<commit_message>
added comaparision between SEQAL and local-pmr
git-svn-id: file://localhost/tmp/svn2git/svn@6572 defb5e50-622e-49ec-a68e-d72c7db87b45
</commit_message>
<xml_diff>
--- a/papers/saga-mr-ngs/data/GS_data.xlsx
+++ b/papers/saga-mr-ngs/data/GS_data.xlsx
@@ -4,14 +4,15 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1460" yWindow="1460" windowWidth="20120" windowHeight="12520" tabRatio="500"/>
+    <workbookView xWindow="30700" yWindow="-2240" windowWidth="26820" windowHeight="12460" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="GS data" sheetId="1" r:id="rId1"/>
     <sheet name="GS data analysis" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId3"/>
+    <externalReference r:id="rId4"/>
   </externalReferences>
   <calcPr calcId="130407" concurrentCalc="0"/>
   <extLst>
@@ -23,7 +24,67 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="128">
+  <si>
+    <t>File Transfer in seconds</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Size of data transferred in MB from Map to reduce phase</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>reduce Output data size in MB</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>duplicate  data size in MB</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Varying Number of chunk size - II</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Varying Number of chunk size - III</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>number of reads</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Number of chunks created</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Time taken to chunk files in seconds</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Map phase Time in seconds - I</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Reduce Phase Time in seconds - I</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Map phase Time in seconds - II</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Reduce Phase Time in seconds-II</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Map phase Time in seconds-III</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>input data</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
   <si>
     <t>mean time taken for map phase</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -33,6 +94,345 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>input 2GB, sequences=3805921, chunksize=128MB, number of reduces=8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sequences per chunk</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Varying Input size - III</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mean chunk time</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>stderr chunk time</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mean map phase</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>stderr in map phase</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mean reduce phase</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>stderr reduce phase</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Varying Input size, chunk size=625000, number  of reduces=8, number of workers=32</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Input data size in GB</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Total Time to solution in  secs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>stderr in chunk time</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Reduce Phase Time in seconds - III</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mean</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>stderr</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mean</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Varying chunk size ,  Input Size = 10GB, Number of workers - 32, Number of reduces -8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>number of reads</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Number of chunks created</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Time taken to chunk files in seconds</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>prq</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2GB</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mean Map phase</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>stderr for map phase</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mean reduce phase</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>stderr for reduce phase</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Mean </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Stdev</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Time to transfer files files between map &amp; reduce phase is </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Data transfer in MB between map &amp; reduce phase is</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Reduced output size  3120 MB  which is 31.2% of input data</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Duplicate output size is 4445MB which is 44.5% of input data</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Remaining is Filedelimiter which I used.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Varying Number of  workers</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Varying Number of  workers - II</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Varying Number of  workers - III</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Number of  subjobs(workers) for both map/reduce phase</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Map phase Time in seconds</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Varying Number of chunk size - I</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>chunk size( lines)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>number of reads</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Input Data size(GB)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Number of chunks created</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Number of  subjobs(workers) for both map/reduce phase</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>number of reduces.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Total Time sec</t>
+  </si>
+  <si>
+    <t>Time taken to chunk files in seconds</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Map phase Time in seconds</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Reduce Phase Time in seconds</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tts</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Input data</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>chunk size</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>map</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>reduce</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tts</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(1+1)2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(2+2)4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(4+4)8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(5+5)10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Map</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Reduce</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>chunks</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>seqal</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Map</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>reduce</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>map</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>intermediate data to be transferred =</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mahine used -sierra</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sequences</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4GB</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>8GB</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Map</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>chunktime</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>chunktime</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>intermediate data</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>comparision.dat</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SEQAL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>local-PMR</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>distributed-PMR</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mean tts</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>std tts</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mean tts</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>stdtts</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>mean time taken for reduce phase</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -130,249 +530,6 @@
   </si>
   <si>
     <t>Varying Input size - II</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Varying Input size - III</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>mean chunk time</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>stderr chunk time</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>mean map phase</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>stderr in map phase</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>mean reduce phase</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>stderr reduce phase</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Varying Input size, chunk size=625000, number  of reduces=8, number of workers=32</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Input data size in GB</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Total Time to solution in  secs</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>stderr in chunk time</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Reduce Phase Time in seconds - III</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Mean</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>stderr</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>mean</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Varying chunk size ,  Input Size = 10GB, Number of workers - 32, Number of reduces -8</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>number of reads</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Number of chunks created</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Time taken to chunk files in seconds</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Mean Map phase</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>stderr for map phase</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>mean reduce phase</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>stderr for reduce phase</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">Mean </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Stdev</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">Time to transfer files files between map &amp; reduce phase is </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Data transfer in MB between map &amp; reduce phase is</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Reduced output size  3120 MB  which is 31.2% of input data</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Duplicate output size is 4445MB which is 44.5% of input data</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Remaining is Filedelimiter which I used.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>+</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Varying Number of  workers</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Varying Number of  workers - II</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Varying Number of  workers - III</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Number of  subjobs(workers) for both map/reduce phase</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Map phase Time in seconds</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Varying Number of chunk size - I</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>chunk size( lines)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>number of reads</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Input Data size(GB)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Number of chunks created</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Number of  subjobs(workers) for both map/reduce phase</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>number of reduces.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Total Time sec</t>
-  </si>
-  <si>
-    <t>Time taken to chunk files in seconds</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Map phase Time in seconds</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Reduce Phase Time in seconds</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>File Transfer in seconds</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Size of data transferred in MB from Map to reduce phase</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>reduce Output data size in MB</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>duplicate  data size in MB</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Varying Number of chunk size - II</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Varying Number of chunk size - III</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>number of reads</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Number of chunks created</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Time taken to chunk files in seconds</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Map phase Time in seconds - I</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Reduce Phase Time in seconds - I</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Map phase Time in seconds - II</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Reduce Phase Time in seconds-II</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Map phase Time in seconds-III</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -530,7 +687,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -614,7 +770,7 @@
             <c:numRef>
               <c:f>'[1]GS Data Analaysis'!$E$5:$E$8</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>2104.295</c:v>
@@ -709,7 +865,7 @@
             <c:numRef>
               <c:f>'[1]GS Data Analaysis'!$G$5:$G$8</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>161.0756666666666</c:v>
@@ -728,11 +884,11 @@
           </c:val>
         </c:ser>
         <c:overlap val="100"/>
-        <c:axId val="499082312"/>
-        <c:axId val="498699992"/>
+        <c:axId val="457805992"/>
+        <c:axId val="74165848"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="499082312"/>
+        <c:axId val="457805992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -753,18 +909,17 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="498699992"/>
+        <c:crossAx val="74165848"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="498699992"/>
+        <c:axId val="74165848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -786,18 +941,16 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
-        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="499082312"/>
+        <c:crossAx val="457805992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -832,7 +985,6 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
             </c:trendlineLbl>
           </c:trendline>
@@ -861,7 +1013,7 @@
             <c:numRef>
               <c:f>'[1]GS Data Analaysis'!$E$5:$E$8</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>2104.295</c:v>
@@ -879,33 +1031,290 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="570139464"/>
-        <c:axId val="570142536"/>
+        <c:axId val="562663864"/>
+        <c:axId val="562666936"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="570139464"/>
+        <c:axId val="562663864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="570142536"/>
+        <c:crossAx val="562666936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="570142536"/>
+        <c:axId val="562666936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:majorGridlines/>
-        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="570139464"/>
+        <c:crossAx val="562663864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="1"/>
+  <c:lang val="en-US"/>
+  <c:style val="17"/>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>SEQAL</c:v>
+          </c:tx>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Sheet1!$N$5:$N$7</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>18.29333333335506</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>114.0978909143999</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>118.9120511601106</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Sheet1!$N$5:$N$7</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>18.29333333335506</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>114.0978909143999</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>118.9120511601106</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+          </c:errBars>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$L$5:$L$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>3.805921E6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.611659E6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.5224713E7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$M$5:$M$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>2862.333333333333</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4903.666666666666</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8736.666666666666</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Local-PMR</c:v>
+          </c:tx>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Sheet1!$Q$12:$Q$14</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>4.097169079209209</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>30.10003705732057</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>10.54038909809311</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Sheet1!$Q$12:$Q$14</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>4.097169079209209</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>30.10003705732057</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>10.54038909809311</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+          </c:errBars>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$L$5:$L$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>3.805921E6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.611659E6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.5224713E7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$P$12:$P$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1544.667</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2909.003666666667</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4941.112333333333</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="562494120"/>
+        <c:axId val="562492616"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="562494120"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Sequences</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="562492616"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="562492616"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>time to solution in seconds</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="562494120"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -944,7 +1353,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -1019,7 +1427,7 @@
             <c:numRef>
               <c:f>'[1]GS Data Analaysis'!$C$51:$C$53</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>3735.89</c:v>
@@ -1102,7 +1510,7 @@
             <c:numRef>
               <c:f>'[1]GS Data Analaysis'!$E$51:$E$53</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>142.433</c:v>
@@ -1118,11 +1526,11 @@
           </c:val>
         </c:ser>
         <c:overlap val="100"/>
-        <c:axId val="499188216"/>
-        <c:axId val="499177208"/>
+        <c:axId val="585720984"/>
+        <c:axId val="562318184"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="499188216"/>
+        <c:axId val="585720984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1143,18 +1551,17 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="499177208"/>
+        <c:crossAx val="562318184"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="499177208"/>
+        <c:axId val="562318184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1176,18 +1583,16 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
-        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="499188216"/>
+        <c:crossAx val="585720984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -1221,7 +1626,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -1296,7 +1700,7 @@
             <c:numRef>
               <c:f>'[1]GS Data Analaysis'!$D$81:$D$83</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>187.717</c:v>
@@ -1379,7 +1783,7 @@
             <c:numRef>
               <c:f>'[1]GS Data Analaysis'!$F$81:$F$83</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>1169.86</c:v>
@@ -1462,7 +1866,7 @@
             <c:numRef>
               <c:f>'[1]GS Data Analaysis'!$H$81:$H$83</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>141.32</c:v>
@@ -1478,11 +1882,11 @@
           </c:val>
         </c:ser>
         <c:overlap val="100"/>
-        <c:axId val="499078760"/>
-        <c:axId val="499070424"/>
+        <c:axId val="562737304"/>
+        <c:axId val="585979016"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="499078760"/>
+        <c:axId val="562737304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1503,18 +1907,17 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="499070424"/>
+        <c:crossAx val="585979016"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="499070424"/>
+        <c:axId val="585979016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1536,18 +1939,16 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
-        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="499078760"/>
+        <c:crossAx val="562737304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -1581,7 +1982,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -1665,7 +2065,7 @@
             <c:numRef>
               <c:f>'[1]GS Data Analaysis'!$E$5:$E$8</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>2104.295</c:v>
@@ -1760,7 +2160,7 @@
             <c:numRef>
               <c:f>'[1]GS Data Analaysis'!$G$5:$G$8</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>161.0756666666666</c:v>
@@ -1779,11 +2179,11 @@
           </c:val>
         </c:ser>
         <c:overlap val="100"/>
-        <c:axId val="497090344"/>
-        <c:axId val="579573240"/>
+        <c:axId val="513759608"/>
+        <c:axId val="512910040"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="497090344"/>
+        <c:axId val="513759608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1804,18 +2204,17 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="579573240"/>
+        <c:crossAx val="512910040"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="579573240"/>
+        <c:axId val="512910040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1837,18 +2236,16 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
-        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="497090344"/>
+        <c:crossAx val="513759608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -1882,7 +2279,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -1957,7 +2353,7 @@
             <c:numRef>
               <c:f>'[1]GS Data Analaysis'!$C$51:$C$53</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>3735.89</c:v>
@@ -2040,7 +2436,7 @@
             <c:numRef>
               <c:f>'[1]GS Data Analaysis'!$E$51:$E$53</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>142.433</c:v>
@@ -2056,11 +2452,11 @@
           </c:val>
         </c:ser>
         <c:overlap val="100"/>
-        <c:axId val="569906440"/>
-        <c:axId val="568437880"/>
+        <c:axId val="562764392"/>
+        <c:axId val="540501144"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="569906440"/>
+        <c:axId val="562764392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2081,18 +2477,17 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="568437880"/>
+        <c:crossAx val="540501144"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="568437880"/>
+        <c:axId val="540501144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2114,18 +2509,16 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
-        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="569906440"/>
+        <c:crossAx val="562764392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -2159,7 +2552,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -2234,7 +2626,7 @@
             <c:numRef>
               <c:f>'[1]GS Data Analaysis'!$D$81:$D$83</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>187.717</c:v>
@@ -2317,7 +2709,7 @@
             <c:numRef>
               <c:f>'[1]GS Data Analaysis'!$F$81:$F$83</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>1169.86</c:v>
@@ -2400,7 +2792,7 @@
             <c:numRef>
               <c:f>'[1]GS Data Analaysis'!$H$81:$H$83</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>141.32</c:v>
@@ -2416,11 +2808,11 @@
           </c:val>
         </c:ser>
         <c:overlap val="100"/>
-        <c:axId val="570972712"/>
-        <c:axId val="571105208"/>
+        <c:axId val="512962536"/>
+        <c:axId val="512968392"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="570972712"/>
+        <c:axId val="512962536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2441,18 +2833,17 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="571105208"/>
+        <c:crossAx val="512968392"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="571105208"/>
+        <c:axId val="512968392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2474,18 +2865,16 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
-        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="570972712"/>
+        <c:crossAx val="512962536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -2519,7 +2908,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout>
@@ -2580,7 +2968,7 @@
             <c:numRef>
               <c:f>'[1]GS Data Analaysis'!$C$5:$C$8</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>2482.182666666667</c:v>
@@ -2599,11 +2987,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="569486808"/>
-        <c:axId val="570986600"/>
+        <c:axId val="512931416"/>
+        <c:axId val="512986568"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="569486808"/>
+        <c:axId val="512931416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2624,16 +3012,15 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="570986600"/>
+        <c:crossAx val="512986568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="570986600"/>
+        <c:axId val="512986568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2655,18 +3042,16 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
-        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="569486808"/>
+        <c:crossAx val="512931416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -2726,7 +3111,7 @@
             <c:numRef>
               <c:f>'[1]GS Data Analaysis'!$B$51:$B$53</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>3890.74</c:v>
@@ -2741,38 +3126,37 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="570093672"/>
-        <c:axId val="570096744"/>
+        <c:axId val="540221112"/>
+        <c:axId val="540224184"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="570093672"/>
+        <c:axId val="540221112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="570096744"/>
+        <c:crossAx val="540224184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="570096744"/>
+        <c:axId val="540224184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:majorGridlines/>
-        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="570093672"/>
+        <c:crossAx val="540221112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -2832,7 +3216,7 @@
             <c:numRef>
               <c:f>'[1]GS Data Analaysis'!$C$81:$C$83</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>1498.897</c:v>
@@ -2847,38 +3231,37 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="570127496"/>
-        <c:axId val="570130568"/>
+        <c:axId val="562637352"/>
+        <c:axId val="562598248"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="570127496"/>
+        <c:axId val="562637352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="570130568"/>
+        <c:crossAx val="562598248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="570130568"/>
+        <c:axId val="562598248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:majorGridlines/>
-        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="570127496"/>
+        <c:crossAx val="562637352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -3192,6 +3575,41 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>203200</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3786,8 +4204,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:Y158"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
-      <selection activeCell="G137" sqref="G137"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A141" sqref="A141:A143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -3800,7 +4218,7 @@
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
       <c r="G1" s="1" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="H1" s="1"/>
       <c r="I1" s="2"/>
@@ -3812,46 +4230,46 @@
     </row>
     <row r="2" spans="1:14" ht="71" thickBot="1">
       <c r="A2" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="I2" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="J2" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="I2" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="J2" s="7" t="s">
-        <v>74</v>
-      </c>
       <c r="K2" s="8" t="s">
-        <v>75</v>
+        <v>0</v>
       </c>
       <c r="L2" s="8" t="s">
-        <v>76</v>
+        <v>1</v>
       </c>
       <c r="M2" s="8" t="s">
-        <v>77</v>
+        <v>2</v>
       </c>
       <c r="N2" s="8" t="s">
-        <v>78</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:14">
@@ -4030,7 +4448,7 @@
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="1" t="s">
-        <v>79</v>
+        <v>4</v>
       </c>
       <c r="H8" s="1"/>
       <c r="I8" s="2"/>
@@ -4042,46 +4460,46 @@
     </row>
     <row r="9" spans="1:14" ht="71" thickBot="1">
       <c r="A9" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="H9" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="I9" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="J9" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="D9" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="I9" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="J9" s="7" t="s">
-        <v>74</v>
-      </c>
       <c r="K9" s="8" t="s">
-        <v>75</v>
+        <v>0</v>
       </c>
       <c r="L9" s="8" t="s">
-        <v>76</v>
+        <v>1</v>
       </c>
       <c r="M9" s="8" t="s">
-        <v>77</v>
+        <v>2</v>
       </c>
       <c r="N9" s="8" t="s">
-        <v>78</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:14">
@@ -4260,7 +4678,7 @@
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
       <c r="G16" s="1" t="s">
-        <v>80</v>
+        <v>5</v>
       </c>
       <c r="H16" s="1"/>
       <c r="I16" s="2"/>
@@ -4272,46 +4690,46 @@
     </row>
     <row r="17" spans="1:19" ht="71" thickBot="1">
       <c r="A17" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="H17" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="I17" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="J17" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="D17" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="G17" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="H17" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="I17" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="J17" s="7" t="s">
-        <v>74</v>
-      </c>
       <c r="K17" s="8" t="s">
-        <v>75</v>
+        <v>0</v>
       </c>
       <c r="L17" s="8" t="s">
-        <v>76</v>
+        <v>1</v>
       </c>
       <c r="M17" s="8" t="s">
-        <v>77</v>
+        <v>2</v>
       </c>
       <c r="N17" s="8" t="s">
-        <v>78</v>
+        <v>3</v>
       </c>
     </row>
     <row r="18" spans="1:19">
@@ -4484,46 +4902,46 @@
     </row>
     <row r="24" spans="1:19" ht="46" thickBot="1">
       <c r="A24" s="3" t="s">
-        <v>81</v>
+        <v>6</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>82</v>
+        <v>7</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>83</v>
+        <v>8</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>84</v>
+        <v>9</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>85</v>
+        <v>10</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>86</v>
+        <v>11</v>
       </c>
       <c r="H24" s="7" t="s">
-        <v>87</v>
+        <v>12</v>
       </c>
       <c r="I24" s="7" t="s">
-        <v>88</v>
+        <v>13</v>
       </c>
       <c r="J24" s="7" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="K24" s="8" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="L24" s="8" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="M24" s="8" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="N24" s="8" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
     </row>
     <row r="25" spans="1:19">
@@ -4720,39 +5138,39 @@
     </row>
     <row r="31" spans="1:19">
       <c r="D31" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
     </row>
     <row r="32" spans="1:19" ht="46" thickBot="1">
       <c r="D32" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="F32" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H32" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="I32" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="J32" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="K32" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="R32" t="s">
         <v>44</v>
       </c>
-      <c r="E32" s="5" t="s">
+      <c r="S32" t="s">
         <v>45</v>
-      </c>
-      <c r="F32" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="G32" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="H32" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="I32" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="J32" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="K32" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="R32" t="s">
-        <v>51</v>
-      </c>
-      <c r="S32" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="33" spans="4:19">
@@ -4782,7 +5200,7 @@
         <v>3.8921515186908202</v>
       </c>
       <c r="M33" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="R33">
         <v>1.59</v>
@@ -4818,7 +5236,7 @@
         <v>1.2000589337377248</v>
       </c>
       <c r="M34" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="R34" s="10">
         <v>9155.6200000000008</v>
@@ -4854,7 +5272,7 @@
         <v>2.2325377438638392</v>
       </c>
       <c r="M35" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
     </row>
     <row r="36" spans="4:19">
@@ -4884,17 +5302,17 @@
         <v>2.6636263501721773</v>
       </c>
       <c r="M36" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
     </row>
     <row r="37" spans="4:19">
       <c r="M37" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
     </row>
     <row r="60" spans="25:25">
       <c r="Y60" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
     </row>
     <row r="65" spans="1:14" ht="15">
@@ -4905,7 +5323,7 @@
       <c r="E65" s="2"/>
       <c r="F65" s="2"/>
       <c r="G65" s="1" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="H65" s="1"/>
       <c r="I65" s="2"/>
@@ -4917,46 +5335,46 @@
     </row>
     <row r="66" spans="1:14" ht="71" thickBot="1">
       <c r="A66" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C66" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D66" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="E66" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F66" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="G66" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="H66" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="B66" s="3" t="s">
+      <c r="I66" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="C66" s="4" t="s">
+      <c r="J66" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="D66" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="E66" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="F66" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="G66" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="H66" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="I66" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="J66" s="7" t="s">
-        <v>74</v>
-      </c>
       <c r="K66" s="8" t="s">
-        <v>75</v>
+        <v>0</v>
       </c>
       <c r="L66" s="8" t="s">
-        <v>76</v>
+        <v>1</v>
       </c>
       <c r="M66" s="8" t="s">
-        <v>77</v>
+        <v>2</v>
       </c>
       <c r="N66" s="8" t="s">
-        <v>78</v>
+        <v>3</v>
       </c>
     </row>
     <row r="67" spans="1:14">
@@ -5093,7 +5511,7 @@
       <c r="E72" s="2"/>
       <c r="F72" s="2"/>
       <c r="G72" s="1" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="H72" s="1"/>
       <c r="I72" s="2"/>
@@ -5105,46 +5523,46 @@
     </row>
     <row r="73" spans="1:14" ht="71" thickBot="1">
       <c r="A73" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B73" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C73" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D73" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="E73" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F73" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="G73" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="H73" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="B73" s="3" t="s">
+      <c r="I73" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="C73" s="4" t="s">
+      <c r="J73" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="D73" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="E73" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="F73" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="G73" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="H73" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="I73" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="J73" s="7" t="s">
-        <v>74</v>
-      </c>
       <c r="K73" s="8" t="s">
-        <v>75</v>
+        <v>0</v>
       </c>
       <c r="L73" s="8" t="s">
-        <v>76</v>
+        <v>1</v>
       </c>
       <c r="M73" s="8" t="s">
-        <v>77</v>
+        <v>2</v>
       </c>
       <c r="N73" s="8" t="s">
-        <v>78</v>
+        <v>3</v>
       </c>
     </row>
     <row r="74" spans="1:14">
@@ -5281,7 +5699,7 @@
       <c r="E79" s="2"/>
       <c r="F79" s="2"/>
       <c r="G79" s="1" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="H79" s="1"/>
       <c r="I79" s="2"/>
@@ -5293,46 +5711,46 @@
     </row>
     <row r="80" spans="1:14" ht="71" thickBot="1">
       <c r="A80" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B80" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C80" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D80" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="E80" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F80" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="G80" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="H80" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="B80" s="3" t="s">
+      <c r="I80" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="C80" s="4" t="s">
+      <c r="J80" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="D80" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="E80" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="F80" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="G80" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="H80" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="I80" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="J80" s="7" t="s">
-        <v>74</v>
-      </c>
       <c r="K80" s="8" t="s">
-        <v>75</v>
+        <v>0</v>
       </c>
       <c r="L80" s="8" t="s">
-        <v>76</v>
+        <v>1</v>
       </c>
       <c r="M80" s="8" t="s">
-        <v>77</v>
+        <v>2</v>
       </c>
       <c r="N80" s="8" t="s">
-        <v>78</v>
+        <v>3</v>
       </c>
     </row>
     <row r="81" spans="1:12">
@@ -5454,40 +5872,40 @@
     </row>
     <row r="87" spans="1:12" ht="71" thickBot="1">
       <c r="A87" s="3" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="B87" s="6" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="C87" s="7" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="D87" s="7" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="E87" s="7" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="F87" s="8" t="s">
-        <v>8</v>
+        <v>108</v>
       </c>
       <c r="G87" s="8" t="s">
-        <v>9</v>
+        <v>109</v>
       </c>
       <c r="H87" s="7" t="s">
-        <v>10</v>
+        <v>110</v>
       </c>
       <c r="I87" s="7" t="s">
-        <v>10</v>
+        <v>110</v>
       </c>
       <c r="J87" s="7" t="s">
-        <v>10</v>
+        <v>110</v>
       </c>
       <c r="K87" s="8" t="s">
-        <v>11</v>
+        <v>111</v>
       </c>
       <c r="L87" s="8" t="s">
-        <v>12</v>
+        <v>112</v>
       </c>
     </row>
     <row r="88" spans="1:12">
@@ -5621,27 +6039,27 @@
     </row>
     <row r="94" spans="1:12">
       <c r="A94" t="s">
-        <v>13</v>
+        <v>113</v>
       </c>
     </row>
     <row r="96" spans="1:12" ht="33" thickBot="1">
       <c r="A96" s="3" t="s">
-        <v>14</v>
+        <v>114</v>
       </c>
       <c r="B96" s="5" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="C96" s="6" t="s">
-        <v>15</v>
+        <v>115</v>
       </c>
       <c r="D96" s="3" t="s">
-        <v>16</v>
+        <v>116</v>
       </c>
       <c r="E96" s="3" t="s">
-        <v>17</v>
+        <v>117</v>
       </c>
       <c r="F96" s="5" t="s">
-        <v>18</v>
+        <v>118</v>
       </c>
       <c r="G96" s="11"/>
     </row>
@@ -5707,7 +6125,7 @@
     </row>
     <row r="100" spans="1:22">
       <c r="V100" t="s">
-        <v>19</v>
+        <v>119</v>
       </c>
     </row>
     <row r="101" spans="1:22">
@@ -5717,27 +6135,27 @@
     </row>
     <row r="105" spans="1:22">
       <c r="I105" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
     </row>
     <row r="106" spans="1:22">
       <c r="I106" t="s">
-        <v>20</v>
+        <v>120</v>
       </c>
     </row>
     <row r="107" spans="1:22">
       <c r="I107" t="s">
-        <v>21</v>
+        <v>121</v>
       </c>
     </row>
     <row r="108" spans="1:22">
       <c r="I108" t="s">
-        <v>22</v>
+        <v>122</v>
       </c>
     </row>
     <row r="109" spans="1:22">
       <c r="I109" t="s">
-        <v>23</v>
+        <v>123</v>
       </c>
     </row>
     <row r="120" spans="1:17" ht="15">
@@ -5748,7 +6166,7 @@
       <c r="E120" s="2"/>
       <c r="F120" s="2"/>
       <c r="G120" s="1" t="s">
-        <v>24</v>
+        <v>124</v>
       </c>
       <c r="H120" s="1"/>
       <c r="I120" s="2"/>
@@ -5760,46 +6178,46 @@
     </row>
     <row r="121" spans="1:17" ht="71" thickBot="1">
       <c r="A121" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B121" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C121" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="D121" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="E121" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F121" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="G121" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="H121" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="B121" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="C121" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D121" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="E121" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="F121" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="G121" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="H121" s="3" t="s">
-        <v>72</v>
-      </c>
       <c r="I121" s="7" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="J121" s="7" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="K121" s="8" t="s">
-        <v>75</v>
+        <v>0</v>
       </c>
       <c r="L121" s="8" t="s">
-        <v>76</v>
+        <v>1</v>
       </c>
       <c r="M121" s="8" t="s">
-        <v>77</v>
+        <v>2</v>
       </c>
       <c r="N121" s="8" t="s">
-        <v>26</v>
+        <v>126</v>
       </c>
     </row>
     <row r="122" spans="1:17">
@@ -5965,7 +6383,7 @@
       <c r="E129" s="2"/>
       <c r="F129" s="2"/>
       <c r="G129" s="1" t="s">
-        <v>27</v>
+        <v>127</v>
       </c>
       <c r="H129" s="1"/>
       <c r="I129" s="2"/>
@@ -5977,46 +6395,46 @@
     </row>
     <row r="130" spans="1:14" ht="71" thickBot="1">
       <c r="A130" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B130" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C130" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D130" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="E130" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F130" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="G130" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="H130" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="B130" s="3" t="s">
+      <c r="I130" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="C130" s="4" t="s">
+      <c r="J130" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="D130" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="E130" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="F130" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="G130" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="H130" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="I130" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="J130" s="7" t="s">
-        <v>74</v>
-      </c>
       <c r="K130" s="8" t="s">
-        <v>75</v>
+        <v>0</v>
       </c>
       <c r="L130" s="8" t="s">
-        <v>76</v>
+        <v>1</v>
       </c>
       <c r="M130" s="8" t="s">
-        <v>77</v>
+        <v>2</v>
       </c>
       <c r="N130" s="8" t="s">
-        <v>78</v>
+        <v>3</v>
       </c>
     </row>
     <row r="131" spans="1:14">
@@ -6156,7 +6574,7 @@
       <c r="E139" s="2"/>
       <c r="F139" s="2"/>
       <c r="G139" s="1" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="H139" s="1"/>
       <c r="I139" s="2"/>
@@ -6168,46 +6586,46 @@
     </row>
     <row r="140" spans="1:14" ht="71" thickBot="1">
       <c r="A140" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B140" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C140" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D140" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="E140" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F140" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="G140" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="H140" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="B140" s="3" t="s">
+      <c r="I140" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="C140" s="4" t="s">
+      <c r="J140" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="D140" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="E140" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="F140" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="G140" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="H140" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="I140" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="J140" s="7" t="s">
-        <v>74</v>
-      </c>
       <c r="K140" s="8" t="s">
-        <v>75</v>
+        <v>0</v>
       </c>
       <c r="L140" s="8" t="s">
-        <v>76</v>
+        <v>1</v>
       </c>
       <c r="M140" s="8" t="s">
-        <v>77</v>
+        <v>2</v>
       </c>
       <c r="N140" s="8" t="s">
-        <v>26</v>
+        <v>126</v>
       </c>
     </row>
     <row r="141" spans="1:14">
@@ -6341,55 +6759,55 @@
     </row>
     <row r="147" spans="1:17" ht="43" thickBot="1">
       <c r="A147" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B147" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C147" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D147" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E147" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="F147" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G147" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H147" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="I147" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="J147" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="K147" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="L147" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="M147" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="B147" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="C147" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="D147" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="E147" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="F147" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="G147" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="H147" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="I147" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="J147" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="K147" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="L147" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="M147" s="7" t="s">
-        <v>74</v>
-      </c>
       <c r="N147" s="7" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="O147" s="7" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="P147" s="8" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="Q147" s="8" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
     </row>
     <row r="148" spans="1:17">
@@ -6553,36 +6971,36 @@
     </row>
     <row r="153" spans="1:17">
       <c r="C153" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
     </row>
     <row r="155" spans="1:17" ht="49" thickBot="1">
       <c r="C155" s="3" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="D155" s="5" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="E155" s="6" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="F155" s="3" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="G155" s="3" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="H155" s="8" t="s">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="I155" s="8" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="J155" s="8" t="s">
-        <v>2</v>
+        <v>102</v>
       </c>
       <c r="K155" s="8" t="s">
-        <v>3</v>
+        <v>103</v>
       </c>
     </row>
     <row r="156" spans="1:17">
@@ -6676,10 +7094,8 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
@@ -6693,41 +7109,41 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A3:I83"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <sheetData>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>104</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="46" thickBot="1">
       <c r="A4" s="3" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>5</v>
+        <v>105</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -6840,15 +7256,15 @@
     </row>
     <row r="31" spans="2:8">
       <c r="G31" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="H31" t="s">
-        <v>6</v>
+        <v>106</v>
       </c>
     </row>
     <row r="32" spans="2:8">
       <c r="B32" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="G32">
         <v>1.59</v>
@@ -6859,7 +7275,7 @@
     </row>
     <row r="33" spans="1:8" ht="15">
       <c r="B33" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="G33" s="10">
         <v>9155.6200000000008</v>
@@ -6870,42 +7286,42 @@
     </row>
     <row r="34" spans="1:8">
       <c r="B34" t="s">
-        <v>7</v>
+        <v>107</v>
       </c>
     </row>
     <row r="35" spans="1:8">
       <c r="B35" t="s">
-        <v>22</v>
+        <v>122</v>
       </c>
     </row>
     <row r="36" spans="1:8">
       <c r="B36" t="s">
-        <v>23</v>
+        <v>123</v>
       </c>
     </row>
     <row r="48" spans="1:8">
       <c r="A48" t="s">
-        <v>13</v>
+        <v>113</v>
       </c>
     </row>
     <row r="50" spans="1:7" ht="33" thickBot="1">
       <c r="A50" s="3" t="s">
-        <v>14</v>
+        <v>114</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="C50" s="6" t="s">
-        <v>15</v>
+        <v>115</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>16</v>
+        <v>116</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>17</v>
+        <v>117</v>
       </c>
       <c r="F50" s="5" t="s">
-        <v>18</v>
+        <v>118</v>
       </c>
       <c r="G50" s="11"/>
     </row>
@@ -6971,15 +7387,15 @@
     </row>
     <row r="64" spans="1:7">
       <c r="B64" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="G64" t="s">
-        <v>19</v>
+        <v>119</v>
       </c>
     </row>
     <row r="65" spans="1:9" ht="15">
       <c r="B65" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="G65">
         <v>9144.5290000000005</v>
@@ -6988,51 +7404,51 @@
     </row>
     <row r="66" spans="1:9">
       <c r="B66" t="s">
-        <v>7</v>
+        <v>107</v>
       </c>
     </row>
     <row r="67" spans="1:9">
       <c r="B67" t="s">
-        <v>22</v>
+        <v>122</v>
       </c>
     </row>
     <row r="68" spans="1:9">
       <c r="B68" t="s">
-        <v>23</v>
+        <v>123</v>
       </c>
     </row>
     <row r="78" spans="1:9">
       <c r="A78" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
     </row>
     <row r="80" spans="1:9" ht="49" thickBot="1">
       <c r="A80" s="3" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="B80" s="5" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="C80" s="6" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="E80" s="3" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="F80" s="8" t="s">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="G80" s="8" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="H80" s="8" t="s">
-        <v>2</v>
+        <v>102</v>
       </c>
       <c r="I80" s="8" t="s">
-        <v>3</v>
+        <v>103</v>
       </c>
     </row>
     <row r="81" spans="1:9">
@@ -7129,7 +7545,615 @@
   <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+  <dimension ref="A2:Q79"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O6" sqref="O6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <sheetData>
+    <row r="2" spans="1:17">
+      <c r="A2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C4" t="s">
+        <v>78</v>
+      </c>
+      <c r="D4" t="s">
+        <v>79</v>
+      </c>
+      <c r="E4" t="s">
+        <v>73</v>
+      </c>
+      <c r="F4" t="s">
+        <v>82</v>
+      </c>
+      <c r="G4" t="s">
+        <v>83</v>
+      </c>
+      <c r="H4" t="s">
+        <v>68</v>
+      </c>
+      <c r="I4" t="s">
+        <v>84</v>
+      </c>
+      <c r="J4" t="s">
+        <v>72</v>
+      </c>
+      <c r="K4" t="s">
+        <v>68</v>
+      </c>
+      <c r="L4" t="s">
+        <v>87</v>
+      </c>
+      <c r="M4" t="s">
+        <v>98</v>
+      </c>
+      <c r="N4" t="s">
+        <v>99</v>
+      </c>
+      <c r="O4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>13</v>
+      </c>
+      <c r="C5">
+        <v>2427</v>
+      </c>
+      <c r="D5">
+        <v>426</v>
+      </c>
+      <c r="E5">
+        <f>C5+D5</f>
+        <v>2853</v>
+      </c>
+      <c r="F5">
+        <v>2438</v>
+      </c>
+      <c r="G5">
+        <v>443</v>
+      </c>
+      <c r="H5">
+        <f>F5+G5</f>
+        <v>2881</v>
+      </c>
+      <c r="I5">
+        <v>2422</v>
+      </c>
+      <c r="J5">
+        <v>431</v>
+      </c>
+      <c r="K5">
+        <f>I5+J5</f>
+        <v>2853</v>
+      </c>
+      <c r="L5">
+        <v>3805921</v>
+      </c>
+      <c r="M5">
+        <f>AVERAGE(E5,H5,K5)</f>
+        <v>2862.3333333333335</v>
+      </c>
+      <c r="N5">
+        <f>1.96 * STDEV(E5,H5,K5)/SQRT(3)</f>
+        <v>18.293333333355065</v>
+      </c>
+      <c r="O5">
+        <f>L5/13</f>
+        <v>292763.15384615387</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>25</v>
+      </c>
+      <c r="C6">
+        <v>4192</v>
+      </c>
+      <c r="D6">
+        <v>824</v>
+      </c>
+      <c r="E6">
+        <f>C6+D6</f>
+        <v>5016</v>
+      </c>
+      <c r="F6">
+        <v>4006</v>
+      </c>
+      <c r="G6">
+        <v>815</v>
+      </c>
+      <c r="H6">
+        <f>F6+G6</f>
+        <v>4821</v>
+      </c>
+      <c r="I6">
+        <v>4053</v>
+      </c>
+      <c r="J6">
+        <v>821</v>
+      </c>
+      <c r="K6">
+        <f>J6+I6</f>
+        <v>4874</v>
+      </c>
+      <c r="L6">
+        <v>7611659</v>
+      </c>
+      <c r="M6">
+        <f t="shared" ref="M6:M7" si="0">AVERAGE(E6,H6,K6)</f>
+        <v>4903.666666666667</v>
+      </c>
+      <c r="N6">
+        <f t="shared" ref="N6:N7" si="1">1.96 * STDEV(E6,H6,K6)/SQRT(3)</f>
+        <v>114.09789091439987</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17">
+      <c r="A7">
+        <v>8</v>
+      </c>
+      <c r="B7">
+        <v>50</v>
+      </c>
+      <c r="C7">
+        <v>7163</v>
+      </c>
+      <c r="D7">
+        <v>1695</v>
+      </c>
+      <c r="E7">
+        <f>C7+D7</f>
+        <v>8858</v>
+      </c>
+      <c r="F7">
+        <v>7015</v>
+      </c>
+      <c r="G7">
+        <v>1660</v>
+      </c>
+      <c r="H7">
+        <f>F7+G7</f>
+        <v>8675</v>
+      </c>
+      <c r="I7">
+        <v>7020</v>
+      </c>
+      <c r="J7">
+        <v>1657</v>
+      </c>
+      <c r="K7">
+        <f>I7+J7</f>
+        <v>8677</v>
+      </c>
+      <c r="L7">
+        <v>15224713</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="0"/>
+        <v>8736.6666666666661</v>
+      </c>
+      <c r="N7">
+        <f t="shared" si="1"/>
+        <v>118.91205116011055</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" t="s">
+        <v>91</v>
+      </c>
+      <c r="C11" t="s">
+        <v>90</v>
+      </c>
+      <c r="D11" t="s">
+        <v>79</v>
+      </c>
+      <c r="E11" t="s">
+        <v>68</v>
+      </c>
+      <c r="F11" t="s">
+        <v>91</v>
+      </c>
+      <c r="G11" t="s">
+        <v>90</v>
+      </c>
+      <c r="H11" t="s">
+        <v>79</v>
+      </c>
+      <c r="I11" t="s">
+        <v>68</v>
+      </c>
+      <c r="J11" t="s">
+        <v>92</v>
+      </c>
+      <c r="K11" t="s">
+        <v>90</v>
+      </c>
+      <c r="L11" t="s">
+        <v>79</v>
+      </c>
+      <c r="M11" t="s">
+        <v>68</v>
+      </c>
+      <c r="N11" t="s">
+        <v>93</v>
+      </c>
+      <c r="P11" t="s">
+        <v>100</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17">
+      <c r="A12">
+        <v>2</v>
+      </c>
+      <c r="B12">
+        <v>24.536999999999999</v>
+      </c>
+      <c r="C12">
+        <v>1480.663</v>
+      </c>
+      <c r="D12">
+        <v>40.225999999999999</v>
+      </c>
+      <c r="E12">
+        <v>1545.4259999999999</v>
+      </c>
+      <c r="F12">
+        <v>24.632000000000001</v>
+      </c>
+      <c r="G12">
+        <v>1475.8620000000001</v>
+      </c>
+      <c r="H12">
+        <v>40.232999999999997</v>
+      </c>
+      <c r="I12">
+        <v>1540.7270000000001</v>
+      </c>
+      <c r="J12">
+        <v>23.358000000000001</v>
+      </c>
+      <c r="K12">
+        <v>1483.2449999999999</v>
+      </c>
+      <c r="L12">
+        <v>41.244999999999997</v>
+      </c>
+      <c r="M12">
+        <f>K12+L12+J12</f>
+        <v>1547.8479999999997</v>
+      </c>
+      <c r="N12">
+        <v>1736.0070000000001</v>
+      </c>
+      <c r="P12">
+        <f>AVERAGE(E12+I12+M12)/3</f>
+        <v>1544.6670000000001</v>
+      </c>
+      <c r="Q12">
+        <f>1.96 * STDEV(E12,I12,M12)/SQRT(3)</f>
+        <v>4.097169079209209</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17">
+      <c r="A13">
+        <v>4</v>
+      </c>
+      <c r="B13">
+        <v>48.817999999999998</v>
+      </c>
+      <c r="C13">
+        <v>2767.5140000000001</v>
+      </c>
+      <c r="D13">
+        <v>71.721000000000004</v>
+      </c>
+      <c r="E13">
+        <v>2888.0540000000001</v>
+      </c>
+      <c r="F13">
+        <v>49.430999999999997</v>
+      </c>
+      <c r="G13">
+        <v>2776.223</v>
+      </c>
+      <c r="H13">
+        <v>74.373000000000005</v>
+      </c>
+      <c r="I13">
+        <v>2900.027</v>
+      </c>
+      <c r="J13">
+        <v>49.23</v>
+      </c>
+      <c r="K13">
+        <v>2812.97</v>
+      </c>
+      <c r="L13">
+        <v>76.73</v>
+      </c>
+      <c r="M13">
+        <v>2938.93</v>
+      </c>
+      <c r="N13">
+        <v>3580.5070000000001</v>
+      </c>
+      <c r="P13">
+        <f t="shared" ref="P13:P14" si="2">AVERAGE(E13+I13+M13)/3</f>
+        <v>2909.003666666667</v>
+      </c>
+      <c r="Q13">
+        <f t="shared" ref="Q13:Q14" si="3">1.96 * STDEV(E13,I13,M13)/SQRT(3)</f>
+        <v>30.100037057320566</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17">
+      <c r="A14">
+        <v>8</v>
+      </c>
+      <c r="B14">
+        <v>98.637</v>
+      </c>
+      <c r="C14">
+        <v>4699.8230000000003</v>
+      </c>
+      <c r="D14">
+        <v>142.68100000000001</v>
+      </c>
+      <c r="E14">
+        <v>4941.1419999999998</v>
+      </c>
+      <c r="F14">
+        <v>99.403999999999996</v>
+      </c>
+      <c r="G14">
+        <v>4709.2629999999999</v>
+      </c>
+      <c r="H14">
+        <v>144.85300000000001</v>
+      </c>
+      <c r="I14">
+        <v>4950.4120000000003</v>
+      </c>
+      <c r="J14">
+        <v>94.57</v>
+      </c>
+      <c r="K14">
+        <v>4689.28</v>
+      </c>
+      <c r="L14">
+        <v>141.83500000000001</v>
+      </c>
+      <c r="M14">
+        <v>4931.7830000000004</v>
+      </c>
+      <c r="N14">
+        <v>7332.8770000000004</v>
+      </c>
+      <c r="P14">
+        <f t="shared" si="2"/>
+        <v>4941.1123333333335</v>
+      </c>
+      <c r="Q14">
+        <f t="shared" si="3"/>
+        <v>10.540389098093113</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12">
+      <c r="D50">
+        <v>1087592</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12">
+      <c r="A53" t="s">
+        <v>69</v>
+      </c>
+      <c r="B53" t="s">
+        <v>70</v>
+      </c>
+      <c r="C53" t="s">
+        <v>71</v>
+      </c>
+      <c r="D53" t="s">
+        <v>72</v>
+      </c>
+      <c r="E53" t="s">
+        <v>73</v>
+      </c>
+      <c r="F53" t="s">
+        <v>71</v>
+      </c>
+      <c r="G53" t="s">
+        <v>72</v>
+      </c>
+      <c r="H53" t="s">
+        <v>68</v>
+      </c>
+      <c r="I53" t="s">
+        <v>71</v>
+      </c>
+      <c r="J53" t="s">
+        <v>72</v>
+      </c>
+      <c r="K53" t="s">
+        <v>68</v>
+      </c>
+      <c r="L53" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12">
+      <c r="A54" t="s">
+        <v>74</v>
+      </c>
+      <c r="B54">
+        <v>1171052</v>
+      </c>
+      <c r="C54">
+        <v>554.67499999999995</v>
+      </c>
+      <c r="D54">
+        <v>11.500999999999999</v>
+      </c>
+      <c r="E54">
+        <v>569.14499999999998</v>
+      </c>
+      <c r="F54">
+        <v>604.90899999999999</v>
+      </c>
+      <c r="G54">
+        <v>7.5179999999999998</v>
+      </c>
+      <c r="H54">
+        <v>615.88599999999997</v>
+      </c>
+      <c r="I54">
+        <v>11.34</v>
+      </c>
+      <c r="J54">
+        <v>588.29200000000003</v>
+      </c>
+      <c r="K54">
+        <v>603.06100000000004</v>
+      </c>
+      <c r="L54">
+        <f>849.742/2</f>
+        <v>424.87099999999998</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12">
+      <c r="A55" t="s">
+        <v>75</v>
+      </c>
+      <c r="B55">
+        <v>1171052</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12">
+      <c r="A56" t="s">
+        <v>76</v>
+      </c>
+      <c r="B56">
+        <v>1171052</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12">
+      <c r="A57" t="s">
+        <v>77</v>
+      </c>
+      <c r="B57">
+        <v>1171052</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12">
+      <c r="A63" t="s">
+        <v>38</v>
+      </c>
+      <c r="B63" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12">
+      <c r="A64" t="s">
+        <v>39</v>
+      </c>
+      <c r="B64">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5">
+      <c r="A65" t="s">
+        <v>88</v>
+      </c>
+      <c r="B65">
+        <f>19*60</f>
+        <v>1140</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5">
+      <c r="A66" t="s">
+        <v>89</v>
+      </c>
+      <c r="B66">
+        <v>2611</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5">
+      <c r="C75" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5">
+      <c r="C76" t="s">
+        <v>95</v>
+      </c>
+      <c r="D76" t="s">
+        <v>96</v>
+      </c>
+      <c r="E76" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5">
+      <c r="B77">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5">
+      <c r="B78">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5">
+      <c r="B79">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">

</xml_diff>

<commit_message>
added rough analysis for performance comparision
git-svn-id: file://localhost/tmp/svn2git/svn@6574 defb5e50-622e-49ec-a68e-d72c7db87b45
</commit_message>
<xml_diff>
--- a/papers/saga-mr-ngs/data/GS_data.xlsx
+++ b/papers/saga-mr-ngs/data/GS_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="30700" yWindow="-2240" windowWidth="26820" windowHeight="12460" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="-940" yWindow="120" windowWidth="26820" windowHeight="12460" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="GS data" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,334 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="131">
+  <si>
+    <t>stderr of map phase</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Reduce Phase Time in seconds</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mean reduce phase</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>stderr of reduce phase</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Varying number of workers, input size = 10 GB, reduces = 8, Number of reads/ chunk=625000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Workers</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mean map phase</t>
+  </si>
+  <si>
+    <t>stderr of map phase</t>
+  </si>
+  <si>
+    <t>mean reduce phase</t>
+  </si>
+  <si>
+    <t>stderr of reduce phase</t>
+  </si>
+  <si>
+    <t>&lt; 1sec</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Data transfer in MB between map &amp; reduce phase is</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Reduced output size  3120 MB  which is 31.2% of input data</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Duplicate output size is 4445MB which is 44.5% of input data</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Remaining is Filedelimiter which I used.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Varying Input size - I</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Input Data size(GB)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>duplicate  data size in GB</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Varying Input size - II</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>at 2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>at 4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>at 8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Reduced output size  3120 MB  which is 31.2% of input data</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Duplicate output size is 4445MB which is 44.5% of input data</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Remaining is Filedelimiter which I used.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Varying Number of  workers</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Varying Number of  workers - II</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Varying Number of  workers - III</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Number of  subjobs(workers) for both map/reduce phase</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Map phase Time in seconds</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Varying Number of chunk size - I</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>chunk size( lines)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>number of reads</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Input Data size(GB)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Number of chunks created</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Number of  subjobs(workers) for both map/reduce phase</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>number of reduces.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Total Time sec</t>
+  </si>
+  <si>
+    <t>Time taken to chunk files in seconds</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Map phase Time in seconds</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Reduce Phase Time in seconds</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tts</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Input data</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>chunk size</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>map</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>reduce</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tts</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(1+1)2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(2+2)4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(4+4)8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(5+5)10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Map</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Reduce</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>chunks</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>seqal</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Map</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>reduce</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>map</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>intermediate data to be transferred =</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mahine used -sierra</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sequences</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4GB</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>8GB</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Map</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>chunktime</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>chunktime</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>intermediate data</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>comparision.dat</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SEQAL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>local-PMR</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>distributed-PMR</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mean tts</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>std tts</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mean tts</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>stdtts</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mean time taken for reduce phase</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>stderr for reduce phase phase time</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Varying chunk size ,  Input Size = 10GB, Number of workers - 32, Number of reduces -8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mean Map phase</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Stdev</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Reduced output size  3120 MB  which is 31.2% of input data</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mean map phase</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
   <si>
     <t>File Transfer in seconds</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -215,321 +542,6 @@
   </si>
   <si>
     <t>Data transfer in MB between map &amp; reduce phase is</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Reduced output size  3120 MB  which is 31.2% of input data</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Duplicate output size is 4445MB which is 44.5% of input data</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Remaining is Filedelimiter which I used.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>+</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Varying Number of  workers</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Varying Number of  workers - II</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Varying Number of  workers - III</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Number of  subjobs(workers) for both map/reduce phase</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Map phase Time in seconds</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Varying Number of chunk size - I</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>chunk size( lines)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>number of reads</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Input Data size(GB)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Number of chunks created</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Number of  subjobs(workers) for both map/reduce phase</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>number of reduces.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Total Time sec</t>
-  </si>
-  <si>
-    <t>Time taken to chunk files in seconds</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Map phase Time in seconds</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Reduce Phase Time in seconds</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>tts</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Input data</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>chunk size</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>map</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>reduce</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>tts</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>(1+1)2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>(2+2)4</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>(4+4)8</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>(5+5)10</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Map</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Reduce</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>chunks</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>seqal</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Map</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>reduce</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>map</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>intermediate data to be transferred =</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>mahine used -sierra</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>sequences</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>4GB</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>8GB</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Map</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>chunktime</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>chunktime</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>intermediate data</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>comparision.dat</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SEQAL</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>local-PMR</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>distributed-PMR</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Mean tts</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>std tts</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>mean tts</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>stdtts</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>mean time taken for reduce phase</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>stderr for reduce phase phase time</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Varying chunk size ,  Input Size = 10GB, Number of workers - 32, Number of reduces -8</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Mean Map phase</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Stdev</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Reduced output size  3120 MB  which is 31.2% of input data</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>mean map phase</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>stderr of map phase</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Reduce Phase Time in seconds</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>mean reduce phase</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>stderr of reduce phase</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Varying number of workers, input size = 10 GB, reduces = 8, Number of reads/ chunk=625000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Workers</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>mean map phase</t>
-  </si>
-  <si>
-    <t>stderr of map phase</t>
-  </si>
-  <si>
-    <t>mean reduce phase</t>
-  </si>
-  <si>
-    <t>stderr of reduce phase</t>
-  </si>
-  <si>
-    <t>&lt; 1sec</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Data transfer in MB between map &amp; reduce phase is</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Reduced output size  3120 MB  which is 31.2% of input data</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Duplicate output size is 4445MB which is 44.5% of input data</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Remaining is Filedelimiter which I used.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Varying Input size - I</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Input Data size(GB)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>duplicate  data size in GB</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Varying Input size - II</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -884,11 +896,11 @@
           </c:val>
         </c:ser>
         <c:overlap val="100"/>
-        <c:axId val="457805992"/>
-        <c:axId val="74165848"/>
+        <c:axId val="536002008"/>
+        <c:axId val="535972216"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="457805992"/>
+        <c:axId val="536002008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -912,14 +924,14 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="74165848"/>
+        <c:crossAx val="535972216"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="74165848"/>
+        <c:axId val="535972216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -944,7 +956,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="457805992"/>
+        <c:crossAx val="536002008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1031,23 +1043,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="562663864"/>
-        <c:axId val="562666936"/>
+        <c:axId val="555140024"/>
+        <c:axId val="555143000"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="562663864"/>
+        <c:axId val="555140024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="562666936"/>
+        <c:crossAx val="555143000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="562666936"/>
+        <c:axId val="555143000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1055,7 +1067,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="562663864"/>
+        <c:crossAx val="555140024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1251,11 +1263,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="562494120"/>
-        <c:axId val="562492616"/>
+        <c:axId val="555195480"/>
+        <c:axId val="555202664"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="562494120"/>
+        <c:axId val="555195480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1280,14 +1292,14 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="562492616"/>
+        <c:crossAx val="555202664"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="562492616"/>
+        <c:axId val="555202664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1312,7 +1324,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="562494120"/>
+        <c:crossAx val="555195480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1526,11 +1538,11 @@
           </c:val>
         </c:ser>
         <c:overlap val="100"/>
-        <c:axId val="585720984"/>
-        <c:axId val="562318184"/>
+        <c:axId val="535899944"/>
+        <c:axId val="535894072"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="585720984"/>
+        <c:axId val="535899944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1554,14 +1566,14 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="562318184"/>
+        <c:crossAx val="535894072"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="562318184"/>
+        <c:axId val="535894072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1586,7 +1598,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="585720984"/>
+        <c:crossAx val="535899944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1882,11 +1894,11 @@
           </c:val>
         </c:ser>
         <c:overlap val="100"/>
-        <c:axId val="562737304"/>
-        <c:axId val="585979016"/>
+        <c:axId val="535852936"/>
+        <c:axId val="535844264"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="562737304"/>
+        <c:axId val="535852936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1910,14 +1922,14 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="585979016"/>
+        <c:crossAx val="535844264"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="585979016"/>
+        <c:axId val="535844264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1942,7 +1954,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="562737304"/>
+        <c:crossAx val="535852936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2179,11 +2191,11 @@
           </c:val>
         </c:ser>
         <c:overlap val="100"/>
-        <c:axId val="513759608"/>
-        <c:axId val="512910040"/>
+        <c:axId val="554900808"/>
+        <c:axId val="554909112"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="513759608"/>
+        <c:axId val="554900808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2207,14 +2219,14 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="512910040"/>
+        <c:crossAx val="554909112"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="512910040"/>
+        <c:axId val="554909112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2239,7 +2251,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="513759608"/>
+        <c:crossAx val="554900808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2452,11 +2464,11 @@
           </c:val>
         </c:ser>
         <c:overlap val="100"/>
-        <c:axId val="562764392"/>
-        <c:axId val="540501144"/>
+        <c:axId val="554945624"/>
+        <c:axId val="554953880"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="562764392"/>
+        <c:axId val="554945624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2480,14 +2492,14 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="540501144"/>
+        <c:crossAx val="554953880"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="540501144"/>
+        <c:axId val="554953880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2512,7 +2524,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="562764392"/>
+        <c:crossAx val="554945624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2808,11 +2820,11 @@
           </c:val>
         </c:ser>
         <c:overlap val="100"/>
-        <c:axId val="512962536"/>
-        <c:axId val="512968392"/>
+        <c:axId val="554999048"/>
+        <c:axId val="555004920"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="512962536"/>
+        <c:axId val="554999048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2836,14 +2848,14 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="512968392"/>
+        <c:crossAx val="555004920"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="512968392"/>
+        <c:axId val="555004920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2868,7 +2880,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="512962536"/>
+        <c:crossAx val="554999048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2987,11 +2999,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="512931416"/>
-        <c:axId val="512986568"/>
+        <c:axId val="555034584"/>
+        <c:axId val="555043400"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="512931416"/>
+        <c:axId val="555034584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3015,12 +3027,12 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="512986568"/>
+        <c:crossAx val="555043400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="512986568"/>
+        <c:axId val="555043400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3045,7 +3057,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="512931416"/>
+        <c:crossAx val="555034584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3126,23 +3138,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="540221112"/>
-        <c:axId val="540224184"/>
+        <c:axId val="555079448"/>
+        <c:axId val="555082424"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="540221112"/>
+        <c:axId val="555079448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="540224184"/>
+        <c:crossAx val="555082424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="540224184"/>
+        <c:axId val="555082424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3150,7 +3162,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="540221112"/>
+        <c:crossAx val="555079448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3231,23 +3243,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="562637352"/>
-        <c:axId val="562598248"/>
+        <c:axId val="555109672"/>
+        <c:axId val="555112648"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="562637352"/>
+        <c:axId val="555109672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="562598248"/>
+        <c:crossAx val="555112648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="562598248"/>
+        <c:axId val="555112648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3255,7 +3267,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="562637352"/>
+        <c:crossAx val="555109672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4218,7 +4230,7 @@
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
       <c r="G1" s="1" t="s">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="H1" s="1"/>
       <c r="I1" s="2"/>
@@ -4230,46 +4242,46 @@
     </row>
     <row r="2" spans="1:14" ht="71" thickBot="1">
       <c r="A2" s="3" t="s">
-        <v>58</v>
+        <v>32</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>59</v>
+        <v>33</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>60</v>
+        <v>34</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>61</v>
+        <v>35</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>62</v>
+        <v>36</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>63</v>
+        <v>37</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>64</v>
+        <v>38</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>65</v>
+        <v>39</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>66</v>
+        <v>40</v>
       </c>
       <c r="J2" s="7" t="s">
-        <v>67</v>
+        <v>41</v>
       </c>
       <c r="K2" s="8" t="s">
-        <v>0</v>
+        <v>83</v>
       </c>
       <c r="L2" s="8" t="s">
-        <v>1</v>
+        <v>84</v>
       </c>
       <c r="M2" s="8" t="s">
-        <v>2</v>
+        <v>85</v>
       </c>
       <c r="N2" s="8" t="s">
-        <v>3</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:14">
@@ -4448,7 +4460,7 @@
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="1" t="s">
-        <v>4</v>
+        <v>87</v>
       </c>
       <c r="H8" s="1"/>
       <c r="I8" s="2"/>
@@ -4460,46 +4472,46 @@
     </row>
     <row r="9" spans="1:14" ht="71" thickBot="1">
       <c r="A9" s="3" t="s">
-        <v>58</v>
+        <v>32</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>59</v>
+        <v>33</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>60</v>
+        <v>34</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>61</v>
+        <v>35</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>62</v>
+        <v>36</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>63</v>
+        <v>37</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>64</v>
+        <v>38</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>65</v>
+        <v>39</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>66</v>
+        <v>40</v>
       </c>
       <c r="J9" s="7" t="s">
-        <v>67</v>
+        <v>41</v>
       </c>
       <c r="K9" s="8" t="s">
-        <v>0</v>
+        <v>83</v>
       </c>
       <c r="L9" s="8" t="s">
-        <v>1</v>
+        <v>84</v>
       </c>
       <c r="M9" s="8" t="s">
-        <v>2</v>
+        <v>85</v>
       </c>
       <c r="N9" s="8" t="s">
-        <v>3</v>
+        <v>86</v>
       </c>
     </row>
     <row r="10" spans="1:14">
@@ -4678,7 +4690,7 @@
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
       <c r="G16" s="1" t="s">
-        <v>5</v>
+        <v>88</v>
       </c>
       <c r="H16" s="1"/>
       <c r="I16" s="2"/>
@@ -4690,46 +4702,46 @@
     </row>
     <row r="17" spans="1:19" ht="71" thickBot="1">
       <c r="A17" s="3" t="s">
-        <v>58</v>
+        <v>32</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>59</v>
+        <v>33</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>60</v>
+        <v>34</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>61</v>
+        <v>35</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>62</v>
+        <v>36</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>63</v>
+        <v>37</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>64</v>
+        <v>38</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>65</v>
+        <v>39</v>
       </c>
       <c r="I17" s="7" t="s">
-        <v>66</v>
+        <v>40</v>
       </c>
       <c r="J17" s="7" t="s">
-        <v>67</v>
+        <v>41</v>
       </c>
       <c r="K17" s="8" t="s">
-        <v>0</v>
+        <v>83</v>
       </c>
       <c r="L17" s="8" t="s">
-        <v>1</v>
+        <v>84</v>
       </c>
       <c r="M17" s="8" t="s">
-        <v>2</v>
+        <v>85</v>
       </c>
       <c r="N17" s="8" t="s">
-        <v>3</v>
+        <v>86</v>
       </c>
     </row>
     <row r="18" spans="1:19">
@@ -4902,46 +4914,46 @@
     </row>
     <row r="24" spans="1:19" ht="46" thickBot="1">
       <c r="A24" s="3" t="s">
-        <v>6</v>
+        <v>89</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>7</v>
+        <v>90</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>64</v>
+        <v>38</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>8</v>
+        <v>91</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>9</v>
+        <v>92</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>10</v>
+        <v>93</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>11</v>
+        <v>94</v>
       </c>
       <c r="H24" s="7" t="s">
-        <v>12</v>
+        <v>95</v>
       </c>
       <c r="I24" s="7" t="s">
-        <v>13</v>
+        <v>96</v>
       </c>
       <c r="J24" s="7" t="s">
-        <v>30</v>
+        <v>113</v>
       </c>
       <c r="K24" s="8" t="s">
-        <v>31</v>
+        <v>114</v>
       </c>
       <c r="L24" s="8" t="s">
-        <v>32</v>
+        <v>115</v>
       </c>
       <c r="M24" s="8" t="s">
-        <v>33</v>
+        <v>116</v>
       </c>
       <c r="N24" s="8" t="s">
-        <v>32</v>
+        <v>115</v>
       </c>
     </row>
     <row r="25" spans="1:19">
@@ -5138,39 +5150,39 @@
     </row>
     <row r="31" spans="1:19">
       <c r="D31" t="s">
-        <v>34</v>
+        <v>117</v>
       </c>
     </row>
     <row r="32" spans="1:19" ht="46" thickBot="1">
       <c r="D32" s="3" t="s">
-        <v>35</v>
+        <v>118</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>36</v>
+        <v>119</v>
       </c>
       <c r="F32" s="6" t="s">
-        <v>64</v>
+        <v>38</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>37</v>
+        <v>120</v>
       </c>
       <c r="H32" s="8" t="s">
-        <v>40</v>
+        <v>123</v>
       </c>
       <c r="I32" s="8" t="s">
-        <v>41</v>
+        <v>124</v>
       </c>
       <c r="J32" s="8" t="s">
-        <v>42</v>
+        <v>125</v>
       </c>
       <c r="K32" s="8" t="s">
-        <v>43</v>
+        <v>126</v>
       </c>
       <c r="R32" t="s">
-        <v>44</v>
+        <v>127</v>
       </c>
       <c r="S32" t="s">
-        <v>45</v>
+        <v>128</v>
       </c>
     </row>
     <row r="33" spans="4:19">
@@ -5200,7 +5212,7 @@
         <v>3.8921515186908202</v>
       </c>
       <c r="M33" t="s">
-        <v>46</v>
+        <v>129</v>
       </c>
       <c r="R33">
         <v>1.59</v>
@@ -5236,7 +5248,7 @@
         <v>1.2000589337377248</v>
       </c>
       <c r="M34" t="s">
-        <v>47</v>
+        <v>130</v>
       </c>
       <c r="R34" s="10">
         <v>9155.6200000000008</v>
@@ -5272,7 +5284,7 @@
         <v>2.2325377438638392</v>
       </c>
       <c r="M35" t="s">
-        <v>48</v>
+        <v>22</v>
       </c>
     </row>
     <row r="36" spans="4:19">
@@ -5302,17 +5314,17 @@
         <v>2.6636263501721773</v>
       </c>
       <c r="M36" t="s">
-        <v>49</v>
+        <v>23</v>
       </c>
     </row>
     <row r="37" spans="4:19">
       <c r="M37" t="s">
-        <v>50</v>
+        <v>24</v>
       </c>
     </row>
     <row r="60" spans="25:25">
       <c r="Y60" t="s">
-        <v>51</v>
+        <v>25</v>
       </c>
     </row>
     <row r="65" spans="1:14" ht="15">
@@ -5323,7 +5335,7 @@
       <c r="E65" s="2"/>
       <c r="F65" s="2"/>
       <c r="G65" s="1" t="s">
-        <v>52</v>
+        <v>26</v>
       </c>
       <c r="H65" s="1"/>
       <c r="I65" s="2"/>
@@ -5335,46 +5347,46 @@
     </row>
     <row r="66" spans="1:14" ht="71" thickBot="1">
       <c r="A66" s="3" t="s">
-        <v>58</v>
+        <v>32</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>59</v>
+        <v>33</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>60</v>
+        <v>34</v>
       </c>
       <c r="D66" s="5" t="s">
-        <v>61</v>
+        <v>35</v>
       </c>
       <c r="E66" s="3" t="s">
-        <v>62</v>
+        <v>36</v>
       </c>
       <c r="F66" s="3" t="s">
-        <v>63</v>
+        <v>37</v>
       </c>
       <c r="G66" s="6" t="s">
-        <v>64</v>
+        <v>38</v>
       </c>
       <c r="H66" s="3" t="s">
-        <v>65</v>
+        <v>39</v>
       </c>
       <c r="I66" s="7" t="s">
-        <v>66</v>
+        <v>40</v>
       </c>
       <c r="J66" s="7" t="s">
-        <v>67</v>
+        <v>41</v>
       </c>
       <c r="K66" s="8" t="s">
-        <v>0</v>
+        <v>83</v>
       </c>
       <c r="L66" s="8" t="s">
-        <v>1</v>
+        <v>84</v>
       </c>
       <c r="M66" s="8" t="s">
-        <v>2</v>
+        <v>85</v>
       </c>
       <c r="N66" s="8" t="s">
-        <v>3</v>
+        <v>86</v>
       </c>
     </row>
     <row r="67" spans="1:14">
@@ -5511,7 +5523,7 @@
       <c r="E72" s="2"/>
       <c r="F72" s="2"/>
       <c r="G72" s="1" t="s">
-        <v>53</v>
+        <v>27</v>
       </c>
       <c r="H72" s="1"/>
       <c r="I72" s="2"/>
@@ -5523,46 +5535,46 @@
     </row>
     <row r="73" spans="1:14" ht="71" thickBot="1">
       <c r="A73" s="3" t="s">
-        <v>58</v>
+        <v>32</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>59</v>
+        <v>33</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>60</v>
+        <v>34</v>
       </c>
       <c r="D73" s="5" t="s">
-        <v>61</v>
+        <v>35</v>
       </c>
       <c r="E73" s="3" t="s">
-        <v>62</v>
+        <v>36</v>
       </c>
       <c r="F73" s="3" t="s">
-        <v>63</v>
+        <v>37</v>
       </c>
       <c r="G73" s="6" t="s">
-        <v>64</v>
+        <v>38</v>
       </c>
       <c r="H73" s="3" t="s">
-        <v>65</v>
+        <v>39</v>
       </c>
       <c r="I73" s="7" t="s">
-        <v>66</v>
+        <v>40</v>
       </c>
       <c r="J73" s="7" t="s">
-        <v>67</v>
+        <v>41</v>
       </c>
       <c r="K73" s="8" t="s">
-        <v>0</v>
+        <v>83</v>
       </c>
       <c r="L73" s="8" t="s">
-        <v>1</v>
+        <v>84</v>
       </c>
       <c r="M73" s="8" t="s">
-        <v>2</v>
+        <v>85</v>
       </c>
       <c r="N73" s="8" t="s">
-        <v>3</v>
+        <v>86</v>
       </c>
     </row>
     <row r="74" spans="1:14">
@@ -5699,7 +5711,7 @@
       <c r="E79" s="2"/>
       <c r="F79" s="2"/>
       <c r="G79" s="1" t="s">
-        <v>54</v>
+        <v>28</v>
       </c>
       <c r="H79" s="1"/>
       <c r="I79" s="2"/>
@@ -5711,46 +5723,46 @@
     </row>
     <row r="80" spans="1:14" ht="71" thickBot="1">
       <c r="A80" s="3" t="s">
-        <v>58</v>
+        <v>32</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>59</v>
+        <v>33</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>60</v>
+        <v>34</v>
       </c>
       <c r="D80" s="5" t="s">
-        <v>61</v>
+        <v>35</v>
       </c>
       <c r="E80" s="3" t="s">
-        <v>62</v>
+        <v>36</v>
       </c>
       <c r="F80" s="3" t="s">
-        <v>63</v>
+        <v>37</v>
       </c>
       <c r="G80" s="6" t="s">
-        <v>64</v>
+        <v>38</v>
       </c>
       <c r="H80" s="3" t="s">
-        <v>65</v>
+        <v>39</v>
       </c>
       <c r="I80" s="7" t="s">
-        <v>66</v>
+        <v>40</v>
       </c>
       <c r="J80" s="7" t="s">
-        <v>67</v>
+        <v>41</v>
       </c>
       <c r="K80" s="8" t="s">
-        <v>0</v>
+        <v>83</v>
       </c>
       <c r="L80" s="8" t="s">
-        <v>1</v>
+        <v>84</v>
       </c>
       <c r="M80" s="8" t="s">
-        <v>2</v>
+        <v>85</v>
       </c>
       <c r="N80" s="8" t="s">
-        <v>3</v>
+        <v>86</v>
       </c>
     </row>
     <row r="81" spans="1:12">
@@ -5872,40 +5884,40 @@
     </row>
     <row r="87" spans="1:12" ht="71" thickBot="1">
       <c r="A87" s="3" t="s">
-        <v>55</v>
+        <v>29</v>
       </c>
       <c r="B87" s="6" t="s">
-        <v>64</v>
+        <v>38</v>
       </c>
       <c r="C87" s="7" t="s">
-        <v>56</v>
+        <v>30</v>
       </c>
       <c r="D87" s="7" t="s">
-        <v>56</v>
+        <v>30</v>
       </c>
       <c r="E87" s="7" t="s">
-        <v>56</v>
+        <v>30</v>
       </c>
       <c r="F87" s="8" t="s">
-        <v>108</v>
+        <v>82</v>
       </c>
       <c r="G87" s="8" t="s">
-        <v>109</v>
+        <v>0</v>
       </c>
       <c r="H87" s="7" t="s">
-        <v>110</v>
+        <v>1</v>
       </c>
       <c r="I87" s="7" t="s">
-        <v>110</v>
+        <v>1</v>
       </c>
       <c r="J87" s="7" t="s">
-        <v>110</v>
+        <v>1</v>
       </c>
       <c r="K87" s="8" t="s">
-        <v>111</v>
+        <v>2</v>
       </c>
       <c r="L87" s="8" t="s">
-        <v>112</v>
+        <v>3</v>
       </c>
     </row>
     <row r="88" spans="1:12">
@@ -6039,27 +6051,27 @@
     </row>
     <row r="94" spans="1:12">
       <c r="A94" t="s">
-        <v>113</v>
+        <v>4</v>
       </c>
     </row>
     <row r="96" spans="1:12" ht="33" thickBot="1">
       <c r="A96" s="3" t="s">
-        <v>114</v>
+        <v>5</v>
       </c>
       <c r="B96" s="5" t="s">
-        <v>64</v>
+        <v>38</v>
       </c>
       <c r="C96" s="6" t="s">
-        <v>115</v>
+        <v>6</v>
       </c>
       <c r="D96" s="3" t="s">
-        <v>116</v>
+        <v>7</v>
       </c>
       <c r="E96" s="3" t="s">
-        <v>117</v>
+        <v>8</v>
       </c>
       <c r="F96" s="5" t="s">
-        <v>118</v>
+        <v>9</v>
       </c>
       <c r="G96" s="11"/>
     </row>
@@ -6125,7 +6137,7 @@
     </row>
     <row r="100" spans="1:22">
       <c r="V100" t="s">
-        <v>119</v>
+        <v>10</v>
       </c>
     </row>
     <row r="101" spans="1:22">
@@ -6135,27 +6147,27 @@
     </row>
     <row r="105" spans="1:22">
       <c r="I105" t="s">
-        <v>46</v>
+        <v>129</v>
       </c>
     </row>
     <row r="106" spans="1:22">
       <c r="I106" t="s">
-        <v>120</v>
+        <v>11</v>
       </c>
     </row>
     <row r="107" spans="1:22">
       <c r="I107" t="s">
-        <v>121</v>
+        <v>12</v>
       </c>
     </row>
     <row r="108" spans="1:22">
       <c r="I108" t="s">
-        <v>122</v>
+        <v>13</v>
       </c>
     </row>
     <row r="109" spans="1:22">
       <c r="I109" t="s">
-        <v>123</v>
+        <v>14</v>
       </c>
     </row>
     <row r="120" spans="1:17" ht="15">
@@ -6166,7 +6178,7 @@
       <c r="E120" s="2"/>
       <c r="F120" s="2"/>
       <c r="G120" s="1" t="s">
-        <v>124</v>
+        <v>15</v>
       </c>
       <c r="H120" s="1"/>
       <c r="I120" s="2"/>
@@ -6178,46 +6190,46 @@
     </row>
     <row r="121" spans="1:17" ht="71" thickBot="1">
       <c r="A121" s="3" t="s">
-        <v>58</v>
+        <v>32</v>
       </c>
       <c r="B121" s="3" t="s">
-        <v>6</v>
+        <v>89</v>
       </c>
       <c r="C121" s="4" t="s">
-        <v>125</v>
+        <v>16</v>
       </c>
       <c r="D121" s="5" t="s">
-        <v>61</v>
+        <v>35</v>
       </c>
       <c r="E121" s="3" t="s">
-        <v>62</v>
+        <v>36</v>
       </c>
       <c r="F121" s="3" t="s">
-        <v>63</v>
+        <v>37</v>
       </c>
       <c r="G121" s="6" t="s">
-        <v>64</v>
+        <v>38</v>
       </c>
       <c r="H121" s="3" t="s">
-        <v>65</v>
+        <v>39</v>
       </c>
       <c r="I121" s="7" t="s">
-        <v>66</v>
+        <v>40</v>
       </c>
       <c r="J121" s="7" t="s">
-        <v>67</v>
+        <v>41</v>
       </c>
       <c r="K121" s="8" t="s">
-        <v>0</v>
+        <v>83</v>
       </c>
       <c r="L121" s="8" t="s">
-        <v>1</v>
+        <v>84</v>
       </c>
       <c r="M121" s="8" t="s">
-        <v>2</v>
+        <v>85</v>
       </c>
       <c r="N121" s="8" t="s">
-        <v>126</v>
+        <v>17</v>
       </c>
     </row>
     <row r="122" spans="1:17">
@@ -6383,7 +6395,7 @@
       <c r="E129" s="2"/>
       <c r="F129" s="2"/>
       <c r="G129" s="1" t="s">
-        <v>127</v>
+        <v>18</v>
       </c>
       <c r="H129" s="1"/>
       <c r="I129" s="2"/>
@@ -6395,46 +6407,46 @@
     </row>
     <row r="130" spans="1:14" ht="71" thickBot="1">
       <c r="A130" s="3" t="s">
-        <v>58</v>
+        <v>32</v>
       </c>
       <c r="B130" s="3" t="s">
-        <v>59</v>
+        <v>33</v>
       </c>
       <c r="C130" s="4" t="s">
-        <v>60</v>
+        <v>34</v>
       </c>
       <c r="D130" s="5" t="s">
-        <v>61</v>
+        <v>35</v>
       </c>
       <c r="E130" s="3" t="s">
-        <v>62</v>
+        <v>36</v>
       </c>
       <c r="F130" s="3" t="s">
-        <v>63</v>
+        <v>37</v>
       </c>
       <c r="G130" s="6" t="s">
-        <v>64</v>
+        <v>38</v>
       </c>
       <c r="H130" s="3" t="s">
-        <v>65</v>
+        <v>39</v>
       </c>
       <c r="I130" s="7" t="s">
-        <v>66</v>
+        <v>40</v>
       </c>
       <c r="J130" s="7" t="s">
-        <v>67</v>
+        <v>41</v>
       </c>
       <c r="K130" s="8" t="s">
-        <v>0</v>
+        <v>83</v>
       </c>
       <c r="L130" s="8" t="s">
-        <v>1</v>
+        <v>84</v>
       </c>
       <c r="M130" s="8" t="s">
-        <v>2</v>
+        <v>85</v>
       </c>
       <c r="N130" s="8" t="s">
-        <v>3</v>
+        <v>86</v>
       </c>
     </row>
     <row r="131" spans="1:14">
@@ -6574,7 +6586,7 @@
       <c r="E139" s="2"/>
       <c r="F139" s="2"/>
       <c r="G139" s="1" t="s">
-        <v>19</v>
+        <v>102</v>
       </c>
       <c r="H139" s="1"/>
       <c r="I139" s="2"/>
@@ -6586,46 +6598,46 @@
     </row>
     <row r="140" spans="1:14" ht="71" thickBot="1">
       <c r="A140" s="3" t="s">
-        <v>58</v>
+        <v>32</v>
       </c>
       <c r="B140" s="3" t="s">
-        <v>59</v>
+        <v>33</v>
       </c>
       <c r="C140" s="4" t="s">
-        <v>60</v>
+        <v>34</v>
       </c>
       <c r="D140" s="5" t="s">
-        <v>61</v>
+        <v>35</v>
       </c>
       <c r="E140" s="3" t="s">
-        <v>62</v>
+        <v>36</v>
       </c>
       <c r="F140" s="3" t="s">
-        <v>63</v>
+        <v>37</v>
       </c>
       <c r="G140" s="6" t="s">
-        <v>64</v>
+        <v>38</v>
       </c>
       <c r="H140" s="3" t="s">
-        <v>65</v>
+        <v>39</v>
       </c>
       <c r="I140" s="7" t="s">
-        <v>66</v>
+        <v>40</v>
       </c>
       <c r="J140" s="7" t="s">
-        <v>67</v>
+        <v>41</v>
       </c>
       <c r="K140" s="8" t="s">
-        <v>0</v>
+        <v>83</v>
       </c>
       <c r="L140" s="8" t="s">
-        <v>1</v>
+        <v>84</v>
       </c>
       <c r="M140" s="8" t="s">
-        <v>2</v>
+        <v>85</v>
       </c>
       <c r="N140" s="8" t="s">
-        <v>126</v>
+        <v>17</v>
       </c>
     </row>
     <row r="141" spans="1:14">
@@ -6759,55 +6771,55 @@
     </row>
     <row r="147" spans="1:17" ht="43" thickBot="1">
       <c r="A147" s="4" t="s">
-        <v>60</v>
+        <v>34</v>
       </c>
       <c r="B147" s="6" t="s">
-        <v>64</v>
+        <v>38</v>
       </c>
       <c r="C147" s="3" t="s">
-        <v>65</v>
+        <v>39</v>
       </c>
       <c r="D147" s="3" t="s">
-        <v>65</v>
+        <v>39</v>
       </c>
       <c r="E147" s="3" t="s">
-        <v>65</v>
+        <v>39</v>
       </c>
       <c r="F147" s="3" t="s">
-        <v>20</v>
+        <v>103</v>
       </c>
       <c r="G147" s="3" t="s">
-        <v>21</v>
+        <v>104</v>
       </c>
       <c r="H147" s="7" t="s">
-        <v>66</v>
+        <v>40</v>
       </c>
       <c r="I147" s="7" t="s">
-        <v>66</v>
+        <v>40</v>
       </c>
       <c r="J147" s="7" t="s">
-        <v>66</v>
+        <v>40</v>
       </c>
       <c r="K147" s="8" t="s">
-        <v>22</v>
+        <v>105</v>
       </c>
       <c r="L147" s="8" t="s">
-        <v>23</v>
+        <v>106</v>
       </c>
       <c r="M147" s="7" t="s">
-        <v>67</v>
+        <v>41</v>
       </c>
       <c r="N147" s="7" t="s">
-        <v>67</v>
+        <v>41</v>
       </c>
       <c r="O147" s="7" t="s">
-        <v>67</v>
+        <v>41</v>
       </c>
       <c r="P147" s="8" t="s">
-        <v>24</v>
+        <v>107</v>
       </c>
       <c r="Q147" s="8" t="s">
-        <v>25</v>
+        <v>108</v>
       </c>
     </row>
     <row r="148" spans="1:17">
@@ -6971,36 +6983,36 @@
     </row>
     <row r="153" spans="1:17">
       <c r="C153" t="s">
-        <v>26</v>
+        <v>109</v>
       </c>
     </row>
     <row r="155" spans="1:17" ht="49" thickBot="1">
       <c r="C155" s="3" t="s">
-        <v>27</v>
+        <v>110</v>
       </c>
       <c r="D155" s="5" t="s">
-        <v>61</v>
+        <v>35</v>
       </c>
       <c r="E155" s="6" t="s">
-        <v>28</v>
+        <v>111</v>
       </c>
       <c r="F155" s="3" t="s">
-        <v>65</v>
+        <v>39</v>
       </c>
       <c r="G155" s="3" t="s">
-        <v>29</v>
+        <v>112</v>
       </c>
       <c r="H155" s="8" t="s">
-        <v>15</v>
+        <v>98</v>
       </c>
       <c r="I155" s="8" t="s">
-        <v>16</v>
+        <v>99</v>
       </c>
       <c r="J155" s="8" t="s">
-        <v>102</v>
+        <v>76</v>
       </c>
       <c r="K155" s="8" t="s">
-        <v>103</v>
+        <v>77</v>
       </c>
     </row>
     <row r="156" spans="1:17">
@@ -7094,6 +7106,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>
@@ -7117,33 +7130,33 @@
   <sheetData>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>104</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="46" thickBot="1">
       <c r="A4" s="3" t="s">
-        <v>59</v>
+        <v>33</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>61</v>
+        <v>35</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>64</v>
+        <v>38</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>65</v>
+        <v>39</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>105</v>
+        <v>79</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>41</v>
+        <v>124</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>42</v>
+        <v>125</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>43</v>
+        <v>126</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -7256,15 +7269,15 @@
     </row>
     <row r="31" spans="2:8">
       <c r="G31" t="s">
-        <v>44</v>
+        <v>127</v>
       </c>
       <c r="H31" t="s">
-        <v>106</v>
+        <v>80</v>
       </c>
     </row>
     <row r="32" spans="2:8">
       <c r="B32" t="s">
-        <v>46</v>
+        <v>129</v>
       </c>
       <c r="G32">
         <v>1.59</v>
@@ -7275,7 +7288,7 @@
     </row>
     <row r="33" spans="1:8" ht="15">
       <c r="B33" t="s">
-        <v>47</v>
+        <v>130</v>
       </c>
       <c r="G33" s="10">
         <v>9155.6200000000008</v>
@@ -7286,42 +7299,42 @@
     </row>
     <row r="34" spans="1:8">
       <c r="B34" t="s">
-        <v>107</v>
+        <v>81</v>
       </c>
     </row>
     <row r="35" spans="1:8">
       <c r="B35" t="s">
-        <v>122</v>
+        <v>13</v>
       </c>
     </row>
     <row r="36" spans="1:8">
       <c r="B36" t="s">
-        <v>123</v>
+        <v>14</v>
       </c>
     </row>
     <row r="48" spans="1:8">
       <c r="A48" t="s">
-        <v>113</v>
+        <v>4</v>
       </c>
     </row>
     <row r="50" spans="1:7" ht="33" thickBot="1">
       <c r="A50" s="3" t="s">
-        <v>114</v>
+        <v>5</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>64</v>
+        <v>38</v>
       </c>
       <c r="C50" s="6" t="s">
-        <v>115</v>
+        <v>6</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>116</v>
+        <v>7</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>117</v>
+        <v>8</v>
       </c>
       <c r="F50" s="5" t="s">
-        <v>118</v>
+        <v>9</v>
       </c>
       <c r="G50" s="11"/>
     </row>
@@ -7387,15 +7400,15 @@
     </row>
     <row r="64" spans="1:7">
       <c r="B64" t="s">
-        <v>46</v>
+        <v>129</v>
       </c>
       <c r="G64" t="s">
-        <v>119</v>
+        <v>10</v>
       </c>
     </row>
     <row r="65" spans="1:9" ht="15">
       <c r="B65" t="s">
-        <v>47</v>
+        <v>130</v>
       </c>
       <c r="G65">
         <v>9144.5290000000005</v>
@@ -7404,51 +7417,51 @@
     </row>
     <row r="66" spans="1:9">
       <c r="B66" t="s">
-        <v>107</v>
+        <v>81</v>
       </c>
     </row>
     <row r="67" spans="1:9">
       <c r="B67" t="s">
-        <v>122</v>
+        <v>13</v>
       </c>
     </row>
     <row r="68" spans="1:9">
       <c r="B68" t="s">
-        <v>123</v>
+        <v>14</v>
       </c>
     </row>
     <row r="78" spans="1:9">
       <c r="A78" t="s">
-        <v>26</v>
+        <v>109</v>
       </c>
     </row>
     <row r="80" spans="1:9" ht="49" thickBot="1">
       <c r="A80" s="3" t="s">
-        <v>27</v>
+        <v>110</v>
       </c>
       <c r="B80" s="5" t="s">
-        <v>61</v>
+        <v>35</v>
       </c>
       <c r="C80" s="6" t="s">
-        <v>28</v>
+        <v>111</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>65</v>
+        <v>39</v>
       </c>
       <c r="E80" s="3" t="s">
-        <v>29</v>
+        <v>112</v>
       </c>
       <c r="F80" s="8" t="s">
-        <v>15</v>
+        <v>98</v>
       </c>
       <c r="G80" s="8" t="s">
-        <v>16</v>
+        <v>99</v>
       </c>
       <c r="H80" s="8" t="s">
-        <v>102</v>
+        <v>76</v>
       </c>
       <c r="I80" s="8" t="s">
-        <v>103</v>
+        <v>77</v>
       </c>
     </row>
     <row r="81" spans="1:9">
@@ -7559,67 +7572,67 @@
   <dimension ref="A2:Q79"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O6" sqref="O6"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <sheetData>
     <row r="2" spans="1:17">
       <c r="A2" t="s">
-        <v>81</v>
+        <v>55</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>100</v>
       </c>
       <c r="H2" t="s">
-        <v>86</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:17">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>97</v>
       </c>
       <c r="B4" t="s">
-        <v>80</v>
+        <v>54</v>
       </c>
       <c r="C4" t="s">
-        <v>78</v>
+        <v>52</v>
       </c>
       <c r="D4" t="s">
-        <v>79</v>
+        <v>53</v>
       </c>
       <c r="E4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F4" t="s">
+        <v>56</v>
+      </c>
+      <c r="G4" t="s">
+        <v>57</v>
+      </c>
+      <c r="H4" t="s">
+        <v>42</v>
+      </c>
+      <c r="I4" t="s">
+        <v>58</v>
+      </c>
+      <c r="J4" t="s">
+        <v>46</v>
+      </c>
+      <c r="K4" t="s">
+        <v>42</v>
+      </c>
+      <c r="L4" t="s">
+        <v>61</v>
+      </c>
+      <c r="M4" t="s">
+        <v>72</v>
+      </c>
+      <c r="N4" t="s">
         <v>73</v>
       </c>
-      <c r="F4" t="s">
-        <v>82</v>
-      </c>
-      <c r="G4" t="s">
-        <v>83</v>
-      </c>
-      <c r="H4" t="s">
-        <v>68</v>
-      </c>
-      <c r="I4" t="s">
-        <v>84</v>
-      </c>
-      <c r="J4" t="s">
-        <v>72</v>
-      </c>
-      <c r="K4" t="s">
-        <v>68</v>
-      </c>
-      <c r="L4" t="s">
-        <v>87</v>
-      </c>
-      <c r="M4" t="s">
-        <v>98</v>
-      </c>
-      <c r="N4" t="s">
-        <v>99</v>
-      </c>
       <c r="O4" t="s">
-        <v>18</v>
+        <v>101</v>
       </c>
     </row>
     <row r="5" spans="1:17">
@@ -7775,52 +7788,52 @@
     </row>
     <row r="11" spans="1:17">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>97</v>
       </c>
       <c r="B11" t="s">
-        <v>91</v>
+        <v>65</v>
       </c>
       <c r="C11" t="s">
-        <v>90</v>
+        <v>64</v>
       </c>
       <c r="D11" t="s">
-        <v>79</v>
+        <v>53</v>
       </c>
       <c r="E11" t="s">
-        <v>68</v>
+        <v>42</v>
       </c>
       <c r="F11" t="s">
-        <v>91</v>
+        <v>65</v>
       </c>
       <c r="G11" t="s">
-        <v>90</v>
+        <v>64</v>
       </c>
       <c r="H11" t="s">
-        <v>79</v>
+        <v>53</v>
       </c>
       <c r="I11" t="s">
-        <v>68</v>
+        <v>42</v>
       </c>
       <c r="J11" t="s">
-        <v>92</v>
+        <v>66</v>
       </c>
       <c r="K11" t="s">
-        <v>90</v>
+        <v>64</v>
       </c>
       <c r="L11" t="s">
-        <v>79</v>
+        <v>53</v>
       </c>
       <c r="M11" t="s">
-        <v>68</v>
+        <v>42</v>
       </c>
       <c r="N11" t="s">
-        <v>93</v>
+        <v>67</v>
       </c>
       <c r="P11" t="s">
-        <v>100</v>
+        <v>74</v>
       </c>
       <c r="Q11" t="s">
-        <v>101</v>
+        <v>75</v>
       </c>
     </row>
     <row r="12" spans="1:17">
@@ -7980,6 +7993,109 @@
         <v>10.540389098093113</v>
       </c>
     </row>
+    <row r="20" spans="2:15">
+      <c r="M20" t="s">
+        <v>19</v>
+      </c>
+      <c r="N20">
+        <f>((M5-P12)/M5)*100</f>
+        <v>46.03469197624316</v>
+      </c>
+      <c r="O20">
+        <f>AVERAGE(N20:N22)</f>
+        <v>43.385208575547772</v>
+      </c>
+    </row>
+    <row r="21" spans="2:15">
+      <c r="M21" t="s">
+        <v>20</v>
+      </c>
+      <c r="N21">
+        <f t="shared" ref="N21:N22" si="4">((M6-P13)/M6)*100</f>
+        <v>40.676969614574126</v>
+      </c>
+      <c r="O21">
+        <f>1.96*STDEV(N20:N22)/SQRT(3)</f>
+        <v>3.0319636073259546</v>
+      </c>
+    </row>
+    <row r="22" spans="2:15">
+      <c r="M22" t="s">
+        <v>21</v>
+      </c>
+      <c r="N22">
+        <f t="shared" si="4"/>
+        <v>43.443964135826015</v>
+      </c>
+    </row>
+    <row r="24" spans="2:15">
+      <c r="B24">
+        <f>AVERAGE(C24:C26)</f>
+        <v>64.21312926960853</v>
+      </c>
+      <c r="C24">
+        <f>C12/C5*100</f>
+        <v>61.007952204367534</v>
+      </c>
+      <c r="D24">
+        <f>(C5-C12)/C5*100</f>
+        <v>38.992047795632466</v>
+      </c>
+      <c r="E24">
+        <f>AVERAGE(D24:D26)</f>
+        <v>35.786870730391477</v>
+      </c>
+    </row>
+    <row r="25" spans="2:15">
+      <c r="B25">
+        <f>1.96 *(STDEV(C24:C26)/SQRT(3))</f>
+        <v>3.1494806557607635</v>
+      </c>
+      <c r="C25">
+        <f t="shared" ref="C25:C26" si="5">C13/C6*100</f>
+        <v>66.018940839694665</v>
+      </c>
+      <c r="D25">
+        <f t="shared" ref="D25:D26" si="6">(C6-C13)/C6*100</f>
+        <v>33.981059160305335</v>
+      </c>
+      <c r="E25">
+        <f>1.96 *(STDEV(D24:D26)/SQRT(3))</f>
+        <v>3.1494806557609487</v>
+      </c>
+    </row>
+    <row r="26" spans="2:15">
+      <c r="C26">
+        <f t="shared" si="5"/>
+        <v>65.612494764763369</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="6"/>
+        <v>34.387505235236624</v>
+      </c>
+    </row>
+    <row r="28" spans="2:15">
+      <c r="B28">
+        <f>(D12/D5)*100</f>
+        <v>9.4427230046948356</v>
+      </c>
+      <c r="C28">
+        <f>AVERAGE(B28:B30)</f>
+        <v>8.854828657052721</v>
+      </c>
+    </row>
+    <row r="29" spans="2:15">
+      <c r="B29">
+        <f t="shared" ref="B29:B30" si="7">(D13/D6)*100</f>
+        <v>8.7040048543689323</v>
+      </c>
+    </row>
+    <row r="30" spans="2:15">
+      <c r="B30">
+        <f t="shared" si="7"/>
+        <v>8.4177581120943969</v>
+      </c>
+    </row>
     <row r="50" spans="1:12">
       <c r="D50">
         <v>1087592</v>
@@ -7987,45 +8103,45 @@
     </row>
     <row r="53" spans="1:12">
       <c r="A53" t="s">
-        <v>69</v>
+        <v>43</v>
       </c>
       <c r="B53" t="s">
-        <v>70</v>
+        <v>44</v>
       </c>
       <c r="C53" t="s">
-        <v>71</v>
+        <v>45</v>
       </c>
       <c r="D53" t="s">
-        <v>72</v>
+        <v>46</v>
       </c>
       <c r="E53" t="s">
-        <v>73</v>
+        <v>47</v>
       </c>
       <c r="F53" t="s">
-        <v>71</v>
+        <v>45</v>
       </c>
       <c r="G53" t="s">
-        <v>72</v>
+        <v>46</v>
       </c>
       <c r="H53" t="s">
-        <v>68</v>
+        <v>42</v>
       </c>
       <c r="I53" t="s">
-        <v>71</v>
+        <v>45</v>
       </c>
       <c r="J53" t="s">
-        <v>72</v>
+        <v>46</v>
       </c>
       <c r="K53" t="s">
-        <v>68</v>
+        <v>42</v>
       </c>
       <c r="L53" t="s">
-        <v>85</v>
+        <v>59</v>
       </c>
     </row>
     <row r="54" spans="1:12">
       <c r="A54" t="s">
-        <v>74</v>
+        <v>48</v>
       </c>
       <c r="B54">
         <v>1171052</v>
@@ -8064,7 +8180,7 @@
     </row>
     <row r="55" spans="1:12">
       <c r="A55" t="s">
-        <v>75</v>
+        <v>49</v>
       </c>
       <c r="B55">
         <v>1171052</v>
@@ -8072,7 +8188,7 @@
     </row>
     <row r="56" spans="1:12">
       <c r="A56" t="s">
-        <v>76</v>
+        <v>50</v>
       </c>
       <c r="B56">
         <v>1171052</v>
@@ -8080,7 +8196,7 @@
     </row>
     <row r="57" spans="1:12">
       <c r="A57" t="s">
-        <v>77</v>
+        <v>51</v>
       </c>
       <c r="B57">
         <v>1171052</v>
@@ -8088,15 +8204,15 @@
     </row>
     <row r="63" spans="1:12">
       <c r="A63" t="s">
-        <v>38</v>
+        <v>121</v>
       </c>
       <c r="B63" t="s">
-        <v>68</v>
+        <v>42</v>
       </c>
     </row>
     <row r="64" spans="1:12">
       <c r="A64" t="s">
-        <v>39</v>
+        <v>122</v>
       </c>
       <c r="B64">
         <v>563</v>
@@ -8104,7 +8220,7 @@
     </row>
     <row r="65" spans="1:5">
       <c r="A65" t="s">
-        <v>88</v>
+        <v>62</v>
       </c>
       <c r="B65">
         <f>19*60</f>
@@ -8113,7 +8229,7 @@
     </row>
     <row r="66" spans="1:5">
       <c r="A66" t="s">
-        <v>89</v>
+        <v>63</v>
       </c>
       <c r="B66">
         <v>2611</v>
@@ -8121,18 +8237,18 @@
     </row>
     <row r="75" spans="1:5">
       <c r="C75" t="s">
-        <v>94</v>
+        <v>68</v>
       </c>
     </row>
     <row r="76" spans="1:5">
       <c r="C76" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="D76" t="s">
-        <v>96</v>
+        <v>70</v>
       </c>
       <c r="E76" t="s">
-        <v>97</v>
+        <v>71</v>
       </c>
     </row>
     <row r="77" spans="1:5">
@@ -8151,9 +8267,9 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">

</xml_diff>

<commit_message>
Deleted ecmls20112.tex as new manuscript is added
git-svn-id: file://localhost/tmp/svn2git/svn@6601 defb5e50-622e-49ec-a68e-d72c7db87b45
</commit_message>
<xml_diff>
--- a/papers/saga-mr-ngs/data/GS_data.xlsx
+++ b/papers/saga-mr-ngs/data/GS_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-940" yWindow="120" windowWidth="26820" windowHeight="12460" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="12620" yWindow="-20" windowWidth="12860" windowHeight="6980" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="GS data" sheetId="1" r:id="rId1"/>
@@ -24,525 +24,577 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="144">
+  <si>
+    <t>Input data</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>chunk size</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>map</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>reduce</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>tts</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>(1+1)2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>(2+2)4</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>(4+4)8</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Map</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Reduce</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>input 2GB, sequences=3805921, chunksize=128MB, number of reduces=8</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mapcompletion</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>shuffle completion</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>reduce completion</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>map phase time</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>setup</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>reduce phase time</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Size of data transferred in MB from Map to reduce phase</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>reduce Output data size in MB</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>duplicate  data size in MB</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Varying Number of chunk size - II</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Varying Number of chunk size - III</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>number of reads</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Number of chunks created</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Time taken to chunk files in seconds</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Map phase Time in seconds - I</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Reduce Phase Time in seconds - I</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>seqal</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>seqal default configs</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>tts</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>mean reduce phase</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>stderr of reduce phase</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Varying number of workers, input size = 10 GB, reduces = 8, Number of reads/ chunk=625000</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Workers</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>mean map phase</t>
+  </si>
   <si>
     <t>stderr of map phase</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mean reduce phase</t>
+  </si>
+  <si>
+    <t>stderr of reduce phase</t>
+  </si>
+  <si>
+    <t>&lt; 1sec</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Data transfer in MB between map &amp; reduce phase is</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Reduced output size  3120 MB  which is 31.2% of input data</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Number of workers=(4+4), sierra and hotel used.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Number of workers=(4+4), india and hotel used.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>835 intermediate data</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>phase times</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Reduced output size  3120 MB  which is 31.2% of input data</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Varying Input size, chunk size=625000, number  of reduces=8, number of workers=32</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Input data size in GB</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Total Time to solution in  secs</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>stderr in chunk time</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Reduce Phase Time in seconds - III</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mean</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>stderr</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>mean</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Varying chunk size ,  Input Size = 10GB, Number of workers - 32, Number of reduces -8</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>number of reads</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Number of chunks created</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Time taken to chunk files in seconds</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>prq</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2GB</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>shuffle phase time</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>averge sort time</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Duplicate output size is 4445MB which is 44.5% of input data</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Remaining is Filedelimiter which I used.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>+</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Varying Number of  workers</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Varying Number of  workers - II</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Varying Number of  workers - III</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Number of  subjobs(workers) for both map/reduce phase</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Map phase Time in seconds</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Varying Number of chunk size - I</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>chunk size( lines)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>number of reads</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mean Map phase</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>stderr for map phase</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>mean reduce phase</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>stderr for reduce phase</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Mean </t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Stdev</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Time to transfer files files between map &amp; reduce phase is </t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Data transfer in MB between map &amp; reduce phase is</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>use default replication factor.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>calculate tim taken for each map task.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>calculate time for launching map task.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Input Data size(GB)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Number of chunks created</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Number of  subjobs(workers) for both map/reduce phase</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>number of reduces.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Total Time sec</t>
+  </si>
+  <si>
+    <t>Time taken to chunk files in seconds</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Map phase Time in seconds</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>Reduce Phase Time in seconds</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>tts</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>caluclate time for sort time.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>chunks</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>seqal</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Map</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>reduce</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>map</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>mahine used -sierra</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>sequences</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>4GB</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>8GB</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Map</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>chunktime</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>chunktime</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>intermediate data</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mean tts</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>std tts</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>mean tts</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>stdtts</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>mean time taken for reduce phase</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>stderr for reduce phase phase time</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Varying chunk size ,  Input Size = 10GB, Number of workers - 32, Number of reduces -8</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mean Map phase</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Stdev</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Reduced output size  3120 MB  which is 31.2% of input data</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>mean map phase</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>File Transfer in seconds</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Map phase Time in seconds - II</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Reduce Phase Time in seconds-II</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Map phase Time in seconds-III</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>input data</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>mean time taken for map phase</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>stderr in map phase time</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>sequences per chunk</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Varying Input size - III</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>mean chunk time</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>stderr chunk time</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>mean map phase</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>stderr in map phase</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>mean reduce phase</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>stderr of reduce phase</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Varying number of workers, input size = 10 GB, reduces = 8, Number of reads/ chunk=625000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Workers</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>mean map phase</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>stderr reduce phase</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>stderr of map phase</t>
-  </si>
-  <si>
-    <t>mean reduce phase</t>
-  </si>
-  <si>
-    <t>stderr of reduce phase</t>
-  </si>
-  <si>
-    <t>&lt; 1sec</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Data transfer in MB between map &amp; reduce phase is</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Reduced output size  3120 MB  which is 31.2% of input data</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Reduce Phase Time in seconds</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>PMR</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>chunk time</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>exchange</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>Duplicate output size is 4445MB which is 44.5% of input data</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>Remaining is Filedelimiter which I used.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>Varying Input size - I</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>Input Data size(GB)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>duplicate  data size in GB</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>Varying Input size - II</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>at 2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>at 4</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>at 8</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Reduced output size  3120 MB  which is 31.2% of input data</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Duplicate output size is 4445MB which is 44.5% of input data</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Remaining is Filedelimiter which I used.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>+</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Varying Number of  workers</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Varying Number of  workers - II</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Varying Number of  workers - III</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Number of  subjobs(workers) for both map/reduce phase</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Map phase Time in seconds</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Varying Number of chunk size - I</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>chunk size( lines)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>number of reads</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Input Data size(GB)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Number of chunks created</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Number of  subjobs(workers) for both map/reduce phase</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>number of reduces.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Total Time sec</t>
-  </si>
-  <si>
-    <t>Time taken to chunk files in seconds</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Map phase Time in seconds</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Reduce Phase Time in seconds</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>tts</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Input data</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>chunk size</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>map</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>reduce</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>tts</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>(1+1)2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>(2+2)4</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>(4+4)8</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>(5+5)10</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Map</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Reduce</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>chunks</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>seqal</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Map</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>reduce</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>map</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>intermediate data to be transferred =</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>mahine used -sierra</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>sequences</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>4GB</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>8GB</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Map</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>chunktime</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>chunktime</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>intermediate data</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>comparision.dat</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SEQAL</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>local-PMR</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>distributed-PMR</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Mean tts</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>std tts</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>mean tts</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>stdtts</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>mean time taken for reduce phase</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>stderr for reduce phase phase time</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Varying chunk size ,  Input Size = 10GB, Number of workers - 32, Number of reduces -8</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Mean Map phase</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Stdev</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Reduced output size  3120 MB  which is 31.2% of input data</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>mean map phase</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>File Transfer in seconds</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Size of data transferred in MB from Map to reduce phase</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>reduce Output data size in MB</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>duplicate  data size in MB</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Varying Number of chunk size - II</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Varying Number of chunk size - III</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>number of reads</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Number of chunks created</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Time taken to chunk files in seconds</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Map phase Time in seconds - I</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Reduce Phase Time in seconds - I</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Map phase Time in seconds - II</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Reduce Phase Time in seconds-II</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Map phase Time in seconds-III</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>input data</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>mean time taken for map phase</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>stderr in map phase time</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>input 2GB, sequences=3805921, chunksize=128MB, number of reduces=8</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>sequences per chunk</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Varying Input size - III</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>mean chunk time</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>stderr chunk time</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>mean map phase</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>stderr in map phase</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>mean reduce phase</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>stderr reduce phase</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Varying Input size, chunk size=625000, number  of reduces=8, number of workers=32</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Input data size in GB</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Total Time to solution in  secs</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>stderr in chunk time</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Reduce Phase Time in seconds - III</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Mean</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>stderr</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>mean</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Varying chunk size ,  Input Size = 10GB, Number of workers - 32, Number of reduces -8</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>number of reads</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Number of chunks created</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Time taken to chunk files in seconds</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>prq</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2GB</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Mean Map phase</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>stderr for map phase</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>mean reduce phase</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>stderr for reduce phase</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">Mean </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Stdev</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">Time to transfer files files between map &amp; reduce phase is </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Data transfer in MB between map &amp; reduce phase is</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -555,7 +607,11 @@
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
+    <font>
+      <sz val="10"/>
+      <name val="Verdana"/>
+    </font>
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -641,31 +697,34 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -896,11 +955,11 @@
           </c:val>
         </c:ser>
         <c:overlap val="100"/>
-        <c:axId val="536002008"/>
-        <c:axId val="535972216"/>
+        <c:axId val="497128904"/>
+        <c:axId val="497627944"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="536002008"/>
+        <c:axId val="497128904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -924,14 +983,14 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="535972216"/>
+        <c:crossAx val="497627944"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="535972216"/>
+        <c:axId val="497627944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -956,7 +1015,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="536002008"/>
+        <c:crossAx val="497128904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1043,23 +1102,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="555140024"/>
-        <c:axId val="555143000"/>
+        <c:axId val="497832056"/>
+        <c:axId val="497835032"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="555140024"/>
+        <c:axId val="497832056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="555143000"/>
+        <c:crossAx val="497835032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="555143000"/>
+        <c:axId val="497835032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1067,7 +1126,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="555140024"/>
+        <c:crossAx val="497832056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1191,7 +1250,7 @@
             <c:errValType val="cust"/>
             <c:plus>
               <c:numRef>
-                <c:f>Sheet1!$Q$12:$Q$14</c:f>
+                <c:f>Sheet1!$Q$27:$Q$29</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
@@ -1209,7 +1268,7 @@
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>Sheet1!$Q$12:$Q$14</c:f>
+                <c:f>Sheet1!$Q$27:$Q$29</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
@@ -1246,7 +1305,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$P$12:$P$14</c:f>
+              <c:f>Sheet1!$P$27:$P$29</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1263,11 +1322,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="555195480"/>
-        <c:axId val="555202664"/>
+        <c:axId val="497902952"/>
+        <c:axId val="497910136"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="555195480"/>
+        <c:axId val="497902952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1292,14 +1351,14 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="555202664"/>
+        <c:crossAx val="497910136"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="555202664"/>
+        <c:axId val="497910136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1324,7 +1383,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="555195480"/>
+        <c:crossAx val="497902952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1538,11 +1597,11 @@
           </c:val>
         </c:ser>
         <c:overlap val="100"/>
-        <c:axId val="535899944"/>
-        <c:axId val="535894072"/>
+        <c:axId val="497522872"/>
+        <c:axId val="497530072"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="535899944"/>
+        <c:axId val="497522872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1566,14 +1625,14 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="535894072"/>
+        <c:crossAx val="497530072"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="535894072"/>
+        <c:axId val="497530072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1598,7 +1657,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="535899944"/>
+        <c:crossAx val="497522872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1894,11 +1953,11 @@
           </c:val>
         </c:ser>
         <c:overlap val="100"/>
-        <c:axId val="535852936"/>
-        <c:axId val="535844264"/>
+        <c:axId val="497544136"/>
+        <c:axId val="497435688"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="535852936"/>
+        <c:axId val="497544136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1922,14 +1981,14 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="535844264"/>
+        <c:crossAx val="497435688"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="535844264"/>
+        <c:axId val="497435688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1954,7 +2013,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="535852936"/>
+        <c:crossAx val="497544136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2191,11 +2250,11 @@
           </c:val>
         </c:ser>
         <c:overlap val="100"/>
-        <c:axId val="554900808"/>
-        <c:axId val="554909112"/>
+        <c:axId val="497384776"/>
+        <c:axId val="497324376"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="554900808"/>
+        <c:axId val="497384776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2219,14 +2278,14 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="554909112"/>
+        <c:crossAx val="497324376"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="554909112"/>
+        <c:axId val="497324376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2251,7 +2310,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="554900808"/>
+        <c:crossAx val="497384776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2464,11 +2523,11 @@
           </c:val>
         </c:ser>
         <c:overlap val="100"/>
-        <c:axId val="554945624"/>
-        <c:axId val="554953880"/>
+        <c:axId val="497639784"/>
+        <c:axId val="497649464"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="554945624"/>
+        <c:axId val="497639784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2492,14 +2551,14 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="554953880"/>
+        <c:crossAx val="497649464"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="554953880"/>
+        <c:axId val="497649464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2524,7 +2583,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="554945624"/>
+        <c:crossAx val="497639784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2820,11 +2879,11 @@
           </c:val>
         </c:ser>
         <c:overlap val="100"/>
-        <c:axId val="554999048"/>
-        <c:axId val="555004920"/>
+        <c:axId val="497694552"/>
+        <c:axId val="497700424"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="554999048"/>
+        <c:axId val="497694552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2848,14 +2907,14 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="555004920"/>
+        <c:crossAx val="497700424"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="555004920"/>
+        <c:axId val="497700424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2880,7 +2939,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="554999048"/>
+        <c:crossAx val="497694552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2999,11 +3058,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="555034584"/>
-        <c:axId val="555043400"/>
+        <c:axId val="497713000"/>
+        <c:axId val="497719208"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="555034584"/>
+        <c:axId val="497713000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3027,12 +3086,12 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="555043400"/>
+        <c:crossAx val="497719208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="555043400"/>
+        <c:axId val="497719208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3057,7 +3116,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="555034584"/>
+        <c:crossAx val="497713000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3138,23 +3197,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="555079448"/>
-        <c:axId val="555082424"/>
+        <c:axId val="497771592"/>
+        <c:axId val="497774568"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="555079448"/>
+        <c:axId val="497771592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="555082424"/>
+        <c:crossAx val="497774568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="555082424"/>
+        <c:axId val="497774568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3162,7 +3221,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="555079448"/>
+        <c:crossAx val="497771592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3243,23 +3302,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="555109672"/>
-        <c:axId val="555112648"/>
+        <c:axId val="497801720"/>
+        <c:axId val="497804696"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="555109672"/>
+        <c:axId val="497801720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="555112648"/>
+        <c:crossAx val="497804696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="555112648"/>
+        <c:axId val="497804696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3267,7 +3326,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="555109672"/>
+        <c:crossAx val="497801720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3599,16 +3658,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>203200</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>139700</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>889000</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>12700</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>698500</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3653,17 +3712,17 @@
       <sheetName val="Sheet9"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="5" refreshError="1"/>
+      <sheetData sheetId="6" refreshError="1"/>
+      <sheetData sheetId="7" refreshError="1"/>
+      <sheetData sheetId="8" refreshError="1"/>
+      <sheetData sheetId="9" refreshError="1"/>
+      <sheetData sheetId="10" refreshError="1"/>
       <sheetData sheetId="11">
         <row r="5">
           <cell r="A5">
@@ -3884,11 +3943,11 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="12"/>
-      <sheetData sheetId="13"/>
-      <sheetData sheetId="14"/>
-      <sheetData sheetId="15"/>
-      <sheetData sheetId="16"/>
+      <sheetData sheetId="12" refreshError="1"/>
+      <sheetData sheetId="13" refreshError="1"/>
+      <sheetData sheetId="14" refreshError="1"/>
+      <sheetData sheetId="15" refreshError="1"/>
+      <sheetData sheetId="16" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -4230,7 +4289,7 @@
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
       <c r="G1" s="1" t="s">
-        <v>31</v>
+        <v>70</v>
       </c>
       <c r="H1" s="1"/>
       <c r="I1" s="2"/>
@@ -4242,46 +4301,46 @@
     </row>
     <row r="2" spans="1:14" ht="71" thickBot="1">
       <c r="A2" s="3" t="s">
-        <v>32</v>
+        <v>71</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>33</v>
+        <v>72</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>34</v>
+        <v>84</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>35</v>
+        <v>85</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>36</v>
+        <v>86</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>37</v>
+        <v>87</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>38</v>
+        <v>88</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>39</v>
+        <v>89</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>40</v>
+        <v>90</v>
       </c>
       <c r="J2" s="7" t="s">
-        <v>41</v>
+        <v>91</v>
       </c>
       <c r="K2" s="8" t="s">
-        <v>83</v>
+        <v>118</v>
       </c>
       <c r="L2" s="8" t="s">
-        <v>84</v>
+        <v>17</v>
       </c>
       <c r="M2" s="8" t="s">
-        <v>85</v>
+        <v>18</v>
       </c>
       <c r="N2" s="8" t="s">
-        <v>86</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:14">
@@ -4460,7 +4519,7 @@
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="1" t="s">
-        <v>87</v>
+        <v>20</v>
       </c>
       <c r="H8" s="1"/>
       <c r="I8" s="2"/>
@@ -4472,46 +4531,46 @@
     </row>
     <row r="9" spans="1:14" ht="71" thickBot="1">
       <c r="A9" s="3" t="s">
-        <v>32</v>
+        <v>71</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>33</v>
+        <v>72</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>34</v>
+        <v>84</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>35</v>
+        <v>85</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>36</v>
+        <v>86</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>37</v>
+        <v>87</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>38</v>
+        <v>88</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>39</v>
+        <v>89</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>40</v>
+        <v>90</v>
       </c>
       <c r="J9" s="7" t="s">
-        <v>41</v>
+        <v>91</v>
       </c>
       <c r="K9" s="8" t="s">
-        <v>83</v>
+        <v>118</v>
       </c>
       <c r="L9" s="8" t="s">
-        <v>84</v>
+        <v>17</v>
       </c>
       <c r="M9" s="8" t="s">
-        <v>85</v>
+        <v>18</v>
       </c>
       <c r="N9" s="8" t="s">
-        <v>86</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:14">
@@ -4690,7 +4749,7 @@
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
       <c r="G16" s="1" t="s">
-        <v>88</v>
+        <v>21</v>
       </c>
       <c r="H16" s="1"/>
       <c r="I16" s="2"/>
@@ -4702,46 +4761,46 @@
     </row>
     <row r="17" spans="1:19" ht="71" thickBot="1">
       <c r="A17" s="3" t="s">
-        <v>32</v>
+        <v>71</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>33</v>
+        <v>72</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>34</v>
+        <v>84</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>35</v>
+        <v>85</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>36</v>
+        <v>86</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>37</v>
+        <v>87</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>38</v>
+        <v>88</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>39</v>
+        <v>89</v>
       </c>
       <c r="I17" s="7" t="s">
-        <v>40</v>
+        <v>90</v>
       </c>
       <c r="J17" s="7" t="s">
-        <v>41</v>
+        <v>91</v>
       </c>
       <c r="K17" s="8" t="s">
-        <v>83</v>
+        <v>118</v>
       </c>
       <c r="L17" s="8" t="s">
-        <v>84</v>
+        <v>17</v>
       </c>
       <c r="M17" s="8" t="s">
-        <v>85</v>
+        <v>18</v>
       </c>
       <c r="N17" s="8" t="s">
-        <v>86</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:19">
@@ -4914,46 +4973,46 @@
     </row>
     <row r="24" spans="1:19" ht="46" thickBot="1">
       <c r="A24" s="3" t="s">
-        <v>89</v>
+        <v>22</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>90</v>
+        <v>23</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>38</v>
+        <v>88</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>91</v>
+        <v>24</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>92</v>
+        <v>25</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>93</v>
+        <v>26</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>94</v>
+        <v>119</v>
       </c>
       <c r="H24" s="7" t="s">
-        <v>95</v>
+        <v>120</v>
       </c>
       <c r="I24" s="7" t="s">
-        <v>96</v>
+        <v>121</v>
       </c>
       <c r="J24" s="7" t="s">
-        <v>113</v>
+        <v>50</v>
       </c>
       <c r="K24" s="8" t="s">
-        <v>114</v>
+        <v>51</v>
       </c>
       <c r="L24" s="8" t="s">
-        <v>115</v>
+        <v>52</v>
       </c>
       <c r="M24" s="8" t="s">
-        <v>116</v>
+        <v>53</v>
       </c>
       <c r="N24" s="8" t="s">
-        <v>115</v>
+        <v>52</v>
       </c>
     </row>
     <row r="25" spans="1:19">
@@ -5150,39 +5209,39 @@
     </row>
     <row r="31" spans="1:19">
       <c r="D31" t="s">
-        <v>117</v>
+        <v>54</v>
       </c>
     </row>
     <row r="32" spans="1:19" ht="46" thickBot="1">
       <c r="D32" s="3" t="s">
-        <v>118</v>
+        <v>55</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>119</v>
+        <v>56</v>
       </c>
       <c r="F32" s="6" t="s">
-        <v>38</v>
+        <v>88</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>120</v>
+        <v>57</v>
       </c>
       <c r="H32" s="8" t="s">
-        <v>123</v>
+        <v>73</v>
       </c>
       <c r="I32" s="8" t="s">
-        <v>124</v>
+        <v>74</v>
       </c>
       <c r="J32" s="8" t="s">
-        <v>125</v>
+        <v>75</v>
       </c>
       <c r="K32" s="8" t="s">
-        <v>126</v>
+        <v>76</v>
       </c>
       <c r="R32" t="s">
-        <v>127</v>
+        <v>77</v>
       </c>
       <c r="S32" t="s">
-        <v>128</v>
+        <v>78</v>
       </c>
     </row>
     <row r="33" spans="4:19">
@@ -5212,7 +5271,7 @@
         <v>3.8921515186908202</v>
       </c>
       <c r="M33" t="s">
-        <v>129</v>
+        <v>79</v>
       </c>
       <c r="R33">
         <v>1.59</v>
@@ -5248,7 +5307,7 @@
         <v>1.2000589337377248</v>
       </c>
       <c r="M34" t="s">
-        <v>130</v>
+        <v>80</v>
       </c>
       <c r="R34" s="10">
         <v>9155.6200000000008</v>
@@ -5284,7 +5343,7 @@
         <v>2.2325377438638392</v>
       </c>
       <c r="M35" t="s">
-        <v>22</v>
+        <v>45</v>
       </c>
     </row>
     <row r="36" spans="4:19">
@@ -5314,17 +5373,17 @@
         <v>2.6636263501721773</v>
       </c>
       <c r="M36" t="s">
-        <v>23</v>
+        <v>62</v>
       </c>
     </row>
     <row r="37" spans="4:19">
       <c r="M37" t="s">
-        <v>24</v>
+        <v>63</v>
       </c>
     </row>
     <row r="60" spans="25:25">
       <c r="Y60" t="s">
-        <v>25</v>
+        <v>64</v>
       </c>
     </row>
     <row r="65" spans="1:14" ht="15">
@@ -5335,7 +5394,7 @@
       <c r="E65" s="2"/>
       <c r="F65" s="2"/>
       <c r="G65" s="1" t="s">
-        <v>26</v>
+        <v>65</v>
       </c>
       <c r="H65" s="1"/>
       <c r="I65" s="2"/>
@@ -5347,46 +5406,46 @@
     </row>
     <row r="66" spans="1:14" ht="71" thickBot="1">
       <c r="A66" s="3" t="s">
-        <v>32</v>
+        <v>71</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>33</v>
+        <v>72</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>34</v>
+        <v>84</v>
       </c>
       <c r="D66" s="5" t="s">
-        <v>35</v>
+        <v>85</v>
       </c>
       <c r="E66" s="3" t="s">
-        <v>36</v>
+        <v>86</v>
       </c>
       <c r="F66" s="3" t="s">
-        <v>37</v>
+        <v>87</v>
       </c>
       <c r="G66" s="6" t="s">
-        <v>38</v>
+        <v>88</v>
       </c>
       <c r="H66" s="3" t="s">
-        <v>39</v>
+        <v>89</v>
       </c>
       <c r="I66" s="7" t="s">
-        <v>40</v>
+        <v>90</v>
       </c>
       <c r="J66" s="7" t="s">
-        <v>41</v>
+        <v>91</v>
       </c>
       <c r="K66" s="8" t="s">
-        <v>83</v>
+        <v>118</v>
       </c>
       <c r="L66" s="8" t="s">
-        <v>84</v>
+        <v>17</v>
       </c>
       <c r="M66" s="8" t="s">
-        <v>85</v>
+        <v>18</v>
       </c>
       <c r="N66" s="8" t="s">
-        <v>86</v>
+        <v>19</v>
       </c>
     </row>
     <row r="67" spans="1:14">
@@ -5523,7 +5582,7 @@
       <c r="E72" s="2"/>
       <c r="F72" s="2"/>
       <c r="G72" s="1" t="s">
-        <v>27</v>
+        <v>66</v>
       </c>
       <c r="H72" s="1"/>
       <c r="I72" s="2"/>
@@ -5535,46 +5594,46 @@
     </row>
     <row r="73" spans="1:14" ht="71" thickBot="1">
       <c r="A73" s="3" t="s">
-        <v>32</v>
+        <v>71</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>33</v>
+        <v>72</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>34</v>
+        <v>84</v>
       </c>
       <c r="D73" s="5" t="s">
-        <v>35</v>
+        <v>85</v>
       </c>
       <c r="E73" s="3" t="s">
-        <v>36</v>
+        <v>86</v>
       </c>
       <c r="F73" s="3" t="s">
-        <v>37</v>
+        <v>87</v>
       </c>
       <c r="G73" s="6" t="s">
-        <v>38</v>
+        <v>88</v>
       </c>
       <c r="H73" s="3" t="s">
-        <v>39</v>
+        <v>89</v>
       </c>
       <c r="I73" s="7" t="s">
-        <v>40</v>
+        <v>90</v>
       </c>
       <c r="J73" s="7" t="s">
-        <v>41</v>
+        <v>91</v>
       </c>
       <c r="K73" s="8" t="s">
-        <v>83</v>
+        <v>118</v>
       </c>
       <c r="L73" s="8" t="s">
-        <v>84</v>
+        <v>17</v>
       </c>
       <c r="M73" s="8" t="s">
-        <v>85</v>
+        <v>18</v>
       </c>
       <c r="N73" s="8" t="s">
-        <v>86</v>
+        <v>19</v>
       </c>
     </row>
     <row r="74" spans="1:14">
@@ -5711,7 +5770,7 @@
       <c r="E79" s="2"/>
       <c r="F79" s="2"/>
       <c r="G79" s="1" t="s">
-        <v>28</v>
+        <v>67</v>
       </c>
       <c r="H79" s="1"/>
       <c r="I79" s="2"/>
@@ -5723,46 +5782,46 @@
     </row>
     <row r="80" spans="1:14" ht="71" thickBot="1">
       <c r="A80" s="3" t="s">
-        <v>32</v>
+        <v>71</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>33</v>
+        <v>72</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>34</v>
+        <v>84</v>
       </c>
       <c r="D80" s="5" t="s">
-        <v>35</v>
+        <v>85</v>
       </c>
       <c r="E80" s="3" t="s">
-        <v>36</v>
+        <v>86</v>
       </c>
       <c r="F80" s="3" t="s">
-        <v>37</v>
+        <v>87</v>
       </c>
       <c r="G80" s="6" t="s">
-        <v>38</v>
+        <v>88</v>
       </c>
       <c r="H80" s="3" t="s">
-        <v>39</v>
+        <v>89</v>
       </c>
       <c r="I80" s="7" t="s">
-        <v>40</v>
+        <v>90</v>
       </c>
       <c r="J80" s="7" t="s">
-        <v>41</v>
+        <v>91</v>
       </c>
       <c r="K80" s="8" t="s">
-        <v>83</v>
+        <v>118</v>
       </c>
       <c r="L80" s="8" t="s">
-        <v>84</v>
+        <v>17</v>
       </c>
       <c r="M80" s="8" t="s">
-        <v>85</v>
+        <v>18</v>
       </c>
       <c r="N80" s="8" t="s">
-        <v>86</v>
+        <v>19</v>
       </c>
     </row>
     <row r="81" spans="1:12">
@@ -5884,40 +5943,40 @@
     </row>
     <row r="87" spans="1:12" ht="71" thickBot="1">
       <c r="A87" s="3" t="s">
-        <v>29</v>
+        <v>68</v>
       </c>
       <c r="B87" s="6" t="s">
-        <v>38</v>
+        <v>88</v>
       </c>
       <c r="C87" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="D87" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="E87" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="F87" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="G87" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="H87" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="I87" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="J87" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="K87" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="D87" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="E87" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="F87" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="G87" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="H87" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="I87" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="J87" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="K87" s="8" t="s">
-        <v>2</v>
-      </c>
       <c r="L87" s="8" t="s">
-        <v>3</v>
+        <v>31</v>
       </c>
     </row>
     <row r="88" spans="1:12">
@@ -6051,27 +6110,27 @@
     </row>
     <row r="94" spans="1:12">
       <c r="A94" t="s">
-        <v>4</v>
+        <v>32</v>
       </c>
     </row>
     <row r="96" spans="1:12" ht="33" thickBot="1">
       <c r="A96" s="3" t="s">
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="B96" s="5" t="s">
-        <v>38</v>
+        <v>88</v>
       </c>
       <c r="C96" s="6" t="s">
-        <v>6</v>
+        <v>34</v>
       </c>
       <c r="D96" s="3" t="s">
-        <v>7</v>
+        <v>35</v>
       </c>
       <c r="E96" s="3" t="s">
-        <v>8</v>
+        <v>36</v>
       </c>
       <c r="F96" s="5" t="s">
-        <v>9</v>
+        <v>37</v>
       </c>
       <c r="G96" s="11"/>
     </row>
@@ -6137,7 +6196,7 @@
     </row>
     <row r="100" spans="1:22">
       <c r="V100" t="s">
-        <v>10</v>
+        <v>38</v>
       </c>
     </row>
     <row r="101" spans="1:22">
@@ -6147,27 +6206,27 @@
     </row>
     <row r="105" spans="1:22">
       <c r="I105" t="s">
-        <v>129</v>
+        <v>79</v>
       </c>
     </row>
     <row r="106" spans="1:22">
       <c r="I106" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
     </row>
     <row r="107" spans="1:22">
       <c r="I107" t="s">
-        <v>12</v>
+        <v>40</v>
       </c>
     </row>
     <row r="108" spans="1:22">
       <c r="I108" t="s">
-        <v>13</v>
+        <v>138</v>
       </c>
     </row>
     <row r="109" spans="1:22">
       <c r="I109" t="s">
-        <v>14</v>
+        <v>139</v>
       </c>
     </row>
     <row r="120" spans="1:17" ht="15">
@@ -6178,7 +6237,7 @@
       <c r="E120" s="2"/>
       <c r="F120" s="2"/>
       <c r="G120" s="1" t="s">
-        <v>15</v>
+        <v>140</v>
       </c>
       <c r="H120" s="1"/>
       <c r="I120" s="2"/>
@@ -6190,46 +6249,46 @@
     </row>
     <row r="121" spans="1:17" ht="71" thickBot="1">
       <c r="A121" s="3" t="s">
-        <v>32</v>
+        <v>71</v>
       </c>
       <c r="B121" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C121" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="D121" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="E121" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="F121" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="G121" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="H121" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="C121" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D121" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="E121" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="F121" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="G121" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="H121" s="3" t="s">
-        <v>39</v>
-      </c>
       <c r="I121" s="7" t="s">
-        <v>40</v>
+        <v>90</v>
       </c>
       <c r="J121" s="7" t="s">
-        <v>41</v>
+        <v>91</v>
       </c>
       <c r="K121" s="8" t="s">
-        <v>83</v>
+        <v>118</v>
       </c>
       <c r="L121" s="8" t="s">
-        <v>84</v>
+        <v>17</v>
       </c>
       <c r="M121" s="8" t="s">
-        <v>85</v>
+        <v>18</v>
       </c>
       <c r="N121" s="8" t="s">
-        <v>17</v>
+        <v>142</v>
       </c>
     </row>
     <row r="122" spans="1:17">
@@ -6395,7 +6454,7 @@
       <c r="E129" s="2"/>
       <c r="F129" s="2"/>
       <c r="G129" s="1" t="s">
-        <v>18</v>
+        <v>143</v>
       </c>
       <c r="H129" s="1"/>
       <c r="I129" s="2"/>
@@ -6407,46 +6466,46 @@
     </row>
     <row r="130" spans="1:14" ht="71" thickBot="1">
       <c r="A130" s="3" t="s">
-        <v>32</v>
+        <v>71</v>
       </c>
       <c r="B130" s="3" t="s">
-        <v>33</v>
+        <v>72</v>
       </c>
       <c r="C130" s="4" t="s">
-        <v>34</v>
+        <v>84</v>
       </c>
       <c r="D130" s="5" t="s">
-        <v>35</v>
+        <v>85</v>
       </c>
       <c r="E130" s="3" t="s">
-        <v>36</v>
+        <v>86</v>
       </c>
       <c r="F130" s="3" t="s">
-        <v>37</v>
+        <v>87</v>
       </c>
       <c r="G130" s="6" t="s">
-        <v>38</v>
+        <v>88</v>
       </c>
       <c r="H130" s="3" t="s">
-        <v>39</v>
+        <v>89</v>
       </c>
       <c r="I130" s="7" t="s">
-        <v>40</v>
+        <v>90</v>
       </c>
       <c r="J130" s="7" t="s">
-        <v>41</v>
+        <v>91</v>
       </c>
       <c r="K130" s="8" t="s">
-        <v>83</v>
+        <v>118</v>
       </c>
       <c r="L130" s="8" t="s">
-        <v>84</v>
+        <v>17</v>
       </c>
       <c r="M130" s="8" t="s">
-        <v>85</v>
+        <v>18</v>
       </c>
       <c r="N130" s="8" t="s">
-        <v>86</v>
+        <v>19</v>
       </c>
     </row>
     <row r="131" spans="1:14">
@@ -6586,7 +6645,7 @@
       <c r="E139" s="2"/>
       <c r="F139" s="2"/>
       <c r="G139" s="1" t="s">
-        <v>102</v>
+        <v>126</v>
       </c>
       <c r="H139" s="1"/>
       <c r="I139" s="2"/>
@@ -6598,46 +6657,46 @@
     </row>
     <row r="140" spans="1:14" ht="71" thickBot="1">
       <c r="A140" s="3" t="s">
-        <v>32</v>
+        <v>71</v>
       </c>
       <c r="B140" s="3" t="s">
-        <v>33</v>
+        <v>72</v>
       </c>
       <c r="C140" s="4" t="s">
-        <v>34</v>
+        <v>84</v>
       </c>
       <c r="D140" s="5" t="s">
-        <v>35</v>
+        <v>85</v>
       </c>
       <c r="E140" s="3" t="s">
-        <v>36</v>
+        <v>86</v>
       </c>
       <c r="F140" s="3" t="s">
-        <v>37</v>
+        <v>87</v>
       </c>
       <c r="G140" s="6" t="s">
-        <v>38</v>
+        <v>88</v>
       </c>
       <c r="H140" s="3" t="s">
-        <v>39</v>
+        <v>89</v>
       </c>
       <c r="I140" s="7" t="s">
-        <v>40</v>
+        <v>90</v>
       </c>
       <c r="J140" s="7" t="s">
-        <v>41</v>
+        <v>91</v>
       </c>
       <c r="K140" s="8" t="s">
-        <v>83</v>
+        <v>118</v>
       </c>
       <c r="L140" s="8" t="s">
-        <v>84</v>
+        <v>17</v>
       </c>
       <c r="M140" s="8" t="s">
-        <v>85</v>
+        <v>18</v>
       </c>
       <c r="N140" s="8" t="s">
-        <v>17</v>
+        <v>142</v>
       </c>
     </row>
     <row r="141" spans="1:14">
@@ -6771,55 +6830,55 @@
     </row>
     <row r="147" spans="1:17" ht="43" thickBot="1">
       <c r="A147" s="4" t="s">
-        <v>34</v>
+        <v>84</v>
       </c>
       <c r="B147" s="6" t="s">
-        <v>38</v>
+        <v>88</v>
       </c>
       <c r="C147" s="3" t="s">
-        <v>39</v>
+        <v>89</v>
       </c>
       <c r="D147" s="3" t="s">
-        <v>39</v>
+        <v>89</v>
       </c>
       <c r="E147" s="3" t="s">
-        <v>39</v>
+        <v>89</v>
       </c>
       <c r="F147" s="3" t="s">
-        <v>103</v>
+        <v>127</v>
       </c>
       <c r="G147" s="3" t="s">
-        <v>104</v>
+        <v>128</v>
       </c>
       <c r="H147" s="7" t="s">
-        <v>40</v>
+        <v>90</v>
       </c>
       <c r="I147" s="7" t="s">
-        <v>40</v>
+        <v>90</v>
       </c>
       <c r="J147" s="7" t="s">
-        <v>40</v>
+        <v>90</v>
       </c>
       <c r="K147" s="8" t="s">
-        <v>105</v>
+        <v>129</v>
       </c>
       <c r="L147" s="8" t="s">
-        <v>106</v>
+        <v>130</v>
       </c>
       <c r="M147" s="7" t="s">
-        <v>41</v>
+        <v>91</v>
       </c>
       <c r="N147" s="7" t="s">
-        <v>41</v>
+        <v>91</v>
       </c>
       <c r="O147" s="7" t="s">
-        <v>41</v>
+        <v>91</v>
       </c>
       <c r="P147" s="8" t="s">
-        <v>107</v>
+        <v>131</v>
       </c>
       <c r="Q147" s="8" t="s">
-        <v>108</v>
+        <v>132</v>
       </c>
     </row>
     <row r="148" spans="1:17">
@@ -6983,36 +7042,36 @@
     </row>
     <row r="153" spans="1:17">
       <c r="C153" t="s">
-        <v>109</v>
+        <v>46</v>
       </c>
     </row>
     <row r="155" spans="1:17" ht="49" thickBot="1">
       <c r="C155" s="3" t="s">
-        <v>110</v>
+        <v>47</v>
       </c>
       <c r="D155" s="5" t="s">
-        <v>35</v>
+        <v>85</v>
       </c>
       <c r="E155" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="F155" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="G155" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H155" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="I155" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="J155" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="F155" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="G155" s="3" t="s">
+      <c r="K155" s="8" t="s">
         <v>112</v>
-      </c>
-      <c r="H155" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="I155" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="J155" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="K155" s="8" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="156" spans="1:17">
@@ -7106,8 +7165,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
-  <phoneticPr fontId="1" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>
   <extLst>
@@ -7122,41 +7180,41 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A3:I83"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <sheetData>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>78</v>
+        <v>113</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="46" thickBot="1">
       <c r="A4" s="3" t="s">
-        <v>33</v>
+        <v>72</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>35</v>
+        <v>85</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>38</v>
+        <v>88</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>39</v>
+        <v>89</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>79</v>
+        <v>114</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>124</v>
+        <v>74</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>125</v>
+        <v>75</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>126</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -7269,15 +7327,15 @@
     </row>
     <row r="31" spans="2:8">
       <c r="G31" t="s">
-        <v>127</v>
+        <v>77</v>
       </c>
       <c r="H31" t="s">
-        <v>80</v>
+        <v>115</v>
       </c>
     </row>
     <row r="32" spans="2:8">
       <c r="B32" t="s">
-        <v>129</v>
+        <v>79</v>
       </c>
       <c r="G32">
         <v>1.59</v>
@@ -7288,7 +7346,7 @@
     </row>
     <row r="33" spans="1:8" ht="15">
       <c r="B33" t="s">
-        <v>130</v>
+        <v>80</v>
       </c>
       <c r="G33" s="10">
         <v>9155.6200000000008</v>
@@ -7299,42 +7357,42 @@
     </row>
     <row r="34" spans="1:8">
       <c r="B34" t="s">
-        <v>81</v>
+        <v>116</v>
       </c>
     </row>
     <row r="35" spans="1:8">
       <c r="B35" t="s">
-        <v>13</v>
+        <v>138</v>
       </c>
     </row>
     <row r="36" spans="1:8">
       <c r="B36" t="s">
-        <v>14</v>
+        <v>139</v>
       </c>
     </row>
     <row r="48" spans="1:8">
       <c r="A48" t="s">
-        <v>4</v>
+        <v>32</v>
       </c>
     </row>
     <row r="50" spans="1:7" ht="33" thickBot="1">
       <c r="A50" s="3" t="s">
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>38</v>
+        <v>88</v>
       </c>
       <c r="C50" s="6" t="s">
-        <v>6</v>
+        <v>34</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>7</v>
+        <v>35</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>8</v>
+        <v>36</v>
       </c>
       <c r="F50" s="5" t="s">
-        <v>9</v>
+        <v>37</v>
       </c>
       <c r="G50" s="11"/>
     </row>
@@ -7400,15 +7458,15 @@
     </row>
     <row r="64" spans="1:7">
       <c r="B64" t="s">
-        <v>129</v>
+        <v>79</v>
       </c>
       <c r="G64" t="s">
-        <v>10</v>
+        <v>38</v>
       </c>
     </row>
     <row r="65" spans="1:9" ht="15">
       <c r="B65" t="s">
-        <v>130</v>
+        <v>80</v>
       </c>
       <c r="G65">
         <v>9144.5290000000005</v>
@@ -7417,51 +7475,51 @@
     </row>
     <row r="66" spans="1:9">
       <c r="B66" t="s">
-        <v>81</v>
+        <v>116</v>
       </c>
     </row>
     <row r="67" spans="1:9">
       <c r="B67" t="s">
-        <v>13</v>
+        <v>138</v>
       </c>
     </row>
     <row r="68" spans="1:9">
       <c r="B68" t="s">
-        <v>14</v>
+        <v>139</v>
       </c>
     </row>
     <row r="78" spans="1:9">
       <c r="A78" t="s">
-        <v>109</v>
+        <v>46</v>
       </c>
     </row>
     <row r="80" spans="1:9" ht="49" thickBot="1">
       <c r="A80" s="3" t="s">
-        <v>110</v>
+        <v>47</v>
       </c>
       <c r="B80" s="5" t="s">
-        <v>35</v>
+        <v>85</v>
       </c>
       <c r="C80" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="D80" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="E80" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F80" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="G80" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="H80" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="D80" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="E80" s="3" t="s">
+      <c r="I80" s="8" t="s">
         <v>112</v>
-      </c>
-      <c r="F80" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="G80" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="H80" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="I80" s="8" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="81" spans="1:9">
@@ -7555,8 +7613,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
-  <phoneticPr fontId="1" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>
   <extLst>
@@ -7569,70 +7626,70 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A2:Q79"/>
+  <dimension ref="A2:Q157"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <sheetData>
     <row r="2" spans="1:17">
       <c r="A2" t="s">
-        <v>55</v>
+        <v>95</v>
       </c>
       <c r="B2" t="s">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="H2" t="s">
-        <v>60</v>
+        <v>99</v>
       </c>
     </row>
     <row r="4" spans="1:17">
       <c r="A4" t="s">
+        <v>122</v>
+      </c>
+      <c r="B4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" t="s">
+        <v>96</v>
+      </c>
+      <c r="G4" t="s">
         <v>97</v>
       </c>
-      <c r="B4" t="s">
-        <v>54</v>
-      </c>
-      <c r="C4" t="s">
-        <v>52</v>
-      </c>
-      <c r="D4" t="s">
-        <v>53</v>
-      </c>
-      <c r="E4" t="s">
-        <v>47</v>
-      </c>
-      <c r="F4" t="s">
-        <v>56</v>
-      </c>
-      <c r="G4" t="s">
-        <v>57</v>
-      </c>
       <c r="H4" t="s">
-        <v>42</v>
+        <v>92</v>
       </c>
       <c r="I4" t="s">
-        <v>58</v>
+        <v>98</v>
       </c>
       <c r="J4" t="s">
-        <v>46</v>
+        <v>3</v>
       </c>
       <c r="K4" t="s">
-        <v>42</v>
+        <v>92</v>
       </c>
       <c r="L4" t="s">
-        <v>61</v>
+        <v>100</v>
       </c>
       <c r="M4" t="s">
-        <v>72</v>
+        <v>107</v>
       </c>
       <c r="N4" t="s">
-        <v>73</v>
+        <v>108</v>
       </c>
       <c r="O4" t="s">
-        <v>101</v>
+        <v>125</v>
       </c>
     </row>
     <row r="5" spans="1:17">
@@ -7786,54 +7843,47 @@
         <v>118.91205116011055</v>
       </c>
     </row>
-    <row r="11" spans="1:17">
-      <c r="A11" t="s">
-        <v>97</v>
-      </c>
-      <c r="B11" t="s">
-        <v>65</v>
-      </c>
-      <c r="C11" t="s">
-        <v>64</v>
-      </c>
-      <c r="D11" t="s">
-        <v>53</v>
-      </c>
-      <c r="E11" t="s">
-        <v>42</v>
-      </c>
-      <c r="F11" t="s">
-        <v>65</v>
-      </c>
-      <c r="G11" t="s">
-        <v>64</v>
-      </c>
-      <c r="H11" t="s">
-        <v>53</v>
-      </c>
-      <c r="I11" t="s">
-        <v>42</v>
-      </c>
-      <c r="J11" t="s">
-        <v>66</v>
-      </c>
-      <c r="K11" t="s">
-        <v>64</v>
-      </c>
-      <c r="L11" t="s">
-        <v>53</v>
+    <row r="10" spans="1:17">
+      <c r="A10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" ht="26">
+      <c r="A11" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G11" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="H11" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="I11" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="J11" s="11" t="s">
+        <v>61</v>
       </c>
       <c r="M11" t="s">
-        <v>42</v>
-      </c>
-      <c r="N11" t="s">
-        <v>67</v>
-      </c>
-      <c r="P11" t="s">
-        <v>74</v>
-      </c>
-      <c r="Q11" t="s">
-        <v>75</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:17">
@@ -7841,104 +7891,103 @@
         <v>2</v>
       </c>
       <c r="B12">
-        <v>24.536999999999999</v>
+        <v>116</v>
       </c>
       <c r="C12">
-        <v>1480.663</v>
+        <v>13</v>
       </c>
       <c r="D12">
-        <v>40.225999999999999</v>
+        <v>2451</v>
       </c>
       <c r="E12">
-        <v>1545.4259999999999</v>
+        <v>2469</v>
       </c>
       <c r="F12">
-        <v>24.632000000000001</v>
+        <f>47*60+41</f>
+        <v>2861</v>
       </c>
       <c r="G12">
-        <v>1475.8620000000001</v>
+        <f>D12-B12</f>
+        <v>2335</v>
       </c>
       <c r="H12">
-        <v>40.232999999999997</v>
+        <f>E12-D12</f>
+        <v>18</v>
       </c>
       <c r="I12">
-        <v>1540.7270000000001</v>
+        <f>F12-E12</f>
+        <v>392</v>
       </c>
       <c r="J12">
-        <v>23.358000000000001</v>
-      </c>
-      <c r="K12">
-        <v>1483.2449999999999</v>
-      </c>
-      <c r="L12">
-        <v>41.244999999999997</v>
-      </c>
-      <c r="M12">
-        <f>K12+L12+J12</f>
-        <v>1547.8479999999997</v>
-      </c>
-      <c r="N12">
-        <v>1736.0070000000001</v>
-      </c>
-      <c r="P12">
-        <f>AVERAGE(E12+I12+M12)/3</f>
-        <v>1544.6670000000001</v>
-      </c>
-      <c r="Q12">
-        <f>1.96 * STDEV(E12,I12,M12)/SQRT(3)</f>
-        <v>4.097169079209209</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="M12" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="N12" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="O12" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="P12" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q12" s="11"/>
     </row>
     <row r="13" spans="1:17">
       <c r="A13">
         <v>4</v>
       </c>
       <c r="B13">
-        <v>48.817999999999998</v>
+        <v>116</v>
       </c>
       <c r="C13">
-        <v>2767.5140000000001</v>
+        <v>25</v>
       </c>
       <c r="D13">
-        <v>71.721000000000004</v>
+        <f>66*60+47</f>
+        <v>4007</v>
       </c>
       <c r="E13">
-        <v>2888.0540000000001</v>
+        <f>67*60+41</f>
+        <v>4061</v>
       </c>
       <c r="F13">
-        <v>49.430999999999997</v>
+        <f>80*60+29</f>
+        <v>4829</v>
       </c>
       <c r="G13">
-        <v>2776.223</v>
+        <f t="shared" ref="G13" si="2">D13-B13</f>
+        <v>3891</v>
       </c>
       <c r="H13">
-        <v>74.373000000000005</v>
+        <f t="shared" ref="H13:H14" si="3">E13-D13</f>
+        <v>54</v>
       </c>
       <c r="I13">
-        <v>2900.027</v>
+        <f t="shared" ref="I13:I14" si="4">F13-E13</f>
+        <v>768</v>
       </c>
       <c r="J13">
-        <v>49.23</v>
-      </c>
-      <c r="K13">
-        <v>2812.97</v>
-      </c>
-      <c r="L13">
-        <v>76.73</v>
+        <v>16</v>
       </c>
       <c r="M13">
-        <v>2938.93</v>
+        <v>2</v>
       </c>
       <c r="N13">
-        <v>3580.5070000000001</v>
+        <v>115</v>
+      </c>
+      <c r="O13">
+        <v>13</v>
       </c>
       <c r="P13">
-        <f t="shared" ref="P13:P14" si="2">AVERAGE(E13+I13+M13)/3</f>
-        <v>2909.003666666667</v>
+        <f>47*60+36</f>
+        <v>2856</v>
       </c>
       <c r="Q13">
-        <f t="shared" ref="Q13:Q14" si="3">1.96 * STDEV(E13,I13,M13)/SQRT(3)</f>
-        <v>30.100037057320566</v>
+        <f>42*60+28</f>
+        <v>2548</v>
       </c>
     </row>
     <row r="14" spans="1:17">
@@ -7946,328 +7995,659 @@
         <v>8</v>
       </c>
       <c r="B14">
+        <v>109</v>
+      </c>
+      <c r="C14">
+        <v>50</v>
+      </c>
+      <c r="D14">
+        <v>7149</v>
+      </c>
+      <c r="E14">
+        <v>7252</v>
+      </c>
+      <c r="F14">
+        <f>2*60*60+26*60+56</f>
+        <v>8816</v>
+      </c>
+      <c r="G14">
+        <f>D14-B14</f>
+        <v>7040</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="3"/>
+        <v>103</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="4"/>
+        <v>1564</v>
+      </c>
+      <c r="J14">
+        <v>11</v>
+      </c>
+      <c r="N14">
+        <v>143</v>
+      </c>
+      <c r="O14">
+        <v>13</v>
+      </c>
+      <c r="P14">
+        <f>49*60+42</f>
+        <v>2982</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17">
+      <c r="N15">
+        <v>139</v>
+      </c>
+      <c r="O15">
+        <v>13</v>
+      </c>
+      <c r="P15">
+        <f>49*60+14</f>
+        <v>2954</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17">
+      <c r="A17" t="s">
+        <v>58</v>
+      </c>
+      <c r="B17" t="s">
+        <v>92</v>
+      </c>
+      <c r="M17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17">
+      <c r="A18" t="s">
+        <v>59</v>
+      </c>
+      <c r="B18">
+        <v>563</v>
+      </c>
+      <c r="M18">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17">
+      <c r="A19" t="s">
+        <v>101</v>
+      </c>
+      <c r="B19">
+        <f>19*60</f>
+        <v>1140</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17">
+      <c r="A20" t="s">
+        <v>102</v>
+      </c>
+      <c r="B20">
+        <v>2611</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17">
+      <c r="A26" t="s">
+        <v>122</v>
+      </c>
+      <c r="B26" t="s">
+        <v>104</v>
+      </c>
+      <c r="C26" t="s">
+        <v>103</v>
+      </c>
+      <c r="D26" t="s">
+        <v>9</v>
+      </c>
+      <c r="E26" t="s">
+        <v>92</v>
+      </c>
+      <c r="F26" t="s">
+        <v>104</v>
+      </c>
+      <c r="G26" t="s">
+        <v>103</v>
+      </c>
+      <c r="H26" t="s">
+        <v>9</v>
+      </c>
+      <c r="I26" t="s">
+        <v>92</v>
+      </c>
+      <c r="J26" t="s">
+        <v>105</v>
+      </c>
+      <c r="K26" t="s">
+        <v>103</v>
+      </c>
+      <c r="L26" t="s">
+        <v>9</v>
+      </c>
+      <c r="M26" t="s">
+        <v>92</v>
+      </c>
+      <c r="N26" t="s">
+        <v>106</v>
+      </c>
+      <c r="P26" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17">
+      <c r="A27">
+        <v>2</v>
+      </c>
+      <c r="B27">
+        <v>24.536999999999999</v>
+      </c>
+      <c r="C27">
+        <v>1480.663</v>
+      </c>
+      <c r="D27">
+        <v>40.225999999999999</v>
+      </c>
+      <c r="E27">
+        <v>1545.4259999999999</v>
+      </c>
+      <c r="F27">
+        <v>24.632000000000001</v>
+      </c>
+      <c r="G27">
+        <v>1475.8620000000001</v>
+      </c>
+      <c r="H27">
+        <v>40.232999999999997</v>
+      </c>
+      <c r="I27">
+        <v>1540.7270000000001</v>
+      </c>
+      <c r="J27">
+        <v>23.358000000000001</v>
+      </c>
+      <c r="K27">
+        <v>1483.2449999999999</v>
+      </c>
+      <c r="L27">
+        <v>41.244999999999997</v>
+      </c>
+      <c r="M27">
+        <f>K27+L27+J27</f>
+        <v>1547.8479999999997</v>
+      </c>
+      <c r="N27">
+        <v>1736.0070000000001</v>
+      </c>
+      <c r="P27">
+        <f>AVERAGE(E27+I27+M27)/3</f>
+        <v>1544.6670000000001</v>
+      </c>
+      <c r="Q27">
+        <f>1.96 * STDEV(E27,I27,M27)/SQRT(3)</f>
+        <v>4.097169079209209</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17">
+      <c r="A28">
+        <v>4</v>
+      </c>
+      <c r="B28">
+        <v>48.817999999999998</v>
+      </c>
+      <c r="C28">
+        <v>2767.5140000000001</v>
+      </c>
+      <c r="D28">
+        <v>71.721000000000004</v>
+      </c>
+      <c r="E28">
+        <v>2888.0540000000001</v>
+      </c>
+      <c r="F28">
+        <v>49.430999999999997</v>
+      </c>
+      <c r="G28">
+        <v>2776.223</v>
+      </c>
+      <c r="H28">
+        <v>74.373000000000005</v>
+      </c>
+      <c r="I28">
+        <v>2900.027</v>
+      </c>
+      <c r="J28">
+        <v>49.23</v>
+      </c>
+      <c r="K28">
+        <v>2812.97</v>
+      </c>
+      <c r="L28">
+        <v>76.73</v>
+      </c>
+      <c r="M28">
+        <v>2938.93</v>
+      </c>
+      <c r="N28">
+        <v>3580.5070000000001</v>
+      </c>
+      <c r="P28">
+        <f t="shared" ref="P28:P29" si="5">AVERAGE(E28+I28+M28)/3</f>
+        <v>2909.003666666667</v>
+      </c>
+      <c r="Q28">
+        <f t="shared" ref="Q28:Q29" si="6">1.96 * STDEV(E28,I28,M28)/SQRT(3)</f>
+        <v>30.100037057320566</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17">
+      <c r="A29">
+        <v>8</v>
+      </c>
+      <c r="B29">
         <v>98.637</v>
       </c>
-      <c r="C14">
+      <c r="C29">
         <v>4699.8230000000003</v>
       </c>
-      <c r="D14">
+      <c r="D29">
         <v>142.68100000000001</v>
       </c>
-      <c r="E14">
+      <c r="E29">
         <v>4941.1419999999998</v>
       </c>
-      <c r="F14">
+      <c r="F29">
         <v>99.403999999999996</v>
       </c>
-      <c r="G14">
+      <c r="G29">
         <v>4709.2629999999999</v>
       </c>
-      <c r="H14">
+      <c r="H29">
         <v>144.85300000000001</v>
       </c>
-      <c r="I14">
+      <c r="I29">
         <v>4950.4120000000003</v>
       </c>
-      <c r="J14">
+      <c r="J29">
         <v>94.57</v>
       </c>
-      <c r="K14">
+      <c r="K29">
         <v>4689.28</v>
       </c>
-      <c r="L14">
+      <c r="L29">
         <v>141.83500000000001</v>
       </c>
-      <c r="M14">
+      <c r="M29">
         <v>4931.7830000000004</v>
       </c>
-      <c r="N14">
+      <c r="N29">
         <v>7332.8770000000004</v>
       </c>
-      <c r="P14">
-        <f t="shared" si="2"/>
+      <c r="P29">
+        <f t="shared" si="5"/>
         <v>4941.1123333333335</v>
       </c>
-      <c r="Q14">
-        <f t="shared" si="3"/>
+      <c r="Q29">
+        <f t="shared" si="6"/>
         <v>10.540389098093113</v>
       </c>
     </row>
-    <row r="20" spans="2:15">
-      <c r="M20" t="s">
-        <v>19</v>
-      </c>
-      <c r="N20">
-        <f>((M5-P12)/M5)*100</f>
-        <v>46.03469197624316</v>
-      </c>
-      <c r="O20">
-        <f>AVERAGE(N20:N22)</f>
-        <v>43.385208575547772</v>
-      </c>
-    </row>
-    <row r="21" spans="2:15">
-      <c r="M21" t="s">
-        <v>20</v>
-      </c>
-      <c r="N21">
-        <f t="shared" ref="N21:N22" si="4">((M6-P13)/M6)*100</f>
-        <v>40.676969614574126</v>
-      </c>
-      <c r="O21">
-        <f>1.96*STDEV(N20:N22)/SQRT(3)</f>
-        <v>3.0319636073259546</v>
-      </c>
-    </row>
-    <row r="22" spans="2:15">
-      <c r="M22" t="s">
-        <v>21</v>
-      </c>
-      <c r="N22">
-        <f t="shared" si="4"/>
-        <v>43.443964135826015</v>
-      </c>
-    </row>
-    <row r="24" spans="2:15">
-      <c r="B24">
-        <f>AVERAGE(C24:C26)</f>
-        <v>64.21312926960853</v>
-      </c>
-      <c r="C24">
-        <f>C12/C5*100</f>
-        <v>61.007952204367534</v>
-      </c>
-      <c r="D24">
-        <f>(C5-C12)/C5*100</f>
-        <v>38.992047795632466</v>
-      </c>
-      <c r="E24">
-        <f>AVERAGE(D24:D26)</f>
-        <v>35.786870730391477</v>
-      </c>
-    </row>
-    <row r="25" spans="2:15">
-      <c r="B25">
-        <f>1.96 *(STDEV(C24:C26)/SQRT(3))</f>
-        <v>3.1494806557607635</v>
-      </c>
-      <c r="C25">
-        <f t="shared" ref="C25:C26" si="5">C13/C6*100</f>
-        <v>66.018940839694665</v>
-      </c>
-      <c r="D25">
-        <f t="shared" ref="D25:D26" si="6">(C6-C13)/C6*100</f>
-        <v>33.981059160305335</v>
-      </c>
-      <c r="E25">
-        <f>1.96 *(STDEV(D24:D26)/SQRT(3))</f>
-        <v>3.1494806557609487</v>
-      </c>
-    </row>
-    <row r="26" spans="2:15">
-      <c r="C26">
-        <f t="shared" si="5"/>
-        <v>65.612494764763369</v>
-      </c>
-      <c r="D26">
-        <f t="shared" si="6"/>
-        <v>34.387505235236624</v>
-      </c>
-    </row>
-    <row r="28" spans="2:15">
-      <c r="B28">
-        <f>(D12/D5)*100</f>
-        <v>9.4427230046948356</v>
-      </c>
-      <c r="C28">
-        <f>AVERAGE(B28:B30)</f>
-        <v>8.854828657052721</v>
-      </c>
-    </row>
-    <row r="29" spans="2:15">
-      <c r="B29">
-        <f t="shared" ref="B29:B30" si="7">(D13/D6)*100</f>
-        <v>8.7040048543689323</v>
-      </c>
-    </row>
-    <row r="30" spans="2:15">
-      <c r="B30">
-        <f t="shared" si="7"/>
-        <v>8.4177581120943969</v>
-      </c>
-    </row>
-    <row r="50" spans="1:12">
-      <c r="D50">
-        <v>1087592</v>
-      </c>
-    </row>
-    <row r="53" spans="1:12">
-      <c r="A53" t="s">
-        <v>43</v>
-      </c>
-      <c r="B53" t="s">
-        <v>44</v>
-      </c>
-      <c r="C53" t="s">
-        <v>45</v>
-      </c>
+    <row r="44" spans="3:3">
+      <c r="C44" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="45" spans="3:3">
+      <c r="C45" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="46" spans="3:3">
+      <c r="C46" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="47" spans="3:3">
+      <c r="C47" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7">
       <c r="D53" t="s">
-        <v>46</v>
-      </c>
-      <c r="E53" t="s">
-        <v>47</v>
-      </c>
-      <c r="F53" t="s">
-        <v>45</v>
-      </c>
-      <c r="G53" t="s">
-        <v>46</v>
-      </c>
-      <c r="H53" t="s">
-        <v>42</v>
-      </c>
-      <c r="I53" t="s">
-        <v>45</v>
-      </c>
-      <c r="J53" t="s">
-        <v>46</v>
-      </c>
-      <c r="K53" t="s">
-        <v>42</v>
-      </c>
-      <c r="L53" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="54" spans="1:12">
-      <c r="A54" t="s">
-        <v>48</v>
-      </c>
-      <c r="B54">
-        <v>1171052</v>
-      </c>
-      <c r="C54">
-        <v>554.67499999999995</v>
-      </c>
-      <c r="D54">
-        <v>11.500999999999999</v>
-      </c>
-      <c r="E54">
-        <v>569.14499999999998</v>
-      </c>
-      <c r="F54">
-        <v>604.90899999999999</v>
-      </c>
-      <c r="G54">
-        <v>7.5179999999999998</v>
-      </c>
-      <c r="H54">
-        <v>615.88599999999997</v>
-      </c>
-      <c r="I54">
-        <v>11.34</v>
-      </c>
-      <c r="J54">
-        <v>588.29200000000003</v>
-      </c>
-      <c r="K54">
-        <v>603.06100000000004</v>
-      </c>
-      <c r="L54">
-        <f>849.742/2</f>
-        <v>424.87099999999998</v>
-      </c>
-    </row>
-    <row r="55" spans="1:12">
-      <c r="A55" t="s">
-        <v>49</v>
-      </c>
-      <c r="B55">
-        <v>1171052</v>
-      </c>
-    </row>
-    <row r="56" spans="1:12">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7">
       <c r="A56" t="s">
-        <v>50</v>
-      </c>
-      <c r="B56">
-        <v>1171052</v>
-      </c>
-    </row>
-    <row r="57" spans="1:12">
+        <v>0</v>
+      </c>
+      <c r="B56" t="s">
+        <v>1</v>
+      </c>
+      <c r="C56" t="s">
+        <v>136</v>
+      </c>
+      <c r="D56" t="s">
+        <v>2</v>
+      </c>
+      <c r="E56" t="s">
+        <v>3</v>
+      </c>
+      <c r="F56" t="s">
+        <v>137</v>
+      </c>
+      <c r="G56" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7">
       <c r="A57" t="s">
-        <v>51</v>
+        <v>5</v>
       </c>
       <c r="B57">
         <v>1171052</v>
       </c>
-    </row>
-    <row r="63" spans="1:12">
-      <c r="A63" t="s">
-        <v>121</v>
-      </c>
-      <c r="B63" t="s">
+      <c r="C57">
+        <f>27.1/2</f>
+        <v>13.55</v>
+      </c>
+      <c r="D57">
+        <v>1514.68</v>
+      </c>
+      <c r="E57">
+        <v>71.5</v>
+      </c>
+      <c r="F57">
+        <v>51.42</v>
+      </c>
+      <c r="G57">
+        <f>C57+D57+E57+F57</f>
+        <v>1651.15</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7">
+      <c r="B58">
+        <v>1171052</v>
+      </c>
+      <c r="C58">
+        <f>27.64/2</f>
+        <v>13.82</v>
+      </c>
+      <c r="D58">
+        <v>1527.62</v>
+      </c>
+      <c r="E58">
+        <v>73.239999999999995</v>
+      </c>
+      <c r="F58">
+        <v>49.51</v>
+      </c>
+      <c r="G58">
+        <f t="shared" ref="G58:G59" si="7">C58+D58+E58+F58</f>
+        <v>1664.1899999999998</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7">
+      <c r="B59">
+        <v>1171052</v>
+      </c>
+      <c r="C59">
+        <f>27.44/2</f>
+        <v>13.72</v>
+      </c>
+      <c r="D59">
+        <v>1538.22</v>
+      </c>
+      <c r="E59">
+        <v>71.010000000000005</v>
+      </c>
+      <c r="F59">
+        <v>49.54</v>
+      </c>
+      <c r="G59">
+        <f t="shared" si="7"/>
+        <v>1672.49</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7">
+      <c r="A61" t="s">
+        <v>6</v>
+      </c>
+      <c r="B61">
+        <v>1171052</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7">
+      <c r="B62">
+        <v>1171052</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7">
+      <c r="B63">
+        <v>1171052</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8">
+      <c r="A66" t="s">
+        <v>7</v>
+      </c>
+      <c r="B66">
+        <v>1171052</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8">
+      <c r="B67">
+        <v>1171052</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8">
+      <c r="B68">
+        <v>1171052</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8">
+      <c r="D76" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="64" spans="1:12">
-      <c r="A64" t="s">
-        <v>122</v>
-      </c>
-      <c r="B64">
+    <row r="79" spans="1:8">
+      <c r="A79" t="s">
+        <v>0</v>
+      </c>
+      <c r="B79" t="s">
+        <v>1</v>
+      </c>
+      <c r="C79" t="s">
+        <v>136</v>
+      </c>
+      <c r="D79" t="s">
+        <v>2</v>
+      </c>
+      <c r="E79" t="s">
+        <v>137</v>
+      </c>
+      <c r="F79" t="s">
+        <v>3</v>
+      </c>
+      <c r="G79" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8">
+      <c r="A80" t="s">
+        <v>5</v>
+      </c>
+      <c r="B80">
+        <v>1171052</v>
+      </c>
+      <c r="C80">
+        <f>33.35/2</f>
+        <v>16.675000000000001</v>
+      </c>
+      <c r="D80">
+        <v>1122.4000000000001</v>
+      </c>
+      <c r="E80">
+        <v>77.94</v>
+      </c>
+      <c r="F80">
+        <v>62.5</v>
+      </c>
+      <c r="G80">
+        <f>C80+D80+E80+F80</f>
+        <v>1279.5150000000001</v>
+      </c>
+      <c r="H80" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7">
+      <c r="B81">
+        <v>1171052</v>
+      </c>
+      <c r="C81">
+        <f>20.3/2</f>
+        <v>10.15</v>
+      </c>
+      <c r="D81">
+        <v>1113.1300000000001</v>
+      </c>
+      <c r="E81">
+        <v>80.67</v>
+      </c>
+      <c r="F81">
+        <v>58.19</v>
+      </c>
+      <c r="G81">
+        <f t="shared" ref="G81:G82" si="8">C81+D81+E81+F81</f>
+        <v>1262.1400000000003</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7">
+      <c r="B82">
+        <v>1171052</v>
+      </c>
+      <c r="C82">
+        <f>20.12/2</f>
+        <v>10.06</v>
+      </c>
+      <c r="D82">
+        <v>1117.4000000000001</v>
+      </c>
+      <c r="E82">
+        <v>82.82</v>
+      </c>
+      <c r="F82">
+        <v>54.21</v>
+      </c>
+      <c r="G82">
+        <f t="shared" si="8"/>
+        <v>1264.49</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7">
+      <c r="A84" t="s">
+        <v>6</v>
+      </c>
+      <c r="B84">
+        <v>1171052</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7">
+      <c r="A85" t="s">
+        <v>7</v>
+      </c>
+      <c r="B85">
+        <v>1171052</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7">
+      <c r="A88" t="s">
+        <v>58</v>
+      </c>
+      <c r="B88" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7">
+      <c r="A89" t="s">
+        <v>59</v>
+      </c>
+      <c r="B89">
         <v>563</v>
       </c>
     </row>
-    <row r="65" spans="1:5">
-      <c r="A65" t="s">
-        <v>62</v>
-      </c>
-      <c r="B65">
+    <row r="90" spans="1:7">
+      <c r="A90" t="s">
+        <v>101</v>
+      </c>
+      <c r="B90">
         <f>19*60</f>
         <v>1140</v>
       </c>
     </row>
-    <row r="66" spans="1:5">
-      <c r="A66" t="s">
-        <v>63</v>
-      </c>
-      <c r="B66">
+    <row r="91" spans="1:7" s="12" customFormat="1">
+      <c r="A91" t="s">
+        <v>102</v>
+      </c>
+      <c r="B91">
         <v>2611</v>
       </c>
-    </row>
-    <row r="75" spans="1:5">
-      <c r="C75" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5">
-      <c r="C76" t="s">
-        <v>69</v>
-      </c>
-      <c r="D76" t="s">
-        <v>70</v>
-      </c>
-      <c r="E76" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5">
-      <c r="B77">
+      <c r="C91"/>
+      <c r="D91"/>
+      <c r="E91"/>
+      <c r="F91"/>
+      <c r="G91"/>
+    </row>
+    <row r="102" spans="7:11" s="11" customFormat="1"/>
+    <row r="111" spans="7:11">
+      <c r="G111" s="11"/>
+      <c r="H111" s="11"/>
+      <c r="I111" s="11"/>
+      <c r="J111" s="11"/>
+      <c r="K111" s="11"/>
+    </row>
+    <row r="144" spans="2:6">
+      <c r="B144" t="s">
+        <v>135</v>
+      </c>
+      <c r="C144" t="s">
+        <v>104</v>
+      </c>
+      <c r="D144" t="s">
+        <v>103</v>
+      </c>
+      <c r="E144" t="s">
+        <v>9</v>
+      </c>
+      <c r="F144" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="145" spans="2:2">
+      <c r="B145">
         <v>2</v>
       </c>
     </row>
-    <row r="78" spans="1:5">
-      <c r="B78">
+    <row r="149" spans="2:2">
+      <c r="B149">
         <v>4</v>
       </c>
     </row>
-    <row r="79" spans="1:5">
-      <c r="B79">
+    <row r="153" spans="2:2">
+      <c r="B153">
         <v>8</v>
       </c>
     </row>
+    <row r="157" spans="2:2">
+      <c r="B157">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
data and figures uploaded
git-svn-id: file://localhost/tmp/svn2git/svn@6607 defb5e50-622e-49ec-a68e-d72c7db87b45
</commit_message>
<xml_diff>
--- a/papers/saga-mr-ngs/data/GS_data.xlsx
+++ b/papers/saga-mr-ngs/data/GS_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="12620" yWindow="-20" windowWidth="12860" windowHeight="6980" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25440" windowHeight="14060" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="GS data" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,135 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="178">
+  <si>
+    <t>avg</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>stderr</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1GB</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2GB</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>4GB</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>initial data transfers</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>tts with intial data transfer</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>232MB</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>943MB</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>445MB</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>max data for a reduce</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>8GB</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>MR type</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SEQAL</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Local-PMR</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>distributed-PMR</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Map</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>reduce</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Chunk</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Push Data</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Shuffle</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Exchange</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Reduce</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Total</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>stderr in cunk</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>stderr in setup</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>stderr in Map</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>sterr in exchange</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>stderr in shuffle</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>stderr in total</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>stderr in dt</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Setup</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
   <si>
     <t>Input data</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -66,6 +194,10 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
+    <t>setup</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
     <t>input 2GB, sequences=3805921, chunksize=128MB, number of reduces=8</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -199,6 +331,10 @@
   </si>
   <si>
     <t>phase times</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>seqal map timings</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -697,7 +833,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -727,6 +863,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1056,6 +1193,7 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
+              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
             </c:trendlineLbl>
           </c:trendline>
@@ -1133,6 +1271,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -1152,7 +1291,17 @@
   <c:chart>
     <c:autoTitleDeleted val="1"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.177270997375328"/>
+          <c:y val="0.111111111111111"/>
+          <c:w val="0.73110542432196"/>
+          <c:h val="0.696871172353456"/>
+        </c:manualLayout>
+      </c:layout>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
@@ -1322,6 +1471,71 @@
             </c:numRef>
           </c:val>
         </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>distributed-PMR</c:v>
+          </c:tx>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Sheet1!$I$57:$I$59</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>12.10328698706824</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>19.03239361660941</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>24.16702109756067</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Sheet1!$I$57:$I$59</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>12.10328698706824</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>19.03239361660941</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>24.16702109756067</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+          </c:errBars>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$R$27:$R$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1633.71047826087</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3087.090623188406</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5297.286246376811</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
         <c:axId val="497902952"/>
         <c:axId val="497910136"/>
       </c:barChart>
@@ -1338,16 +1552,23 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr/>
+                  <a:defRPr sz="1100"/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" sz="1100"/>
                   <a:t>Sequences</a:t>
                 </a:r>
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.447668635170604"/>
+              <c:y val="0.906481481481481"/>
+            </c:manualLayout>
+          </c:layout>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
@@ -1370,11 +1591,11 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr/>
+                  <a:defRPr sz="1100"/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>time to solution in seconds</a:t>
+                  <a:rPr lang="en-US" sz="1100"/>
+                  <a:t>Runtime (in seconds)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -1390,7 +1611,513 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.227820866141732"/>
+          <c:y val="0.0549795858850977"/>
+          <c:w val="0.491623578302712"/>
+          <c:h val="0.107633056284631"/>
+        </c:manualLayout>
+      </c:layout>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="1"/>
+  <c:lang val="en-US"/>
+  <c:style val="18"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.1046274290255"/>
+          <c:y val="0.0509259259259259"/>
+          <c:w val="0.844949432926389"/>
+          <c:h val="0.799648950131234"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$K$72</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>SEQAL</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Sheet1!$P$79:$W$79</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="8"/>
+                  <c:pt idx="0">
+                    <c:v>7.441688726208064</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>3.974071519794642</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>95.10208690314496</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>1.131606527611667</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>23.90700129901929</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>118.9120511601106</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Sheet1!$P$79:$W$79</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="8"/>
+                  <c:pt idx="0">
+                    <c:v>7.441688726208064</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>3.974071519794642</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>95.10208690314496</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>1.131606527611667</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>23.90700129901929</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>118.9120511601106</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+          </c:errBars>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$L$71:$S$71</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Push Data</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Chunk</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Setup</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Map</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Shuffle</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Exchange</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Reduce</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Total</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$L$72:$S$72</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>356.1739130434783</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>109.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7066.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>103.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1670.666666666667</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9304.840579710144</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$K$73</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Local-PMR</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Sheet1!$P$80:$W$80</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="8"/>
+                  <c:pt idx="0">
+                    <c:v>7.441688726208064</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>2.93986693476621</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>11.31218638858732</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>5.185672569686598</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>1.131606527611667</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>1.761676959264712</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>10.54038909809311</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Sheet1!$P$80:$W$80</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="8"/>
+                  <c:pt idx="0">
+                    <c:v>7.441688726208064</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>2.93986693476621</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>11.31218638858732</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>5.185672569686598</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>1.131606527611667</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>1.761676959264712</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>10.54038909809311</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+          </c:errBars>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$L$71:$S$71</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Push Data</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Chunk</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Setup</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Map</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Shuffle</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Exchange</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Reduce</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Total</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$L$73:$S$73</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>356.1739130434783</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>98.637</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4699.455333333332</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>250.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>143.123</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5547.38924637681</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$K$74</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>distributed-PMR</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Sheet1!$P$81:$W$81</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="8"/>
+                  <c:pt idx="1">
+                    <c:v>0.634641960303525</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>23.77030017401586</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>1.728557523113877</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>2.076212744396057</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>24.16702109756067</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Sheet1!$P$81:$W$81</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="8"/>
+                  <c:pt idx="1">
+                    <c:v>0.634641960303525</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>23.77030017401586</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>1.728557523113877</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>2.076212744396057</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>24.16702109756067</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+          </c:errBars>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$L$71:$S$71</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Push Data</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Chunk</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Setup</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Map</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Shuffle</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Exchange</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Reduce</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Total</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$L$74:$S$74</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>35.85666666666666</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4756.134666666666</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1922.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>142.12</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6856.111333333333</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="632776056"/>
+        <c:axId val="632991096"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="632776056"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr rot="0" vert="horz" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1100"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="632991096"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="632991096"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1100"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1100"/>
+                  <a:t>Runtime(in seconds)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="632776056"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.305081449107852"/>
+          <c:y val="0.0364610673665792"/>
+          <c:w val="0.493083688506826"/>
+          <c:h val="0.0937441673957422"/>
+        </c:manualLayout>
+      </c:layout>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -2053,6 +2780,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -2275,6 +3003,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
@@ -2307,6 +3036,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
@@ -2317,6 +3047,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -2979,6 +3710,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout>
@@ -3083,6 +3815,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
@@ -3113,6 +3846,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
@@ -3123,6 +3857,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -3658,16 +4393,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>889000</xdr:colOff>
-      <xdr:row>51</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>622300</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>698500</xdr:colOff>
-      <xdr:row>68</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>431800</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3685,6 +4420,36 @@
       </a:graphic>
     </xdr:graphicFrame>
     <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>317500</xdr:colOff>
+      <xdr:row>78</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>787400</xdr:colOff>
+      <xdr:row>96</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData fLocksWithSheet="0"/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
@@ -4289,7 +5054,7 @@
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
       <c r="G1" s="1" t="s">
-        <v>70</v>
+        <v>104</v>
       </c>
       <c r="H1" s="1"/>
       <c r="I1" s="2"/>
@@ -4301,46 +5066,46 @@
     </row>
     <row r="2" spans="1:14" ht="71" thickBot="1">
       <c r="A2" s="3" t="s">
-        <v>71</v>
+        <v>105</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>72</v>
+        <v>106</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>84</v>
+        <v>118</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>85</v>
+        <v>119</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>86</v>
+        <v>120</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>87</v>
+        <v>121</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>88</v>
+        <v>122</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>89</v>
+        <v>123</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>90</v>
+        <v>124</v>
       </c>
       <c r="J2" s="7" t="s">
-        <v>91</v>
+        <v>125</v>
       </c>
       <c r="K2" s="8" t="s">
-        <v>118</v>
+        <v>152</v>
       </c>
       <c r="L2" s="8" t="s">
-        <v>17</v>
+        <v>50</v>
       </c>
       <c r="M2" s="8" t="s">
-        <v>18</v>
+        <v>51</v>
       </c>
       <c r="N2" s="8" t="s">
-        <v>19</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:14">
@@ -4519,7 +5284,7 @@
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="1" t="s">
-        <v>20</v>
+        <v>53</v>
       </c>
       <c r="H8" s="1"/>
       <c r="I8" s="2"/>
@@ -4531,46 +5296,46 @@
     </row>
     <row r="9" spans="1:14" ht="71" thickBot="1">
       <c r="A9" s="3" t="s">
-        <v>71</v>
+        <v>105</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>72</v>
+        <v>106</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>84</v>
+        <v>118</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>85</v>
+        <v>119</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>86</v>
+        <v>120</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>87</v>
+        <v>121</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>88</v>
+        <v>122</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>89</v>
+        <v>123</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>90</v>
+        <v>124</v>
       </c>
       <c r="J9" s="7" t="s">
-        <v>91</v>
+        <v>125</v>
       </c>
       <c r="K9" s="8" t="s">
-        <v>118</v>
+        <v>152</v>
       </c>
       <c r="L9" s="8" t="s">
-        <v>17</v>
+        <v>50</v>
       </c>
       <c r="M9" s="8" t="s">
-        <v>18</v>
+        <v>51</v>
       </c>
       <c r="N9" s="8" t="s">
-        <v>19</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:14">
@@ -4749,7 +5514,7 @@
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
       <c r="G16" s="1" t="s">
-        <v>21</v>
+        <v>54</v>
       </c>
       <c r="H16" s="1"/>
       <c r="I16" s="2"/>
@@ -4761,46 +5526,46 @@
     </row>
     <row r="17" spans="1:19" ht="71" thickBot="1">
       <c r="A17" s="3" t="s">
-        <v>71</v>
+        <v>105</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>72</v>
+        <v>106</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>84</v>
+        <v>118</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>85</v>
+        <v>119</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>86</v>
+        <v>120</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>87</v>
+        <v>121</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>88</v>
+        <v>122</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>89</v>
+        <v>123</v>
       </c>
       <c r="I17" s="7" t="s">
-        <v>90</v>
+        <v>124</v>
       </c>
       <c r="J17" s="7" t="s">
-        <v>91</v>
+        <v>125</v>
       </c>
       <c r="K17" s="8" t="s">
-        <v>118</v>
+        <v>152</v>
       </c>
       <c r="L17" s="8" t="s">
-        <v>17</v>
+        <v>50</v>
       </c>
       <c r="M17" s="8" t="s">
-        <v>18</v>
+        <v>51</v>
       </c>
       <c r="N17" s="8" t="s">
-        <v>19</v>
+        <v>52</v>
       </c>
     </row>
     <row r="18" spans="1:19">
@@ -4973,46 +5738,46 @@
     </row>
     <row r="24" spans="1:19" ht="46" thickBot="1">
       <c r="A24" s="3" t="s">
-        <v>22</v>
+        <v>55</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>23</v>
+        <v>56</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>88</v>
+        <v>122</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>24</v>
+        <v>57</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>25</v>
+        <v>58</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>26</v>
+        <v>59</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>119</v>
+        <v>153</v>
       </c>
       <c r="H24" s="7" t="s">
-        <v>120</v>
+        <v>154</v>
       </c>
       <c r="I24" s="7" t="s">
-        <v>121</v>
+        <v>155</v>
       </c>
       <c r="J24" s="7" t="s">
-        <v>50</v>
+        <v>84</v>
       </c>
       <c r="K24" s="8" t="s">
-        <v>51</v>
+        <v>85</v>
       </c>
       <c r="L24" s="8" t="s">
-        <v>52</v>
+        <v>86</v>
       </c>
       <c r="M24" s="8" t="s">
-        <v>53</v>
+        <v>87</v>
       </c>
       <c r="N24" s="8" t="s">
-        <v>52</v>
+        <v>86</v>
       </c>
     </row>
     <row r="25" spans="1:19">
@@ -5209,39 +5974,39 @@
     </row>
     <row r="31" spans="1:19">
       <c r="D31" t="s">
-        <v>54</v>
+        <v>88</v>
       </c>
     </row>
     <row r="32" spans="1:19" ht="46" thickBot="1">
       <c r="D32" s="3" t="s">
-        <v>55</v>
+        <v>89</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>56</v>
+        <v>90</v>
       </c>
       <c r="F32" s="6" t="s">
-        <v>88</v>
+        <v>122</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>57</v>
+        <v>91</v>
       </c>
       <c r="H32" s="8" t="s">
-        <v>73</v>
+        <v>107</v>
       </c>
       <c r="I32" s="8" t="s">
-        <v>74</v>
+        <v>108</v>
       </c>
       <c r="J32" s="8" t="s">
-        <v>75</v>
+        <v>109</v>
       </c>
       <c r="K32" s="8" t="s">
-        <v>76</v>
+        <v>110</v>
       </c>
       <c r="R32" t="s">
-        <v>77</v>
+        <v>111</v>
       </c>
       <c r="S32" t="s">
-        <v>78</v>
+        <v>112</v>
       </c>
     </row>
     <row r="33" spans="4:19">
@@ -5271,7 +6036,7 @@
         <v>3.8921515186908202</v>
       </c>
       <c r="M33" t="s">
-        <v>79</v>
+        <v>113</v>
       </c>
       <c r="R33">
         <v>1.59</v>
@@ -5307,7 +6072,7 @@
         <v>1.2000589337377248</v>
       </c>
       <c r="M34" t="s">
-        <v>80</v>
+        <v>114</v>
       </c>
       <c r="R34" s="10">
         <v>9155.6200000000008</v>
@@ -5343,7 +6108,7 @@
         <v>2.2325377438638392</v>
       </c>
       <c r="M35" t="s">
-        <v>45</v>
+        <v>79</v>
       </c>
     </row>
     <row r="36" spans="4:19">
@@ -5373,17 +6138,17 @@
         <v>2.6636263501721773</v>
       </c>
       <c r="M36" t="s">
-        <v>62</v>
+        <v>96</v>
       </c>
     </row>
     <row r="37" spans="4:19">
       <c r="M37" t="s">
-        <v>63</v>
+        <v>97</v>
       </c>
     </row>
     <row r="60" spans="25:25">
       <c r="Y60" t="s">
-        <v>64</v>
+        <v>98</v>
       </c>
     </row>
     <row r="65" spans="1:14" ht="15">
@@ -5394,7 +6159,7 @@
       <c r="E65" s="2"/>
       <c r="F65" s="2"/>
       <c r="G65" s="1" t="s">
-        <v>65</v>
+        <v>99</v>
       </c>
       <c r="H65" s="1"/>
       <c r="I65" s="2"/>
@@ -5406,46 +6171,46 @@
     </row>
     <row r="66" spans="1:14" ht="71" thickBot="1">
       <c r="A66" s="3" t="s">
-        <v>71</v>
+        <v>105</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>72</v>
+        <v>106</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>84</v>
+        <v>118</v>
       </c>
       <c r="D66" s="5" t="s">
-        <v>85</v>
+        <v>119</v>
       </c>
       <c r="E66" s="3" t="s">
-        <v>86</v>
+        <v>120</v>
       </c>
       <c r="F66" s="3" t="s">
-        <v>87</v>
+        <v>121</v>
       </c>
       <c r="G66" s="6" t="s">
-        <v>88</v>
+        <v>122</v>
       </c>
       <c r="H66" s="3" t="s">
-        <v>89</v>
+        <v>123</v>
       </c>
       <c r="I66" s="7" t="s">
-        <v>90</v>
+        <v>124</v>
       </c>
       <c r="J66" s="7" t="s">
-        <v>91</v>
+        <v>125</v>
       </c>
       <c r="K66" s="8" t="s">
-        <v>118</v>
+        <v>152</v>
       </c>
       <c r="L66" s="8" t="s">
-        <v>17</v>
+        <v>50</v>
       </c>
       <c r="M66" s="8" t="s">
-        <v>18</v>
+        <v>51</v>
       </c>
       <c r="N66" s="8" t="s">
-        <v>19</v>
+        <v>52</v>
       </c>
     </row>
     <row r="67" spans="1:14">
@@ -5582,7 +6347,7 @@
       <c r="E72" s="2"/>
       <c r="F72" s="2"/>
       <c r="G72" s="1" t="s">
-        <v>66</v>
+        <v>100</v>
       </c>
       <c r="H72" s="1"/>
       <c r="I72" s="2"/>
@@ -5594,46 +6359,46 @@
     </row>
     <row r="73" spans="1:14" ht="71" thickBot="1">
       <c r="A73" s="3" t="s">
-        <v>71</v>
+        <v>105</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>72</v>
+        <v>106</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>84</v>
+        <v>118</v>
       </c>
       <c r="D73" s="5" t="s">
-        <v>85</v>
+        <v>119</v>
       </c>
       <c r="E73" s="3" t="s">
-        <v>86</v>
+        <v>120</v>
       </c>
       <c r="F73" s="3" t="s">
-        <v>87</v>
+        <v>121</v>
       </c>
       <c r="G73" s="6" t="s">
-        <v>88</v>
+        <v>122</v>
       </c>
       <c r="H73" s="3" t="s">
-        <v>89</v>
+        <v>123</v>
       </c>
       <c r="I73" s="7" t="s">
-        <v>90</v>
+        <v>124</v>
       </c>
       <c r="J73" s="7" t="s">
-        <v>91</v>
+        <v>125</v>
       </c>
       <c r="K73" s="8" t="s">
-        <v>118</v>
+        <v>152</v>
       </c>
       <c r="L73" s="8" t="s">
-        <v>17</v>
+        <v>50</v>
       </c>
       <c r="M73" s="8" t="s">
-        <v>18</v>
+        <v>51</v>
       </c>
       <c r="N73" s="8" t="s">
-        <v>19</v>
+        <v>52</v>
       </c>
     </row>
     <row r="74" spans="1:14">
@@ -5770,7 +6535,7 @@
       <c r="E79" s="2"/>
       <c r="F79" s="2"/>
       <c r="G79" s="1" t="s">
-        <v>67</v>
+        <v>101</v>
       </c>
       <c r="H79" s="1"/>
       <c r="I79" s="2"/>
@@ -5782,46 +6547,46 @@
     </row>
     <row r="80" spans="1:14" ht="71" thickBot="1">
       <c r="A80" s="3" t="s">
-        <v>71</v>
+        <v>105</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>72</v>
+        <v>106</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>84</v>
+        <v>118</v>
       </c>
       <c r="D80" s="5" t="s">
-        <v>85</v>
+        <v>119</v>
       </c>
       <c r="E80" s="3" t="s">
-        <v>86</v>
+        <v>120</v>
       </c>
       <c r="F80" s="3" t="s">
-        <v>87</v>
+        <v>121</v>
       </c>
       <c r="G80" s="6" t="s">
-        <v>88</v>
+        <v>122</v>
       </c>
       <c r="H80" s="3" t="s">
-        <v>89</v>
+        <v>123</v>
       </c>
       <c r="I80" s="7" t="s">
-        <v>90</v>
+        <v>124</v>
       </c>
       <c r="J80" s="7" t="s">
-        <v>91</v>
+        <v>125</v>
       </c>
       <c r="K80" s="8" t="s">
-        <v>118</v>
+        <v>152</v>
       </c>
       <c r="L80" s="8" t="s">
-        <v>17</v>
+        <v>50</v>
       </c>
       <c r="M80" s="8" t="s">
-        <v>18</v>
+        <v>51</v>
       </c>
       <c r="N80" s="8" t="s">
-        <v>19</v>
+        <v>52</v>
       </c>
     </row>
     <row r="81" spans="1:12">
@@ -5943,40 +6708,40 @@
     </row>
     <row r="87" spans="1:12" ht="71" thickBot="1">
       <c r="A87" s="3" t="s">
-        <v>68</v>
+        <v>102</v>
       </c>
       <c r="B87" s="6" t="s">
-        <v>88</v>
+        <v>122</v>
       </c>
       <c r="C87" s="7" t="s">
-        <v>69</v>
+        <v>103</v>
       </c>
       <c r="D87" s="7" t="s">
-        <v>69</v>
+        <v>103</v>
       </c>
       <c r="E87" s="7" t="s">
-        <v>69</v>
+        <v>103</v>
       </c>
       <c r="F87" s="8" t="s">
-        <v>117</v>
+        <v>151</v>
       </c>
       <c r="G87" s="8" t="s">
-        <v>133</v>
+        <v>167</v>
       </c>
       <c r="H87" s="7" t="s">
-        <v>134</v>
+        <v>168</v>
       </c>
       <c r="I87" s="7" t="s">
-        <v>134</v>
+        <v>168</v>
       </c>
       <c r="J87" s="7" t="s">
-        <v>134</v>
+        <v>168</v>
       </c>
       <c r="K87" s="8" t="s">
-        <v>30</v>
+        <v>63</v>
       </c>
       <c r="L87" s="8" t="s">
-        <v>31</v>
+        <v>64</v>
       </c>
     </row>
     <row r="88" spans="1:12">
@@ -6110,27 +6875,27 @@
     </row>
     <row r="94" spans="1:12">
       <c r="A94" t="s">
-        <v>32</v>
+        <v>65</v>
       </c>
     </row>
     <row r="96" spans="1:12" ht="33" thickBot="1">
       <c r="A96" s="3" t="s">
-        <v>33</v>
+        <v>66</v>
       </c>
       <c r="B96" s="5" t="s">
-        <v>88</v>
+        <v>122</v>
       </c>
       <c r="C96" s="6" t="s">
-        <v>34</v>
+        <v>67</v>
       </c>
       <c r="D96" s="3" t="s">
-        <v>35</v>
+        <v>68</v>
       </c>
       <c r="E96" s="3" t="s">
-        <v>36</v>
+        <v>69</v>
       </c>
       <c r="F96" s="5" t="s">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="G96" s="11"/>
     </row>
@@ -6196,7 +6961,7 @@
     </row>
     <row r="100" spans="1:22">
       <c r="V100" t="s">
-        <v>38</v>
+        <v>71</v>
       </c>
     </row>
     <row r="101" spans="1:22">
@@ -6206,27 +6971,27 @@
     </row>
     <row r="105" spans="1:22">
       <c r="I105" t="s">
-        <v>79</v>
+        <v>113</v>
       </c>
     </row>
     <row r="106" spans="1:22">
       <c r="I106" t="s">
-        <v>39</v>
+        <v>72</v>
       </c>
     </row>
     <row r="107" spans="1:22">
       <c r="I107" t="s">
-        <v>40</v>
+        <v>73</v>
       </c>
     </row>
     <row r="108" spans="1:22">
       <c r="I108" t="s">
-        <v>138</v>
+        <v>172</v>
       </c>
     </row>
     <row r="109" spans="1:22">
       <c r="I109" t="s">
-        <v>139</v>
+        <v>173</v>
       </c>
     </row>
     <row r="120" spans="1:17" ht="15">
@@ -6237,7 +7002,7 @@
       <c r="E120" s="2"/>
       <c r="F120" s="2"/>
       <c r="G120" s="1" t="s">
-        <v>140</v>
+        <v>174</v>
       </c>
       <c r="H120" s="1"/>
       <c r="I120" s="2"/>
@@ -6249,46 +7014,46 @@
     </row>
     <row r="121" spans="1:17" ht="71" thickBot="1">
       <c r="A121" s="3" t="s">
-        <v>71</v>
+        <v>105</v>
       </c>
       <c r="B121" s="3" t="s">
-        <v>22</v>
+        <v>55</v>
       </c>
       <c r="C121" s="4" t="s">
-        <v>141</v>
+        <v>175</v>
       </c>
       <c r="D121" s="5" t="s">
-        <v>85</v>
+        <v>119</v>
       </c>
       <c r="E121" s="3" t="s">
-        <v>86</v>
+        <v>120</v>
       </c>
       <c r="F121" s="3" t="s">
-        <v>87</v>
+        <v>121</v>
       </c>
       <c r="G121" s="6" t="s">
-        <v>88</v>
+        <v>122</v>
       </c>
       <c r="H121" s="3" t="s">
-        <v>89</v>
+        <v>123</v>
       </c>
       <c r="I121" s="7" t="s">
-        <v>90</v>
+        <v>124</v>
       </c>
       <c r="J121" s="7" t="s">
-        <v>91</v>
+        <v>125</v>
       </c>
       <c r="K121" s="8" t="s">
-        <v>118</v>
+        <v>152</v>
       </c>
       <c r="L121" s="8" t="s">
-        <v>17</v>
+        <v>50</v>
       </c>
       <c r="M121" s="8" t="s">
-        <v>18</v>
+        <v>51</v>
       </c>
       <c r="N121" s="8" t="s">
-        <v>142</v>
+        <v>176</v>
       </c>
     </row>
     <row r="122" spans="1:17">
@@ -6454,7 +7219,7 @@
       <c r="E129" s="2"/>
       <c r="F129" s="2"/>
       <c r="G129" s="1" t="s">
-        <v>143</v>
+        <v>177</v>
       </c>
       <c r="H129" s="1"/>
       <c r="I129" s="2"/>
@@ -6466,46 +7231,46 @@
     </row>
     <row r="130" spans="1:14" ht="71" thickBot="1">
       <c r="A130" s="3" t="s">
-        <v>71</v>
+        <v>105</v>
       </c>
       <c r="B130" s="3" t="s">
-        <v>72</v>
+        <v>106</v>
       </c>
       <c r="C130" s="4" t="s">
-        <v>84</v>
+        <v>118</v>
       </c>
       <c r="D130" s="5" t="s">
-        <v>85</v>
+        <v>119</v>
       </c>
       <c r="E130" s="3" t="s">
-        <v>86</v>
+        <v>120</v>
       </c>
       <c r="F130" s="3" t="s">
-        <v>87</v>
+        <v>121</v>
       </c>
       <c r="G130" s="6" t="s">
-        <v>88</v>
+        <v>122</v>
       </c>
       <c r="H130" s="3" t="s">
-        <v>89</v>
+        <v>123</v>
       </c>
       <c r="I130" s="7" t="s">
-        <v>90</v>
+        <v>124</v>
       </c>
       <c r="J130" s="7" t="s">
-        <v>91</v>
+        <v>125</v>
       </c>
       <c r="K130" s="8" t="s">
-        <v>118</v>
+        <v>152</v>
       </c>
       <c r="L130" s="8" t="s">
-        <v>17</v>
+        <v>50</v>
       </c>
       <c r="M130" s="8" t="s">
-        <v>18</v>
+        <v>51</v>
       </c>
       <c r="N130" s="8" t="s">
-        <v>19</v>
+        <v>52</v>
       </c>
     </row>
     <row r="131" spans="1:14">
@@ -6645,7 +7410,7 @@
       <c r="E139" s="2"/>
       <c r="F139" s="2"/>
       <c r="G139" s="1" t="s">
-        <v>126</v>
+        <v>160</v>
       </c>
       <c r="H139" s="1"/>
       <c r="I139" s="2"/>
@@ -6657,46 +7422,46 @@
     </row>
     <row r="140" spans="1:14" ht="71" thickBot="1">
       <c r="A140" s="3" t="s">
-        <v>71</v>
+        <v>105</v>
       </c>
       <c r="B140" s="3" t="s">
-        <v>72</v>
+        <v>106</v>
       </c>
       <c r="C140" s="4" t="s">
-        <v>84</v>
+        <v>118</v>
       </c>
       <c r="D140" s="5" t="s">
-        <v>85</v>
+        <v>119</v>
       </c>
       <c r="E140" s="3" t="s">
-        <v>86</v>
+        <v>120</v>
       </c>
       <c r="F140" s="3" t="s">
-        <v>87</v>
+        <v>121</v>
       </c>
       <c r="G140" s="6" t="s">
-        <v>88</v>
+        <v>122</v>
       </c>
       <c r="H140" s="3" t="s">
-        <v>89</v>
+        <v>123</v>
       </c>
       <c r="I140" s="7" t="s">
-        <v>90</v>
+        <v>124</v>
       </c>
       <c r="J140" s="7" t="s">
-        <v>91</v>
+        <v>125</v>
       </c>
       <c r="K140" s="8" t="s">
-        <v>118</v>
+        <v>152</v>
       </c>
       <c r="L140" s="8" t="s">
-        <v>17</v>
+        <v>50</v>
       </c>
       <c r="M140" s="8" t="s">
-        <v>18</v>
+        <v>51</v>
       </c>
       <c r="N140" s="8" t="s">
-        <v>142</v>
+        <v>176</v>
       </c>
     </row>
     <row r="141" spans="1:14">
@@ -6830,55 +7595,55 @@
     </row>
     <row r="147" spans="1:17" ht="43" thickBot="1">
       <c r="A147" s="4" t="s">
-        <v>84</v>
+        <v>118</v>
       </c>
       <c r="B147" s="6" t="s">
-        <v>88</v>
+        <v>122</v>
       </c>
       <c r="C147" s="3" t="s">
-        <v>89</v>
+        <v>123</v>
       </c>
       <c r="D147" s="3" t="s">
-        <v>89</v>
+        <v>123</v>
       </c>
       <c r="E147" s="3" t="s">
-        <v>89</v>
+        <v>123</v>
       </c>
       <c r="F147" s="3" t="s">
-        <v>127</v>
+        <v>161</v>
       </c>
       <c r="G147" s="3" t="s">
-        <v>128</v>
+        <v>162</v>
       </c>
       <c r="H147" s="7" t="s">
-        <v>90</v>
+        <v>124</v>
       </c>
       <c r="I147" s="7" t="s">
-        <v>90</v>
+        <v>124</v>
       </c>
       <c r="J147" s="7" t="s">
-        <v>90</v>
+        <v>124</v>
       </c>
       <c r="K147" s="8" t="s">
-        <v>129</v>
+        <v>163</v>
       </c>
       <c r="L147" s="8" t="s">
-        <v>130</v>
+        <v>164</v>
       </c>
       <c r="M147" s="7" t="s">
-        <v>91</v>
+        <v>125</v>
       </c>
       <c r="N147" s="7" t="s">
-        <v>91</v>
+        <v>125</v>
       </c>
       <c r="O147" s="7" t="s">
-        <v>91</v>
+        <v>125</v>
       </c>
       <c r="P147" s="8" t="s">
-        <v>131</v>
+        <v>165</v>
       </c>
       <c r="Q147" s="8" t="s">
-        <v>132</v>
+        <v>166</v>
       </c>
     </row>
     <row r="148" spans="1:17">
@@ -7042,36 +7807,36 @@
     </row>
     <row r="153" spans="1:17">
       <c r="C153" t="s">
-        <v>46</v>
+        <v>80</v>
       </c>
     </row>
     <row r="155" spans="1:17" ht="49" thickBot="1">
       <c r="C155" s="3" t="s">
-        <v>47</v>
+        <v>81</v>
       </c>
       <c r="D155" s="5" t="s">
-        <v>85</v>
+        <v>119</v>
       </c>
       <c r="E155" s="6" t="s">
-        <v>48</v>
+        <v>82</v>
       </c>
       <c r="F155" s="3" t="s">
-        <v>89</v>
+        <v>123</v>
       </c>
       <c r="G155" s="3" t="s">
-        <v>49</v>
+        <v>83</v>
       </c>
       <c r="H155" s="8" t="s">
-        <v>123</v>
+        <v>157</v>
       </c>
       <c r="I155" s="8" t="s">
-        <v>124</v>
+        <v>158</v>
       </c>
       <c r="J155" s="8" t="s">
-        <v>111</v>
+        <v>145</v>
       </c>
       <c r="K155" s="8" t="s">
-        <v>112</v>
+        <v>146</v>
       </c>
     </row>
     <row r="156" spans="1:17">
@@ -7165,6 +7930,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>
@@ -7188,33 +7954,33 @@
   <sheetData>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>113</v>
+        <v>147</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="46" thickBot="1">
       <c r="A4" s="3" t="s">
-        <v>72</v>
+        <v>106</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>85</v>
+        <v>119</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>88</v>
+        <v>122</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>89</v>
+        <v>123</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>114</v>
+        <v>148</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>74</v>
+        <v>108</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>75</v>
+        <v>109</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>76</v>
+        <v>110</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -7327,15 +8093,15 @@
     </row>
     <row r="31" spans="2:8">
       <c r="G31" t="s">
-        <v>77</v>
+        <v>111</v>
       </c>
       <c r="H31" t="s">
-        <v>115</v>
+        <v>149</v>
       </c>
     </row>
     <row r="32" spans="2:8">
       <c r="B32" t="s">
-        <v>79</v>
+        <v>113</v>
       </c>
       <c r="G32">
         <v>1.59</v>
@@ -7346,7 +8112,7 @@
     </row>
     <row r="33" spans="1:8" ht="15">
       <c r="B33" t="s">
-        <v>80</v>
+        <v>114</v>
       </c>
       <c r="G33" s="10">
         <v>9155.6200000000008</v>
@@ -7357,42 +8123,42 @@
     </row>
     <row r="34" spans="1:8">
       <c r="B34" t="s">
-        <v>116</v>
+        <v>150</v>
       </c>
     </row>
     <row r="35" spans="1:8">
       <c r="B35" t="s">
-        <v>138</v>
+        <v>172</v>
       </c>
     </row>
     <row r="36" spans="1:8">
       <c r="B36" t="s">
-        <v>139</v>
+        <v>173</v>
       </c>
     </row>
     <row r="48" spans="1:8">
       <c r="A48" t="s">
-        <v>32</v>
+        <v>65</v>
       </c>
     </row>
     <row r="50" spans="1:7" ht="33" thickBot="1">
       <c r="A50" s="3" t="s">
-        <v>33</v>
+        <v>66</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>88</v>
+        <v>122</v>
       </c>
       <c r="C50" s="6" t="s">
-        <v>34</v>
+        <v>67</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>35</v>
+        <v>68</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>36</v>
+        <v>69</v>
       </c>
       <c r="F50" s="5" t="s">
-        <v>37</v>
+        <v>70</v>
       </c>
       <c r="G50" s="11"/>
     </row>
@@ -7458,15 +8224,15 @@
     </row>
     <row r="64" spans="1:7">
       <c r="B64" t="s">
-        <v>79</v>
+        <v>113</v>
       </c>
       <c r="G64" t="s">
-        <v>38</v>
+        <v>71</v>
       </c>
     </row>
     <row r="65" spans="1:9" ht="15">
       <c r="B65" t="s">
-        <v>80</v>
+        <v>114</v>
       </c>
       <c r="G65">
         <v>9144.5290000000005</v>
@@ -7475,51 +8241,51 @@
     </row>
     <row r="66" spans="1:9">
       <c r="B66" t="s">
-        <v>116</v>
+        <v>150</v>
       </c>
     </row>
     <row r="67" spans="1:9">
       <c r="B67" t="s">
-        <v>138</v>
+        <v>172</v>
       </c>
     </row>
     <row r="68" spans="1:9">
       <c r="B68" t="s">
-        <v>139</v>
+        <v>173</v>
       </c>
     </row>
     <row r="78" spans="1:9">
       <c r="A78" t="s">
-        <v>46</v>
+        <v>80</v>
       </c>
     </row>
     <row r="80" spans="1:9" ht="49" thickBot="1">
       <c r="A80" s="3" t="s">
-        <v>47</v>
+        <v>81</v>
       </c>
       <c r="B80" s="5" t="s">
-        <v>85</v>
+        <v>119</v>
       </c>
       <c r="C80" s="6" t="s">
-        <v>48</v>
+        <v>82</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>89</v>
+        <v>123</v>
       </c>
       <c r="E80" s="3" t="s">
-        <v>49</v>
+        <v>83</v>
       </c>
       <c r="F80" s="8" t="s">
-        <v>123</v>
+        <v>157</v>
       </c>
       <c r="G80" s="8" t="s">
-        <v>124</v>
+        <v>158</v>
       </c>
       <c r="H80" s="8" t="s">
-        <v>111</v>
+        <v>145</v>
       </c>
       <c r="I80" s="8" t="s">
-        <v>112</v>
+        <v>146</v>
       </c>
     </row>
     <row r="81" spans="1:9">
@@ -7613,6 +8379,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>
@@ -7626,73 +8393,73 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A2:Q157"/>
+  <dimension ref="A2:W157"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="E39" sqref="E39"/>
+    <sheetView tabSelected="1" topLeftCell="D76" workbookViewId="0">
+      <selection activeCell="P91" sqref="P91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <sheetData>
-    <row r="2" spans="1:17">
+    <row r="2" spans="1:21">
       <c r="A2" t="s">
-        <v>95</v>
+        <v>129</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>43</v>
       </c>
       <c r="H2" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21">
       <c r="A4" t="s">
-        <v>122</v>
+        <v>156</v>
       </c>
       <c r="B4" t="s">
-        <v>94</v>
+        <v>128</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="D4" t="s">
-        <v>9</v>
+        <v>41</v>
       </c>
       <c r="E4" t="s">
-        <v>4</v>
+        <v>36</v>
       </c>
       <c r="F4" t="s">
-        <v>96</v>
+        <v>130</v>
       </c>
       <c r="G4" t="s">
-        <v>97</v>
+        <v>131</v>
       </c>
       <c r="H4" t="s">
-        <v>92</v>
+        <v>126</v>
       </c>
       <c r="I4" t="s">
-        <v>98</v>
+        <v>132</v>
       </c>
       <c r="J4" t="s">
-        <v>3</v>
+        <v>35</v>
       </c>
       <c r="K4" t="s">
-        <v>92</v>
+        <v>126</v>
       </c>
       <c r="L4" t="s">
-        <v>100</v>
+        <v>134</v>
       </c>
       <c r="M4" t="s">
-        <v>107</v>
+        <v>141</v>
       </c>
       <c r="N4" t="s">
-        <v>108</v>
+        <v>142</v>
       </c>
       <c r="O4" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21">
       <c r="A5">
         <v>2</v>
       </c>
@@ -7745,7 +8512,7 @@
         <v>292763.15384615387</v>
       </c>
     </row>
-    <row r="6" spans="1:17">
+    <row r="6" spans="1:21">
       <c r="A6">
         <v>4</v>
       </c>
@@ -7794,7 +8561,7 @@
         <v>114.09789091439987</v>
       </c>
     </row>
-    <row r="7" spans="1:17">
+    <row r="7" spans="1:21">
       <c r="A7">
         <v>8</v>
       </c>
@@ -7843,50 +8610,53 @@
         <v>118.91205116011055</v>
       </c>
     </row>
-    <row r="10" spans="1:17">
+    <row r="10" spans="1:21">
       <c r="A10" t="s">
-        <v>27</v>
+        <v>60</v>
       </c>
       <c r="B10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" ht="26">
+      <c r="A11" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="D11" s="11" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="11" spans="1:17" ht="26">
-      <c r="A11" s="11" t="s">
-        <v>122</v>
-      </c>
-      <c r="B11" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" s="11" t="s">
+      <c r="E11" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="G11" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="H11" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="D11" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E11" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="F11" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="G11" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="H11" s="11" t="s">
-        <v>60</v>
-      </c>
       <c r="I11" s="11" t="s">
-        <v>16</v>
+        <v>49</v>
       </c>
       <c r="J11" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="M11" t="s">
         <v>61</v>
       </c>
-      <c r="M11" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17">
+      <c r="R11" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21">
       <c r="A12">
         <v>2</v>
       </c>
@@ -7922,20 +8692,32 @@
         <v>9</v>
       </c>
       <c r="M12" s="11" t="s">
-        <v>122</v>
+        <v>156</v>
       </c>
       <c r="N12" s="11" t="s">
-        <v>15</v>
+        <v>48</v>
       </c>
       <c r="O12" s="11" t="s">
-        <v>94</v>
+        <v>128</v>
       </c>
       <c r="P12" s="11" t="s">
-        <v>29</v>
+        <v>62</v>
       </c>
       <c r="Q12" s="11"/>
-    </row>
-    <row r="13" spans="1:17">
+      <c r="R12" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="S12" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="T12" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="U12" s="11" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21">
       <c r="A13">
         <v>4</v>
       </c>
@@ -7985,12 +8767,11 @@
         <f>47*60+36</f>
         <v>2856</v>
       </c>
-      <c r="Q13">
-        <f>42*60+28</f>
-        <v>2548</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17">
+      <c r="R13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21">
       <c r="A14">
         <v>8</v>
       </c>
@@ -8036,7 +8817,7 @@
         <v>2982</v>
       </c>
     </row>
-    <row r="15" spans="1:17">
+    <row r="15" spans="1:21">
       <c r="N15">
         <v>139</v>
       </c>
@@ -8048,96 +8829,165 @@
         <v>2954</v>
       </c>
     </row>
-    <row r="17" spans="1:17">
+    <row r="17" spans="1:18">
       <c r="A17" t="s">
-        <v>58</v>
+        <v>92</v>
       </c>
       <c r="B17" t="s">
-        <v>92</v>
+        <v>126</v>
       </c>
       <c r="M17">
         <v>4</v>
       </c>
-    </row>
-    <row r="18" spans="1:17">
+      <c r="N17">
+        <v>115</v>
+      </c>
+      <c r="O17">
+        <v>25</v>
+      </c>
+      <c r="P17">
+        <v>5006</v>
+      </c>
+      <c r="R17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18">
       <c r="A18" t="s">
-        <v>59</v>
+        <v>93</v>
       </c>
       <c r="B18">
         <v>563</v>
       </c>
-      <c r="M18">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17">
+      <c r="N18">
+        <v>123</v>
+      </c>
+      <c r="O18">
+        <v>25</v>
+      </c>
+      <c r="P18">
+        <v>4731</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18">
       <c r="A19" t="s">
-        <v>101</v>
+        <v>135</v>
       </c>
       <c r="B19">
         <f>19*60</f>
         <v>1140</v>
       </c>
-    </row>
-    <row r="20" spans="1:17">
+      <c r="N19">
+        <v>116</v>
+      </c>
+      <c r="O19">
+        <v>25</v>
+      </c>
+      <c r="P19">
+        <v>4804</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18">
       <c r="A20" t="s">
-        <v>102</v>
+        <v>136</v>
       </c>
       <c r="B20">
         <v>2611</v>
       </c>
     </row>
-    <row r="26" spans="1:17">
+    <row r="21" spans="1:18">
+      <c r="M21">
+        <v>8</v>
+      </c>
+      <c r="N21">
+        <v>116</v>
+      </c>
+      <c r="O21">
+        <v>50</v>
+      </c>
+      <c r="P21">
+        <v>8765</v>
+      </c>
+      <c r="R21">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18">
+      <c r="N22">
+        <v>115</v>
+      </c>
+      <c r="O22">
+        <v>50</v>
+      </c>
+      <c r="P22">
+        <v>8546</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18">
+      <c r="N23">
+        <v>136</v>
+      </c>
+      <c r="O23">
+        <v>50</v>
+      </c>
+      <c r="P23">
+        <v>8579</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18">
       <c r="A26" t="s">
-        <v>122</v>
+        <v>156</v>
       </c>
       <c r="B26" t="s">
-        <v>104</v>
+        <v>138</v>
       </c>
       <c r="C26" t="s">
-        <v>103</v>
+        <v>137</v>
       </c>
       <c r="D26" t="s">
-        <v>9</v>
+        <v>41</v>
       </c>
       <c r="E26" t="s">
-        <v>92</v>
+        <v>126</v>
       </c>
       <c r="F26" t="s">
-        <v>104</v>
+        <v>138</v>
       </c>
       <c r="G26" t="s">
-        <v>103</v>
+        <v>137</v>
       </c>
       <c r="H26" t="s">
-        <v>9</v>
+        <v>41</v>
       </c>
       <c r="I26" t="s">
-        <v>92</v>
+        <v>126</v>
       </c>
       <c r="J26" t="s">
-        <v>105</v>
+        <v>139</v>
       </c>
       <c r="K26" t="s">
-        <v>103</v>
+        <v>137</v>
       </c>
       <c r="L26" t="s">
-        <v>9</v>
+        <v>41</v>
       </c>
       <c r="M26" t="s">
-        <v>92</v>
+        <v>126</v>
       </c>
       <c r="N26" t="s">
-        <v>106</v>
+        <v>140</v>
       </c>
       <c r="P26" t="s">
-        <v>109</v>
+        <v>143</v>
       </c>
       <c r="Q26" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="27" spans="1:17">
+        <v>144</v>
+      </c>
+      <c r="R26" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18">
       <c r="A27">
         <v>2</v>
       </c>
@@ -8189,8 +9039,12 @@
         <f>1.96 * STDEV(E27,I27,M27)/SQRT(3)</f>
         <v>4.097169079209209</v>
       </c>
-    </row>
-    <row r="28" spans="1:17">
+      <c r="R27">
+        <f>P27+I34</f>
+        <v>1633.7104782608696</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18">
       <c r="A28">
         <v>4</v>
       </c>
@@ -8241,8 +9095,12 @@
         <f t="shared" ref="Q28:Q29" si="6">1.96 * STDEV(E28,I28,M28)/SQRT(3)</f>
         <v>30.100037057320566</v>
       </c>
-    </row>
-    <row r="29" spans="1:17">
+      <c r="R28">
+        <f>P28+J34</f>
+        <v>3087.090623188406</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18">
       <c r="A29">
         <v>8</v>
       </c>
@@ -8293,58 +9151,133 @@
         <f t="shared" si="6"/>
         <v>10.540389098093113</v>
       </c>
-    </row>
-    <row r="44" spans="3:3">
+      <c r="R29">
+        <f>P29+K34</f>
+        <v>5297.2862463768115</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18">
+      <c r="I32" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="3:11">
+      <c r="I33" t="s">
+        <v>2</v>
+      </c>
+      <c r="J33" t="s">
+        <v>3</v>
+      </c>
+      <c r="K33" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="3:11">
+      <c r="I34">
+        <v>89.043478260869563</v>
+      </c>
+      <c r="J34">
+        <v>178.08695652173913</v>
+      </c>
+      <c r="K34">
+        <v>356.17391304347825</v>
+      </c>
+    </row>
+    <row r="35" spans="3:11">
+      <c r="K35">
+        <f>4096/11.2</f>
+        <v>365.71428571428572</v>
+      </c>
+    </row>
+    <row r="36" spans="3:11">
+      <c r="K36">
+        <f>4096/11.6</f>
+        <v>353.10344827586209</v>
+      </c>
+    </row>
+    <row r="37" spans="3:11">
+      <c r="D37">
+        <f>30446636</f>
+        <v>30446636</v>
+      </c>
+      <c r="E37">
+        <f>D37-E38</f>
+        <v>-716</v>
+      </c>
+    </row>
+    <row r="38" spans="3:11">
+      <c r="E38">
+        <f>1171052*26</f>
+        <v>30447352</v>
+      </c>
+      <c r="F38">
+        <f>716/4</f>
+        <v>179</v>
+      </c>
+    </row>
+    <row r="41" spans="3:11">
+      <c r="H41" s="13"/>
+    </row>
+    <row r="44" spans="3:11">
       <c r="C44" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="45" spans="3:3">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="45" spans="3:11">
       <c r="C45" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="46" spans="3:3">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="46" spans="3:11">
       <c r="C46" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="47" spans="3:3">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="47" spans="3:11">
       <c r="C47" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11">
       <c r="D53" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11">
       <c r="A56" t="s">
+        <v>32</v>
+      </c>
+      <c r="B56" t="s">
+        <v>33</v>
+      </c>
+      <c r="C56" t="s">
+        <v>170</v>
+      </c>
+      <c r="D56" t="s">
+        <v>34</v>
+      </c>
+      <c r="E56" t="s">
+        <v>171</v>
+      </c>
+      <c r="F56" t="s">
+        <v>35</v>
+      </c>
+      <c r="G56" t="s">
+        <v>36</v>
+      </c>
+      <c r="H56" t="s">
         <v>0</v>
       </c>
-      <c r="B56" t="s">
+      <c r="I56" t="s">
         <v>1</v>
       </c>
-      <c r="C56" t="s">
-        <v>136</v>
-      </c>
-      <c r="D56" t="s">
-        <v>2</v>
-      </c>
-      <c r="E56" t="s">
-        <v>3</v>
-      </c>
-      <c r="F56" t="s">
-        <v>137</v>
-      </c>
-      <c r="G56" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7">
+      <c r="K56" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11">
       <c r="A57" t="s">
-        <v>5</v>
+        <v>37</v>
       </c>
       <c r="B57">
         <v>1171052</v>
@@ -8357,17 +9290,28 @@
         <v>1514.68</v>
       </c>
       <c r="E57">
+        <v>451</v>
+      </c>
+      <c r="F57">
         <v>71.5</v>
       </c>
-      <c r="F57">
-        <v>51.42</v>
-      </c>
       <c r="G57">
-        <f>C57+D57+E57+F57</f>
-        <v>1651.15</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7">
+        <f>C57+D57+F57+E57</f>
+        <v>2050.73</v>
+      </c>
+      <c r="H57">
+        <f>AVERAGE(G57:G59)</f>
+        <v>2062.12</v>
+      </c>
+      <c r="I57">
+        <f>1.96*(STDEV(G57:G59)/SQRT(3))</f>
+        <v>12.103286987068245</v>
+      </c>
+      <c r="K57" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11">
       <c r="B58">
         <v>1171052</v>
       </c>
@@ -8379,17 +9323,23 @@
         <v>1527.62</v>
       </c>
       <c r="E58">
+        <v>449</v>
+      </c>
+      <c r="F58">
         <v>73.239999999999995</v>
       </c>
-      <c r="F58">
-        <v>49.51</v>
-      </c>
       <c r="G58">
-        <f t="shared" ref="G58:G59" si="7">C58+D58+E58+F58</f>
-        <v>1664.1899999999998</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7">
+        <f>C58+D58+F58+E58</f>
+        <v>2063.6799999999998</v>
+      </c>
+      <c r="H58">
+        <v>3847.2836666666662</v>
+      </c>
+      <c r="I58">
+        <v>19.032393616609415</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11">
       <c r="B59">
         <v>1171052</v>
       </c>
@@ -8401,83 +9351,370 @@
         <v>1538.22</v>
       </c>
       <c r="E59">
+        <v>449</v>
+      </c>
+      <c r="F59">
         <v>71.010000000000005</v>
       </c>
-      <c r="F59">
-        <v>49.54</v>
-      </c>
       <c r="G59">
-        <f t="shared" si="7"/>
-        <v>1672.49</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7">
+        <f>C59+D59+F59+E59</f>
+        <v>2071.9499999999998</v>
+      </c>
+      <c r="H59">
+        <v>6855.4446666666663</v>
+      </c>
+      <c r="I59">
+        <v>24.167021097560671</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11">
       <c r="A61" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
       <c r="B61">
         <v>1171052</v>
       </c>
-    </row>
-    <row r="62" spans="1:7">
+      <c r="C61">
+        <f>57.14/2</f>
+        <v>28.57</v>
+      </c>
+      <c r="D61">
+        <v>2762.45</v>
+      </c>
+      <c r="E61">
+        <v>952</v>
+      </c>
+      <c r="F61">
+        <v>90.721000000000004</v>
+      </c>
+      <c r="G61">
+        <f>C61+D61+E61+F61</f>
+        <v>3833.741</v>
+      </c>
+      <c r="H61">
+        <f>AVERAGE(G61:G63)</f>
+        <v>3847.2836666666662</v>
+      </c>
+      <c r="I61">
+        <f>1.96*(STDEV(G61:G63)/SQRT(3))</f>
+        <v>19.032393616609415</v>
+      </c>
+      <c r="K61" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11">
       <c r="B62">
         <v>1171052</v>
       </c>
-    </row>
-    <row r="63" spans="1:7">
+      <c r="C62">
+        <v>25.68</v>
+      </c>
+      <c r="D62">
+        <v>2792.7</v>
+      </c>
+      <c r="E62">
+        <v>958</v>
+      </c>
+      <c r="F62">
+        <v>89.73</v>
+      </c>
+      <c r="G62">
+        <f t="shared" ref="G62:G63" si="7">C62+D62+E62+F62</f>
+        <v>3866.1099999999997</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11">
       <c r="B63">
         <v>1171052</v>
       </c>
-    </row>
-    <row r="66" spans="1:8">
+      <c r="C63">
+        <f>42.48/2</f>
+        <v>21.24</v>
+      </c>
+      <c r="D63">
+        <v>2770.53</v>
+      </c>
+      <c r="E63">
+        <f>16*60</f>
+        <v>960</v>
+      </c>
+      <c r="F63">
+        <v>90.23</v>
+      </c>
+      <c r="G63">
+        <f t="shared" si="7"/>
+        <v>3842</v>
+      </c>
+    </row>
+    <row r="66" spans="1:23">
       <c r="A66" t="s">
-        <v>7</v>
+        <v>39</v>
       </c>
       <c r="B66">
         <v>1171052</v>
       </c>
-    </row>
-    <row r="67" spans="1:8">
+      <c r="C66">
+        <f>72.3/2</f>
+        <v>36.15</v>
+      </c>
+      <c r="D66">
+        <v>4742.82</v>
+      </c>
+      <c r="E66">
+        <f>32*60</f>
+        <v>1920</v>
+      </c>
+      <c r="F66">
+        <v>140.9</v>
+      </c>
+      <c r="G66">
+        <f>C66+D66+E66+F66</f>
+        <v>6839.869999999999</v>
+      </c>
+      <c r="H66">
+        <f>AVERAGE(G66:G68)</f>
+        <v>6855.4446666666663</v>
+      </c>
+      <c r="I66">
+        <f>1.96*(STDEV(G66:G68)/SQRT(3))</f>
+        <v>24.167021097560671</v>
+      </c>
+      <c r="K66" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="67" spans="1:23">
       <c r="B67">
         <v>1171052</v>
       </c>
-    </row>
-    <row r="68" spans="1:8">
+      <c r="C67">
+        <v>35.21</v>
+      </c>
+      <c r="D67">
+        <v>4780.3500000000004</v>
+      </c>
+      <c r="E67">
+        <f>1923</f>
+        <v>1923</v>
+      </c>
+      <c r="F67">
+        <v>141.22999999999999</v>
+      </c>
+      <c r="G67">
+        <f t="shared" ref="G67:G68" si="8">C67+D67+E67+F67</f>
+        <v>6879.79</v>
+      </c>
+    </row>
+    <row r="68" spans="1:23">
       <c r="B68">
         <v>1171052</v>
       </c>
-    </row>
-    <row r="76" spans="1:8">
+      <c r="C68">
+        <v>36.21</v>
+      </c>
+      <c r="D68">
+        <v>4745.2340000000004</v>
+      </c>
+      <c r="E68">
+        <v>1921</v>
+      </c>
+      <c r="F68">
+        <v>144.22999999999999</v>
+      </c>
+      <c r="G68">
+        <f t="shared" si="8"/>
+        <v>6846.674</v>
+      </c>
+    </row>
+    <row r="71" spans="1:23">
+      <c r="K71" t="s">
+        <v>12</v>
+      </c>
+      <c r="L71" t="s">
+        <v>19</v>
+      </c>
+      <c r="M71" t="s">
+        <v>18</v>
+      </c>
+      <c r="N71" t="s">
+        <v>31</v>
+      </c>
+      <c r="O71" t="s">
+        <v>16</v>
+      </c>
+      <c r="P71" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q71" t="s">
+        <v>21</v>
+      </c>
+      <c r="R71" t="s">
+        <v>22</v>
+      </c>
+      <c r="S71" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="72" spans="1:23">
+      <c r="J72" t="s">
+        <v>11</v>
+      </c>
+      <c r="K72" t="s">
+        <v>13</v>
+      </c>
+      <c r="L72">
+        <v>356.17391304347825</v>
+      </c>
+      <c r="N72">
+        <v>109</v>
+      </c>
+      <c r="O72">
+        <f>AVERAGE(C7,F7,I7)</f>
+        <v>7066</v>
+      </c>
+      <c r="P72">
+        <v>103</v>
+      </c>
+      <c r="R72">
+        <f>AVERAGE(D7,G7,J7)</f>
+        <v>1670.6666666666667</v>
+      </c>
+      <c r="S72">
+        <f>SUM(L72:R72)</f>
+        <v>9304.8405797101441</v>
+      </c>
+    </row>
+    <row r="73" spans="1:23">
+      <c r="K73" t="s">
+        <v>14</v>
+      </c>
+      <c r="L73">
+        <v>356.17391304347825</v>
+      </c>
+      <c r="M73">
+        <v>98.637</v>
+      </c>
+      <c r="O73">
+        <f>AVERAGE(C29,G29,K29)</f>
+        <v>4699.4553333333324</v>
+      </c>
+      <c r="P73">
+        <f>250</f>
+        <v>250</v>
+      </c>
+      <c r="R73">
+        <f>AVERAGE(D29,H29,L29)</f>
+        <v>143.12300000000002</v>
+      </c>
+      <c r="S73">
+        <f>SUM(L73:R73)</f>
+        <v>5547.3892463768107</v>
+      </c>
+    </row>
+    <row r="74" spans="1:23">
+      <c r="K74" t="s">
+        <v>15</v>
+      </c>
+      <c r="L74">
+        <v>0</v>
+      </c>
+      <c r="M74">
+        <f>AVERAGE(C66:C68)</f>
+        <v>35.856666666666662</v>
+      </c>
+      <c r="O74">
+        <f>AVERAGE(D66:D68)</f>
+        <v>4756.1346666666668</v>
+      </c>
+      <c r="Q74">
+        <f>1922</f>
+        <v>1922</v>
+      </c>
+      <c r="R74">
+        <f>AVERAGE(F66:F68)</f>
+        <v>142.12</v>
+      </c>
+      <c r="S74">
+        <f t="shared" ref="S73:S74" si="9">SUM(M74:R74)</f>
+        <v>6856.1113333333333</v>
+      </c>
+    </row>
+    <row r="76" spans="1:23">
       <c r="D76" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="79" spans="1:8">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="78" spans="1:23">
+      <c r="P78" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q78" t="s">
+        <v>24</v>
+      </c>
+      <c r="R78" t="s">
+        <v>25</v>
+      </c>
+      <c r="S78" t="s">
+        <v>26</v>
+      </c>
+      <c r="T78" t="s">
+        <v>28</v>
+      </c>
+      <c r="U78" t="s">
+        <v>27</v>
+      </c>
+      <c r="V78" t="s">
+        <v>17</v>
+      </c>
+      <c r="W78" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="79" spans="1:23">
       <c r="A79" t="s">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="B79" t="s">
-        <v>1</v>
+        <v>33</v>
       </c>
       <c r="C79" t="s">
-        <v>136</v>
+        <v>170</v>
       </c>
       <c r="D79" t="s">
-        <v>2</v>
+        <v>34</v>
       </c>
       <c r="E79" t="s">
-        <v>137</v>
+        <v>171</v>
       </c>
       <c r="F79" t="s">
-        <v>3</v>
+        <v>35</v>
       </c>
       <c r="G79" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="80" spans="1:8">
+        <v>126</v>
+      </c>
+      <c r="P79">
+        <v>7.4416887262080644</v>
+      </c>
+      <c r="R79">
+        <v>3.9740715197946423</v>
+      </c>
+      <c r="S79">
+        <v>95.102086903144965</v>
+      </c>
+      <c r="T79">
+        <v>1.1316065276116667</v>
+      </c>
+      <c r="V79">
+        <v>23.907001299019289</v>
+      </c>
+      <c r="W79">
+        <v>118.91205116011056</v>
+      </c>
+    </row>
+    <row r="80" spans="1:23">
       <c r="A80" t="s">
-        <v>5</v>
+        <v>37</v>
       </c>
       <c r="B80">
         <v>1171052</v>
@@ -8500,10 +9737,31 @@
         <v>1279.5150000000001</v>
       </c>
       <c r="H80" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="81" spans="1:7">
+        <v>76</v>
+      </c>
+      <c r="P80">
+        <v>7.4416887262080644</v>
+      </c>
+      <c r="Q80">
+        <v>2.9398669347662096</v>
+      </c>
+      <c r="S80">
+        <v>11.312186388587316</v>
+      </c>
+      <c r="T80">
+        <v>5.1856725696865977</v>
+      </c>
+      <c r="U80">
+        <v>1.1316065276116667</v>
+      </c>
+      <c r="V80">
+        <v>1.7616769592647126</v>
+      </c>
+      <c r="W80">
+        <v>10.540389098093113</v>
+      </c>
+    </row>
+    <row r="81" spans="1:23">
       <c r="B81">
         <v>1171052</v>
       </c>
@@ -8521,11 +9779,26 @@
         <v>58.19</v>
       </c>
       <c r="G81">
-        <f t="shared" ref="G81:G82" si="8">C81+D81+E81+F81</f>
+        <f t="shared" ref="G81:G82" si="10">C81+D81+E81+F81</f>
         <v>1262.1400000000003</v>
       </c>
-    </row>
-    <row r="82" spans="1:7">
+      <c r="Q81">
+        <v>0.63464196030352471</v>
+      </c>
+      <c r="S81">
+        <v>23.770300174015858</v>
+      </c>
+      <c r="U81">
+        <v>1.728557523113877</v>
+      </c>
+      <c r="V81">
+        <v>2.0762127443960567</v>
+      </c>
+      <c r="W81">
+        <v>24.167021097560671</v>
+      </c>
+    </row>
+    <row r="82" spans="1:23">
       <c r="B82">
         <v>1171052</v>
       </c>
@@ -8543,54 +9816,54 @@
         <v>54.21</v>
       </c>
       <c r="G82">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>1264.49</v>
       </c>
     </row>
-    <row r="84" spans="1:7">
+    <row r="84" spans="1:23">
       <c r="A84" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
       <c r="B84">
         <v>1171052</v>
       </c>
     </row>
-    <row r="85" spans="1:7">
+    <row r="85" spans="1:23">
       <c r="A85" t="s">
-        <v>7</v>
+        <v>39</v>
       </c>
       <c r="B85">
         <v>1171052</v>
       </c>
     </row>
-    <row r="88" spans="1:7">
+    <row r="88" spans="1:23">
       <c r="A88" t="s">
-        <v>58</v>
+        <v>92</v>
       </c>
       <c r="B88" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="89" spans="1:7">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="89" spans="1:23">
       <c r="A89" t="s">
-        <v>59</v>
+        <v>93</v>
       </c>
       <c r="B89">
         <v>563</v>
       </c>
     </row>
-    <row r="90" spans="1:7">
+    <row r="90" spans="1:23">
       <c r="A90" t="s">
-        <v>101</v>
+        <v>135</v>
       </c>
       <c r="B90">
         <f>19*60</f>
         <v>1140</v>
       </c>
     </row>
-    <row r="91" spans="1:7" s="12" customFormat="1">
+    <row r="91" spans="1:23" s="12" customFormat="1">
       <c r="A91" t="s">
-        <v>102</v>
+        <v>136</v>
       </c>
       <c r="B91">
         <v>2611</v>
@@ -8611,19 +9884,19 @@
     </row>
     <row r="144" spans="2:6">
       <c r="B144" t="s">
-        <v>135</v>
+        <v>169</v>
       </c>
       <c r="C144" t="s">
-        <v>104</v>
+        <v>138</v>
       </c>
       <c r="D144" t="s">
-        <v>103</v>
+        <v>137</v>
       </c>
       <c r="E144" t="s">
-        <v>9</v>
+        <v>41</v>
       </c>
       <c r="F144" t="s">
-        <v>92</v>
+        <v>126</v>
       </c>
     </row>
     <row r="145" spans="2:2">

</xml_diff>

<commit_message>
new figures in the excel sheets
git-svn-id: file://localhost/tmp/svn2git/svn@6637 defb5e50-622e-49ec-a68e-d72c7db87b45
</commit_message>
<xml_diff>
--- a/papers/saga-mr-ngs/data/GS_data.xlsx
+++ b/papers/saga-mr-ngs/data/GS_data.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="21405"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="29160" yWindow="-6700" windowWidth="25440" windowHeight="14060" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="GS data" sheetId="1" r:id="rId1"/>
@@ -13,11 +13,10 @@
   </sheets>
   <externalReferences>
     <externalReference r:id="rId4"/>
-    <externalReference r:id="rId5"/>
   </externalReferences>
-  <calcPr calcId="130407" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
@@ -779,14 +778,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-  </numFmts>
-  <fonts count="8">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -921,7 +914,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
 </file>
 
@@ -929,7 +922,15 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="1"/>
   <c:lang val="en-US"/>
-  <c:style val="18"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -947,22 +948,26 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
+      <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:v>Map Phase time</c:v>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:errBars>
             <c:errBarType val="both"/>
             <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
                 <c:f>'[1]GS Data Analaysis'!$F$5:$F$8</c:f>
@@ -1055,9 +1060,11 @@
           <c:tx>
             <c:v>Reduce phase time</c:v>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:errBars>
             <c:errBarType val="both"/>
             <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
                 <c:f>'[1]GS Data Analaysis'!$H$5:$H$8</c:f>
@@ -1144,15 +1151,25 @@
             </c:numRef>
           </c:val>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="584352072"/>
-        <c:axId val="587060568"/>
+        <c:axId val="511901880"/>
+        <c:axId val="512701240"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="584352072"/>
+        <c:axId val="511901880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -1170,21 +1187,25 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="587060568"/>
+        <c:crossAx val="512701240"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="587060568"/>
+        <c:axId val="512701240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:title>
@@ -1203,20 +1224,24 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="584352072"/>
+        <c:crossAx val="511901880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -1230,12 +1255,22 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="1"/>
   <c:lang val="en-US"/>
-  <c:style val="2"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -1295,32 +1330,47 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
+          <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="578459624"/>
-        <c:axId val="584090904"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="573481896"/>
+        <c:axId val="454300232"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="578459624"/>
+        <c:axId val="573481896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="584090904"/>
+        <c:crossAx val="454300232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="584090904"/>
+        <c:axId val="454300232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="578459624"/>
+        <c:crossAx val="573481896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1328,8 +1378,11 @@
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -1343,7 +1396,15 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="1"/>
   <c:lang val="en-US"/>
-  <c:style val="2"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:autoTitleDeleted val="1"/>
     <c:plotArea>
@@ -1361,15 +1422,18 @@
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:v>SEQAL</c:v>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:errBars>
             <c:errBarType val="both"/>
             <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
                 <c:f>Sheet1!$N$5:$N$7</c:f>
@@ -1377,13 +1441,13 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
                   <c:pt idx="0">
-                    <c:v>18.29333333335506</c:v>
+                    <c:v>18.29333333333334</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>114.0978909143999</c:v>
+                    <c:v>114.0978909143859</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>118.9120511601106</c:v>
+                    <c:v>118.9120511601373</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1395,13 +1459,13 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
                   <c:pt idx="0">
-                    <c:v>18.29333333335506</c:v>
+                    <c:v>18.29333333333334</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>114.0978909143999</c:v>
+                    <c:v>114.0978909143859</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>118.9120511601106</c:v>
+                    <c:v>118.9120511601373</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1450,9 +1514,11 @@
           <c:tx>
             <c:v>Local-PMR</c:v>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:errBars>
             <c:errBarType val="both"/>
             <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
                 <c:f>Sheet1!$Q$27:$Q$29</c:f>
@@ -1460,13 +1526,13 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
                   <c:pt idx="0">
-                    <c:v>4.097169079209209</c:v>
+                    <c:v>4.09716907931949</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>30.10003705732057</c:v>
+                    <c:v>30.10003705736206</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>10.54038909809311</c:v>
+                    <c:v>10.54038909769669</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1478,13 +1544,13 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
                   <c:pt idx="0">
-                    <c:v>4.097169079209209</c:v>
+                    <c:v>4.09716907931949</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>30.10003705732057</c:v>
+                    <c:v>30.10003705736206</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>10.54038909809311</c:v>
+                    <c:v>10.54038909769669</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1533,9 +1599,11 @@
           <c:tx>
             <c:v>distributed-PMR</c:v>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:errBars>
             <c:errBarType val="both"/>
             <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
                 <c:f>Sheet1!$I$57:$I$59</c:f>
@@ -1543,7 +1611,7 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
                   <c:pt idx="0">
-                    <c:v>12.10328698706824</c:v>
+                    <c:v>12.10328698715066</c:v>
                   </c:pt>
                   <c:pt idx="1">
                     <c:v>19.03239361660941</c:v>
@@ -1561,7 +1629,7 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
                   <c:pt idx="0">
-                    <c:v>12.10328698706824</c:v>
+                    <c:v>12.10328698715066</c:v>
                   </c:pt>
                   <c:pt idx="1">
                     <c:v>19.03239361660941</c:v>
@@ -1610,14 +1678,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="509676376"/>
-        <c:axId val="536533288"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="573411576"/>
+        <c:axId val="457303368"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="509676376"/>
+        <c:axId val="573411576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -1643,8 +1721,11 @@
               <c:y val="0.900806562677764"/>
             </c:manualLayout>
           </c:layout>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:txPr>
           <a:bodyPr/>
@@ -1656,17 +1737,19 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="536533288"/>
+        <c:crossAx val="457303368"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="536533288"/>
+        <c:axId val="457303368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:title>
           <c:tx>
@@ -1685,8 +1768,11 @@
             </c:rich>
           </c:tx>
           <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:txPr>
           <a:bodyPr/>
@@ -1698,16 +1784,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="509676376"/>
+        <c:crossAx val="573411576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:spPr>
-        <a:ln>
+        <a:ln w="19050">
           <a:solidFill>
-            <a:schemeClr val="bg1">
-              <a:lumMod val="65000"/>
-            </a:schemeClr>
+            <a:schemeClr val="tx1"/>
           </a:solidFill>
         </a:ln>
       </c:spPr>
@@ -1720,23 +1804,31 @@
           <c:yMode val="edge"/>
           <c:x val="0.215173891600483"/>
           <c:y val="0.105704096770512"/>
-          <c:w val="0.318285403309467"/>
-          <c:h val="0.183719901860094"/>
+          <c:w val="0.383080219724154"/>
+          <c:h val="0.256183669976036"/>
         </c:manualLayout>
       </c:layout>
+      <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400"/>
+            <a:defRPr sz="1600"/>
           </a:pPr>
           <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
+  <c:spPr>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
@@ -1749,8 +1841,17 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="1"/>
   <c:lang val="en-US"/>
-  <c:style val="18"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout>
         <c:manualLayout>
@@ -1766,6 +1867,7 @@
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -1780,9 +1882,11 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:errBars>
             <c:errBarType val="both"/>
             <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
                 <c:f>Sheet1!$P$79:$W$79</c:f>
@@ -1912,9 +2016,11 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:errBars>
             <c:errBarType val="both"/>
             <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
                 <c:f>Sheet1!$P$80:$W$80</c:f>
@@ -2050,9 +2156,11 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:errBars>
             <c:errBarType val="both"/>
             <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
                 <c:f>Sheet1!$P$81:$W$81</c:f>
@@ -2162,15 +2270,27 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="596695816"/>
-        <c:axId val="586960408"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="395021240"/>
+        <c:axId val="573509080"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="596695816"/>
+        <c:axId val="395021240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:txPr>
           <a:bodyPr rot="0" vert="horz" anchor="ctr" anchorCtr="1"/>
@@ -2182,17 +2302,19 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="586960408"/>
+        <c:crossAx val="573509080"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="586960408"/>
+        <c:axId val="573509080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:title>
           <c:tx>
@@ -2211,8 +2333,11 @@
             </c:rich>
           </c:tx>
           <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:txPr>
           <a:bodyPr/>
@@ -2224,7 +2349,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="596695816"/>
+        <c:crossAx val="395021240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2250,6 +2375,7 @@
           <c:h val="0.0937441673957422"/>
         </c:manualLayout>
       </c:layout>
+      <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
         <a:lstStyle/>
@@ -2262,6 +2388,8 @@
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -2275,8 +2403,17 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="1"/>
   <c:lang val="en-US"/>
-  <c:style val="18"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout>
         <c:manualLayout>
@@ -2292,6 +2429,7 @@
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -2306,9 +2444,11 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:errBars>
             <c:errBarType val="both"/>
             <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
                 <c:f>Sheet1!$U$110:$Y$110</c:f>
@@ -2420,9 +2560,11 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:errBars>
             <c:errBarType val="both"/>
             <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
                 <c:f>Sheet1!$U$111:$Y$111</c:f>
@@ -2534,9 +2676,11 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:errBars>
             <c:errBarType val="both"/>
             <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
                 <c:f>Sheet1!$U$112:$Y$112</c:f>
@@ -2634,15 +2778,27 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="760008184"/>
-        <c:axId val="597456808"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="456775288"/>
+        <c:axId val="456536472"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="760008184"/>
+        <c:axId val="456775288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:txPr>
           <a:bodyPr/>
@@ -2654,17 +2810,19 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="597456808"/>
+        <c:crossAx val="456536472"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="597456808"/>
+        <c:axId val="456536472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:title>
           <c:tx>
@@ -2683,8 +2841,11 @@
             </c:rich>
           </c:tx>
           <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:txPr>
           <a:bodyPr/>
@@ -2696,16 +2857,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="760008184"/>
+        <c:crossAx val="456775288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:spPr>
-        <a:ln>
+        <a:ln w="19050">
           <a:solidFill>
-            <a:schemeClr val="bg1">
-              <a:lumMod val="65000"/>
-            </a:schemeClr>
+            <a:schemeClr val="tx1"/>
           </a:solidFill>
         </a:ln>
       </c:spPr>
@@ -2722,6 +2881,7 @@
           <c:h val="0.241094286291137"/>
         </c:manualLayout>
       </c:layout>
+      <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
         <a:lstStyle/>
@@ -2734,7 +2894,14 @@
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
+  <c:spPr>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
@@ -2747,7 +2914,15 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="1"/>
   <c:lang val="en-US"/>
-  <c:style val="2"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -2765,22 +2940,26 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
+      <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:v>Map Phase time</c:v>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:errBars>
             <c:errBarType val="both"/>
             <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
                 <c:f>'[1]GS Data Analaysis'!$D$51:$D$53</c:f>
@@ -2861,9 +3040,11 @@
           <c:tx>
             <c:v>Reduce phase time</c:v>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:errBars>
             <c:errBarType val="both"/>
             <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
                 <c:f>'[1]GS Data Analaysis'!$F$51:$F$53</c:f>
@@ -2938,15 +3119,25 @@
             </c:numRef>
           </c:val>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="527914440"/>
-        <c:axId val="584302760"/>
+        <c:axId val="457275624"/>
+        <c:axId val="573138856"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="527914440"/>
+        <c:axId val="457275624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -2964,21 +3155,758 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="584302760"/>
+        <c:crossAx val="573138856"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="584302760"/>
+        <c:axId val="573138856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Time to solution in seconds</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="457275624"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="1"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Varying Input size, chunk size=62500 reads, number of reduces=8, number of workers=32</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>chunk time</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>'[1]GS Data Analaysis'!$E$81:$E$83</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>1.754000000000283</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>3.576333333336287</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>24.97066666666846</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>'[1]GS Data Analaysis'!$E$81:$E$83</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>1.754000000000283</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>3.576333333336287</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>24.97066666666846</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+          </c:errBars>
+          <c:cat>
+            <c:numRef>
+              <c:f>'[1]GS Data Analaysis'!$A$81:$A$83</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'[1]GS Data Analaysis'!$D$81:$D$83</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>187.717</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>396.5783333333333</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>860.7486666666667</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Map phase time</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>'[1]GS Data Analaysis'!$G$81:$G$83</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>19.67843770052061</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>13.90201619669563</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>67.3443622683438</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>'[1]GS Data Analaysis'!$G$81:$G$83</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>19.67843770052061</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>13.90201619669563</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>67.3443622683438</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+          </c:errBars>
+          <c:cat>
+            <c:numRef>
+              <c:f>'[1]GS Data Analaysis'!$A$81:$A$83</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'[1]GS Data Analaysis'!$F$81:$F$83</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1169.86</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2174.028</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4351.129</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Reduce phase time</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>'[1]GS Data Analaysis'!$I$81:$I$83</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>2.663626350172177</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>10.87379759380782</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>5.753053517722344</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>'[1]GS Data Analaysis'!$I$81:$I$83</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>2.663626350172177</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>10.87379759380782</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>5.753053517722344</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+          </c:errBars>
+          <c:cat>
+            <c:numRef>
+              <c:f>'[1]GS Data Analaysis'!$A$81:$A$83</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'[1]GS Data Analaysis'!$H$81:$H$83</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>141.32</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>302.1166666666667</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>671.0963333333332</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="100"/>
+        <c:axId val="454962632"/>
+        <c:axId val="573542152"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="454962632"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>input size in GB</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="573542152"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="573542152"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>time to solution in seconds</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="454962632"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="1"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Varying chunk size, Input size = 10GB, number of workers =32, Number of reduces = 8</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Map Phase time</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>'[1]GS Data Analaysis'!$F$5:$F$8</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="4"/>
+                  <c:pt idx="0">
+                    <c:v>0.951133183659104</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>25.90289232885597</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>15.29989664816251</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>19.67843770052061</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>'[1]GS Data Analaysis'!$F$5:$F$8</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="4"/>
+                  <c:pt idx="0">
+                    <c:v>0.951133183659104</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>25.90289232885597</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>15.29989664816251</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>19.67843770052061</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+          </c:errBars>
+          <c:cat>
+            <c:numRef>
+              <c:f>'[1]GS Data Analaysis'!$A$5:$A$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>78125.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>156250.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>312500.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>625000.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'[1]GS Data Analaysis'!$E$5:$E$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2104.295</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1504.33</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1283.610666666667</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1169.86</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Reduce phase time</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>'[1]GS Data Analaysis'!$H$5:$H$8</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="4"/>
+                  <c:pt idx="0">
+                    <c:v>3.89215151869082</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>1.200058933737725</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>2.23253774386384</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>2.663626350172177</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>'[1]GS Data Analaysis'!$H$5:$H$8</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="4"/>
+                  <c:pt idx="0">
+                    <c:v>3.89215151869082</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>1.200058933737725</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>2.23253774386384</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>2.663626350172177</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+          </c:errBars>
+          <c:cat>
+            <c:numRef>
+              <c:f>'[1]GS Data Analaysis'!$A$5:$A$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>78125.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>156250.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>312500.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>625000.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'[1]GS Data Analaysis'!$G$5:$G$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>161.0756666666666</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>145.6316666666667</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>146.4826666666667</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>141.32</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="100"/>
+        <c:axId val="456763208"/>
+        <c:axId val="511963832"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="456763208"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Number of sequence reads/chunk</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="511963832"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="511963832"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:title>
@@ -2998,10 +3926,13 @@
             </c:rich>
           </c:tx>
           <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="527914440"/>
+        <c:crossAx val="456763208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3009,665 +3940,11 @@
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="1"/>
-  <c:lang val="en-US"/>
-  <c:style val="18"/>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Varying Input size, chunk size=62500 reads, number of reduces=8, number of workers=32</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-    </c:title>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="stacked"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:v>chunk time</c:v>
-          </c:tx>
-          <c:errBars>
-            <c:errBarType val="both"/>
-            <c:errValType val="cust"/>
-            <c:plus>
-              <c:numRef>
-                <c:f>'[1]GS Data Analaysis'!$E$81:$E$83</c:f>
-                <c:numCache>
-                  <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="3"/>
-                  <c:pt idx="0">
-                    <c:v>1.754000000000283</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>3.576333333336287</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>24.97066666666846</c:v>
-                  </c:pt>
-                </c:numCache>
-              </c:numRef>
-            </c:plus>
-            <c:minus>
-              <c:numRef>
-                <c:f>'[1]GS Data Analaysis'!$E$81:$E$83</c:f>
-                <c:numCache>
-                  <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="3"/>
-                  <c:pt idx="0">
-                    <c:v>1.754000000000283</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>3.576333333336287</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>24.97066666666846</c:v>
-                  </c:pt>
-                </c:numCache>
-              </c:numRef>
-            </c:minus>
-          </c:errBars>
-          <c:cat>
-            <c:numRef>
-              <c:f>'[1]GS Data Analaysis'!$A$81:$A$83</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>10.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>20.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>40.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'[1]GS Data Analaysis'!$D$81:$D$83</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>187.717</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>396.5783333333333</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>860.7486666666667</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:v>Map phase time</c:v>
-          </c:tx>
-          <c:errBars>
-            <c:errBarType val="both"/>
-            <c:errValType val="cust"/>
-            <c:plus>
-              <c:numRef>
-                <c:f>'[1]GS Data Analaysis'!$G$81:$G$83</c:f>
-                <c:numCache>
-                  <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="3"/>
-                  <c:pt idx="0">
-                    <c:v>19.67843770052061</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>13.90201619669563</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>67.3443622683438</c:v>
-                  </c:pt>
-                </c:numCache>
-              </c:numRef>
-            </c:plus>
-            <c:minus>
-              <c:numRef>
-                <c:f>'[1]GS Data Analaysis'!$G$81:$G$83</c:f>
-                <c:numCache>
-                  <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="3"/>
-                  <c:pt idx="0">
-                    <c:v>19.67843770052061</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>13.90201619669563</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>67.3443622683438</c:v>
-                  </c:pt>
-                </c:numCache>
-              </c:numRef>
-            </c:minus>
-          </c:errBars>
-          <c:cat>
-            <c:numRef>
-              <c:f>'[1]GS Data Analaysis'!$A$81:$A$83</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>10.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>20.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>40.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'[1]GS Data Analaysis'!$F$81:$F$83</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>1169.86</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2174.028</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4351.129</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:v>Reduce phase time</c:v>
-          </c:tx>
-          <c:errBars>
-            <c:errBarType val="both"/>
-            <c:errValType val="cust"/>
-            <c:plus>
-              <c:numRef>
-                <c:f>'[1]GS Data Analaysis'!$I$81:$I$83</c:f>
-                <c:numCache>
-                  <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="3"/>
-                  <c:pt idx="0">
-                    <c:v>2.663626350172177</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>10.87379759380782</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>5.753053517722344</c:v>
-                  </c:pt>
-                </c:numCache>
-              </c:numRef>
-            </c:plus>
-            <c:minus>
-              <c:numRef>
-                <c:f>'[1]GS Data Analaysis'!$I$81:$I$83</c:f>
-                <c:numCache>
-                  <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="3"/>
-                  <c:pt idx="0">
-                    <c:v>2.663626350172177</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>10.87379759380782</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>5.753053517722344</c:v>
-                  </c:pt>
-                </c:numCache>
-              </c:numRef>
-            </c:minus>
-          </c:errBars>
-          <c:cat>
-            <c:numRef>
-              <c:f>'[1]GS Data Analaysis'!$A$81:$A$83</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>10.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>20.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>40.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'[1]GS Data Analaysis'!$H$81:$H$83</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>141.32</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>302.1166666666667</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>671.0963333333332</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:overlap val="100"/>
-        <c:axId val="586883816"/>
-        <c:axId val="586983752"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="586883816"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>input size in GB</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="586983752"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="586983752"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>time to solution in seconds</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="586883816"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="1"/>
-  <c:lang val="en-US"/>
-  <c:style val="18"/>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Varying chunk size, Input size = 10GB, number of workers =32, Number of reduces = 8</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-    </c:title>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="stacked"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:v>Map Phase time</c:v>
-          </c:tx>
-          <c:errBars>
-            <c:errBarType val="both"/>
-            <c:errValType val="cust"/>
-            <c:plus>
-              <c:numRef>
-                <c:f>'[1]GS Data Analaysis'!$F$5:$F$8</c:f>
-                <c:numCache>
-                  <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="4"/>
-                  <c:pt idx="0">
-                    <c:v>0.951133183659104</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>25.90289232885597</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>15.29989664816251</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>19.67843770052061</c:v>
-                  </c:pt>
-                </c:numCache>
-              </c:numRef>
-            </c:plus>
-            <c:minus>
-              <c:numRef>
-                <c:f>'[1]GS Data Analaysis'!$F$5:$F$8</c:f>
-                <c:numCache>
-                  <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="4"/>
-                  <c:pt idx="0">
-                    <c:v>0.951133183659104</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>25.90289232885597</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>15.29989664816251</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>19.67843770052061</c:v>
-                  </c:pt>
-                </c:numCache>
-              </c:numRef>
-            </c:minus>
-          </c:errBars>
-          <c:cat>
-            <c:numRef>
-              <c:f>'[1]GS Data Analaysis'!$A$5:$A$8</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>78125.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>156250.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>312500.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>625000.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'[1]GS Data Analaysis'!$E$5:$E$8</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>2104.295</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1504.33</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1283.610666666667</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1169.86</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:v>Reduce phase time</c:v>
-          </c:tx>
-          <c:errBars>
-            <c:errBarType val="both"/>
-            <c:errValType val="cust"/>
-            <c:plus>
-              <c:numRef>
-                <c:f>'[1]GS Data Analaysis'!$H$5:$H$8</c:f>
-                <c:numCache>
-                  <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="4"/>
-                  <c:pt idx="0">
-                    <c:v>3.89215151869082</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>1.200058933737725</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>2.23253774386384</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>2.663626350172177</c:v>
-                  </c:pt>
-                </c:numCache>
-              </c:numRef>
-            </c:plus>
-            <c:minus>
-              <c:numRef>
-                <c:f>'[1]GS Data Analaysis'!$H$5:$H$8</c:f>
-                <c:numCache>
-                  <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="4"/>
-                  <c:pt idx="0">
-                    <c:v>3.89215151869082</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>1.200058933737725</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>2.23253774386384</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>2.663626350172177</c:v>
-                  </c:pt>
-                </c:numCache>
-              </c:numRef>
-            </c:minus>
-          </c:errBars>
-          <c:cat>
-            <c:numRef>
-              <c:f>'[1]GS Data Analaysis'!$A$5:$A$8</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>78125.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>156250.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>312500.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>625000.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'[1]GS Data Analaysis'!$G$5:$G$8</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>161.0756666666666</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>145.6316666666667</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>146.4826666666667</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>141.32</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:overlap val="100"/>
-        <c:axId val="585075864"/>
-        <c:axId val="584554856"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="585075864"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Number of sequence reads/chunk</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="584554856"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="584554856"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Time to solution in seconds</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="585075864"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -3681,7 +3958,15 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="1"/>
   <c:lang val="en-US"/>
-  <c:style val="2"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:autoTitleDeleted val="1"/>
     <c:plotArea>
@@ -3699,15 +3984,18 @@
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:v>Map</c:v>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:errBars>
             <c:errBarType val="both"/>
             <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
                 <c:f>'[1]GS Data Analaysis'!$D$51:$D$53</c:f>
@@ -3788,9 +4076,11 @@
           <c:tx>
             <c:v>Reduce</c:v>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:errBars>
             <c:errBarType val="both"/>
             <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
                 <c:f>'[1]GS Data Analaysis'!$F$51:$F$53</c:f>
@@ -3865,15 +4155,25 @@
             </c:numRef>
           </c:val>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="587114216"/>
-        <c:axId val="578083688"/>
+        <c:axId val="456340600"/>
+        <c:axId val="379835704"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="587114216"/>
+        <c:axId val="456340600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -3886,14 +4186,17 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US" sz="1800"/>
-                  <a:t>Nodes</a:t>
+                  <a:t># of Nodes</a:t>
                 </a:r>
               </a:p>
             </c:rich>
           </c:tx>
           <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:txPr>
           <a:bodyPr/>
@@ -3905,17 +4208,19 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="578083688"/>
+        <c:crossAx val="379835704"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="578083688"/>
+        <c:axId val="379835704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:title>
           <c:tx>
@@ -3934,8 +4239,11 @@
             </c:rich>
           </c:tx>
           <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:txPr>
           <a:bodyPr/>
@@ -3947,16 +4255,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="587114216"/>
+        <c:crossAx val="456340600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:spPr>
-        <a:ln w="3175" cmpd="sng">
+        <a:ln w="19050" cmpd="sng">
           <a:solidFill>
-            <a:schemeClr val="bg1">
-              <a:lumMod val="65000"/>
-            </a:schemeClr>
+            <a:schemeClr val="tx1"/>
           </a:solidFill>
         </a:ln>
       </c:spPr>
@@ -3967,12 +4273,13 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.345150751610594"/>
-          <c:y val="0.151813420061623"/>
+          <c:x val="0.507013286310386"/>
+          <c:y val="0.15614241401643"/>
           <c:w val="0.340303793843951"/>
           <c:h val="0.157242725094146"/>
         </c:manualLayout>
       </c:layout>
+      <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
         <a:lstStyle/>
@@ -3985,7 +4292,14 @@
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
+  <c:spPr>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
@@ -3998,7 +4312,15 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="1"/>
   <c:lang val="en-US"/>
-  <c:style val="18"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:autoTitleDeleted val="1"/>
     <c:plotArea>
@@ -4016,15 +4338,18 @@
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:v>Chunk</c:v>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:errBars>
             <c:errBarType val="both"/>
             <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
                 <c:f>'[1]GS Data Analaysis'!$E$81:$E$83</c:f>
@@ -4105,9 +4430,11 @@
           <c:tx>
             <c:v>Map</c:v>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:errBars>
             <c:errBarType val="both"/>
             <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
                 <c:f>'[1]GS Data Analaysis'!$G$81:$G$83</c:f>
@@ -4188,9 +4515,11 @@
           <c:tx>
             <c:v>Reduce</c:v>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:errBars>
             <c:errBarType val="both"/>
             <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
                 <c:f>'[1]GS Data Analaysis'!$I$81:$I$83</c:f>
@@ -4265,15 +4594,25 @@
             </c:numRef>
           </c:val>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="509719880"/>
-        <c:axId val="584817256"/>
+        <c:axId val="511885576"/>
+        <c:axId val="511891112"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="509719880"/>
+        <c:axId val="511885576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -4299,9 +4638,15 @@
               <c:y val="0.869026548672566"/>
             </c:manualLayout>
           </c:layout>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="19050"/>
+        </c:spPr>
         <c:txPr>
           <a:bodyPr/>
           <a:lstStyle/>
@@ -4312,17 +4657,19 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="584817256"/>
+        <c:crossAx val="511891112"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="584817256"/>
+        <c:axId val="511891112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:title>
           <c:tx>
@@ -4341,8 +4688,11 @@
             </c:rich>
           </c:tx>
           <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:txPr>
           <a:bodyPr/>
@@ -4354,16 +4704,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="509719880"/>
+        <c:crossAx val="511885576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:spPr>
-        <a:ln w="9525">
+        <a:ln w="19050">
           <a:solidFill>
-            <a:schemeClr val="bg1">
-              <a:lumMod val="65000"/>
-            </a:schemeClr>
+            <a:schemeClr val="tx1"/>
           </a:solidFill>
         </a:ln>
       </c:spPr>
@@ -4380,6 +4728,7 @@
           <c:h val="0.142693540519824"/>
         </c:manualLayout>
       </c:layout>
+      <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
         <a:lstStyle/>
@@ -4392,7 +4741,14 @@
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
+  <c:spPr>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
@@ -4405,7 +4761,15 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="1"/>
   <c:lang val="en-US"/>
-  <c:style val="2"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -4424,7 +4788,9 @@
         </c:rich>
       </c:tx>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout>
         <c:manualLayout>
@@ -4439,6 +4805,7 @@
       </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -4503,14 +4870,23 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="585019848"/>
-        <c:axId val="536853016"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="573254792"/>
+        <c:axId val="573260248"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="585019848"/>
+        <c:axId val="573254792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -4529,18 +4905,22 @@
             </c:rich>
           </c:tx>
           <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="536853016"/>
+        <c:crossAx val="573260248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="536853016"/>
+        <c:axId val="573260248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:title>
@@ -4560,10 +4940,13 @@
             </c:rich>
           </c:tx>
           <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="585019848"/>
+        <c:crossAx val="573254792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4571,8 +4954,11 @@
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -4586,12 +4972,22 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="1"/>
   <c:lang val="en-US"/>
-  <c:style val="2"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -4645,32 +5041,47 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
+          <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="597134904"/>
-        <c:axId val="586422184"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="456396168"/>
+        <c:axId val="454681576"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="597134904"/>
+        <c:axId val="456396168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="586422184"/>
+        <c:crossAx val="454681576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="586422184"/>
+        <c:axId val="454681576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="597134904"/>
+        <c:crossAx val="456396168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4678,8 +5089,11 @@
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -4693,12 +5107,22 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="1"/>
   <c:lang val="en-US"/>
-  <c:style val="2"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -4752,32 +5176,47 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
+          <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="509726344"/>
-        <c:axId val="527822744"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="573389960"/>
+        <c:axId val="573392920"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="509726344"/>
+        <c:axId val="573389960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="527822744"/>
+        <c:crossAx val="573392920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="527822744"/>
+        <c:axId val="573392920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="509726344"/>
+        <c:crossAx val="573389960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4785,8 +5224,11 @@
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -5170,16 +5612,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>889000</xdr:colOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>812800</xdr:colOff>
       <xdr:row>84</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:rowOff>139700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>381000</xdr:colOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
       <xdr:row>102</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:rowOff>139700</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5460,19 +5902,6 @@
       <sheetData sheetId="14"/>
       <sheetData sheetId="15"/>
       <sheetData sheetId="16"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="GS Data Analaysis"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -5797,14 +6226,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y158"/>
   <sheetViews>
     <sheetView topLeftCell="A130" workbookViewId="0">
       <selection activeCell="H6" sqref="H6:J6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:14" ht="15">
       <c r="A1" s="1"/>
@@ -6577,7 +7006,7 @@
       </c>
       <c r="L25">
         <f>STDEV(E25,G25,I25)/SQRT(3)</f>
-        <v>0.95113318365910415</v>
+        <v>0.95113318380418077</v>
       </c>
       <c r="M25">
         <f>AVERAGE(F25,H25,J25)</f>
@@ -6585,7 +7014,7 @@
       </c>
       <c r="N25">
         <f>STDEV(F25,H25,J25)/SQRT(3)</f>
-        <v>3.8921515186908215</v>
+        <v>3.8921515186904561</v>
       </c>
     </row>
     <row r="26" spans="1:19">
@@ -6625,7 +7054,7 @@
       </c>
       <c r="L26">
         <f>STDEV(E26,G26,I26)/SQRT(3)</f>
-        <v>25.902892328855973</v>
+        <v>25.902892328850076</v>
       </c>
       <c r="M26">
         <f>AVERAGE(F26,H26,J26)</f>
@@ -6633,7 +7062,7 @@
       </c>
       <c r="N26">
         <f>STDEV(F26,H26,J26)/SQRT(3)</f>
-        <v>1.2000589337377248</v>
+        <v>1.2000589337380267</v>
       </c>
     </row>
     <row r="27" spans="1:19">
@@ -6673,7 +7102,7 @@
       </c>
       <c r="L27">
         <f>STDEV(E27,G27,I27)/SQRT(3)</f>
-        <v>15.299896648162512</v>
+        <v>15.299896648162221</v>
       </c>
       <c r="M27">
         <f>AVERAGE(F27,H27,J27)</f>
@@ -6681,7 +7110,7 @@
       </c>
       <c r="N27">
         <f>STDEV(F27,H27,J27)/SQRT(3)</f>
-        <v>2.2325377438638392</v>
+        <v>2.2325377438640941</v>
       </c>
     </row>
     <row r="28" spans="1:19">
@@ -6721,7 +7150,7 @@
       </c>
       <c r="L28">
         <f>STDEV(E28,G28,I28)/SQRT(3)</f>
-        <v>19.678437700520611</v>
+        <v>19.678437700522181</v>
       </c>
       <c r="M28">
         <f>AVERAGE(F28,H28,J28)</f>
@@ -6729,7 +7158,7 @@
       </c>
       <c r="N28">
         <f>STDEV(F28,H28,J28)/SQRT(3)</f>
-        <v>2.6636263501721773</v>
+        <v>2.6636263501725166</v>
       </c>
     </row>
     <row r="31" spans="1:19">
@@ -7527,7 +7956,7 @@
       </c>
       <c r="G88">
         <f>STDEV(C88,D88,E88)/SQRT(3)</f>
-        <v>44.339394594427489</v>
+        <v>44.33939459442368</v>
       </c>
       <c r="H88">
         <v>128.80500000000001</v>
@@ -7544,7 +7973,7 @@
       </c>
       <c r="L88">
         <f>STDEV(H88,I88,J88)/SQRT(3)</f>
-        <v>7.5428862071049236</v>
+        <v>7.5428862071048961</v>
       </c>
     </row>
     <row r="89" spans="1:12">
@@ -7570,7 +7999,7 @@
       </c>
       <c r="G89">
         <f>STDEV(C89,D89,E89)/SQRT(3)</f>
-        <v>58.385792408006402</v>
+        <v>58.385792408008861</v>
       </c>
       <c r="H89">
         <v>140.238</v>
@@ -7587,7 +8016,7 @@
       </c>
       <c r="L89">
         <f>STDEV(H89,I89,J89)/SQRT(3)</f>
-        <v>4.1344438965032166</v>
+        <v>4.1344438965032886</v>
       </c>
     </row>
     <row r="90" spans="1:12">
@@ -7613,7 +8042,7 @@
       </c>
       <c r="G90">
         <f>STDEV(C90,D90,E90)/SQRT(3)</f>
-        <v>19.678437700520611</v>
+        <v>19.678437700522181</v>
       </c>
       <c r="H90">
         <v>136.01</v>
@@ -7630,7 +8059,7 @@
       </c>
       <c r="L90">
         <f>STDEV(H90,I90,J90)/SQRT(3)</f>
-        <v>2.6636263501721773</v>
+        <v>2.6636263501725166</v>
       </c>
     </row>
     <row r="94" spans="1:12">
@@ -7870,7 +8299,7 @@
       </c>
       <c r="Q122">
         <f>STDEV(O122:O123)</f>
-        <v>1.0748023074035887E-2</v>
+        <v>1.0748023074035516E-2</v>
       </c>
     </row>
     <row r="123" spans="1:17">
@@ -8422,7 +8851,7 @@
       </c>
       <c r="G148">
         <f>STDEV(C148,D148,E148)/SQRT(3)</f>
-        <v>1.7540000000002831</v>
+        <v>1.7540000000000004</v>
       </c>
       <c r="H148">
         <v>1209.1849999999999</v>
@@ -8439,7 +8868,7 @@
       </c>
       <c r="L148">
         <f>STDEV(H148,I148,J148)/SQRT(3)</f>
-        <v>19.678437700520611</v>
+        <v>19.678437700522181</v>
       </c>
       <c r="M148">
         <v>136.01</v>
@@ -8456,7 +8885,7 @@
       </c>
       <c r="Q148">
         <f>STDEV(M148,N148,O148)/SQRT(3)</f>
-        <v>2.6636263501721773</v>
+        <v>2.6636263501725166</v>
       </c>
     </row>
     <row r="149" spans="1:17">
@@ -8475,7 +8904,7 @@
       </c>
       <c r="G149">
         <f>STDEV(C149,D149,E149)/SQRT(3)</f>
-        <v>3.5763333333362866</v>
+        <v>3.5763333333333285</v>
       </c>
       <c r="H149">
         <v>2187.7220000000002</v>
@@ -8492,7 +8921,7 @@
       </c>
       <c r="L149">
         <f>STDEV(H149,I149,J149)/SQRT(3)</f>
-        <v>13.902016196695632</v>
+        <v>13.902016196700965</v>
       </c>
       <c r="M149">
         <v>323.47300000000001</v>
@@ -8509,7 +8938,7 @@
       </c>
       <c r="Q149">
         <f>STDEV(M149,N149,O149)/SQRT(3)</f>
-        <v>10.873797593807824</v>
+        <v>10.8737975938083</v>
       </c>
     </row>
     <row r="150" spans="1:17">
@@ -8528,7 +8957,7 @@
       </c>
       <c r="G150">
         <f>STDEV(C150,D150,E150)/SQRT(3)</f>
-        <v>24.97066666666846</v>
+        <v>24.970666666666681</v>
       </c>
       <c r="H150">
         <v>4227.183</v>
@@ -8545,7 +8974,7 @@
       </c>
       <c r="L150">
         <f>STDEV(H150,I150,J150)/SQRT(3)</f>
-        <v>67.344362268343815</v>
+        <v>67.344362268369153</v>
       </c>
       <c r="M150">
         <v>673.399</v>
@@ -8562,7 +8991,7 @@
       </c>
       <c r="Q150">
         <f>STDEV(M150,N150,O150)/SQRT(3)</f>
-        <v>5.7530535177223436</v>
+        <v>5.7530535177223614</v>
       </c>
     </row>
     <row r="153" spans="1:17">
@@ -8694,7 +9123,7 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
@@ -8702,14 +9131,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:I85"/>
   <sheetViews>
-    <sheetView topLeftCell="A92" workbookViewId="0">
-      <selection activeCell="G60" sqref="G60"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="H73" sqref="H73"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
@@ -9165,7 +9594,7 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
@@ -9173,14 +9602,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:Z157"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K83" workbookViewId="0">
-      <selection activeCell="T108" sqref="T108"/>
+    <sheetView tabSelected="1" topLeftCell="N72" workbookViewId="0">
+      <selection activeCell="AA102" sqref="AA102"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="2" spans="1:21">
       <c r="A2" t="s">
@@ -9286,7 +9715,7 @@
       </c>
       <c r="N5">
         <f>1.96 * STDEV(E5,H5,K5)/SQRT(3)</f>
-        <v>18.293333333355065</v>
+        <v>18.293333333333337</v>
       </c>
       <c r="O5">
         <f>L5/13</f>
@@ -9339,7 +9768,7 @@
       </c>
       <c r="N6">
         <f t="shared" ref="N6:N7" si="1">1.96 * STDEV(E6,H6,K6)/SQRT(3)</f>
-        <v>114.09789091439987</v>
+        <v>114.09789091438593</v>
       </c>
     </row>
     <row r="7" spans="1:21">
@@ -9388,7 +9817,7 @@
       </c>
       <c r="N7">
         <f t="shared" si="1"/>
-        <v>118.91205116011055</v>
+        <v>118.91205116013731</v>
       </c>
     </row>
     <row r="9" spans="1:21">
@@ -9879,7 +10308,7 @@
       </c>
       <c r="Q27">
         <f>1.96 * STDEV(E27,I27,M27)/SQRT(3)</f>
-        <v>4.097169079209209</v>
+        <v>4.0971690793194897</v>
       </c>
       <c r="R27">
         <f>P27+I34</f>
@@ -9935,7 +10364,7 @@
       </c>
       <c r="Q28">
         <f t="shared" ref="Q28:Q29" si="6">1.96 * STDEV(E28,I28,M28)/SQRT(3)</f>
-        <v>30.100037057320566</v>
+        <v>30.100037057362055</v>
       </c>
       <c r="R28">
         <f>P28+J34</f>
@@ -9991,7 +10420,7 @@
       </c>
       <c r="Q29">
         <f t="shared" si="6"/>
-        <v>10.540389098093113</v>
+        <v>10.540389097696695</v>
       </c>
       <c r="R29">
         <f>P29+K34</f>
@@ -10158,7 +10587,7 @@
       </c>
       <c r="I57">
         <f>1.96*(STDEV(G57:G59)/SQRT(3))</f>
-        <v>12.103286987068245</v>
+        <v>12.103286987150657</v>
       </c>
       <c r="K57" t="s">
         <v>138</v>
@@ -10250,7 +10679,7 @@
       </c>
       <c r="I61">
         <f>1.96*(STDEV(G61:G63)/SQRT(3))</f>
-        <v>19.032393616609415</v>
+        <v>19.032393616362871</v>
       </c>
       <c r="K61" t="s">
         <v>140</v>
@@ -10331,7 +10760,7 @@
       </c>
       <c r="I66">
         <f>1.96*(STDEV(G66:G68)/SQRT(3))</f>
-        <v>24.167021097560671</v>
+        <v>24.16702109730387</v>
       </c>
       <c r="K66" t="s">
         <v>139</v>
@@ -10916,13 +11345,12 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>

</xml_diff>

<commit_message>
adding 2BG in crossbow
git-svn-id: file://localhost/tmp/svn2git/svn@6652 defb5e50-622e-49ec-a68e-d72c7db87b45
</commit_message>
<xml_diff>
--- a/papers/saga-mr-ngs/data/GS_data.xlsx
+++ b/papers/saga-mr-ngs/data/GS_data.xlsx
@@ -24,12 +24,633 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="211">
+  <si>
+    <t>Mean Map phase</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>stderr for map phase</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>mean reduce phase</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>stderr for reduce phase</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Mean </t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Stdev</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Remaining is Filedelimiter which I used.</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Varying Input size - I</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Input Data size(GB)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>duplicate  data size in GB</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Varying Input size - II</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>calculate tim taken for each map task.</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>calculate time for launching map task.</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Input Data size(GB)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Number of chunks created</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Number of  subjobs(workers) for both map/reduce phase</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>number of reduces.</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Total Time sec</t>
+  </si>
+  <si>
+    <t>Time taken to chunk files in seconds</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Map phase Time in seconds</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Reduce Phase Time in seconds</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>tts</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>caluclate time for sort time.</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>chunks</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Map</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>reduce</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>map</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>sequences</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>4GB</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>8GB</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Map</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>chunktime</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>chunktime</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>intermediate data</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mean tts</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>std tts</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>mean tts</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>stdtts</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>mean time taken for reduce phase</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>stderr for reduce phase phase time</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>crossbow</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>tts</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Varying Input size - III</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>mean chunk time</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Map phase Time in seconds - I</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Reduce Phase Time in seconds - I</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>seqal default configs</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>tts</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>mean reduce phase</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Reduce Phase Time in seconds</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>chunk time</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>exchange</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Duplicate output size is 4445MB which is 44.5% of input data</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>stderr of map phase</t>
+  </si>
+  <si>
+    <t>mean reduce phase</t>
+  </si>
+  <si>
+    <t>stderr of reduce phase</t>
+  </si>
+  <si>
+    <t>&lt; 1sec</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Data transfer in MB between map &amp; reduce phase is</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Reduced output size  3120 MB  which is 31.2% of input data</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Number of workers=(4+4), sierra and hotel used.</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Number of workers=(4+4), india and hotel used.</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>835 intermediate data</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>seqal map timings</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Reduced output size  3120 MB  which is 31.2% of input data</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Varying Input size, chunk size=625000, number  of reduces=8, number of workers=32</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Input data size in GB</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Total Time to solution in  secs</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>stderr in chunk time</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Reduce Phase Time in seconds - III</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mean</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>stderr</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>mean</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Varying chunk size ,  Input Size = 10GB, Number of workers - 32, Number of reduces -8</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>number of reads</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Number of chunks created</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>stderr chunk time</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>mean map phase</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>stderr in map phase</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>mean reduce phase</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>stderr reduce phase</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>stderr of map phase</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Varying Input size, chunk size=62500 reads, number of reduces=8, number of workers=32</t>
+  </si>
+  <si>
+    <t>Varying number of workers, input size = 10 GB, reduces = 8, Number of reads/ chunk=625000</t>
+  </si>
+  <si>
+    <t>Setup</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Map</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Shuffle</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Reduce</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Total</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>stderr in setup</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>stderr in map</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>stderr I shuffle</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>number of reads</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>chunk size( lines)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>stderr of reduce phase</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Varying number of workers, input size = 10 GB, reduces = 8, Number of reads/ chunk=625000</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Workers</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>mean map phase</t>
+  </si>
+  <si>
+    <t>map align only</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Time to transfer files files between map &amp; reduce phase is </t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Data transfer in MB between map &amp; reduce phase is</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>use default replication factor.</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>avg</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>stderr</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>1GB</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2GB</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>4GB</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>initial data transfers</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>tts with intial data transfer</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>232MB</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>943MB</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>445MB</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>max data for a reduce</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>8GB</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>MR type</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
   <si>
     <t>SEQAL</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
+    <t>Local-PMR</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>distributed-PMR</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Map</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>reduce</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Chunk</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Push Data</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Shuffle</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Exchange</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Reduce</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Total</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>stderr in cunk</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>stderr in setup</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>stderr in Map</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>sterr in exchange</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>stderr in shuffle</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>stderr in total</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>stderr in dt</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Setup</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Input data</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>chunk size</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>map</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>reduce</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>tts</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>(1+1)2</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>(2+2)4</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>(4+4)8</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Map</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Reduce</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>setup</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Varying chunk size ,  Input Size = 10GB, Number of workers - 32, Number of reduces -8</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mean Map phase</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Stdev</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Reduced output size  3120 MB  which is 31.2% of input data</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>mean map phase</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>File Transfer in seconds</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Map phase Time in seconds - II</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Reduce Phase Time in seconds-II</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Map phase Time in seconds-III</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>input data</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>mean time taken for map phase</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>stderr in map phase time</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>sequences per chunk</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SEQAL</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
     <t>local-PMR(bwa)</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -239,619 +860,6 @@
   </si>
   <si>
     <t>Varying Number of chunk size - I</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>chunk size( lines)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>stderr of reduce phase</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Varying number of workers, input size = 10 GB, reduces = 8, Number of reads/ chunk=625000</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Workers</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>mean map phase</t>
-  </si>
-  <si>
-    <t>map align only</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">Time to transfer files files between map &amp; reduce phase is </t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Data transfer in MB between map &amp; reduce phase is</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>use default replication factor.</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>avg</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>stderr</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>1GB</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>2GB</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>4GB</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>initial data transfers</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>tts with intial data transfer</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>232MB</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>943MB</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>445MB</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>max data for a reduce</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>8GB</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>MR type</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>SEQAL</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Local-PMR</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>distributed-PMR</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Map</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>reduce</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Chunk</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Push Data</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Shuffle</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Exchange</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Reduce</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Total</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>stderr in cunk</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>stderr in setup</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>stderr in Map</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>sterr in exchange</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>stderr in shuffle</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>stderr in total</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>stderr in dt</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Setup</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Input data</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>chunk size</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>map</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>reduce</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>tts</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>(1+1)2</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>(2+2)4</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>(4+4)8</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Map</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Reduce</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>setup</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Varying chunk size ,  Input Size = 10GB, Number of workers - 32, Number of reduces -8</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Mean Map phase</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Stdev</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Reduced output size  3120 MB  which is 31.2% of input data</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>mean map phase</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>File Transfer in seconds</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Map phase Time in seconds - II</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Reduce Phase Time in seconds-II</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Map phase Time in seconds-III</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>input data</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>mean time taken for map phase</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>stderr in map phase time</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>sequences per chunk</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Varying Input size - III</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>mean chunk time</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Map phase Time in seconds - I</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Reduce Phase Time in seconds - I</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>seqal default configs</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>tts</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>mean reduce phase</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Reduce Phase Time in seconds</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>chunk time</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>exchange</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Duplicate output size is 4445MB which is 44.5% of input data</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>stderr of map phase</t>
-  </si>
-  <si>
-    <t>mean reduce phase</t>
-  </si>
-  <si>
-    <t>stderr of reduce phase</t>
-  </si>
-  <si>
-    <t>&lt; 1sec</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Data transfer in MB between map &amp; reduce phase is</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Reduced output size  3120 MB  which is 31.2% of input data</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Number of workers=(4+4), sierra and hotel used.</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Number of workers=(4+4), india and hotel used.</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>835 intermediate data</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>seqal map timings</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Reduced output size  3120 MB  which is 31.2% of input data</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Varying Input size, chunk size=625000, number  of reduces=8, number of workers=32</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Input data size in GB</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Total Time to solution in  secs</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>stderr in chunk time</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Reduce Phase Time in seconds - III</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Mean</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>stderr</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>mean</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Varying chunk size ,  Input Size = 10GB, Number of workers - 32, Number of reduces -8</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>number of reads</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Number of chunks created</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>stderr chunk time</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>mean map phase</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>stderr in map phase</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>mean reduce phase</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>stderr reduce phase</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>stderr of map phase</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Varying Input size, chunk size=62500 reads, number of reduces=8, number of workers=32</t>
-  </si>
-  <si>
-    <t>Varying number of workers, input size = 10 GB, reduces = 8, Number of reads/ chunk=625000</t>
-  </si>
-  <si>
-    <t>Setup</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Map</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Shuffle</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Reduce</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Total</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>stderr in setup</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>stderr in map</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>stderr I shuffle</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>number of reads</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Mean Map phase</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>stderr for map phase</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>mean reduce phase</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>stderr for reduce phase</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">Mean </t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Stdev</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Remaining is Filedelimiter which I used.</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Varying Input size - I</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Input Data size(GB)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>duplicate  data size in GB</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Varying Input size - II</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>calculate tim taken for each map task.</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>calculate time for launching map task.</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Input Data size(GB)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Number of chunks created</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Number of  subjobs(workers) for both map/reduce phase</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>number of reduces.</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Total Time sec</t>
-  </si>
-  <si>
-    <t>Time taken to chunk files in seconds</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Map phase Time in seconds</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Reduce Phase Time in seconds</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>tts</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>caluclate time for sort time.</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>chunks</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Map</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>reduce</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>map</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>sequences</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>4GB</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>8GB</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Map</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>chunktime</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>chunktime</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>intermediate data</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Mean tts</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>std tts</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>mean tts</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>stdtts</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>mean time taken for reduce phase</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>stderr for reduce phase phase time</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -859,12 +867,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-  </numFmts>
   <fonts count="9">
     <font>
       <sz val="10"/>
@@ -1228,13 +1230,12 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls/>
         <c:overlap val="100"/>
-        <c:axId val="483217336"/>
-        <c:axId val="482932280"/>
+        <c:axId val="567752136"/>
+        <c:axId val="567764152"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="483217336"/>
+        <c:axId val="567752136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1258,14 +1259,14 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="482932280"/>
+        <c:crossAx val="567764152"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="482932280"/>
+        <c:axId val="567764152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1290,7 +1291,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="483217336"/>
+        <c:crossAx val="567752136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1332,7 +1333,6 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
             </c:trendlineLbl>
           </c:trendline>
@@ -1379,24 +1379,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="482750024"/>
-        <c:axId val="482753064"/>
+        <c:axId val="570573976"/>
+        <c:axId val="570563944"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="482750024"/>
+        <c:axId val="570573976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="482753064"/>
+        <c:crossAx val="570563944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="482753064"/>
+        <c:axId val="570563944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1404,14 +1403,13 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="482750024"/>
+        <c:crossAx val="570573976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
@@ -1462,13 +1460,13 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
                   <c:pt idx="0">
-                    <c:v>18.29333333333334</c:v>
+                    <c:v>18.29333333335506</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>114.0978909143859</c:v>
+                    <c:v>114.0978909143999</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>118.9120511601373</c:v>
+                    <c:v>118.9120511601106</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1480,13 +1478,13 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
                   <c:pt idx="0">
-                    <c:v>18.29333333333334</c:v>
+                    <c:v>18.29333333335506</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>114.0978909143859</c:v>
+                    <c:v>114.0978909143999</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>118.9120511601373</c:v>
+                    <c:v>118.9120511601106</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1545,13 +1543,13 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
                   <c:pt idx="0">
-                    <c:v>4.09716907931949</c:v>
+                    <c:v>4.097169079209209</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>30.10003705736206</c:v>
+                    <c:v>30.10003705732057</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>10.54038909769669</c:v>
+                    <c:v>10.54038909809311</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1563,13 +1561,13 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
                   <c:pt idx="0">
-                    <c:v>4.09716907931949</c:v>
+                    <c:v>4.097169079209209</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>30.10003705736206</c:v>
+                    <c:v>30.10003705732057</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>10.54038909769669</c:v>
+                    <c:v>10.54038909809311</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1628,7 +1626,7 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
                   <c:pt idx="0">
-                    <c:v>12.10328698715066</c:v>
+                    <c:v>12.10328698706824</c:v>
                   </c:pt>
                   <c:pt idx="1">
                     <c:v>19.03239361660941</c:v>
@@ -1646,7 +1644,7 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
                   <c:pt idx="0">
-                    <c:v>12.10328698715066</c:v>
+                    <c:v>12.10328698706824</c:v>
                   </c:pt>
                   <c:pt idx="1">
                     <c:v>19.03239361660941</c:v>
@@ -1695,12 +1693,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="482528168"/>
-        <c:axId val="482535576"/>
+        <c:axId val="552521080"/>
+        <c:axId val="552528488"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="482528168"/>
+        <c:axId val="552521080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1742,14 +1739,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="482535576"/>
+        <c:crossAx val="552528488"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="482535576"/>
+        <c:axId val="552528488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1784,7 +1781,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="482528168"/>
+        <c:crossAx val="552521080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2252,12 +2249,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="482827896"/>
-        <c:axId val="482831224"/>
+        <c:axId val="552571704"/>
+        <c:axId val="552575032"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="482827896"/>
+        <c:axId val="552571704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2273,14 +2269,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="482831224"/>
+        <c:crossAx val="552575032"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="482831224"/>
+        <c:axId val="552575032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2315,7 +2311,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="482827896"/>
+        <c:crossAx val="552571704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2726,12 +2722,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="483334440"/>
-        <c:axId val="483337768"/>
+        <c:axId val="570774696"/>
+        <c:axId val="570926136"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="483334440"/>
+        <c:axId val="570774696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2747,14 +2742,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="483337768"/>
+        <c:crossAx val="570926136"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="483337768"/>
+        <c:axId val="570926136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2789,7 +2784,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="483334440"/>
+        <c:crossAx val="570774696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3158,11 +3153,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="603852168"/>
-        <c:axId val="603855336"/>
+        <c:axId val="570880376"/>
+        <c:axId val="551907800"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="603852168"/>
+        <c:axId val="570880376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3197,14 +3192,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="603855336"/>
+        <c:crossAx val="551907800"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="603855336"/>
+        <c:axId val="551907800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3239,7 +3234,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="603852168"/>
+        <c:crossAx val="570880376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3480,13 +3475,12 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls/>
         <c:overlap val="100"/>
-        <c:axId val="482994088"/>
-        <c:axId val="483001352"/>
+        <c:axId val="567856600"/>
+        <c:axId val="567830088"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="482994088"/>
+        <c:axId val="567856600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3510,14 +3504,14 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="483001352"/>
+        <c:crossAx val="567830088"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="483001352"/>
+        <c:axId val="567830088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3542,7 +3536,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="482994088"/>
+        <c:crossAx val="567856600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3583,7 +3577,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -3839,13 +3832,12 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls/>
         <c:overlap val="100"/>
-        <c:axId val="483234840"/>
-        <c:axId val="482395256"/>
+        <c:axId val="589567432"/>
+        <c:axId val="589574712"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="483234840"/>
+        <c:axId val="589567432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3866,18 +3858,17 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="482395256"/>
+        <c:crossAx val="589574712"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="482395256"/>
+        <c:axId val="589574712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3899,18 +3890,16 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="483234840"/>
+        <c:crossAx val="589567432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
@@ -3945,7 +3934,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -4142,13 +4130,12 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls/>
         <c:overlap val="100"/>
-        <c:axId val="483087080"/>
-        <c:axId val="483241288"/>
+        <c:axId val="570744040"/>
+        <c:axId val="570749832"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="483087080"/>
+        <c:axId val="570744040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4169,18 +4156,17 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="483241288"/>
+        <c:crossAx val="570749832"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="483241288"/>
+        <c:axId val="570749832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4202,18 +4188,16 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="483087080"/>
+        <c:crossAx val="570744040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
@@ -4414,13 +4398,12 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls/>
         <c:overlap val="100"/>
-        <c:axId val="482623976"/>
-        <c:axId val="482631320"/>
+        <c:axId val="570630328"/>
+        <c:axId val="570826840"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="482623976"/>
+        <c:axId val="570630328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4441,7 +4424,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
@@ -4455,14 +4437,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="482631320"/>
+        <c:crossAx val="570826840"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="482631320"/>
+        <c:axId val="570826840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4483,7 +4465,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
@@ -4497,7 +4478,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="482623976"/>
+        <c:crossAx val="570630328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4819,13 +4800,12 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls/>
         <c:overlap val="100"/>
-        <c:axId val="483275672"/>
-        <c:axId val="482423896"/>
+        <c:axId val="568028824"/>
+        <c:axId val="568149208"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="483275672"/>
+        <c:axId val="568028824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4870,14 +4850,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="482423896"/>
+        <c:crossAx val="568149208"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="482423896"/>
+        <c:axId val="568149208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4898,7 +4878,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
@@ -4912,7 +4891,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="483275672"/>
+        <c:crossAx val="568028824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4985,7 +4964,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout>
@@ -5065,12 +5043,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="482608984"/>
-        <c:axId val="482812168"/>
+        <c:axId val="570836376"/>
+        <c:axId val="568157848"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="482608984"/>
+        <c:axId val="570836376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5091,16 +5068,15 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="482812168"/>
+        <c:crossAx val="568157848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="482812168"/>
+        <c:axId val="568157848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5122,18 +5098,16 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="482608984"/>
+        <c:crossAx val="570836376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
@@ -5169,7 +5143,6 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
             </c:trendlineLbl>
           </c:trendline>
@@ -5210,24 +5183,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="482684584"/>
-        <c:axId val="482687624"/>
+        <c:axId val="570577544"/>
+        <c:axId val="570437880"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="482684584"/>
+        <c:axId val="570577544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="482687624"/>
+        <c:crossAx val="570437880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="482687624"/>
+        <c:axId val="570437880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5235,14 +5207,13 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="482684584"/>
+        <c:crossAx val="570577544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
@@ -5278,7 +5249,6 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
             </c:trendlineLbl>
           </c:trendline>
@@ -5319,24 +5289,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="482717224"/>
-        <c:axId val="482720264"/>
+        <c:axId val="570467224"/>
+        <c:axId val="570470264"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="482717224"/>
+        <c:axId val="570467224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="482720264"/>
+        <c:crossAx val="570470264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="482720264"/>
+        <c:axId val="570470264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5344,14 +5313,13 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="482717224"/>
+        <c:crossAx val="570467224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
@@ -6399,7 +6367,7 @@
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
       <c r="G1" s="1" t="s">
-        <v>53</v>
+        <v>210</v>
       </c>
       <c r="H1" s="1"/>
       <c r="I1" s="2"/>
@@ -6411,46 +6379,46 @@
     </row>
     <row r="2" spans="1:14" ht="71" thickBot="1">
       <c r="A2" s="3" t="s">
-        <v>54</v>
+        <v>92</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>168</v>
+        <v>91</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>182</v>
+        <v>13</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>183</v>
+        <v>14</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>184</v>
+        <v>15</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>185</v>
+        <v>16</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>186</v>
+        <v>17</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>187</v>
+        <v>18</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>188</v>
+        <v>19</v>
       </c>
       <c r="J2" s="7" t="s">
-        <v>189</v>
+        <v>20</v>
       </c>
       <c r="K2" s="8" t="s">
-        <v>111</v>
+        <v>149</v>
       </c>
       <c r="L2" s="8" t="s">
-        <v>17</v>
+        <v>174</v>
       </c>
       <c r="M2" s="8" t="s">
-        <v>18</v>
+        <v>175</v>
       </c>
       <c r="N2" s="8" t="s">
-        <v>19</v>
+        <v>176</v>
       </c>
     </row>
     <row r="3" spans="1:14">
@@ -6629,7 +6597,7 @@
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="1" t="s">
-        <v>20</v>
+        <v>177</v>
       </c>
       <c r="H8" s="1"/>
       <c r="I8" s="2"/>
@@ -6641,46 +6609,46 @@
     </row>
     <row r="9" spans="1:14" ht="71" thickBot="1">
       <c r="A9" s="3" t="s">
-        <v>54</v>
+        <v>92</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>168</v>
+        <v>91</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>182</v>
+        <v>13</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>183</v>
+        <v>14</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>184</v>
+        <v>15</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>185</v>
+        <v>16</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>186</v>
+        <v>17</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>187</v>
+        <v>18</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>188</v>
+        <v>19</v>
       </c>
       <c r="J9" s="7" t="s">
-        <v>189</v>
+        <v>20</v>
       </c>
       <c r="K9" s="8" t="s">
-        <v>111</v>
+        <v>149</v>
       </c>
       <c r="L9" s="8" t="s">
-        <v>17</v>
+        <v>174</v>
       </c>
       <c r="M9" s="8" t="s">
-        <v>18</v>
+        <v>175</v>
       </c>
       <c r="N9" s="8" t="s">
-        <v>19</v>
+        <v>176</v>
       </c>
     </row>
     <row r="10" spans="1:14">
@@ -6859,7 +6827,7 @@
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
       <c r="G16" s="1" t="s">
-        <v>21</v>
+        <v>178</v>
       </c>
       <c r="H16" s="1"/>
       <c r="I16" s="2"/>
@@ -6871,46 +6839,46 @@
     </row>
     <row r="17" spans="1:19" ht="71" thickBot="1">
       <c r="A17" s="3" t="s">
-        <v>54</v>
+        <v>92</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>168</v>
+        <v>91</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>182</v>
+        <v>13</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>183</v>
+        <v>14</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>184</v>
+        <v>15</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>185</v>
+        <v>16</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>186</v>
+        <v>17</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>187</v>
+        <v>18</v>
       </c>
       <c r="I17" s="7" t="s">
-        <v>188</v>
+        <v>19</v>
       </c>
       <c r="J17" s="7" t="s">
-        <v>189</v>
+        <v>20</v>
       </c>
       <c r="K17" s="8" t="s">
-        <v>111</v>
+        <v>149</v>
       </c>
       <c r="L17" s="8" t="s">
-        <v>17</v>
+        <v>174</v>
       </c>
       <c r="M17" s="8" t="s">
-        <v>18</v>
+        <v>175</v>
       </c>
       <c r="N17" s="8" t="s">
-        <v>19</v>
+        <v>176</v>
       </c>
     </row>
     <row r="18" spans="1:19">
@@ -7083,46 +7051,46 @@
     </row>
     <row r="24" spans="1:19" ht="46" thickBot="1">
       <c r="A24" s="3" t="s">
-        <v>22</v>
+        <v>179</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>23</v>
+        <v>180</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>186</v>
+        <v>17</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>24</v>
+        <v>181</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>121</v>
+        <v>44</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>122</v>
+        <v>45</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>112</v>
+        <v>150</v>
       </c>
       <c r="H24" s="7" t="s">
-        <v>113</v>
+        <v>151</v>
       </c>
       <c r="I24" s="7" t="s">
-        <v>114</v>
+        <v>152</v>
       </c>
       <c r="J24" s="7" t="s">
-        <v>145</v>
+        <v>68</v>
       </c>
       <c r="K24" s="8" t="s">
-        <v>146</v>
+        <v>69</v>
       </c>
       <c r="L24" s="8" t="s">
-        <v>147</v>
+        <v>70</v>
       </c>
       <c r="M24" s="8" t="s">
-        <v>148</v>
+        <v>71</v>
       </c>
       <c r="N24" s="8" t="s">
-        <v>147</v>
+        <v>70</v>
       </c>
     </row>
     <row r="25" spans="1:19">
@@ -7162,7 +7130,7 @@
       </c>
       <c r="L25">
         <f>STDEV(E25,G25,I25)/SQRT(3)</f>
-        <v>0.95113318380418077</v>
+        <v>0.95113318365910415</v>
       </c>
       <c r="M25">
         <f>AVERAGE(F25,H25,J25)</f>
@@ -7170,7 +7138,7 @@
       </c>
       <c r="N25">
         <f>STDEV(F25,H25,J25)/SQRT(3)</f>
-        <v>3.8921515186904561</v>
+        <v>3.8921515186908215</v>
       </c>
     </row>
     <row r="26" spans="1:19">
@@ -7210,7 +7178,7 @@
       </c>
       <c r="L26">
         <f>STDEV(E26,G26,I26)/SQRT(3)</f>
-        <v>25.902892328850076</v>
+        <v>25.902892328855973</v>
       </c>
       <c r="M26">
         <f>AVERAGE(F26,H26,J26)</f>
@@ -7218,7 +7186,7 @@
       </c>
       <c r="N26">
         <f>STDEV(F26,H26,J26)/SQRT(3)</f>
-        <v>1.2000589337380267</v>
+        <v>1.2000589337377248</v>
       </c>
     </row>
     <row r="27" spans="1:19">
@@ -7258,7 +7226,7 @@
       </c>
       <c r="L27">
         <f>STDEV(E27,G27,I27)/SQRT(3)</f>
-        <v>15.299896648162221</v>
+        <v>15.299896648162512</v>
       </c>
       <c r="M27">
         <f>AVERAGE(F27,H27,J27)</f>
@@ -7266,7 +7234,7 @@
       </c>
       <c r="N27">
         <f>STDEV(F27,H27,J27)/SQRT(3)</f>
-        <v>2.2325377438640941</v>
+        <v>2.2325377438638392</v>
       </c>
     </row>
     <row r="28" spans="1:19">
@@ -7306,7 +7274,7 @@
       </c>
       <c r="L28">
         <f>STDEV(E28,G28,I28)/SQRT(3)</f>
-        <v>19.678437700522181</v>
+        <v>19.678437700520611</v>
       </c>
       <c r="M28">
         <f>AVERAGE(F28,H28,J28)</f>
@@ -7314,44 +7282,44 @@
       </c>
       <c r="N28">
         <f>STDEV(F28,H28,J28)/SQRT(3)</f>
-        <v>2.6636263501725166</v>
+        <v>2.6636263501721773</v>
       </c>
     </row>
     <row r="31" spans="1:19">
       <c r="D31" t="s">
-        <v>149</v>
+        <v>72</v>
       </c>
     </row>
     <row r="32" spans="1:19" ht="46" thickBot="1">
       <c r="D32" s="3" t="s">
-        <v>150</v>
+        <v>73</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>151</v>
+        <v>74</v>
       </c>
       <c r="F32" s="6" t="s">
-        <v>186</v>
+        <v>17</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>40</v>
+        <v>197</v>
       </c>
       <c r="H32" s="8" t="s">
-        <v>169</v>
+        <v>0</v>
       </c>
       <c r="I32" s="8" t="s">
-        <v>170</v>
+        <v>1</v>
       </c>
       <c r="J32" s="8" t="s">
-        <v>171</v>
+        <v>2</v>
       </c>
       <c r="K32" s="8" t="s">
-        <v>172</v>
+        <v>3</v>
       </c>
       <c r="R32" t="s">
-        <v>173</v>
+        <v>4</v>
       </c>
       <c r="S32" t="s">
-        <v>174</v>
+        <v>5</v>
       </c>
     </row>
     <row r="33" spans="4:19">
@@ -7381,7 +7349,7 @@
         <v>3.8921515186908202</v>
       </c>
       <c r="M33" t="s">
-        <v>60</v>
+        <v>98</v>
       </c>
       <c r="R33">
         <v>1.59</v>
@@ -7417,7 +7385,7 @@
         <v>1.2000589337377248</v>
       </c>
       <c r="M34" t="s">
-        <v>61</v>
+        <v>99</v>
       </c>
       <c r="R34" s="10">
         <v>9155.6200000000008</v>
@@ -7453,7 +7421,7 @@
         <v>2.2325377438638392</v>
       </c>
       <c r="M35" t="s">
-        <v>140</v>
+        <v>63</v>
       </c>
     </row>
     <row r="36" spans="4:19">
@@ -7483,17 +7451,17 @@
         <v>2.6636263501721773</v>
       </c>
       <c r="M36" t="s">
-        <v>45</v>
+        <v>202</v>
       </c>
     </row>
     <row r="37" spans="4:19">
       <c r="M37" t="s">
-        <v>46</v>
+        <v>203</v>
       </c>
     </row>
     <row r="60" spans="25:25">
       <c r="Y60" t="s">
-        <v>47</v>
+        <v>204</v>
       </c>
     </row>
     <row r="65" spans="1:14" ht="15">
@@ -7504,7 +7472,7 @@
       <c r="E65" s="2"/>
       <c r="F65" s="2"/>
       <c r="G65" s="1" t="s">
-        <v>48</v>
+        <v>205</v>
       </c>
       <c r="H65" s="1"/>
       <c r="I65" s="2"/>
@@ -7516,46 +7484,46 @@
     </row>
     <row r="66" spans="1:14" ht="71" thickBot="1">
       <c r="A66" s="3" t="s">
-        <v>54</v>
+        <v>92</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>168</v>
+        <v>91</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>182</v>
+        <v>13</v>
       </c>
       <c r="D66" s="5" t="s">
-        <v>183</v>
+        <v>14</v>
       </c>
       <c r="E66" s="3" t="s">
-        <v>184</v>
+        <v>15</v>
       </c>
       <c r="F66" s="3" t="s">
-        <v>185</v>
+        <v>16</v>
       </c>
       <c r="G66" s="6" t="s">
-        <v>186</v>
+        <v>17</v>
       </c>
       <c r="H66" s="3" t="s">
-        <v>187</v>
+        <v>18</v>
       </c>
       <c r="I66" s="7" t="s">
-        <v>188</v>
+        <v>19</v>
       </c>
       <c r="J66" s="7" t="s">
-        <v>189</v>
+        <v>20</v>
       </c>
       <c r="K66" s="8" t="s">
-        <v>111</v>
+        <v>149</v>
       </c>
       <c r="L66" s="8" t="s">
-        <v>17</v>
+        <v>174</v>
       </c>
       <c r="M66" s="8" t="s">
-        <v>18</v>
+        <v>175</v>
       </c>
       <c r="N66" s="8" t="s">
-        <v>19</v>
+        <v>176</v>
       </c>
     </row>
     <row r="67" spans="1:14">
@@ -7692,7 +7660,7 @@
       <c r="E72" s="2"/>
       <c r="F72" s="2"/>
       <c r="G72" s="1" t="s">
-        <v>49</v>
+        <v>206</v>
       </c>
       <c r="H72" s="1"/>
       <c r="I72" s="2"/>
@@ -7704,46 +7672,46 @@
     </row>
     <row r="73" spans="1:14" ht="71" thickBot="1">
       <c r="A73" s="3" t="s">
-        <v>54</v>
+        <v>92</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>168</v>
+        <v>91</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>182</v>
+        <v>13</v>
       </c>
       <c r="D73" s="5" t="s">
-        <v>183</v>
+        <v>14</v>
       </c>
       <c r="E73" s="3" t="s">
-        <v>184</v>
+        <v>15</v>
       </c>
       <c r="F73" s="3" t="s">
-        <v>185</v>
+        <v>16</v>
       </c>
       <c r="G73" s="6" t="s">
-        <v>186</v>
+        <v>17</v>
       </c>
       <c r="H73" s="3" t="s">
-        <v>187</v>
+        <v>18</v>
       </c>
       <c r="I73" s="7" t="s">
-        <v>188</v>
+        <v>19</v>
       </c>
       <c r="J73" s="7" t="s">
-        <v>189</v>
+        <v>20</v>
       </c>
       <c r="K73" s="8" t="s">
-        <v>111</v>
+        <v>149</v>
       </c>
       <c r="L73" s="8" t="s">
-        <v>17</v>
+        <v>174</v>
       </c>
       <c r="M73" s="8" t="s">
-        <v>18</v>
+        <v>175</v>
       </c>
       <c r="N73" s="8" t="s">
-        <v>19</v>
+        <v>176</v>
       </c>
     </row>
     <row r="74" spans="1:14">
@@ -7880,7 +7848,7 @@
       <c r="E79" s="2"/>
       <c r="F79" s="2"/>
       <c r="G79" s="1" t="s">
-        <v>50</v>
+        <v>207</v>
       </c>
       <c r="H79" s="1"/>
       <c r="I79" s="2"/>
@@ -7892,46 +7860,46 @@
     </row>
     <row r="80" spans="1:14" ht="71" thickBot="1">
       <c r="A80" s="3" t="s">
-        <v>54</v>
+        <v>92</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>168</v>
+        <v>91</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>182</v>
+        <v>13</v>
       </c>
       <c r="D80" s="5" t="s">
-        <v>183</v>
+        <v>14</v>
       </c>
       <c r="E80" s="3" t="s">
-        <v>184</v>
+        <v>15</v>
       </c>
       <c r="F80" s="3" t="s">
-        <v>185</v>
+        <v>16</v>
       </c>
       <c r="G80" s="6" t="s">
-        <v>186</v>
+        <v>17</v>
       </c>
       <c r="H80" s="3" t="s">
-        <v>187</v>
+        <v>18</v>
       </c>
       <c r="I80" s="7" t="s">
-        <v>188</v>
+        <v>19</v>
       </c>
       <c r="J80" s="7" t="s">
-        <v>189</v>
+        <v>20</v>
       </c>
       <c r="K80" s="8" t="s">
-        <v>111</v>
+        <v>149</v>
       </c>
       <c r="L80" s="8" t="s">
-        <v>17</v>
+        <v>174</v>
       </c>
       <c r="M80" s="8" t="s">
-        <v>18</v>
+        <v>175</v>
       </c>
       <c r="N80" s="8" t="s">
-        <v>19</v>
+        <v>176</v>
       </c>
     </row>
     <row r="81" spans="1:12">
@@ -8053,40 +8021,40 @@
     </row>
     <row r="87" spans="1:12" ht="71" thickBot="1">
       <c r="A87" s="3" t="s">
-        <v>51</v>
+        <v>208</v>
       </c>
       <c r="B87" s="6" t="s">
-        <v>186</v>
+        <v>17</v>
       </c>
       <c r="C87" s="7" t="s">
-        <v>52</v>
+        <v>209</v>
       </c>
       <c r="D87" s="7" t="s">
-        <v>52</v>
+        <v>209</v>
       </c>
       <c r="E87" s="7" t="s">
-        <v>52</v>
+        <v>209</v>
       </c>
       <c r="F87" s="8" t="s">
-        <v>110</v>
+        <v>148</v>
       </c>
       <c r="G87" s="8" t="s">
-        <v>157</v>
+        <v>80</v>
       </c>
       <c r="H87" s="7" t="s">
-        <v>126</v>
+        <v>49</v>
       </c>
       <c r="I87" s="7" t="s">
-        <v>126</v>
+        <v>49</v>
       </c>
       <c r="J87" s="7" t="s">
-        <v>126</v>
+        <v>49</v>
       </c>
       <c r="K87" s="8" t="s">
-        <v>125</v>
+        <v>48</v>
       </c>
       <c r="L87" s="8" t="s">
-        <v>55</v>
+        <v>93</v>
       </c>
     </row>
     <row r="88" spans="1:12">
@@ -8112,7 +8080,7 @@
       </c>
       <c r="G88">
         <f>STDEV(C88,D88,E88)/SQRT(3)</f>
-        <v>44.33939459442368</v>
+        <v>44.339394594427489</v>
       </c>
       <c r="H88">
         <v>128.80500000000001</v>
@@ -8129,7 +8097,7 @@
       </c>
       <c r="L88">
         <f>STDEV(H88,I88,J88)/SQRT(3)</f>
-        <v>7.5428862071048961</v>
+        <v>7.5428862071049236</v>
       </c>
     </row>
     <row r="89" spans="1:12">
@@ -8155,7 +8123,7 @@
       </c>
       <c r="G89">
         <f>STDEV(C89,D89,E89)/SQRT(3)</f>
-        <v>58.385792408008861</v>
+        <v>58.385792408006402</v>
       </c>
       <c r="H89">
         <v>140.238</v>
@@ -8172,7 +8140,7 @@
       </c>
       <c r="L89">
         <f>STDEV(H89,I89,J89)/SQRT(3)</f>
-        <v>4.1344438965032886</v>
+        <v>4.1344438965032166</v>
       </c>
     </row>
     <row r="90" spans="1:12">
@@ -8198,7 +8166,7 @@
       </c>
       <c r="G90">
         <f>STDEV(C90,D90,E90)/SQRT(3)</f>
-        <v>19.678437700522181</v>
+        <v>19.678437700520611</v>
       </c>
       <c r="H90">
         <v>136.01</v>
@@ -8215,32 +8183,32 @@
       </c>
       <c r="L90">
         <f>STDEV(H90,I90,J90)/SQRT(3)</f>
-        <v>2.6636263501725166</v>
+        <v>2.6636263501721773</v>
       </c>
     </row>
     <row r="94" spans="1:12">
       <c r="A94" t="s">
-        <v>56</v>
+        <v>94</v>
       </c>
     </row>
     <row r="96" spans="1:12" ht="33" thickBot="1">
       <c r="A96" s="3" t="s">
-        <v>57</v>
+        <v>95</v>
       </c>
       <c r="B96" s="5" t="s">
-        <v>186</v>
+        <v>17</v>
       </c>
       <c r="C96" s="6" t="s">
-        <v>58</v>
+        <v>96</v>
       </c>
       <c r="D96" s="3" t="s">
-        <v>130</v>
+        <v>53</v>
       </c>
       <c r="E96" s="3" t="s">
-        <v>131</v>
+        <v>54</v>
       </c>
       <c r="F96" s="5" t="s">
-        <v>132</v>
+        <v>55</v>
       </c>
       <c r="G96" s="11"/>
     </row>
@@ -8306,7 +8274,7 @@
     </row>
     <row r="100" spans="1:22">
       <c r="V100" t="s">
-        <v>133</v>
+        <v>56</v>
       </c>
     </row>
     <row r="101" spans="1:22">
@@ -8316,27 +8284,27 @@
     </row>
     <row r="105" spans="1:22">
       <c r="I105" t="s">
-        <v>60</v>
+        <v>98</v>
       </c>
     </row>
     <row r="106" spans="1:22">
       <c r="I106" t="s">
-        <v>134</v>
+        <v>57</v>
       </c>
     </row>
     <row r="107" spans="1:22">
       <c r="I107" t="s">
-        <v>135</v>
+        <v>58</v>
       </c>
     </row>
     <row r="108" spans="1:22">
       <c r="I108" t="s">
-        <v>129</v>
+        <v>52</v>
       </c>
     </row>
     <row r="109" spans="1:22">
       <c r="I109" t="s">
-        <v>175</v>
+        <v>6</v>
       </c>
     </row>
     <row r="120" spans="1:17" ht="15">
@@ -8347,7 +8315,7 @@
       <c r="E120" s="2"/>
       <c r="F120" s="2"/>
       <c r="G120" s="1" t="s">
-        <v>176</v>
+        <v>7</v>
       </c>
       <c r="H120" s="1"/>
       <c r="I120" s="2"/>
@@ -8359,46 +8327,46 @@
     </row>
     <row r="121" spans="1:17" ht="71" thickBot="1">
       <c r="A121" s="3" t="s">
-        <v>54</v>
+        <v>92</v>
       </c>
       <c r="B121" s="3" t="s">
-        <v>22</v>
+        <v>179</v>
       </c>
       <c r="C121" s="4" t="s">
-        <v>177</v>
+        <v>8</v>
       </c>
       <c r="D121" s="5" t="s">
-        <v>183</v>
+        <v>14</v>
       </c>
       <c r="E121" s="3" t="s">
-        <v>184</v>
+        <v>15</v>
       </c>
       <c r="F121" s="3" t="s">
-        <v>185</v>
+        <v>16</v>
       </c>
       <c r="G121" s="6" t="s">
-        <v>186</v>
+        <v>17</v>
       </c>
       <c r="H121" s="3" t="s">
-        <v>187</v>
+        <v>18</v>
       </c>
       <c r="I121" s="7" t="s">
-        <v>188</v>
+        <v>19</v>
       </c>
       <c r="J121" s="7" t="s">
-        <v>189</v>
+        <v>20</v>
       </c>
       <c r="K121" s="8" t="s">
-        <v>111</v>
+        <v>149</v>
       </c>
       <c r="L121" s="8" t="s">
-        <v>17</v>
+        <v>174</v>
       </c>
       <c r="M121" s="8" t="s">
-        <v>18</v>
+        <v>175</v>
       </c>
       <c r="N121" s="8" t="s">
-        <v>178</v>
+        <v>9</v>
       </c>
     </row>
     <row r="122" spans="1:17">
@@ -8455,7 +8423,7 @@
       </c>
       <c r="Q122">
         <f>STDEV(O122:O123)</f>
-        <v>1.0748023074035516E-2</v>
+        <v>1.0748023074035887E-2</v>
       </c>
     </row>
     <row r="123" spans="1:17">
@@ -8564,7 +8532,7 @@
       <c r="E129" s="2"/>
       <c r="F129" s="2"/>
       <c r="G129" s="1" t="s">
-        <v>179</v>
+        <v>10</v>
       </c>
       <c r="H129" s="1"/>
       <c r="I129" s="2"/>
@@ -8576,46 +8544,46 @@
     </row>
     <row r="130" spans="1:14" ht="71" thickBot="1">
       <c r="A130" s="3" t="s">
-        <v>54</v>
+        <v>92</v>
       </c>
       <c r="B130" s="3" t="s">
-        <v>168</v>
+        <v>91</v>
       </c>
       <c r="C130" s="4" t="s">
-        <v>182</v>
+        <v>13</v>
       </c>
       <c r="D130" s="5" t="s">
-        <v>183</v>
+        <v>14</v>
       </c>
       <c r="E130" s="3" t="s">
-        <v>184</v>
+        <v>15</v>
       </c>
       <c r="F130" s="3" t="s">
-        <v>185</v>
+        <v>16</v>
       </c>
       <c r="G130" s="6" t="s">
-        <v>186</v>
+        <v>17</v>
       </c>
       <c r="H130" s="3" t="s">
-        <v>187</v>
+        <v>18</v>
       </c>
       <c r="I130" s="7" t="s">
-        <v>188</v>
+        <v>19</v>
       </c>
       <c r="J130" s="7" t="s">
-        <v>189</v>
+        <v>20</v>
       </c>
       <c r="K130" s="8" t="s">
-        <v>111</v>
+        <v>149</v>
       </c>
       <c r="L130" s="8" t="s">
-        <v>17</v>
+        <v>174</v>
       </c>
       <c r="M130" s="8" t="s">
-        <v>18</v>
+        <v>175</v>
       </c>
       <c r="N130" s="8" t="s">
-        <v>19</v>
+        <v>176</v>
       </c>
     </row>
     <row r="131" spans="1:14">
@@ -8755,7 +8723,7 @@
       <c r="E139" s="2"/>
       <c r="F139" s="2"/>
       <c r="G139" s="1" t="s">
-        <v>119</v>
+        <v>42</v>
       </c>
       <c r="H139" s="1"/>
       <c r="I139" s="2"/>
@@ -8767,46 +8735,46 @@
     </row>
     <row r="140" spans="1:14" ht="71" thickBot="1">
       <c r="A140" s="3" t="s">
-        <v>54</v>
+        <v>92</v>
       </c>
       <c r="B140" s="3" t="s">
-        <v>168</v>
+        <v>91</v>
       </c>
       <c r="C140" s="4" t="s">
-        <v>182</v>
+        <v>13</v>
       </c>
       <c r="D140" s="5" t="s">
-        <v>183</v>
+        <v>14</v>
       </c>
       <c r="E140" s="3" t="s">
-        <v>184</v>
+        <v>15</v>
       </c>
       <c r="F140" s="3" t="s">
-        <v>185</v>
+        <v>16</v>
       </c>
       <c r="G140" s="6" t="s">
-        <v>186</v>
+        <v>17</v>
       </c>
       <c r="H140" s="3" t="s">
-        <v>187</v>
+        <v>18</v>
       </c>
       <c r="I140" s="7" t="s">
-        <v>188</v>
+        <v>19</v>
       </c>
       <c r="J140" s="7" t="s">
-        <v>189</v>
+        <v>20</v>
       </c>
       <c r="K140" s="8" t="s">
-        <v>111</v>
+        <v>149</v>
       </c>
       <c r="L140" s="8" t="s">
-        <v>17</v>
+        <v>174</v>
       </c>
       <c r="M140" s="8" t="s">
-        <v>18</v>
+        <v>175</v>
       </c>
       <c r="N140" s="8" t="s">
-        <v>178</v>
+        <v>9</v>
       </c>
     </row>
     <row r="141" spans="1:14">
@@ -8940,55 +8908,55 @@
     </row>
     <row r="147" spans="1:17" ht="43" thickBot="1">
       <c r="A147" s="4" t="s">
-        <v>182</v>
+        <v>13</v>
       </c>
       <c r="B147" s="6" t="s">
-        <v>186</v>
+        <v>17</v>
       </c>
       <c r="C147" s="3" t="s">
-        <v>187</v>
+        <v>18</v>
       </c>
       <c r="D147" s="3" t="s">
-        <v>187</v>
+        <v>18</v>
       </c>
       <c r="E147" s="3" t="s">
-        <v>187</v>
+        <v>18</v>
       </c>
       <c r="F147" s="3" t="s">
-        <v>120</v>
+        <v>43</v>
       </c>
       <c r="G147" s="3" t="s">
-        <v>152</v>
+        <v>75</v>
       </c>
       <c r="H147" s="7" t="s">
-        <v>188</v>
+        <v>19</v>
       </c>
       <c r="I147" s="7" t="s">
-        <v>188</v>
+        <v>19</v>
       </c>
       <c r="J147" s="7" t="s">
-        <v>188</v>
+        <v>19</v>
       </c>
       <c r="K147" s="8" t="s">
-        <v>153</v>
+        <v>76</v>
       </c>
       <c r="L147" s="8" t="s">
-        <v>154</v>
+        <v>77</v>
       </c>
       <c r="M147" s="7" t="s">
-        <v>189</v>
+        <v>20</v>
       </c>
       <c r="N147" s="7" t="s">
-        <v>189</v>
+        <v>20</v>
       </c>
       <c r="O147" s="7" t="s">
-        <v>189</v>
+        <v>20</v>
       </c>
       <c r="P147" s="8" t="s">
-        <v>155</v>
+        <v>78</v>
       </c>
       <c r="Q147" s="8" t="s">
-        <v>156</v>
+        <v>79</v>
       </c>
     </row>
     <row r="148" spans="1:17">
@@ -9007,7 +8975,7 @@
       </c>
       <c r="G148">
         <f>STDEV(C148,D148,E148)/SQRT(3)</f>
-        <v>1.7540000000000004</v>
+        <v>1.7540000000002831</v>
       </c>
       <c r="H148">
         <v>1209.1849999999999</v>
@@ -9024,7 +8992,7 @@
       </c>
       <c r="L148">
         <f>STDEV(H148,I148,J148)/SQRT(3)</f>
-        <v>19.678437700522181</v>
+        <v>19.678437700520611</v>
       </c>
       <c r="M148">
         <v>136.01</v>
@@ -9041,7 +9009,7 @@
       </c>
       <c r="Q148">
         <f>STDEV(M148,N148,O148)/SQRT(3)</f>
-        <v>2.6636263501725166</v>
+        <v>2.6636263501721773</v>
       </c>
     </row>
     <row r="149" spans="1:17">
@@ -9060,7 +9028,7 @@
       </c>
       <c r="G149">
         <f>STDEV(C149,D149,E149)/SQRT(3)</f>
-        <v>3.5763333333333285</v>
+        <v>3.5763333333362866</v>
       </c>
       <c r="H149">
         <v>2187.7220000000002</v>
@@ -9077,7 +9045,7 @@
       </c>
       <c r="L149">
         <f>STDEV(H149,I149,J149)/SQRT(3)</f>
-        <v>13.902016196700965</v>
+        <v>13.902016196695632</v>
       </c>
       <c r="M149">
         <v>323.47300000000001</v>
@@ -9094,7 +9062,7 @@
       </c>
       <c r="Q149">
         <f>STDEV(M149,N149,O149)/SQRT(3)</f>
-        <v>10.8737975938083</v>
+        <v>10.873797593807824</v>
       </c>
     </row>
     <row r="150" spans="1:17">
@@ -9113,7 +9081,7 @@
       </c>
       <c r="G150">
         <f>STDEV(C150,D150,E150)/SQRT(3)</f>
-        <v>24.970666666666681</v>
+        <v>24.97066666666846</v>
       </c>
       <c r="H150">
         <v>4227.183</v>
@@ -9130,7 +9098,7 @@
       </c>
       <c r="L150">
         <f>STDEV(H150,I150,J150)/SQRT(3)</f>
-        <v>67.344362268369153</v>
+        <v>67.344362268343815</v>
       </c>
       <c r="M150">
         <v>673.399</v>
@@ -9147,41 +9115,41 @@
       </c>
       <c r="Q150">
         <f>STDEV(M150,N150,O150)/SQRT(3)</f>
-        <v>5.7530535177223614</v>
+        <v>5.7530535177223436</v>
       </c>
     </row>
     <row r="153" spans="1:17">
       <c r="C153" t="s">
-        <v>141</v>
+        <v>64</v>
       </c>
     </row>
     <row r="155" spans="1:17" ht="49" thickBot="1">
       <c r="C155" s="3" t="s">
-        <v>142</v>
+        <v>65</v>
       </c>
       <c r="D155" s="5" t="s">
-        <v>183</v>
+        <v>14</v>
       </c>
       <c r="E155" s="6" t="s">
-        <v>143</v>
+        <v>66</v>
       </c>
       <c r="F155" s="3" t="s">
-        <v>187</v>
+        <v>18</v>
       </c>
       <c r="G155" s="3" t="s">
-        <v>144</v>
+        <v>67</v>
       </c>
       <c r="H155" s="8" t="s">
-        <v>116</v>
+        <v>154</v>
       </c>
       <c r="I155" s="8" t="s">
-        <v>117</v>
+        <v>155</v>
       </c>
       <c r="J155" s="8" t="s">
-        <v>207</v>
+        <v>38</v>
       </c>
       <c r="K155" s="8" t="s">
-        <v>208</v>
+        <v>39</v>
       </c>
     </row>
     <row r="156" spans="1:17">
@@ -9298,33 +9266,33 @@
   <sheetData>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>106</v>
+        <v>144</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="46" thickBot="1">
       <c r="A4" s="3" t="s">
-        <v>168</v>
+        <v>91</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>183</v>
+        <v>14</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>186</v>
+        <v>17</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>187</v>
+        <v>18</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>107</v>
+        <v>145</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>170</v>
+        <v>1</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>171</v>
+        <v>2</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>172</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -9437,15 +9405,15 @@
     </row>
     <row r="31" spans="2:8">
       <c r="G31" t="s">
-        <v>173</v>
+        <v>4</v>
       </c>
       <c r="H31" t="s">
-        <v>108</v>
+        <v>146</v>
       </c>
     </row>
     <row r="32" spans="2:8">
       <c r="B32" t="s">
-        <v>60</v>
+        <v>98</v>
       </c>
       <c r="G32">
         <v>1.59</v>
@@ -9456,7 +9424,7 @@
     </row>
     <row r="33" spans="1:8" ht="15">
       <c r="B33" t="s">
-        <v>61</v>
+        <v>99</v>
       </c>
       <c r="G33" s="10">
         <v>9155.6200000000008</v>
@@ -9467,42 +9435,42 @@
     </row>
     <row r="34" spans="1:8">
       <c r="B34" t="s">
-        <v>109</v>
+        <v>147</v>
       </c>
     </row>
     <row r="35" spans="1:8">
       <c r="B35" t="s">
-        <v>129</v>
+        <v>52</v>
       </c>
     </row>
     <row r="36" spans="1:8">
       <c r="B36" t="s">
-        <v>175</v>
+        <v>6</v>
       </c>
     </row>
     <row r="48" spans="1:8">
       <c r="A48" t="s">
-        <v>56</v>
+        <v>94</v>
       </c>
     </row>
     <row r="50" spans="1:9" ht="33" thickBot="1">
       <c r="A50" s="3" t="s">
-        <v>57</v>
+        <v>95</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>186</v>
+        <v>17</v>
       </c>
       <c r="C50" s="6" t="s">
-        <v>58</v>
+        <v>96</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>130</v>
+        <v>53</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>131</v>
+        <v>54</v>
       </c>
       <c r="F50" s="5" t="s">
-        <v>132</v>
+        <v>55</v>
       </c>
       <c r="G50" s="11"/>
     </row>
@@ -9546,7 +9514,7 @@
         <v>4.1344438965032166</v>
       </c>
       <c r="I52" s="14" t="s">
-        <v>159</v>
+        <v>82</v>
       </c>
     </row>
     <row r="53" spans="1:9">
@@ -9571,15 +9539,15 @@
     </row>
     <row r="64" spans="1:9">
       <c r="B64" t="s">
-        <v>60</v>
+        <v>98</v>
       </c>
       <c r="G64" t="s">
-        <v>133</v>
+        <v>56</v>
       </c>
     </row>
     <row r="65" spans="1:9" ht="15">
       <c r="B65" t="s">
-        <v>61</v>
+        <v>99</v>
       </c>
       <c r="G65">
         <v>9144.5290000000005</v>
@@ -9588,17 +9556,17 @@
     </row>
     <row r="66" spans="1:9">
       <c r="B66" t="s">
-        <v>109</v>
+        <v>147</v>
       </c>
     </row>
     <row r="67" spans="1:9">
       <c r="B67" t="s">
-        <v>129</v>
+        <v>52</v>
       </c>
     </row>
     <row r="68" spans="1:9">
       <c r="B68" t="s">
-        <v>175</v>
+        <v>6</v>
       </c>
     </row>
     <row r="71" spans="1:9">
@@ -9618,36 +9586,36 @@
     </row>
     <row r="78" spans="1:9">
       <c r="A78" t="s">
-        <v>141</v>
+        <v>64</v>
       </c>
     </row>
     <row r="80" spans="1:9" ht="49" thickBot="1">
       <c r="A80" s="3" t="s">
-        <v>142</v>
+        <v>65</v>
       </c>
       <c r="B80" s="5" t="s">
-        <v>183</v>
+        <v>14</v>
       </c>
       <c r="C80" s="6" t="s">
-        <v>143</v>
+        <v>66</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>187</v>
+        <v>18</v>
       </c>
       <c r="E80" s="3" t="s">
-        <v>144</v>
+        <v>67</v>
       </c>
       <c r="F80" s="8" t="s">
-        <v>116</v>
+        <v>154</v>
       </c>
       <c r="G80" s="8" t="s">
-        <v>117</v>
+        <v>155</v>
       </c>
       <c r="H80" s="8" t="s">
-        <v>207</v>
+        <v>38</v>
       </c>
       <c r="I80" s="8" t="s">
-        <v>208</v>
+        <v>39</v>
       </c>
     </row>
     <row r="81" spans="1:9">
@@ -9742,11 +9710,10 @@
     </row>
     <row r="85" spans="1:9" ht="23">
       <c r="C85" s="14" t="s">
-        <v>158</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>
@@ -9760,72 +9727,72 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A2:Z149"/>
+  <dimension ref="A2:Z162"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A110" workbookViewId="0">
-      <selection activeCell="O131" sqref="O131"/>
+    <sheetView tabSelected="1" topLeftCell="A124" workbookViewId="0">
+      <selection activeCell="B158" sqref="B158"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <sheetData>
     <row r="2" spans="1:24">
       <c r="A2" s="15" t="s">
-        <v>30</v>
+        <v>187</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>33</v>
+        <v>190</v>
       </c>
       <c r="C2" s="15"/>
       <c r="I2" s="15"/>
       <c r="K2" s="15" t="s">
-        <v>31</v>
+        <v>188</v>
       </c>
     </row>
     <row r="4" spans="1:24">
       <c r="A4" t="s">
-        <v>115</v>
+        <v>153</v>
       </c>
       <c r="B4" t="s">
-        <v>192</v>
+        <v>23</v>
       </c>
       <c r="C4" t="s">
-        <v>103</v>
+        <v>141</v>
       </c>
       <c r="D4" t="s">
-        <v>104</v>
+        <v>142</v>
       </c>
       <c r="E4" t="s">
-        <v>99</v>
+        <v>137</v>
       </c>
       <c r="F4" t="s">
-        <v>193</v>
+        <v>24</v>
       </c>
       <c r="G4" t="s">
-        <v>194</v>
+        <v>25</v>
       </c>
       <c r="H4" t="s">
-        <v>190</v>
+        <v>21</v>
       </c>
       <c r="I4" t="s">
-        <v>195</v>
+        <v>26</v>
       </c>
       <c r="J4" t="s">
-        <v>98</v>
+        <v>136</v>
       </c>
       <c r="K4" t="s">
-        <v>190</v>
+        <v>21</v>
       </c>
       <c r="L4" t="s">
-        <v>196</v>
+        <v>27</v>
       </c>
       <c r="M4" t="s">
-        <v>203</v>
+        <v>34</v>
       </c>
       <c r="N4" t="s">
-        <v>204</v>
+        <v>35</v>
       </c>
       <c r="O4" t="s">
-        <v>118</v>
+        <v>156</v>
       </c>
     </row>
     <row r="5" spans="1:24">
@@ -9874,7 +9841,7 @@
       </c>
       <c r="N5">
         <f>1.96 * STDEV(E5,H5,K5)/SQRT(3)</f>
-        <v>18.293333333333337</v>
+        <v>18.293333333355065</v>
       </c>
       <c r="O5">
         <f>L5/13</f>
@@ -9927,7 +9894,7 @@
       </c>
       <c r="N6">
         <f t="shared" ref="N6:N7" si="1">1.96 * STDEV(E6,H6,K6)/SQRT(3)</f>
-        <v>114.09789091438593</v>
+        <v>114.09789091439987</v>
       </c>
     </row>
     <row r="7" spans="1:24">
@@ -9976,7 +9943,7 @@
       </c>
       <c r="N7">
         <f t="shared" si="1"/>
-        <v>118.91205116013731</v>
+        <v>118.91205116011055</v>
       </c>
     </row>
     <row r="9" spans="1:24">
@@ -9987,48 +9954,48 @@
     </row>
     <row r="10" spans="1:24">
       <c r="A10" s="15" t="s">
-        <v>28</v>
+        <v>185</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>29</v>
+        <v>186</v>
       </c>
     </row>
     <row r="11" spans="1:24" ht="26">
       <c r="A11" s="11" t="s">
-        <v>115</v>
+        <v>153</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>15</v>
+        <v>172</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>192</v>
+        <v>23</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>11</v>
+        <v>168</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>12</v>
+        <v>169</v>
       </c>
       <c r="F11" s="11" t="s">
-        <v>13</v>
+        <v>170</v>
       </c>
       <c r="G11" s="11" t="s">
-        <v>14</v>
+        <v>171</v>
       </c>
       <c r="H11" s="11" t="s">
-        <v>43</v>
+        <v>200</v>
       </c>
       <c r="I11" s="11" t="s">
-        <v>16</v>
+        <v>173</v>
       </c>
       <c r="J11" s="11" t="s">
-        <v>44</v>
+        <v>201</v>
       </c>
       <c r="M11" t="s">
-        <v>123</v>
+        <v>46</v>
       </c>
       <c r="R11" t="s">
-        <v>139</v>
+        <v>62</v>
       </c>
     </row>
     <row r="12" spans="1:24" ht="26">
@@ -10067,38 +10034,38 @@
         <v>9</v>
       </c>
       <c r="M12" s="11" t="s">
-        <v>115</v>
+        <v>153</v>
       </c>
       <c r="N12" s="11" t="s">
-        <v>15</v>
+        <v>172</v>
       </c>
       <c r="O12" s="11" t="s">
-        <v>192</v>
+        <v>23</v>
       </c>
       <c r="P12" s="11" t="s">
-        <v>124</v>
+        <v>47</v>
       </c>
       <c r="Q12" s="11"/>
       <c r="R12" s="11" t="s">
-        <v>115</v>
+        <v>153</v>
       </c>
       <c r="S12" s="11" t="s">
-        <v>105</v>
+        <v>143</v>
       </c>
       <c r="T12" s="11" t="s">
-        <v>59</v>
+        <v>97</v>
       </c>
       <c r="U12" s="11" t="s">
-        <v>6</v>
+        <v>163</v>
       </c>
       <c r="V12" s="11" t="s">
-        <v>7</v>
+        <v>164</v>
       </c>
       <c r="W12" s="11" t="s">
-        <v>8</v>
+        <v>165</v>
       </c>
       <c r="X12" s="11" t="s">
-        <v>9</v>
+        <v>166</v>
       </c>
     </row>
     <row r="13" spans="1:24">
@@ -10253,10 +10220,10 @@
     </row>
     <row r="17" spans="1:24">
       <c r="A17" t="s">
-        <v>41</v>
+        <v>198</v>
       </c>
       <c r="B17" t="s">
-        <v>190</v>
+        <v>21</v>
       </c>
       <c r="M17">
         <v>4</v>
@@ -10295,7 +10262,7 @@
     </row>
     <row r="18" spans="1:24">
       <c r="A18" t="s">
-        <v>42</v>
+        <v>199</v>
       </c>
       <c r="B18">
         <v>563</v>
@@ -10323,7 +10290,7 @@
     </row>
     <row r="19" spans="1:24">
       <c r="A19" t="s">
-        <v>197</v>
+        <v>28</v>
       </c>
       <c r="B19">
         <f>19*60</f>
@@ -10352,7 +10319,7 @@
     </row>
     <row r="20" spans="1:24">
       <c r="A20" t="s">
-        <v>198</v>
+        <v>29</v>
       </c>
       <c r="B20">
         <v>2611</v>
@@ -10437,63 +10404,63 @@
     </row>
     <row r="24" spans="1:24">
       <c r="H24" s="15" t="s">
-        <v>26</v>
+        <v>183</v>
       </c>
       <c r="I24" s="15" t="s">
-        <v>27</v>
+        <v>184</v>
       </c>
     </row>
     <row r="26" spans="1:24">
       <c r="A26" t="s">
-        <v>115</v>
+        <v>153</v>
       </c>
       <c r="B26" t="s">
-        <v>200</v>
+        <v>31</v>
       </c>
       <c r="C26" t="s">
-        <v>199</v>
+        <v>30</v>
       </c>
       <c r="D26" t="s">
-        <v>104</v>
+        <v>142</v>
       </c>
       <c r="E26" t="s">
-        <v>190</v>
+        <v>21</v>
       </c>
       <c r="F26" t="s">
-        <v>200</v>
+        <v>31</v>
       </c>
       <c r="G26" t="s">
-        <v>199</v>
+        <v>30</v>
       </c>
       <c r="H26" t="s">
-        <v>104</v>
+        <v>142</v>
       </c>
       <c r="I26" t="s">
-        <v>190</v>
+        <v>21</v>
       </c>
       <c r="J26" t="s">
-        <v>201</v>
+        <v>32</v>
       </c>
       <c r="K26" t="s">
-        <v>199</v>
+        <v>30</v>
       </c>
       <c r="L26" t="s">
-        <v>104</v>
+        <v>142</v>
       </c>
       <c r="M26" t="s">
-        <v>190</v>
+        <v>21</v>
       </c>
       <c r="N26" t="s">
-        <v>202</v>
+        <v>33</v>
       </c>
       <c r="P26" t="s">
-        <v>205</v>
+        <v>36</v>
       </c>
       <c r="Q26" t="s">
-        <v>206</v>
+        <v>37</v>
       </c>
       <c r="R26" t="s">
-        <v>69</v>
+        <v>107</v>
       </c>
     </row>
     <row r="27" spans="1:24">
@@ -10546,7 +10513,7 @@
       </c>
       <c r="Q27">
         <f>1.96 * STDEV(E27,I27,M27)/SQRT(3)</f>
-        <v>4.0971690793194897</v>
+        <v>4.097169079209209</v>
       </c>
       <c r="R27">
         <f>P27+I34</f>
@@ -10602,7 +10569,7 @@
       </c>
       <c r="Q28">
         <f t="shared" ref="Q28:Q29" si="7">1.96 * STDEV(E28,I28,M28)/SQRT(3)</f>
-        <v>30.100037057362055</v>
+        <v>30.100037057320566</v>
       </c>
       <c r="R28">
         <f>P28+J34</f>
@@ -10658,7 +10625,7 @@
       </c>
       <c r="Q29">
         <f t="shared" si="7"/>
-        <v>10.540389097696695</v>
+        <v>10.540389098093113</v>
       </c>
       <c r="R29">
         <f>P29+K34</f>
@@ -10667,26 +10634,26 @@
     </row>
     <row r="32" spans="1:24">
       <c r="I32" t="s">
-        <v>68</v>
+        <v>106</v>
       </c>
     </row>
     <row r="33" spans="3:17">
       <c r="I33" t="s">
-        <v>65</v>
+        <v>103</v>
       </c>
       <c r="J33" t="s">
-        <v>66</v>
+        <v>104</v>
       </c>
       <c r="K33" t="s">
-        <v>67</v>
+        <v>105</v>
       </c>
     </row>
     <row r="34" spans="3:17">
       <c r="D34" t="s">
-        <v>10</v>
+        <v>167</v>
       </c>
       <c r="E34" t="s">
-        <v>9</v>
+        <v>166</v>
       </c>
       <c r="I34">
         <v>89.043478260869563</v>
@@ -10755,7 +10722,7 @@
     </row>
     <row r="44" spans="3:17">
       <c r="C44" t="s">
-        <v>62</v>
+        <v>100</v>
       </c>
       <c r="Q44">
         <v>4</v>
@@ -10763,7 +10730,7 @@
     </row>
     <row r="45" spans="3:17">
       <c r="C45" t="s">
-        <v>180</v>
+        <v>11</v>
       </c>
       <c r="Q45">
         <v>8</v>
@@ -10771,54 +10738,54 @@
     </row>
     <row r="46" spans="3:17">
       <c r="C46" t="s">
-        <v>181</v>
+        <v>12</v>
       </c>
     </row>
     <row r="47" spans="3:17">
       <c r="C47" t="s">
-        <v>191</v>
+        <v>22</v>
       </c>
     </row>
     <row r="53" spans="1:11">
       <c r="D53" t="s">
-        <v>136</v>
+        <v>59</v>
       </c>
     </row>
     <row r="56" spans="1:11">
       <c r="A56" t="s">
-        <v>95</v>
+        <v>133</v>
       </c>
       <c r="B56" t="s">
-        <v>96</v>
+        <v>134</v>
       </c>
       <c r="C56" t="s">
-        <v>127</v>
+        <v>50</v>
       </c>
       <c r="D56" t="s">
-        <v>97</v>
+        <v>135</v>
       </c>
       <c r="E56" t="s">
-        <v>128</v>
+        <v>51</v>
       </c>
       <c r="F56" t="s">
-        <v>98</v>
+        <v>136</v>
       </c>
       <c r="G56" t="s">
-        <v>99</v>
+        <v>137</v>
       </c>
       <c r="H56" t="s">
-        <v>63</v>
+        <v>101</v>
       </c>
       <c r="I56" t="s">
-        <v>64</v>
+        <v>102</v>
       </c>
       <c r="K56" t="s">
-        <v>73</v>
+        <v>111</v>
       </c>
     </row>
     <row r="57" spans="1:11">
       <c r="A57" t="s">
-        <v>100</v>
+        <v>138</v>
       </c>
       <c r="B57">
         <v>1171052</v>
@@ -10846,10 +10813,10 @@
       </c>
       <c r="I57">
         <f>1.96*(STDEV(G57:G59)/SQRT(3))</f>
-        <v>12.103286987150657</v>
+        <v>12.103286987068245</v>
       </c>
       <c r="K57" t="s">
-        <v>70</v>
+        <v>108</v>
       </c>
     </row>
     <row r="58" spans="1:11">
@@ -10910,7 +10877,7 @@
     </row>
     <row r="61" spans="1:11">
       <c r="A61" t="s">
-        <v>101</v>
+        <v>139</v>
       </c>
       <c r="B61">
         <v>1171052</v>
@@ -10938,10 +10905,10 @@
       </c>
       <c r="I61">
         <f>1.96*(STDEV(G61:G63)/SQRT(3))</f>
-        <v>19.032393616362871</v>
+        <v>19.032393616609415</v>
       </c>
       <c r="K61" t="s">
-        <v>72</v>
+        <v>110</v>
       </c>
     </row>
     <row r="62" spans="1:11">
@@ -10990,7 +10957,7 @@
     </row>
     <row r="66" spans="1:26">
       <c r="A66" t="s">
-        <v>102</v>
+        <v>140</v>
       </c>
       <c r="B66">
         <v>1171052</v>
@@ -11019,10 +10986,10 @@
       </c>
       <c r="I66">
         <f>1.96*(STDEV(G66:G68)/SQRT(3))</f>
-        <v>24.16702109730387</v>
+        <v>24.167021097560671</v>
       </c>
       <c r="K66" t="s">
-        <v>71</v>
+        <v>109</v>
       </c>
     </row>
     <row r="67" spans="1:26">
@@ -11070,10 +11037,10 @@
     </row>
     <row r="70" spans="1:26">
       <c r="E70" t="s">
-        <v>10</v>
+        <v>167</v>
       </c>
       <c r="F70" t="s">
-        <v>9</v>
+        <v>166</v>
       </c>
     </row>
     <row r="71" spans="1:26">
@@ -11089,46 +11056,46 @@
         <v>13.340925888849769</v>
       </c>
       <c r="K71" t="s">
-        <v>75</v>
+        <v>113</v>
       </c>
       <c r="L71" t="s">
-        <v>82</v>
+        <v>120</v>
       </c>
       <c r="M71" t="s">
-        <v>81</v>
+        <v>119</v>
       </c>
       <c r="N71" t="s">
-        <v>94</v>
+        <v>132</v>
       </c>
       <c r="O71" t="s">
-        <v>79</v>
+        <v>117</v>
       </c>
       <c r="P71" t="s">
+        <v>121</v>
+      </c>
+      <c r="Q71" t="s">
+        <v>122</v>
+      </c>
+      <c r="R71" t="s">
+        <v>123</v>
+      </c>
+      <c r="S71" t="s">
+        <v>124</v>
+      </c>
+      <c r="V71" t="s">
         <v>83</v>
       </c>
-      <c r="Q71" t="s">
+      <c r="W71" t="s">
         <v>84</v>
       </c>
-      <c r="R71" t="s">
+      <c r="X71" t="s">
         <v>85</v>
       </c>
-      <c r="S71" t="s">
+      <c r="Y71" t="s">
         <v>86</v>
       </c>
-      <c r="V71" t="s">
-        <v>160</v>
-      </c>
-      <c r="W71" t="s">
-        <v>161</v>
-      </c>
-      <c r="X71" t="s">
-        <v>162</v>
-      </c>
-      <c r="Y71" t="s">
-        <v>163</v>
-      </c>
       <c r="Z71" t="s">
-        <v>164</v>
+        <v>87</v>
       </c>
     </row>
     <row r="72" spans="1:26">
@@ -11144,10 +11111,10 @@
         <v>8.4817664826547219</v>
       </c>
       <c r="J72" t="s">
-        <v>74</v>
+        <v>112</v>
       </c>
       <c r="K72" t="s">
-        <v>76</v>
+        <v>114</v>
       </c>
       <c r="L72">
         <v>356.17391304347825</v>
@@ -11171,7 +11138,7 @@
         <v>9304.8405797101441</v>
       </c>
       <c r="U72" t="s">
-        <v>76</v>
+        <v>114</v>
       </c>
       <c r="V72">
         <f>L72+N72</f>
@@ -11204,7 +11171,7 @@
         <v>979.58801708376609</v>
       </c>
       <c r="K73" t="s">
-        <v>77</v>
+        <v>115</v>
       </c>
       <c r="L73">
         <v>356.17391304347825</v>
@@ -11229,7 +11196,7 @@
         <v>5547.3892463768107</v>
       </c>
       <c r="U73" t="s">
-        <v>77</v>
+        <v>115</v>
       </c>
       <c r="V73">
         <f>L73+M73</f>
@@ -11251,7 +11218,7 @@
     </row>
     <row r="74" spans="1:26">
       <c r="K74" t="s">
-        <v>78</v>
+        <v>116</v>
       </c>
       <c r="L74">
         <v>0</v>
@@ -11277,7 +11244,7 @@
         <v>6856.1113333333333</v>
       </c>
       <c r="U74" t="s">
-        <v>78</v>
+        <v>116</v>
       </c>
       <c r="V74">
         <f>M74</f>
@@ -11299,56 +11266,56 @@
     </row>
     <row r="76" spans="1:26">
       <c r="D76" t="s">
-        <v>137</v>
+        <v>60</v>
       </c>
     </row>
     <row r="78" spans="1:26">
       <c r="P78" t="s">
-        <v>93</v>
+        <v>131</v>
       </c>
       <c r="Q78" t="s">
-        <v>87</v>
+        <v>125</v>
       </c>
       <c r="R78" t="s">
-        <v>88</v>
+        <v>126</v>
       </c>
       <c r="S78" t="s">
-        <v>89</v>
+        <v>127</v>
       </c>
       <c r="T78" t="s">
-        <v>91</v>
+        <v>129</v>
       </c>
       <c r="U78" t="s">
-        <v>90</v>
+        <v>128</v>
       </c>
       <c r="V78" t="s">
-        <v>80</v>
+        <v>118</v>
       </c>
       <c r="W78" t="s">
-        <v>92</v>
+        <v>130</v>
       </c>
     </row>
     <row r="79" spans="1:26">
       <c r="A79" t="s">
-        <v>95</v>
+        <v>133</v>
       </c>
       <c r="B79" t="s">
-        <v>96</v>
+        <v>134</v>
       </c>
       <c r="C79" t="s">
-        <v>127</v>
+        <v>50</v>
       </c>
       <c r="D79" t="s">
-        <v>97</v>
+        <v>135</v>
       </c>
       <c r="E79" t="s">
-        <v>128</v>
+        <v>51</v>
       </c>
       <c r="F79" t="s">
-        <v>98</v>
+        <v>136</v>
       </c>
       <c r="G79" t="s">
-        <v>190</v>
+        <v>21</v>
       </c>
       <c r="P79">
         <v>7.44168872620806</v>
@@ -11371,7 +11338,7 @@
     </row>
     <row r="80" spans="1:26">
       <c r="A80" t="s">
-        <v>100</v>
+        <v>138</v>
       </c>
       <c r="B80">
         <v>1171052</v>
@@ -11394,7 +11361,7 @@
         <v>1279.5150000000001</v>
       </c>
       <c r="H80" t="s">
-        <v>138</v>
+        <v>61</v>
       </c>
       <c r="P80">
         <v>7.4416887262080644</v>
@@ -11479,7 +11446,7 @@
     </row>
     <row r="84" spans="1:23">
       <c r="A84" t="s">
-        <v>101</v>
+        <v>139</v>
       </c>
       <c r="B84">
         <v>1171052</v>
@@ -11487,7 +11454,7 @@
     </row>
     <row r="85" spans="1:23">
       <c r="A85" t="s">
-        <v>102</v>
+        <v>140</v>
       </c>
       <c r="B85">
         <v>1171052</v>
@@ -11495,15 +11462,15 @@
     </row>
     <row r="88" spans="1:23">
       <c r="A88" t="s">
-        <v>41</v>
+        <v>198</v>
       </c>
       <c r="B88" t="s">
-        <v>190</v>
+        <v>21</v>
       </c>
     </row>
     <row r="89" spans="1:23">
       <c r="A89" t="s">
-        <v>42</v>
+        <v>199</v>
       </c>
       <c r="B89">
         <v>563</v>
@@ -11511,7 +11478,7 @@
     </row>
     <row r="90" spans="1:23">
       <c r="A90" t="s">
-        <v>197</v>
+        <v>28</v>
       </c>
       <c r="B90">
         <f>19*60</f>
@@ -11520,7 +11487,7 @@
     </row>
     <row r="91" spans="1:23" s="12" customFormat="1">
       <c r="A91" t="s">
-        <v>198</v>
+        <v>29</v>
       </c>
       <c r="B91">
         <v>2611</v>
@@ -11534,19 +11501,19 @@
     <row r="102" spans="7:25" s="11" customFormat="1"/>
     <row r="109" spans="7:25">
       <c r="U109" t="s">
-        <v>165</v>
+        <v>88</v>
       </c>
       <c r="V109" t="s">
-        <v>166</v>
+        <v>89</v>
       </c>
       <c r="W109" t="s">
-        <v>167</v>
+        <v>90</v>
       </c>
       <c r="X109" t="s">
-        <v>80</v>
+        <v>118</v>
       </c>
       <c r="Y109" t="s">
-        <v>92</v>
+        <v>130</v>
       </c>
     </row>
     <row r="110" spans="7:25">
@@ -11609,54 +11576,54 @@
     </row>
     <row r="114" spans="1:17">
       <c r="A114" t="s">
-        <v>25</v>
+        <v>182</v>
       </c>
       <c r="B114" t="s">
-        <v>32</v>
+        <v>189</v>
       </c>
       <c r="K114" t="s">
-        <v>34</v>
+        <v>191</v>
       </c>
       <c r="L114" t="s">
-        <v>35</v>
+        <v>192</v>
       </c>
     </row>
     <row r="115" spans="1:17">
       <c r="B115" t="s">
-        <v>96</v>
+        <v>134</v>
       </c>
       <c r="C115" t="s">
-        <v>127</v>
+        <v>50</v>
       </c>
       <c r="D115" t="s">
-        <v>195</v>
+        <v>26</v>
       </c>
       <c r="E115" t="s">
-        <v>99</v>
+        <v>137</v>
       </c>
       <c r="F115" t="s">
-        <v>63</v>
+        <v>101</v>
       </c>
       <c r="G115" t="s">
-        <v>64</v>
+        <v>102</v>
       </c>
       <c r="L115" t="s">
-        <v>96</v>
+        <v>134</v>
       </c>
       <c r="M115" t="s">
-        <v>127</v>
+        <v>50</v>
       </c>
       <c r="N115" t="s">
-        <v>195</v>
+        <v>26</v>
       </c>
       <c r="O115" t="s">
-        <v>99</v>
+        <v>137</v>
       </c>
       <c r="P115" t="s">
-        <v>63</v>
+        <v>101</v>
       </c>
       <c r="Q115" t="s">
-        <v>64</v>
+        <v>102</v>
       </c>
     </row>
     <row r="116" spans="1:17">
@@ -11684,7 +11651,7 @@
         <v>13.935673511291871</v>
       </c>
       <c r="K116" t="s">
-        <v>36</v>
+        <v>193</v>
       </c>
       <c r="L116">
         <v>1171052</v>
@@ -11790,7 +11757,7 @@
         <v>7.8781625077026014</v>
       </c>
       <c r="K121" t="s">
-        <v>37</v>
+        <v>194</v>
       </c>
       <c r="L121">
         <v>1171052</v>
@@ -11896,7 +11863,7 @@
         <v>4.6431871871022583</v>
       </c>
       <c r="K126" t="s">
-        <v>38</v>
+        <v>195</v>
       </c>
       <c r="L126">
         <v>1171052</v>
@@ -11979,27 +11946,27 @@
     </row>
     <row r="137" spans="5:11">
       <c r="I137" t="s">
-        <v>39</v>
+        <v>196</v>
       </c>
     </row>
     <row r="141" spans="5:11" s="11" customFormat="1" ht="26">
       <c r="F141" s="11" t="s">
-        <v>0</v>
+        <v>157</v>
       </c>
       <c r="G141" s="11" t="s">
-        <v>1</v>
+        <v>158</v>
       </c>
       <c r="H141" s="11" t="s">
-        <v>2</v>
+        <v>159</v>
       </c>
       <c r="I141" s="11" t="s">
-        <v>3</v>
+        <v>160</v>
       </c>
       <c r="J141" s="11" t="s">
-        <v>4</v>
+        <v>161</v>
       </c>
       <c r="K141" s="11" t="s">
-        <v>5</v>
+        <v>162</v>
       </c>
     </row>
     <row r="142" spans="5:11">
@@ -12062,24 +12029,24 @@
         <v>1684.1916666666666</v>
       </c>
     </row>
-    <row r="146" spans="6:10">
+    <row r="146" spans="1:10">
       <c r="F146" t="s">
-        <v>9</v>
+        <v>166</v>
       </c>
       <c r="G146" t="s">
-        <v>9</v>
+        <v>166</v>
       </c>
       <c r="H146" t="s">
-        <v>9</v>
+        <v>166</v>
       </c>
       <c r="I146" t="s">
-        <v>9</v>
+        <v>166</v>
       </c>
       <c r="J146" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="147" spans="6:10">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="147" spans="1:10">
       <c r="F147">
         <v>90.643966766199668</v>
       </c>
@@ -12096,7 +12063,7 @@
         <v>1.6668740844330987</v>
       </c>
     </row>
-    <row r="148" spans="6:10">
+    <row r="148" spans="1:10">
       <c r="F148">
         <v>99.177635471794702</v>
       </c>
@@ -12113,7 +12080,7 @@
         <v>7.3775567566892803</v>
       </c>
     </row>
-    <row r="149" spans="6:10">
+    <row r="149" spans="1:10">
       <c r="F149">
         <v>48.174196873825352</v>
       </c>
@@ -12130,10 +12097,49 @@
         <v>5.9110665054272307</v>
       </c>
     </row>
+    <row r="153" spans="1:10">
+      <c r="A153" t="s">
+        <v>40</v>
+      </c>
+      <c r="B153" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="154" spans="1:10">
+      <c r="A154">
+        <v>2</v>
+      </c>
+      <c r="B154">
+        <f>10*60+46</f>
+        <v>646</v>
+      </c>
+    </row>
+    <row r="155" spans="1:10">
+      <c r="B155">
+        <f>9*60+33</f>
+        <v>573</v>
+      </c>
+    </row>
+    <row r="156" spans="1:10">
+      <c r="B156">
+        <f>9*60+35</f>
+        <v>575</v>
+      </c>
+    </row>
+    <row r="158" spans="1:10">
+      <c r="A158">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1">
+      <c r="A162">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">

</xml_diff>

<commit_message>
Crossbow data update -  2GB,4GB,8GB
git-svn-id: file://localhost/tmp/svn2git/svn@6676 defb5e50-622e-49ec-a68e-d72c7db87b45
</commit_message>
<xml_diff>
--- a/papers/saga-mr-ngs/data/GS_data.xlsx
+++ b/papers/saga-mr-ngs/data/GS_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="-20" windowWidth="24600" windowHeight="14220" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="6680" yWindow="2980" windowWidth="29580" windowHeight="18620" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="GS data" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
   <externalReferences>
     <externalReference r:id="rId4"/>
   </externalReferences>
-  <calcPr calcId="130407" concurrentCalc="0"/>
+  <calcPr calcId="130000" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:ArchID Flags="2"/>
@@ -24,12 +24,645 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="217">
+  <si>
+    <t>Varying Number of chunk size - III</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>number of reads</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Number of chunks created</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Time taken to chunk files in seconds</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bowtie</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Local PMR</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>(BWA)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>seqal</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>phase times</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>seqal</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>mahine used -sierra</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>(8 workers/ 2 workers/node, 4 node requested, number of reduces=8)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>input 2GB, sequences=3805921, chunksize=128MB, number of reduces=8,nodes=4, numberofworkers/node=2</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bowtie</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>(8 workers(4 on each machine)/ 2 workers/node, 4 node requested(2 on each machine), number of reduces=8)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>(1GB+1GB)2</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>(2+2)4</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>(4+4)8</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Map Function</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Time taken to chunk files in seconds</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>prq</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2GB</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>shuffle phase time</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>averge sort time</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Duplicate output size is 4445MB which is 44.5% of input data</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Remaining is Filedelimiter which I used.</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>+</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Varying Number of  workers</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Varying Number of  workers - II</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Varying Number of  workers - III</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Number of  subjobs(workers) for both map/reduce phase</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Map phase Time in seconds</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Varying Number of chunk size - I</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2GB</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>4GB</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>8GB</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Align Stage</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SNPs Stage</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Align</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SNPs</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>max data for a reduce</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>8GB</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>MR type</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SEQAL</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Local-PMR</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>distributed-PMR</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Map</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>reduce</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Chunk</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Push Data</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Shuffle</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Exchange</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Reduce</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Total</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>stderr in cunk</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>stderr in setup</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>stderr in Map</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>sterr in exchange</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>stderr in shuffle</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>stderr in total</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>stderr in dt</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Setup</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Input data</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>chunk size</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>map</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>reduce</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>tts</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>(1+1)2</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>(2+2)4</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>(4+4)8</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Map</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Reduce</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>setup</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Varying chunk size ,  Input Size = 10GB, Number of workers - 32, Number of reduces -8</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
   <si>
     <t>Mean Map phase</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
+    <t>Stdev</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Reduced output size  3120 MB  which is 31.2% of input data</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>mean map phase</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>File Transfer in seconds</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Map phase Time in seconds - II</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Reduce Phase Time in seconds-II</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Map phase Time in seconds-III</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>input data</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>mean time taken for map phase</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>stderr in map phase time</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>sequences per chunk</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>SEQAL</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>local-PMR(bwa)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>distribtued-PMR(bwa)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>local-PMR(bowtie)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>distributed-PMR(bowtie)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Crossbow</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>setup</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>tts</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>average</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>stderr</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>maps</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mapcompletion</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>shuffle completion</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>reduce completion</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>map phase time</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>setup</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>reduce phase time</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Size of data transferred in MB from Map to reduce phase</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>reduce Output data size in MB</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>duplicate  data size in MB</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Varying Number of chunk size - II</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Number of workers=(4+4), sierra and hotel used.</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Number of workers=(4+4), india and hotel used.</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>835 intermediate data</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>seqal map timings</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Reduced output size  3120 MB  which is 31.2% of input data</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Varying Input size, chunk size=625000, number  of reduces=8, number of workers=32</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Input data size in GB</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Total Time to solution in  secs</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>stderr in chunk time</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Reduce Phase Time in seconds - III</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mean</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>stderr</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>mean</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Varying chunk size ,  Input Size = 10GB, Number of workers - 32, Number of reduces -8</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>number of reads</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Number of chunks created</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>stderr chunk time</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>mean map phase</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>stderr in map phase</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>mean reduce phase</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>stderr reduce phase</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>stderr of map phase</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Varying Input size, chunk size=62500 reads, number of reduces=8, number of workers=32</t>
+  </si>
+  <si>
+    <t>Varying number of workers, input size = 10 GB, reduces = 8, Number of reads/ chunk=625000</t>
+  </si>
+  <si>
+    <t>Setup</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Map</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Shuffle</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Reduce</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Total</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>stderr in setup</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>stderr in map</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>stderr I shuffle</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>number of reads</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>chunk size( lines)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>stderr of reduce phase</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Varying number of workers, input size = 10 GB, reduces = 8, Number of reads/ chunk=625000</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Workers</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>mean map phase</t>
+  </si>
+  <si>
+    <t>map align only</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Time to transfer files files between map &amp; reduce phase is </t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Data transfer in MB between map &amp; reduce phase is</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>use default replication factor.</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>avg</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>stderr</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>1GB</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2GB</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>4GB</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>initial data transfers</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>tts with intial data transfer</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>232MB</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>943MB</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>445MB</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mean Map phase</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
     <t>stderr for map phase</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -189,34 +822,30 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
+    <t>Varying Input size - III</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>mean chunk time</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Map phase Time in seconds - I</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Reduce Phase Time in seconds - I</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>seqal default configs</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
     <t>tts</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>Varying Input size - III</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>mean chunk time</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Map phase Time in seconds - I</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Reduce Phase Time in seconds - I</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>seqal default configs</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>tts</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>mean reduce phase</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -255,611 +884,6 @@
   </si>
   <si>
     <t>Reduced output size  3120 MB  which is 31.2% of input data</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Number of workers=(4+4), sierra and hotel used.</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Number of workers=(4+4), india and hotel used.</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>835 intermediate data</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>seqal map timings</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Reduced output size  3120 MB  which is 31.2% of input data</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Varying Input size, chunk size=625000, number  of reduces=8, number of workers=32</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Input data size in GB</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Total Time to solution in  secs</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>stderr in chunk time</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Reduce Phase Time in seconds - III</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Mean</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>stderr</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>mean</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Varying chunk size ,  Input Size = 10GB, Number of workers - 32, Number of reduces -8</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>number of reads</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Number of chunks created</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>stderr chunk time</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>mean map phase</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>stderr in map phase</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>mean reduce phase</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>stderr reduce phase</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>stderr of map phase</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Varying Input size, chunk size=62500 reads, number of reduces=8, number of workers=32</t>
-  </si>
-  <si>
-    <t>Varying number of workers, input size = 10 GB, reduces = 8, Number of reads/ chunk=625000</t>
-  </si>
-  <si>
-    <t>Setup</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Map</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Shuffle</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Reduce</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Total</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>stderr in setup</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>stderr in map</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>stderr I shuffle</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>number of reads</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>chunk size( lines)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>stderr of reduce phase</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Varying number of workers, input size = 10 GB, reduces = 8, Number of reads/ chunk=625000</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Workers</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>mean map phase</t>
-  </si>
-  <si>
-    <t>map align only</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">Time to transfer files files between map &amp; reduce phase is </t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Data transfer in MB between map &amp; reduce phase is</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>use default replication factor.</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>avg</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>stderr</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>1GB</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>2GB</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>4GB</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>initial data transfers</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>tts with intial data transfer</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>232MB</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>943MB</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>445MB</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>max data for a reduce</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>8GB</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>MR type</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>SEQAL</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Local-PMR</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>distributed-PMR</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Map</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>reduce</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Chunk</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Push Data</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Shuffle</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Exchange</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Reduce</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Total</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>stderr in cunk</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>stderr in setup</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>stderr in Map</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>sterr in exchange</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>stderr in shuffle</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>stderr in total</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>stderr in dt</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Setup</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Input data</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>chunk size</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>map</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>reduce</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>tts</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>(1+1)2</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>(2+2)4</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>(4+4)8</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Map</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Reduce</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>setup</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Varying chunk size ,  Input Size = 10GB, Number of workers - 32, Number of reduces -8</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Mean Map phase</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Stdev</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Reduced output size  3120 MB  which is 31.2% of input data</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>mean map phase</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>File Transfer in seconds</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Map phase Time in seconds - II</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Reduce Phase Time in seconds-II</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Map phase Time in seconds-III</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>input data</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>mean time taken for map phase</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>stderr in map phase time</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>sequences per chunk</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>SEQAL</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>local-PMR(bwa)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>distribtued-PMR(bwa)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>local-PMR(bowtie)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>distributed-PMR(bowtie)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Crossbow</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>setup</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>tts</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>average</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>stderr</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>maps</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Mapcompletion</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>shuffle completion</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>reduce completion</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>map phase time</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>setup</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>reduce phase time</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Size of data transferred in MB from Map to reduce phase</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>reduce Output data size in MB</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>duplicate  data size in MB</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Varying Number of chunk size - II</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Varying Number of chunk size - III</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>number of reads</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Number of chunks created</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Time taken to chunk files in seconds</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Bowtie</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Local PMR</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>(BWA)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>seqal</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>phase times</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>seqal</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>mahine used -sierra</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>(8 workers/ 2 workers/node, 4 node requested, number of reduces=8)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>input 2GB, sequences=3805921, chunksize=128MB, number of reduces=8,nodes=4, numberofworkers/node=2</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Bowtie</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>(8 workers(4 on each machine)/ 2 workers/node, 4 node requested(2 on each machine), number of reduces=8)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>(1GB+1GB)2</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>(2+2)4</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>(4+4)8</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Map Function</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Time taken to chunk files in seconds</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>prq</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>2GB</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>shuffle phase time</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>averge sort time</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Duplicate output size is 4445MB which is 44.5% of input data</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Remaining is Filedelimiter which I used.</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>+</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Varying Number of  workers</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Varying Number of  workers - II</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Varying Number of  workers - III</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Number of  subjobs(workers) for both map/reduce phase</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Map phase Time in seconds</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Varying Number of chunk size - I</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -867,6 +891,14 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="6">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="h:mm:ss"/>
+    <numFmt numFmtId="166" formatCode="ss"/>
+  </numFmts>
   <fonts count="9">
     <font>
       <sz val="10"/>
@@ -918,7 +950,7 @@
       <name val="Verdana"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -937,8 +969,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="51"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -964,11 +1002,91 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -1003,6 +1121,20 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="21" fontId="0" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="21" fontId="0" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1231,11 +1363,11 @@
           </c:val>
         </c:ser>
         <c:overlap val="100"/>
-        <c:axId val="567752136"/>
-        <c:axId val="567764152"/>
+        <c:axId val="520980344"/>
+        <c:axId val="521012312"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="567752136"/>
+        <c:axId val="520980344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1259,14 +1391,14 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="567764152"/>
+        <c:crossAx val="521012312"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="567764152"/>
+        <c:axId val="521012312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1291,7 +1423,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="567752136"/>
+        <c:crossAx val="520980344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1379,23 +1511,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="570573976"/>
-        <c:axId val="570563944"/>
+        <c:axId val="497310904"/>
+        <c:axId val="497313880"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="570573976"/>
+        <c:axId val="497310904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="570563944"/>
+        <c:crossAx val="497313880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="570563944"/>
+        <c:axId val="497313880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1403,7 +1535,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="570573976"/>
+        <c:crossAx val="497310904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1693,11 +1825,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="552521080"/>
-        <c:axId val="552528488"/>
+        <c:axId val="497424328"/>
+        <c:axId val="497430328"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="552521080"/>
+        <c:axId val="497424328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1739,14 +1871,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="552528488"/>
+        <c:crossAx val="497430328"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="552528488"/>
+        <c:axId val="497430328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1767,7 +1899,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
@@ -1781,7 +1912,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="552521080"/>
+        <c:crossAx val="497424328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2249,11 +2380,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="552571704"/>
-        <c:axId val="552575032"/>
+        <c:axId val="497473912"/>
+        <c:axId val="497477192"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="552571704"/>
+        <c:axId val="497473912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2269,14 +2400,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="552575032"/>
+        <c:crossAx val="497477192"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="552575032"/>
+        <c:axId val="497477192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2297,7 +2428,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
@@ -2311,7 +2441,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="552571704"/>
+        <c:crossAx val="497473912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2722,11 +2852,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="570774696"/>
-        <c:axId val="570926136"/>
+        <c:axId val="497519944"/>
+        <c:axId val="497523224"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="570774696"/>
+        <c:axId val="497519944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2742,14 +2872,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="570926136"/>
+        <c:crossAx val="497523224"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="570926136"/>
+        <c:axId val="497523224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2770,7 +2900,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
@@ -2784,7 +2913,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="570774696"/>
+        <c:crossAx val="497519944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3153,11 +3282,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="570880376"/>
-        <c:axId val="551907800"/>
+        <c:axId val="497572744"/>
+        <c:axId val="497578824"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="570880376"/>
+        <c:axId val="497572744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3192,14 +3321,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="551907800"/>
+        <c:crossAx val="497578824"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="551907800"/>
+        <c:axId val="497578824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3234,7 +3363,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="570880376"/>
+        <c:crossAx val="497572744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3270,6 +3399,217 @@
           <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="1"/>
+  <c:lang val="en-US"/>
+  <c:style val="18"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Crossbow</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$J$158</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Align</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$I$159:$I$161</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$J$159:$J$161</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>996.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1296.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2378.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$K$158</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>SNPs</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$I$159:$I$161</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$K$159:$K$161</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>6280.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6395.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7137.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="500312504"/>
+        <c:axId val="494680104"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="500312504"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Data Size [GB]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="494680104"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="494680104"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Total Runtime [sec]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="500312504"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -3476,11 +3816,11 @@
           </c:val>
         </c:ser>
         <c:overlap val="100"/>
-        <c:axId val="567856600"/>
-        <c:axId val="567830088"/>
+        <c:axId val="521076648"/>
+        <c:axId val="521082504"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="567856600"/>
+        <c:axId val="521076648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3504,14 +3844,14 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="567830088"/>
+        <c:crossAx val="521082504"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="567830088"/>
+        <c:axId val="521082504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3536,7 +3876,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="567856600"/>
+        <c:crossAx val="521076648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3833,11 +4173,11 @@
           </c:val>
         </c:ser>
         <c:overlap val="100"/>
-        <c:axId val="589567432"/>
-        <c:axId val="589574712"/>
+        <c:axId val="521121320"/>
+        <c:axId val="497030904"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="589567432"/>
+        <c:axId val="521121320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3861,14 +4201,14 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="589574712"/>
+        <c:crossAx val="497030904"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="589574712"/>
+        <c:axId val="497030904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3893,7 +4233,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="589567432"/>
+        <c:crossAx val="521121320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4131,11 +4471,11 @@
           </c:val>
         </c:ser>
         <c:overlap val="100"/>
-        <c:axId val="570744040"/>
-        <c:axId val="570749832"/>
+        <c:axId val="497078040"/>
+        <c:axId val="497086312"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="570744040"/>
+        <c:axId val="497078040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4159,14 +4499,14 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="570749832"/>
+        <c:crossAx val="497086312"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="570749832"/>
+        <c:axId val="497086312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4191,7 +4531,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="570744040"/>
+        <c:crossAx val="497078040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4399,11 +4739,11 @@
           </c:val>
         </c:ser>
         <c:overlap val="100"/>
-        <c:axId val="570630328"/>
-        <c:axId val="570826840"/>
+        <c:axId val="497151320"/>
+        <c:axId val="497158600"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="570630328"/>
+        <c:axId val="497151320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4437,14 +4777,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="570826840"/>
+        <c:crossAx val="497158600"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="570826840"/>
+        <c:axId val="497158600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4478,7 +4818,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="570630328"/>
+        <c:crossAx val="497151320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4801,11 +5141,11 @@
           </c:val>
         </c:ser>
         <c:overlap val="100"/>
-        <c:axId val="568028824"/>
-        <c:axId val="568149208"/>
+        <c:axId val="497200472"/>
+        <c:axId val="497206600"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="568028824"/>
+        <c:axId val="497200472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4850,14 +5190,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="568149208"/>
+        <c:crossAx val="497206600"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="568149208"/>
+        <c:axId val="497206600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4891,7 +5231,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="568028824"/>
+        <c:crossAx val="497200472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5043,11 +5383,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="570836376"/>
-        <c:axId val="568157848"/>
+        <c:axId val="497175784"/>
+        <c:axId val="497215800"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="570836376"/>
+        <c:axId val="497175784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5071,12 +5411,12 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="568157848"/>
+        <c:crossAx val="497215800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="568157848"/>
+        <c:axId val="497215800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5101,7 +5441,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="570836376"/>
+        <c:crossAx val="497175784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5183,23 +5523,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="570577544"/>
-        <c:axId val="570437880"/>
+        <c:axId val="497251384"/>
+        <c:axId val="497254360"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="570577544"/>
+        <c:axId val="497251384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="570437880"/>
+        <c:crossAx val="497254360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="570437880"/>
+        <c:axId val="497254360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5207,7 +5547,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="570577544"/>
+        <c:crossAx val="497251384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5289,23 +5629,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="570467224"/>
-        <c:axId val="570470264"/>
+        <c:axId val="497281160"/>
+        <c:axId val="497284136"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="570467224"/>
+        <c:axId val="497281160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="570470264"/>
+        <c:crossAx val="497284136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="570470264"/>
+        <c:axId val="497284136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5313,7 +5653,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="570467224"/>
+        <c:crossAx val="497281160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5759,6 +6099,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>469900</xdr:colOff>
+      <xdr:row>142</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>393700</xdr:colOff>
+      <xdr:row>164</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="9" name="Chart 8"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -6351,6 +6721,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+  <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:Y158"/>
   <sheetViews>
     <sheetView topLeftCell="A190" workbookViewId="0">
@@ -6367,7 +6738,7 @@
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
       <c r="G1" s="1" t="s">
-        <v>210</v>
+        <v>32</v>
       </c>
       <c r="H1" s="1"/>
       <c r="I1" s="2"/>
@@ -6379,46 +6750,46 @@
     </row>
     <row r="2" spans="1:14" ht="71" thickBot="1">
       <c r="A2" s="3" t="s">
-        <v>92</v>
+        <v>140</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>91</v>
+        <v>139</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>13</v>
+        <v>172</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>14</v>
+        <v>173</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>15</v>
+        <v>174</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>16</v>
+        <v>175</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>17</v>
+        <v>176</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>18</v>
+        <v>177</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>19</v>
+        <v>178</v>
       </c>
       <c r="J2" s="7" t="s">
-        <v>20</v>
+        <v>179</v>
       </c>
       <c r="K2" s="8" t="s">
-        <v>149</v>
+        <v>78</v>
       </c>
       <c r="L2" s="8" t="s">
-        <v>174</v>
+        <v>103</v>
       </c>
       <c r="M2" s="8" t="s">
-        <v>175</v>
+        <v>104</v>
       </c>
       <c r="N2" s="8" t="s">
-        <v>176</v>
+        <v>105</v>
       </c>
     </row>
     <row r="3" spans="1:14">
@@ -6597,7 +6968,7 @@
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="1" t="s">
-        <v>177</v>
+        <v>106</v>
       </c>
       <c r="H8" s="1"/>
       <c r="I8" s="2"/>
@@ -6609,46 +6980,46 @@
     </row>
     <row r="9" spans="1:14" ht="71" thickBot="1">
       <c r="A9" s="3" t="s">
-        <v>92</v>
+        <v>140</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>91</v>
+        <v>139</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>13</v>
+        <v>172</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>14</v>
+        <v>173</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>15</v>
+        <v>174</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>16</v>
+        <v>175</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>17</v>
+        <v>176</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>18</v>
+        <v>177</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>19</v>
+        <v>178</v>
       </c>
       <c r="J9" s="7" t="s">
-        <v>20</v>
+        <v>179</v>
       </c>
       <c r="K9" s="8" t="s">
-        <v>149</v>
+        <v>78</v>
       </c>
       <c r="L9" s="8" t="s">
-        <v>174</v>
+        <v>103</v>
       </c>
       <c r="M9" s="8" t="s">
-        <v>175</v>
+        <v>104</v>
       </c>
       <c r="N9" s="8" t="s">
-        <v>176</v>
+        <v>105</v>
       </c>
     </row>
     <row r="10" spans="1:14">
@@ -6827,7 +7198,7 @@
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
       <c r="G16" s="1" t="s">
-        <v>178</v>
+        <v>0</v>
       </c>
       <c r="H16" s="1"/>
       <c r="I16" s="2"/>
@@ -6839,46 +7210,46 @@
     </row>
     <row r="17" spans="1:19" ht="71" thickBot="1">
       <c r="A17" s="3" t="s">
-        <v>92</v>
+        <v>140</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>91</v>
+        <v>139</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>13</v>
+        <v>172</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>14</v>
+        <v>173</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>15</v>
+        <v>174</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>16</v>
+        <v>175</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>17</v>
+        <v>176</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>18</v>
+        <v>177</v>
       </c>
       <c r="I17" s="7" t="s">
-        <v>19</v>
+        <v>178</v>
       </c>
       <c r="J17" s="7" t="s">
-        <v>20</v>
+        <v>179</v>
       </c>
       <c r="K17" s="8" t="s">
-        <v>149</v>
+        <v>78</v>
       </c>
       <c r="L17" s="8" t="s">
-        <v>174</v>
+        <v>103</v>
       </c>
       <c r="M17" s="8" t="s">
-        <v>175</v>
+        <v>104</v>
       </c>
       <c r="N17" s="8" t="s">
-        <v>176</v>
+        <v>105</v>
       </c>
     </row>
     <row r="18" spans="1:19">
@@ -7051,46 +7422,46 @@
     </row>
     <row r="24" spans="1:19" ht="46" thickBot="1">
       <c r="A24" s="3" t="s">
-        <v>179</v>
+        <v>1</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>180</v>
+        <v>2</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>17</v>
+        <v>176</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>181</v>
+        <v>3</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>44</v>
+        <v>202</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>45</v>
+        <v>203</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>150</v>
+        <v>79</v>
       </c>
       <c r="H24" s="7" t="s">
-        <v>151</v>
+        <v>80</v>
       </c>
       <c r="I24" s="7" t="s">
-        <v>152</v>
+        <v>81</v>
       </c>
       <c r="J24" s="7" t="s">
-        <v>68</v>
+        <v>116</v>
       </c>
       <c r="K24" s="8" t="s">
-        <v>69</v>
+        <v>117</v>
       </c>
       <c r="L24" s="8" t="s">
-        <v>70</v>
+        <v>118</v>
       </c>
       <c r="M24" s="8" t="s">
-        <v>71</v>
+        <v>119</v>
       </c>
       <c r="N24" s="8" t="s">
-        <v>70</v>
+        <v>118</v>
       </c>
     </row>
     <row r="25" spans="1:19">
@@ -7287,39 +7658,39 @@
     </row>
     <row r="31" spans="1:19">
       <c r="D31" t="s">
-        <v>72</v>
+        <v>120</v>
       </c>
     </row>
     <row r="32" spans="1:19" ht="46" thickBot="1">
       <c r="D32" s="3" t="s">
-        <v>73</v>
+        <v>121</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>74</v>
+        <v>122</v>
       </c>
       <c r="F32" s="6" t="s">
-        <v>17</v>
+        <v>176</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>197</v>
+        <v>19</v>
       </c>
       <c r="H32" s="8" t="s">
-        <v>0</v>
+        <v>159</v>
       </c>
       <c r="I32" s="8" t="s">
-        <v>1</v>
+        <v>160</v>
       </c>
       <c r="J32" s="8" t="s">
-        <v>2</v>
+        <v>161</v>
       </c>
       <c r="K32" s="8" t="s">
-        <v>3</v>
+        <v>162</v>
       </c>
       <c r="R32" t="s">
-        <v>4</v>
+        <v>163</v>
       </c>
       <c r="S32" t="s">
-        <v>5</v>
+        <v>164</v>
       </c>
     </row>
     <row r="33" spans="4:19">
@@ -7349,7 +7720,7 @@
         <v>3.8921515186908202</v>
       </c>
       <c r="M33" t="s">
-        <v>98</v>
+        <v>146</v>
       </c>
       <c r="R33">
         <v>1.59</v>
@@ -7385,7 +7756,7 @@
         <v>1.2000589337377248</v>
       </c>
       <c r="M34" t="s">
-        <v>99</v>
+        <v>147</v>
       </c>
       <c r="R34" s="10">
         <v>9155.6200000000008</v>
@@ -7421,7 +7792,7 @@
         <v>2.2325377438638392</v>
       </c>
       <c r="M35" t="s">
-        <v>63</v>
+        <v>111</v>
       </c>
     </row>
     <row r="36" spans="4:19">
@@ -7451,17 +7822,17 @@
         <v>2.6636263501721773</v>
       </c>
       <c r="M36" t="s">
-        <v>202</v>
+        <v>24</v>
       </c>
     </row>
     <row r="37" spans="4:19">
       <c r="M37" t="s">
-        <v>203</v>
+        <v>25</v>
       </c>
     </row>
     <row r="60" spans="25:25">
       <c r="Y60" t="s">
-        <v>204</v>
+        <v>26</v>
       </c>
     </row>
     <row r="65" spans="1:14" ht="15">
@@ -7472,7 +7843,7 @@
       <c r="E65" s="2"/>
       <c r="F65" s="2"/>
       <c r="G65" s="1" t="s">
-        <v>205</v>
+        <v>27</v>
       </c>
       <c r="H65" s="1"/>
       <c r="I65" s="2"/>
@@ -7484,46 +7855,46 @@
     </row>
     <row r="66" spans="1:14" ht="71" thickBot="1">
       <c r="A66" s="3" t="s">
-        <v>92</v>
+        <v>140</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>91</v>
+        <v>139</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>13</v>
+        <v>172</v>
       </c>
       <c r="D66" s="5" t="s">
-        <v>14</v>
+        <v>173</v>
       </c>
       <c r="E66" s="3" t="s">
-        <v>15</v>
+        <v>174</v>
       </c>
       <c r="F66" s="3" t="s">
-        <v>16</v>
+        <v>175</v>
       </c>
       <c r="G66" s="6" t="s">
-        <v>17</v>
+        <v>176</v>
       </c>
       <c r="H66" s="3" t="s">
-        <v>18</v>
+        <v>177</v>
       </c>
       <c r="I66" s="7" t="s">
-        <v>19</v>
+        <v>178</v>
       </c>
       <c r="J66" s="7" t="s">
-        <v>20</v>
+        <v>179</v>
       </c>
       <c r="K66" s="8" t="s">
-        <v>149</v>
+        <v>78</v>
       </c>
       <c r="L66" s="8" t="s">
-        <v>174</v>
+        <v>103</v>
       </c>
       <c r="M66" s="8" t="s">
-        <v>175</v>
+        <v>104</v>
       </c>
       <c r="N66" s="8" t="s">
-        <v>176</v>
+        <v>105</v>
       </c>
     </row>
     <row r="67" spans="1:14">
@@ -7660,7 +8031,7 @@
       <c r="E72" s="2"/>
       <c r="F72" s="2"/>
       <c r="G72" s="1" t="s">
-        <v>206</v>
+        <v>28</v>
       </c>
       <c r="H72" s="1"/>
       <c r="I72" s="2"/>
@@ -7672,46 +8043,46 @@
     </row>
     <row r="73" spans="1:14" ht="71" thickBot="1">
       <c r="A73" s="3" t="s">
-        <v>92</v>
+        <v>140</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>91</v>
+        <v>139</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>13</v>
+        <v>172</v>
       </c>
       <c r="D73" s="5" t="s">
-        <v>14</v>
+        <v>173</v>
       </c>
       <c r="E73" s="3" t="s">
-        <v>15</v>
+        <v>174</v>
       </c>
       <c r="F73" s="3" t="s">
-        <v>16</v>
+        <v>175</v>
       </c>
       <c r="G73" s="6" t="s">
-        <v>17</v>
+        <v>176</v>
       </c>
       <c r="H73" s="3" t="s">
-        <v>18</v>
+        <v>177</v>
       </c>
       <c r="I73" s="7" t="s">
-        <v>19</v>
+        <v>178</v>
       </c>
       <c r="J73" s="7" t="s">
-        <v>20</v>
+        <v>179</v>
       </c>
       <c r="K73" s="8" t="s">
-        <v>149</v>
+        <v>78</v>
       </c>
       <c r="L73" s="8" t="s">
-        <v>174</v>
+        <v>103</v>
       </c>
       <c r="M73" s="8" t="s">
-        <v>175</v>
+        <v>104</v>
       </c>
       <c r="N73" s="8" t="s">
-        <v>176</v>
+        <v>105</v>
       </c>
     </row>
     <row r="74" spans="1:14">
@@ -7848,7 +8219,7 @@
       <c r="E79" s="2"/>
       <c r="F79" s="2"/>
       <c r="G79" s="1" t="s">
-        <v>207</v>
+        <v>29</v>
       </c>
       <c r="H79" s="1"/>
       <c r="I79" s="2"/>
@@ -7860,46 +8231,46 @@
     </row>
     <row r="80" spans="1:14" ht="71" thickBot="1">
       <c r="A80" s="3" t="s">
-        <v>92</v>
+        <v>140</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>91</v>
+        <v>139</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>13</v>
+        <v>172</v>
       </c>
       <c r="D80" s="5" t="s">
-        <v>14</v>
+        <v>173</v>
       </c>
       <c r="E80" s="3" t="s">
-        <v>15</v>
+        <v>174</v>
       </c>
       <c r="F80" s="3" t="s">
-        <v>16</v>
+        <v>175</v>
       </c>
       <c r="G80" s="6" t="s">
-        <v>17</v>
+        <v>176</v>
       </c>
       <c r="H80" s="3" t="s">
-        <v>18</v>
+        <v>177</v>
       </c>
       <c r="I80" s="7" t="s">
-        <v>19</v>
+        <v>178</v>
       </c>
       <c r="J80" s="7" t="s">
-        <v>20</v>
+        <v>179</v>
       </c>
       <c r="K80" s="8" t="s">
-        <v>149</v>
+        <v>78</v>
       </c>
       <c r="L80" s="8" t="s">
-        <v>174</v>
+        <v>103</v>
       </c>
       <c r="M80" s="8" t="s">
-        <v>175</v>
+        <v>104</v>
       </c>
       <c r="N80" s="8" t="s">
-        <v>176</v>
+        <v>105</v>
       </c>
     </row>
     <row r="81" spans="1:12">
@@ -8021,40 +8392,40 @@
     </row>
     <row r="87" spans="1:12" ht="71" thickBot="1">
       <c r="A87" s="3" t="s">
-        <v>208</v>
+        <v>30</v>
       </c>
       <c r="B87" s="6" t="s">
-        <v>17</v>
+        <v>176</v>
       </c>
       <c r="C87" s="7" t="s">
-        <v>209</v>
+        <v>31</v>
       </c>
       <c r="D87" s="7" t="s">
-        <v>209</v>
+        <v>31</v>
       </c>
       <c r="E87" s="7" t="s">
-        <v>209</v>
+        <v>31</v>
       </c>
       <c r="F87" s="8" t="s">
-        <v>148</v>
+        <v>77</v>
       </c>
       <c r="G87" s="8" t="s">
-        <v>80</v>
+        <v>128</v>
       </c>
       <c r="H87" s="7" t="s">
-        <v>49</v>
+        <v>207</v>
       </c>
       <c r="I87" s="7" t="s">
-        <v>49</v>
+        <v>207</v>
       </c>
       <c r="J87" s="7" t="s">
-        <v>49</v>
+        <v>207</v>
       </c>
       <c r="K87" s="8" t="s">
-        <v>48</v>
+        <v>206</v>
       </c>
       <c r="L87" s="8" t="s">
-        <v>93</v>
+        <v>141</v>
       </c>
     </row>
     <row r="88" spans="1:12">
@@ -8188,27 +8559,27 @@
     </row>
     <row r="94" spans="1:12">
       <c r="A94" t="s">
-        <v>94</v>
+        <v>142</v>
       </c>
     </row>
     <row r="96" spans="1:12" ht="33" thickBot="1">
       <c r="A96" s="3" t="s">
-        <v>95</v>
+        <v>143</v>
       </c>
       <c r="B96" s="5" t="s">
-        <v>17</v>
+        <v>176</v>
       </c>
       <c r="C96" s="6" t="s">
-        <v>96</v>
+        <v>144</v>
       </c>
       <c r="D96" s="3" t="s">
-        <v>53</v>
+        <v>211</v>
       </c>
       <c r="E96" s="3" t="s">
-        <v>54</v>
+        <v>212</v>
       </c>
       <c r="F96" s="5" t="s">
-        <v>55</v>
+        <v>213</v>
       </c>
       <c r="G96" s="11"/>
     </row>
@@ -8274,7 +8645,7 @@
     </row>
     <row r="100" spans="1:22">
       <c r="V100" t="s">
-        <v>56</v>
+        <v>214</v>
       </c>
     </row>
     <row r="101" spans="1:22">
@@ -8284,27 +8655,27 @@
     </row>
     <row r="105" spans="1:22">
       <c r="I105" t="s">
-        <v>98</v>
+        <v>146</v>
       </c>
     </row>
     <row r="106" spans="1:22">
       <c r="I106" t="s">
-        <v>57</v>
+        <v>215</v>
       </c>
     </row>
     <row r="107" spans="1:22">
       <c r="I107" t="s">
-        <v>58</v>
+        <v>216</v>
       </c>
     </row>
     <row r="108" spans="1:22">
       <c r="I108" t="s">
-        <v>52</v>
+        <v>210</v>
       </c>
     </row>
     <row r="109" spans="1:22">
       <c r="I109" t="s">
-        <v>6</v>
+        <v>165</v>
       </c>
     </row>
     <row r="120" spans="1:17" ht="15">
@@ -8315,7 +8686,7 @@
       <c r="E120" s="2"/>
       <c r="F120" s="2"/>
       <c r="G120" s="1" t="s">
-        <v>7</v>
+        <v>166</v>
       </c>
       <c r="H120" s="1"/>
       <c r="I120" s="2"/>
@@ -8327,46 +8698,46 @@
     </row>
     <row r="121" spans="1:17" ht="71" thickBot="1">
       <c r="A121" s="3" t="s">
-        <v>92</v>
+        <v>140</v>
       </c>
       <c r="B121" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C121" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="D121" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="E121" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="F121" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="G121" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="H121" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="I121" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="J121" s="7" t="s">
         <v>179</v>
       </c>
-      <c r="C121" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D121" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E121" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F121" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G121" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="H121" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="I121" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="J121" s="7" t="s">
-        <v>20</v>
-      </c>
       <c r="K121" s="8" t="s">
-        <v>149</v>
+        <v>78</v>
       </c>
       <c r="L121" s="8" t="s">
-        <v>174</v>
+        <v>103</v>
       </c>
       <c r="M121" s="8" t="s">
-        <v>175</v>
+        <v>104</v>
       </c>
       <c r="N121" s="8" t="s">
-        <v>9</v>
+        <v>168</v>
       </c>
     </row>
     <row r="122" spans="1:17">
@@ -8532,7 +8903,7 @@
       <c r="E129" s="2"/>
       <c r="F129" s="2"/>
       <c r="G129" s="1" t="s">
-        <v>10</v>
+        <v>169</v>
       </c>
       <c r="H129" s="1"/>
       <c r="I129" s="2"/>
@@ -8544,46 +8915,46 @@
     </row>
     <row r="130" spans="1:14" ht="71" thickBot="1">
       <c r="A130" s="3" t="s">
-        <v>92</v>
+        <v>140</v>
       </c>
       <c r="B130" s="3" t="s">
-        <v>91</v>
+        <v>139</v>
       </c>
       <c r="C130" s="4" t="s">
-        <v>13</v>
+        <v>172</v>
       </c>
       <c r="D130" s="5" t="s">
-        <v>14</v>
+        <v>173</v>
       </c>
       <c r="E130" s="3" t="s">
-        <v>15</v>
+        <v>174</v>
       </c>
       <c r="F130" s="3" t="s">
-        <v>16</v>
+        <v>175</v>
       </c>
       <c r="G130" s="6" t="s">
-        <v>17</v>
+        <v>176</v>
       </c>
       <c r="H130" s="3" t="s">
-        <v>18</v>
+        <v>177</v>
       </c>
       <c r="I130" s="7" t="s">
-        <v>19</v>
+        <v>178</v>
       </c>
       <c r="J130" s="7" t="s">
-        <v>20</v>
+        <v>179</v>
       </c>
       <c r="K130" s="8" t="s">
-        <v>149</v>
+        <v>78</v>
       </c>
       <c r="L130" s="8" t="s">
-        <v>174</v>
+        <v>103</v>
       </c>
       <c r="M130" s="8" t="s">
-        <v>175</v>
+        <v>104</v>
       </c>
       <c r="N130" s="8" t="s">
-        <v>176</v>
+        <v>105</v>
       </c>
     </row>
     <row r="131" spans="1:14">
@@ -8723,7 +9094,7 @@
       <c r="E139" s="2"/>
       <c r="F139" s="2"/>
       <c r="G139" s="1" t="s">
-        <v>42</v>
+        <v>200</v>
       </c>
       <c r="H139" s="1"/>
       <c r="I139" s="2"/>
@@ -8735,46 +9106,46 @@
     </row>
     <row r="140" spans="1:14" ht="71" thickBot="1">
       <c r="A140" s="3" t="s">
-        <v>92</v>
+        <v>140</v>
       </c>
       <c r="B140" s="3" t="s">
-        <v>91</v>
+        <v>139</v>
       </c>
       <c r="C140" s="4" t="s">
-        <v>13</v>
+        <v>172</v>
       </c>
       <c r="D140" s="5" t="s">
-        <v>14</v>
+        <v>173</v>
       </c>
       <c r="E140" s="3" t="s">
-        <v>15</v>
+        <v>174</v>
       </c>
       <c r="F140" s="3" t="s">
-        <v>16</v>
+        <v>175</v>
       </c>
       <c r="G140" s="6" t="s">
-        <v>17</v>
+        <v>176</v>
       </c>
       <c r="H140" s="3" t="s">
-        <v>18</v>
+        <v>177</v>
       </c>
       <c r="I140" s="7" t="s">
-        <v>19</v>
+        <v>178</v>
       </c>
       <c r="J140" s="7" t="s">
-        <v>20</v>
+        <v>179</v>
       </c>
       <c r="K140" s="8" t="s">
-        <v>149</v>
+        <v>78</v>
       </c>
       <c r="L140" s="8" t="s">
-        <v>174</v>
+        <v>103</v>
       </c>
       <c r="M140" s="8" t="s">
-        <v>175</v>
+        <v>104</v>
       </c>
       <c r="N140" s="8" t="s">
-        <v>9</v>
+        <v>168</v>
       </c>
     </row>
     <row r="141" spans="1:14">
@@ -8908,55 +9279,55 @@
     </row>
     <row r="147" spans="1:17" ht="43" thickBot="1">
       <c r="A147" s="4" t="s">
-        <v>13</v>
+        <v>172</v>
       </c>
       <c r="B147" s="6" t="s">
-        <v>17</v>
+        <v>176</v>
       </c>
       <c r="C147" s="3" t="s">
-        <v>18</v>
+        <v>177</v>
       </c>
       <c r="D147" s="3" t="s">
-        <v>18</v>
+        <v>177</v>
       </c>
       <c r="E147" s="3" t="s">
-        <v>18</v>
+        <v>177</v>
       </c>
       <c r="F147" s="3" t="s">
-        <v>43</v>
+        <v>201</v>
       </c>
       <c r="G147" s="3" t="s">
-        <v>75</v>
+        <v>123</v>
       </c>
       <c r="H147" s="7" t="s">
-        <v>19</v>
+        <v>178</v>
       </c>
       <c r="I147" s="7" t="s">
-        <v>19</v>
+        <v>178</v>
       </c>
       <c r="J147" s="7" t="s">
-        <v>19</v>
+        <v>178</v>
       </c>
       <c r="K147" s="8" t="s">
-        <v>76</v>
+        <v>124</v>
       </c>
       <c r="L147" s="8" t="s">
-        <v>77</v>
+        <v>125</v>
       </c>
       <c r="M147" s="7" t="s">
-        <v>20</v>
+        <v>179</v>
       </c>
       <c r="N147" s="7" t="s">
-        <v>20</v>
+        <v>179</v>
       </c>
       <c r="O147" s="7" t="s">
-        <v>20</v>
+        <v>179</v>
       </c>
       <c r="P147" s="8" t="s">
-        <v>78</v>
+        <v>126</v>
       </c>
       <c r="Q147" s="8" t="s">
-        <v>79</v>
+        <v>127</v>
       </c>
     </row>
     <row r="148" spans="1:17">
@@ -9120,36 +9491,36 @@
     </row>
     <row r="153" spans="1:17">
       <c r="C153" t="s">
-        <v>64</v>
+        <v>112</v>
       </c>
     </row>
     <row r="155" spans="1:17" ht="49" thickBot="1">
       <c r="C155" s="3" t="s">
-        <v>65</v>
+        <v>113</v>
       </c>
       <c r="D155" s="5" t="s">
-        <v>14</v>
+        <v>173</v>
       </c>
       <c r="E155" s="6" t="s">
-        <v>66</v>
+        <v>114</v>
       </c>
       <c r="F155" s="3" t="s">
-        <v>18</v>
+        <v>177</v>
       </c>
       <c r="G155" s="3" t="s">
-        <v>67</v>
+        <v>115</v>
       </c>
       <c r="H155" s="8" t="s">
-        <v>154</v>
+        <v>83</v>
       </c>
       <c r="I155" s="8" t="s">
-        <v>155</v>
+        <v>84</v>
       </c>
       <c r="J155" s="8" t="s">
-        <v>38</v>
+        <v>197</v>
       </c>
       <c r="K155" s="8" t="s">
-        <v>39</v>
+        <v>198</v>
       </c>
     </row>
     <row r="156" spans="1:17">
@@ -9256,6 +9627,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+  <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A3:I85"/>
   <sheetViews>
     <sheetView topLeftCell="A85" workbookViewId="0">
@@ -9266,33 +9638,33 @@
   <sheetData>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>144</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="46" thickBot="1">
       <c r="A4" s="3" t="s">
-        <v>91</v>
+        <v>139</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>14</v>
+        <v>173</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>17</v>
+        <v>176</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>18</v>
+        <v>177</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>145</v>
+        <v>74</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>1</v>
+        <v>160</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>2</v>
+        <v>161</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>3</v>
+        <v>162</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -9405,15 +9777,15 @@
     </row>
     <row r="31" spans="2:8">
       <c r="G31" t="s">
-        <v>4</v>
+        <v>163</v>
       </c>
       <c r="H31" t="s">
-        <v>146</v>
+        <v>75</v>
       </c>
     </row>
     <row r="32" spans="2:8">
       <c r="B32" t="s">
-        <v>98</v>
+        <v>146</v>
       </c>
       <c r="G32">
         <v>1.59</v>
@@ -9424,7 +9796,7 @@
     </row>
     <row r="33" spans="1:8" ht="15">
       <c r="B33" t="s">
-        <v>99</v>
+        <v>147</v>
       </c>
       <c r="G33" s="10">
         <v>9155.6200000000008</v>
@@ -9435,42 +9807,42 @@
     </row>
     <row r="34" spans="1:8">
       <c r="B34" t="s">
-        <v>147</v>
+        <v>76</v>
       </c>
     </row>
     <row r="35" spans="1:8">
       <c r="B35" t="s">
-        <v>52</v>
+        <v>210</v>
       </c>
     </row>
     <row r="36" spans="1:8">
       <c r="B36" t="s">
-        <v>6</v>
+        <v>165</v>
       </c>
     </row>
     <row r="48" spans="1:8">
       <c r="A48" t="s">
-        <v>94</v>
+        <v>142</v>
       </c>
     </row>
     <row r="50" spans="1:9" ht="33" thickBot="1">
       <c r="A50" s="3" t="s">
-        <v>95</v>
+        <v>143</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>17</v>
+        <v>176</v>
       </c>
       <c r="C50" s="6" t="s">
-        <v>96</v>
+        <v>144</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>53</v>
+        <v>211</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>54</v>
+        <v>212</v>
       </c>
       <c r="F50" s="5" t="s">
-        <v>55</v>
+        <v>213</v>
       </c>
       <c r="G50" s="11"/>
     </row>
@@ -9514,7 +9886,7 @@
         <v>4.1344438965032166</v>
       </c>
       <c r="I52" s="14" t="s">
-        <v>82</v>
+        <v>130</v>
       </c>
     </row>
     <row r="53" spans="1:9">
@@ -9539,15 +9911,15 @@
     </row>
     <row r="64" spans="1:9">
       <c r="B64" t="s">
-        <v>98</v>
+        <v>146</v>
       </c>
       <c r="G64" t="s">
-        <v>56</v>
+        <v>214</v>
       </c>
     </row>
     <row r="65" spans="1:9" ht="15">
       <c r="B65" t="s">
-        <v>99</v>
+        <v>147</v>
       </c>
       <c r="G65">
         <v>9144.5290000000005</v>
@@ -9556,17 +9928,17 @@
     </row>
     <row r="66" spans="1:9">
       <c r="B66" t="s">
-        <v>147</v>
+        <v>76</v>
       </c>
     </row>
     <row r="67" spans="1:9">
       <c r="B67" t="s">
-        <v>52</v>
+        <v>210</v>
       </c>
     </row>
     <row r="68" spans="1:9">
       <c r="B68" t="s">
-        <v>6</v>
+        <v>165</v>
       </c>
     </row>
     <row r="71" spans="1:9">
@@ -9586,36 +9958,36 @@
     </row>
     <row r="78" spans="1:9">
       <c r="A78" t="s">
-        <v>64</v>
+        <v>112</v>
       </c>
     </row>
     <row r="80" spans="1:9" ht="49" thickBot="1">
       <c r="A80" s="3" t="s">
-        <v>65</v>
+        <v>113</v>
       </c>
       <c r="B80" s="5" t="s">
-        <v>14</v>
+        <v>173</v>
       </c>
       <c r="C80" s="6" t="s">
-        <v>66</v>
+        <v>114</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>18</v>
+        <v>177</v>
       </c>
       <c r="E80" s="3" t="s">
-        <v>67</v>
+        <v>115</v>
       </c>
       <c r="F80" s="8" t="s">
-        <v>154</v>
+        <v>83</v>
       </c>
       <c r="G80" s="8" t="s">
-        <v>155</v>
+        <v>84</v>
       </c>
       <c r="H80" s="8" t="s">
-        <v>38</v>
+        <v>197</v>
       </c>
       <c r="I80" s="8" t="s">
-        <v>39</v>
+        <v>198</v>
       </c>
     </row>
     <row r="81" spans="1:9">
@@ -9710,7 +10082,7 @@
     </row>
     <row r="85" spans="1:9" ht="23">
       <c r="C85" s="14" t="s">
-        <v>81</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -9727,72 +10099,73 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A2:Z162"/>
+  <sheetPr published="0" enableFormatConditionsCalculation="0"/>
+  <dimension ref="A2:Z165"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A124" workbookViewId="0">
-      <selection activeCell="B158" sqref="B158"/>
+    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
+      <selection activeCell="S153" sqref="S153"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <sheetData>
     <row r="2" spans="1:24">
       <c r="A2" s="15" t="s">
-        <v>187</v>
+        <v>9</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>190</v>
+        <v>12</v>
       </c>
       <c r="C2" s="15"/>
       <c r="I2" s="15"/>
       <c r="K2" s="15" t="s">
-        <v>188</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:24">
       <c r="A4" t="s">
-        <v>153</v>
+        <v>82</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
+        <v>182</v>
       </c>
       <c r="C4" t="s">
-        <v>141</v>
+        <v>70</v>
       </c>
       <c r="D4" t="s">
-        <v>142</v>
+        <v>71</v>
       </c>
       <c r="E4" t="s">
-        <v>137</v>
+        <v>66</v>
       </c>
       <c r="F4" t="s">
-        <v>24</v>
+        <v>183</v>
       </c>
       <c r="G4" t="s">
-        <v>25</v>
+        <v>184</v>
       </c>
       <c r="H4" t="s">
-        <v>21</v>
+        <v>180</v>
       </c>
       <c r="I4" t="s">
-        <v>26</v>
+        <v>185</v>
       </c>
       <c r="J4" t="s">
-        <v>136</v>
+        <v>65</v>
       </c>
       <c r="K4" t="s">
-        <v>21</v>
+        <v>180</v>
       </c>
       <c r="L4" t="s">
-        <v>27</v>
+        <v>186</v>
       </c>
       <c r="M4" t="s">
-        <v>34</v>
+        <v>193</v>
       </c>
       <c r="N4" t="s">
-        <v>35</v>
+        <v>194</v>
       </c>
       <c r="O4" t="s">
-        <v>156</v>
+        <v>85</v>
       </c>
     </row>
     <row r="5" spans="1:24">
@@ -9954,48 +10327,48 @@
     </row>
     <row r="10" spans="1:24">
       <c r="A10" s="15" t="s">
-        <v>185</v>
+        <v>7</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>186</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:24" ht="26">
       <c r="A11" s="11" t="s">
-        <v>153</v>
+        <v>82</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>172</v>
+        <v>101</v>
       </c>
       <c r="C11" s="11" t="s">
+        <v>182</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="G11" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="H11" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="I11" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="J11" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="D11" s="11" t="s">
-        <v>168</v>
-      </c>
-      <c r="E11" s="11" t="s">
-        <v>169</v>
-      </c>
-      <c r="F11" s="11" t="s">
-        <v>170</v>
-      </c>
-      <c r="G11" s="11" t="s">
-        <v>171</v>
-      </c>
-      <c r="H11" s="11" t="s">
-        <v>200</v>
-      </c>
-      <c r="I11" s="11" t="s">
-        <v>173</v>
-      </c>
-      <c r="J11" s="11" t="s">
-        <v>201</v>
-      </c>
       <c r="M11" t="s">
-        <v>46</v>
+        <v>204</v>
       </c>
       <c r="R11" t="s">
-        <v>62</v>
+        <v>110</v>
       </c>
     </row>
     <row r="12" spans="1:24" ht="26">
@@ -10034,38 +10407,38 @@
         <v>9</v>
       </c>
       <c r="M12" s="11" t="s">
-        <v>153</v>
+        <v>82</v>
       </c>
       <c r="N12" s="11" t="s">
-        <v>172</v>
+        <v>101</v>
       </c>
       <c r="O12" s="11" t="s">
-        <v>23</v>
+        <v>182</v>
       </c>
       <c r="P12" s="11" t="s">
-        <v>47</v>
+        <v>205</v>
       </c>
       <c r="Q12" s="11"/>
       <c r="R12" s="11" t="s">
-        <v>153</v>
+        <v>82</v>
       </c>
       <c r="S12" s="11" t="s">
-        <v>143</v>
+        <v>72</v>
       </c>
       <c r="T12" s="11" t="s">
-        <v>97</v>
+        <v>145</v>
       </c>
       <c r="U12" s="11" t="s">
-        <v>163</v>
+        <v>92</v>
       </c>
       <c r="V12" s="11" t="s">
-        <v>164</v>
+        <v>93</v>
       </c>
       <c r="W12" s="11" t="s">
-        <v>165</v>
+        <v>94</v>
       </c>
       <c r="X12" s="11" t="s">
-        <v>166</v>
+        <v>95</v>
       </c>
     </row>
     <row r="13" spans="1:24">
@@ -10220,10 +10593,10 @@
     </row>
     <row r="17" spans="1:24">
       <c r="A17" t="s">
-        <v>198</v>
+        <v>20</v>
       </c>
       <c r="B17" t="s">
-        <v>21</v>
+        <v>180</v>
       </c>
       <c r="M17">
         <v>4</v>
@@ -10262,7 +10635,7 @@
     </row>
     <row r="18" spans="1:24">
       <c r="A18" t="s">
-        <v>199</v>
+        <v>21</v>
       </c>
       <c r="B18">
         <v>563</v>
@@ -10290,7 +10663,7 @@
     </row>
     <row r="19" spans="1:24">
       <c r="A19" t="s">
-        <v>28</v>
+        <v>187</v>
       </c>
       <c r="B19">
         <f>19*60</f>
@@ -10319,7 +10692,7 @@
     </row>
     <row r="20" spans="1:24">
       <c r="A20" t="s">
-        <v>29</v>
+        <v>188</v>
       </c>
       <c r="B20">
         <v>2611</v>
@@ -10404,63 +10777,63 @@
     </row>
     <row r="24" spans="1:24">
       <c r="H24" s="15" t="s">
-        <v>183</v>
+        <v>5</v>
       </c>
       <c r="I24" s="15" t="s">
-        <v>184</v>
+        <v>6</v>
       </c>
     </row>
     <row r="26" spans="1:24">
       <c r="A26" t="s">
-        <v>153</v>
+        <v>82</v>
       </c>
       <c r="B26" t="s">
-        <v>31</v>
+        <v>190</v>
       </c>
       <c r="C26" t="s">
-        <v>30</v>
+        <v>189</v>
       </c>
       <c r="D26" t="s">
-        <v>142</v>
+        <v>71</v>
       </c>
       <c r="E26" t="s">
-        <v>21</v>
+        <v>180</v>
       </c>
       <c r="F26" t="s">
-        <v>31</v>
+        <v>190</v>
       </c>
       <c r="G26" t="s">
-        <v>30</v>
+        <v>189</v>
       </c>
       <c r="H26" t="s">
-        <v>142</v>
+        <v>71</v>
       </c>
       <c r="I26" t="s">
-        <v>21</v>
+        <v>180</v>
       </c>
       <c r="J26" t="s">
-        <v>32</v>
+        <v>191</v>
       </c>
       <c r="K26" t="s">
-        <v>30</v>
+        <v>189</v>
       </c>
       <c r="L26" t="s">
-        <v>142</v>
+        <v>71</v>
       </c>
       <c r="M26" t="s">
-        <v>21</v>
+        <v>180</v>
       </c>
       <c r="N26" t="s">
-        <v>33</v>
+        <v>192</v>
       </c>
       <c r="P26" t="s">
-        <v>36</v>
+        <v>195</v>
       </c>
       <c r="Q26" t="s">
-        <v>37</v>
+        <v>196</v>
       </c>
       <c r="R26" t="s">
-        <v>107</v>
+        <v>155</v>
       </c>
     </row>
     <row r="27" spans="1:24">
@@ -10634,26 +11007,26 @@
     </row>
     <row r="32" spans="1:24">
       <c r="I32" t="s">
-        <v>106</v>
+        <v>154</v>
       </c>
     </row>
     <row r="33" spans="3:17">
       <c r="I33" t="s">
-        <v>103</v>
+        <v>151</v>
       </c>
       <c r="J33" t="s">
-        <v>104</v>
+        <v>152</v>
       </c>
       <c r="K33" t="s">
-        <v>105</v>
+        <v>153</v>
       </c>
     </row>
     <row r="34" spans="3:17">
       <c r="D34" t="s">
-        <v>167</v>
+        <v>96</v>
       </c>
       <c r="E34" t="s">
-        <v>166</v>
+        <v>95</v>
       </c>
       <c r="I34">
         <v>89.043478260869563</v>
@@ -10722,7 +11095,7 @@
     </row>
     <row r="44" spans="3:17">
       <c r="C44" t="s">
-        <v>100</v>
+        <v>148</v>
       </c>
       <c r="Q44">
         <v>4</v>
@@ -10730,7 +11103,7 @@
     </row>
     <row r="45" spans="3:17">
       <c r="C45" t="s">
-        <v>11</v>
+        <v>170</v>
       </c>
       <c r="Q45">
         <v>8</v>
@@ -10738,54 +11111,54 @@
     </row>
     <row r="46" spans="3:17">
       <c r="C46" t="s">
-        <v>12</v>
+        <v>171</v>
       </c>
     </row>
     <row r="47" spans="3:17">
       <c r="C47" t="s">
-        <v>22</v>
+        <v>181</v>
       </c>
     </row>
     <row r="53" spans="1:11">
       <c r="D53" t="s">
-        <v>59</v>
+        <v>107</v>
       </c>
     </row>
     <row r="56" spans="1:11">
       <c r="A56" t="s">
-        <v>133</v>
+        <v>62</v>
       </c>
       <c r="B56" t="s">
-        <v>134</v>
+        <v>63</v>
       </c>
       <c r="C56" t="s">
-        <v>50</v>
+        <v>208</v>
       </c>
       <c r="D56" t="s">
-        <v>135</v>
+        <v>64</v>
       </c>
       <c r="E56" t="s">
-        <v>51</v>
+        <v>209</v>
       </c>
       <c r="F56" t="s">
-        <v>136</v>
+        <v>65</v>
       </c>
       <c r="G56" t="s">
-        <v>137</v>
+        <v>66</v>
       </c>
       <c r="H56" t="s">
-        <v>101</v>
+        <v>149</v>
       </c>
       <c r="I56" t="s">
-        <v>102</v>
+        <v>150</v>
       </c>
       <c r="K56" t="s">
-        <v>111</v>
+        <v>40</v>
       </c>
     </row>
     <row r="57" spans="1:11">
       <c r="A57" t="s">
-        <v>138</v>
+        <v>67</v>
       </c>
       <c r="B57">
         <v>1171052</v>
@@ -10816,7 +11189,7 @@
         <v>12.103286987068245</v>
       </c>
       <c r="K57" t="s">
-        <v>108</v>
+        <v>156</v>
       </c>
     </row>
     <row r="58" spans="1:11">
@@ -10877,7 +11250,7 @@
     </row>
     <row r="61" spans="1:11">
       <c r="A61" t="s">
-        <v>139</v>
+        <v>68</v>
       </c>
       <c r="B61">
         <v>1171052</v>
@@ -10908,7 +11281,7 @@
         <v>19.032393616609415</v>
       </c>
       <c r="K61" t="s">
-        <v>110</v>
+        <v>158</v>
       </c>
     </row>
     <row r="62" spans="1:11">
@@ -10957,7 +11330,7 @@
     </row>
     <row r="66" spans="1:26">
       <c r="A66" t="s">
-        <v>140</v>
+        <v>69</v>
       </c>
       <c r="B66">
         <v>1171052</v>
@@ -10989,7 +11362,7 @@
         <v>24.167021097560671</v>
       </c>
       <c r="K66" t="s">
-        <v>109</v>
+        <v>157</v>
       </c>
     </row>
     <row r="67" spans="1:26">
@@ -11037,10 +11410,10 @@
     </row>
     <row r="70" spans="1:26">
       <c r="E70" t="s">
-        <v>167</v>
+        <v>96</v>
       </c>
       <c r="F70" t="s">
-        <v>166</v>
+        <v>95</v>
       </c>
     </row>
     <row r="71" spans="1:26">
@@ -11056,46 +11429,46 @@
         <v>13.340925888849769</v>
       </c>
       <c r="K71" t="s">
-        <v>113</v>
+        <v>42</v>
       </c>
       <c r="L71" t="s">
-        <v>120</v>
+        <v>49</v>
       </c>
       <c r="M71" t="s">
-        <v>119</v>
+        <v>48</v>
       </c>
       <c r="N71" t="s">
+        <v>61</v>
+      </c>
+      <c r="O71" t="s">
+        <v>46</v>
+      </c>
+      <c r="P71" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q71" t="s">
+        <v>51</v>
+      </c>
+      <c r="R71" t="s">
+        <v>52</v>
+      </c>
+      <c r="S71" t="s">
+        <v>53</v>
+      </c>
+      <c r="V71" t="s">
+        <v>131</v>
+      </c>
+      <c r="W71" t="s">
         <v>132</v>
       </c>
-      <c r="O71" t="s">
-        <v>117</v>
-      </c>
-      <c r="P71" t="s">
-        <v>121</v>
-      </c>
-      <c r="Q71" t="s">
-        <v>122</v>
-      </c>
-      <c r="R71" t="s">
-        <v>123</v>
-      </c>
-      <c r="S71" t="s">
-        <v>124</v>
-      </c>
-      <c r="V71" t="s">
-        <v>83</v>
-      </c>
-      <c r="W71" t="s">
-        <v>84</v>
-      </c>
       <c r="X71" t="s">
-        <v>85</v>
+        <v>133</v>
       </c>
       <c r="Y71" t="s">
-        <v>86</v>
+        <v>134</v>
       </c>
       <c r="Z71" t="s">
-        <v>87</v>
+        <v>135</v>
       </c>
     </row>
     <row r="72" spans="1:26">
@@ -11111,10 +11484,10 @@
         <v>8.4817664826547219</v>
       </c>
       <c r="J72" t="s">
-        <v>112</v>
+        <v>41</v>
       </c>
       <c r="K72" t="s">
-        <v>114</v>
+        <v>43</v>
       </c>
       <c r="L72">
         <v>356.17391304347825</v>
@@ -11138,7 +11511,7 @@
         <v>9304.8405797101441</v>
       </c>
       <c r="U72" t="s">
-        <v>114</v>
+        <v>43</v>
       </c>
       <c r="V72">
         <f>L72+N72</f>
@@ -11171,7 +11544,7 @@
         <v>979.58801708376609</v>
       </c>
       <c r="K73" t="s">
-        <v>115</v>
+        <v>44</v>
       </c>
       <c r="L73">
         <v>356.17391304347825</v>
@@ -11196,7 +11569,7 @@
         <v>5547.3892463768107</v>
       </c>
       <c r="U73" t="s">
-        <v>115</v>
+        <v>44</v>
       </c>
       <c r="V73">
         <f>L73+M73</f>
@@ -11218,7 +11591,7 @@
     </row>
     <row r="74" spans="1:26">
       <c r="K74" t="s">
-        <v>116</v>
+        <v>45</v>
       </c>
       <c r="L74">
         <v>0</v>
@@ -11244,7 +11617,7 @@
         <v>6856.1113333333333</v>
       </c>
       <c r="U74" t="s">
-        <v>116</v>
+        <v>45</v>
       </c>
       <c r="V74">
         <f>M74</f>
@@ -11266,56 +11639,56 @@
     </row>
     <row r="76" spans="1:26">
       <c r="D76" t="s">
-        <v>60</v>
+        <v>108</v>
       </c>
     </row>
     <row r="78" spans="1:26">
       <c r="P78" t="s">
-        <v>131</v>
+        <v>60</v>
       </c>
       <c r="Q78" t="s">
-        <v>125</v>
+        <v>54</v>
       </c>
       <c r="R78" t="s">
-        <v>126</v>
+        <v>55</v>
       </c>
       <c r="S78" t="s">
-        <v>127</v>
+        <v>56</v>
       </c>
       <c r="T78" t="s">
-        <v>129</v>
+        <v>58</v>
       </c>
       <c r="U78" t="s">
-        <v>128</v>
+        <v>57</v>
       </c>
       <c r="V78" t="s">
-        <v>118</v>
+        <v>47</v>
       </c>
       <c r="W78" t="s">
-        <v>130</v>
+        <v>59</v>
       </c>
     </row>
     <row r="79" spans="1:26">
       <c r="A79" t="s">
-        <v>133</v>
+        <v>62</v>
       </c>
       <c r="B79" t="s">
-        <v>134</v>
+        <v>63</v>
       </c>
       <c r="C79" t="s">
-        <v>50</v>
+        <v>208</v>
       </c>
       <c r="D79" t="s">
-        <v>135</v>
+        <v>64</v>
       </c>
       <c r="E79" t="s">
-        <v>51</v>
+        <v>209</v>
       </c>
       <c r="F79" t="s">
-        <v>136</v>
+        <v>65</v>
       </c>
       <c r="G79" t="s">
-        <v>21</v>
+        <v>180</v>
       </c>
       <c r="P79">
         <v>7.44168872620806</v>
@@ -11338,7 +11711,7 @@
     </row>
     <row r="80" spans="1:26">
       <c r="A80" t="s">
-        <v>138</v>
+        <v>67</v>
       </c>
       <c r="B80">
         <v>1171052</v>
@@ -11361,7 +11734,7 @@
         <v>1279.5150000000001</v>
       </c>
       <c r="H80" t="s">
-        <v>61</v>
+        <v>109</v>
       </c>
       <c r="P80">
         <v>7.4416887262080644</v>
@@ -11446,7 +11819,7 @@
     </row>
     <row r="84" spans="1:23">
       <c r="A84" t="s">
-        <v>139</v>
+        <v>68</v>
       </c>
       <c r="B84">
         <v>1171052</v>
@@ -11454,7 +11827,7 @@
     </row>
     <row r="85" spans="1:23">
       <c r="A85" t="s">
-        <v>140</v>
+        <v>69</v>
       </c>
       <c r="B85">
         <v>1171052</v>
@@ -11462,15 +11835,15 @@
     </row>
     <row r="88" spans="1:23">
       <c r="A88" t="s">
-        <v>198</v>
+        <v>20</v>
       </c>
       <c r="B88" t="s">
-        <v>21</v>
+        <v>180</v>
       </c>
     </row>
     <row r="89" spans="1:23">
       <c r="A89" t="s">
-        <v>199</v>
+        <v>21</v>
       </c>
       <c r="B89">
         <v>563</v>
@@ -11478,7 +11851,7 @@
     </row>
     <row r="90" spans="1:23">
       <c r="A90" t="s">
-        <v>28</v>
+        <v>187</v>
       </c>
       <c r="B90">
         <f>19*60</f>
@@ -11487,7 +11860,7 @@
     </row>
     <row r="91" spans="1:23" s="12" customFormat="1">
       <c r="A91" t="s">
-        <v>29</v>
+        <v>188</v>
       </c>
       <c r="B91">
         <v>2611</v>
@@ -11501,19 +11874,19 @@
     <row r="102" spans="7:25" s="11" customFormat="1"/>
     <row r="109" spans="7:25">
       <c r="U109" t="s">
-        <v>88</v>
+        <v>136</v>
       </c>
       <c r="V109" t="s">
-        <v>89</v>
+        <v>137</v>
       </c>
       <c r="W109" t="s">
-        <v>90</v>
+        <v>138</v>
       </c>
       <c r="X109" t="s">
-        <v>118</v>
+        <v>47</v>
       </c>
       <c r="Y109" t="s">
-        <v>130</v>
+        <v>59</v>
       </c>
     </row>
     <row r="110" spans="7:25">
@@ -11576,54 +11949,54 @@
     </row>
     <row r="114" spans="1:17">
       <c r="A114" t="s">
-        <v>182</v>
+        <v>4</v>
       </c>
       <c r="B114" t="s">
-        <v>189</v>
+        <v>11</v>
       </c>
       <c r="K114" t="s">
-        <v>191</v>
+        <v>13</v>
       </c>
       <c r="L114" t="s">
-        <v>192</v>
+        <v>14</v>
       </c>
     </row>
     <row r="115" spans="1:17">
       <c r="B115" t="s">
-        <v>134</v>
+        <v>63</v>
       </c>
       <c r="C115" t="s">
-        <v>50</v>
+        <v>208</v>
       </c>
       <c r="D115" t="s">
-        <v>26</v>
+        <v>185</v>
       </c>
       <c r="E115" t="s">
-        <v>137</v>
+        <v>66</v>
       </c>
       <c r="F115" t="s">
-        <v>101</v>
+        <v>149</v>
       </c>
       <c r="G115" t="s">
-        <v>102</v>
+        <v>150</v>
       </c>
       <c r="L115" t="s">
-        <v>134</v>
+        <v>63</v>
       </c>
       <c r="M115" t="s">
-        <v>50</v>
+        <v>208</v>
       </c>
       <c r="N115" t="s">
-        <v>26</v>
+        <v>185</v>
       </c>
       <c r="O115" t="s">
-        <v>137</v>
+        <v>66</v>
       </c>
       <c r="P115" t="s">
-        <v>101</v>
+        <v>149</v>
       </c>
       <c r="Q115" t="s">
-        <v>102</v>
+        <v>150</v>
       </c>
     </row>
     <row r="116" spans="1:17">
@@ -11651,7 +12024,7 @@
         <v>13.935673511291871</v>
       </c>
       <c r="K116" t="s">
-        <v>193</v>
+        <v>15</v>
       </c>
       <c r="L116">
         <v>1171052</v>
@@ -11757,7 +12130,7 @@
         <v>7.8781625077026014</v>
       </c>
       <c r="K121" t="s">
-        <v>194</v>
+        <v>16</v>
       </c>
       <c r="L121">
         <v>1171052</v>
@@ -11863,7 +12236,7 @@
         <v>4.6431871871022583</v>
       </c>
       <c r="K126" t="s">
-        <v>195</v>
+        <v>17</v>
       </c>
       <c r="L126">
         <v>1171052</v>
@@ -11946,27 +12319,27 @@
     </row>
     <row r="137" spans="5:11">
       <c r="I137" t="s">
-        <v>196</v>
+        <v>18</v>
       </c>
     </row>
     <row r="141" spans="5:11" s="11" customFormat="1" ht="26">
       <c r="F141" s="11" t="s">
-        <v>157</v>
+        <v>86</v>
       </c>
       <c r="G141" s="11" t="s">
-        <v>158</v>
+        <v>87</v>
       </c>
       <c r="H141" s="11" t="s">
-        <v>159</v>
+        <v>88</v>
       </c>
       <c r="I141" s="11" t="s">
-        <v>160</v>
+        <v>89</v>
       </c>
       <c r="J141" s="11" t="s">
-        <v>161</v>
+        <v>90</v>
       </c>
       <c r="K141" s="11" t="s">
-        <v>162</v>
+        <v>91</v>
       </c>
     </row>
     <row r="142" spans="5:11">
@@ -12029,24 +12402,24 @@
         <v>1684.1916666666666</v>
       </c>
     </row>
-    <row r="146" spans="1:10">
+    <row r="146" spans="1:12">
       <c r="F146" t="s">
-        <v>166</v>
+        <v>95</v>
       </c>
       <c r="G146" t="s">
-        <v>166</v>
+        <v>95</v>
       </c>
       <c r="H146" t="s">
-        <v>166</v>
+        <v>95</v>
       </c>
       <c r="I146" t="s">
-        <v>166</v>
+        <v>95</v>
       </c>
       <c r="J146" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="147" spans="1:10">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="147" spans="1:12">
       <c r="F147">
         <v>90.643966766199668</v>
       </c>
@@ -12063,7 +12436,7 @@
         <v>1.6668740844330987</v>
       </c>
     </row>
-    <row r="148" spans="1:10">
+    <row r="148" spans="1:12">
       <c r="F148">
         <v>99.177635471794702</v>
       </c>
@@ -12080,7 +12453,7 @@
         <v>7.3775567566892803</v>
       </c>
     </row>
-    <row r="149" spans="1:10">
+    <row r="149" spans="1:12">
       <c r="F149">
         <v>48.174196873825352</v>
       </c>
@@ -12097,49 +12470,320 @@
         <v>5.9110665054272307</v>
       </c>
     </row>
-    <row r="153" spans="1:10">
+    <row r="153" spans="1:12">
       <c r="A153" t="s">
-        <v>40</v>
+        <v>199</v>
       </c>
       <c r="B153" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="154" spans="1:10">
-      <c r="A154">
+        <v>36</v>
+      </c>
+      <c r="C153" t="s">
+        <v>37</v>
+      </c>
+      <c r="J153" t="s">
+        <v>38</v>
+      </c>
+      <c r="K153" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="154" spans="1:12">
+      <c r="A154" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="B154" s="19">
+        <f>E155-E154</f>
+        <v>9.490740740740744E-3</v>
+      </c>
+      <c r="C154" s="20">
+        <f>E156-E155</f>
+        <v>7.2210648148148149E-2</v>
+      </c>
+      <c r="E154" s="16">
+        <v>0.51013888888888892</v>
+      </c>
+      <c r="F154" s="16">
+        <v>0.59953703703703709</v>
+      </c>
+      <c r="G154" s="17">
+        <v>0.34256944444444448</v>
+      </c>
+      <c r="I154">
         <v>2</v>
       </c>
-      <c r="B154">
-        <f>10*60+46</f>
-        <v>646</v>
-      </c>
-    </row>
-    <row r="155" spans="1:10">
-      <c r="B155">
-        <f>9*60+33</f>
-        <v>573</v>
-      </c>
-    </row>
-    <row r="156" spans="1:10">
-      <c r="B156">
-        <f>9*60+35</f>
-        <v>575</v>
-      </c>
-    </row>
-    <row r="158" spans="1:10">
-      <c r="A158">
+      <c r="J154" s="16">
+        <f>B157</f>
+        <v>1.1527777777777729E-2</v>
+      </c>
+      <c r="K154" s="16">
+        <f>C157</f>
+        <v>7.2681327160493817E-2</v>
+      </c>
+    </row>
+    <row r="155" spans="1:12">
+      <c r="A155" s="21"/>
+      <c r="B155" s="22">
+        <f>F155-F154</f>
+        <v>7.8472222222221166E-3</v>
+      </c>
+      <c r="C155" s="23">
+        <f>F156-F155</f>
+        <v>7.1192129629629619E-2</v>
+      </c>
+      <c r="E155" s="16">
+        <v>0.51962962962962966</v>
+      </c>
+      <c r="F155" s="16">
+        <v>0.60738425925925921</v>
+      </c>
+      <c r="G155" s="17">
+        <v>0.35981481481481481</v>
+      </c>
+      <c r="I155">
         <v>4</v>
       </c>
-    </row>
-    <row r="162" spans="1:1">
-      <c r="A162">
+      <c r="J155" s="16">
+        <f>B161</f>
+        <v>1.500385802469136E-2</v>
+      </c>
+      <c r="K155" s="16">
+        <f>C161</f>
+        <v>7.4020061728395023E-2</v>
+      </c>
+      <c r="L155" s="16"/>
+    </row>
+    <row r="156" spans="1:12">
+      <c r="A156" s="21"/>
+      <c r="B156" s="24">
+        <f>G155-G154</f>
+        <v>1.7245370370370328E-2</v>
+      </c>
+      <c r="C156" s="25">
+        <f>G156-G155</f>
+        <v>7.4641203703703696E-2</v>
+      </c>
+      <c r="E156" s="16">
+        <v>0.59184027777777781</v>
+      </c>
+      <c r="F156" s="16">
+        <v>0.67857638888888883</v>
+      </c>
+      <c r="G156" s="17">
+        <v>0.43445601851851851</v>
+      </c>
+      <c r="I156">
         <v>8</v>
+      </c>
+      <c r="J156" s="16">
+        <f>B165</f>
+        <v>2.7519290123456785E-2</v>
+      </c>
+      <c r="K156" s="16">
+        <f>C165</f>
+        <v>8.2600308641975331E-2</v>
+      </c>
+      <c r="L156" s="16"/>
+    </row>
+    <row r="157" spans="1:12">
+      <c r="A157" s="26"/>
+      <c r="B157" s="27">
+        <f>AVERAGE(B154:B156)</f>
+        <v>1.1527777777777729E-2</v>
+      </c>
+      <c r="C157" s="28">
+        <f>AVERAGE(C154:C156)</f>
+        <v>7.2681327160493817E-2</v>
+      </c>
+      <c r="L157" s="16"/>
+    </row>
+    <row r="158" spans="1:12">
+      <c r="A158" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="B158" s="19">
+        <f>E159-E158</f>
+        <v>1.4409722222222254E-2</v>
+      </c>
+      <c r="C158" s="20">
+        <f>E160-E159</f>
+        <v>7.3935185185185159E-2</v>
+      </c>
+      <c r="E158" s="16">
+        <v>0.60547453703703702</v>
+      </c>
+      <c r="F158" s="16">
+        <v>0.76245370370370369</v>
+      </c>
+      <c r="G158" s="17">
+        <v>0.34256944444444448</v>
+      </c>
+      <c r="J158" t="s">
+        <v>38</v>
+      </c>
+      <c r="K158" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="159" spans="1:12">
+      <c r="A159" s="21"/>
+      <c r="B159" s="22">
+        <f>F159-F158</f>
+        <v>1.3356481481481497E-2</v>
+      </c>
+      <c r="C159" s="23">
+        <f>F160-F159</f>
+        <v>7.34837962962962E-2</v>
+      </c>
+      <c r="E159" s="16">
+        <v>0.61988425925925927</v>
+      </c>
+      <c r="F159" s="16">
+        <v>0.77581018518518519</v>
+      </c>
+      <c r="G159" s="17">
+        <v>0.35981481481481481</v>
+      </c>
+      <c r="I159">
+        <v>2</v>
+      </c>
+      <c r="J159" s="29">
+        <f>16*60+36</f>
+        <v>996</v>
+      </c>
+      <c r="K159" s="29">
+        <f>1*60*60+44*60+40</f>
+        <v>6280</v>
+      </c>
+    </row>
+    <row r="160" spans="1:12">
+      <c r="A160" s="21"/>
+      <c r="B160" s="24">
+        <f>G159-G158</f>
+        <v>1.7245370370370328E-2</v>
+      </c>
+      <c r="C160" s="25">
+        <f>G160-G159</f>
+        <v>7.4641203703703696E-2</v>
+      </c>
+      <c r="E160" s="16">
+        <v>0.69381944444444443</v>
+      </c>
+      <c r="F160" s="16">
+        <v>0.84929398148148139</v>
+      </c>
+      <c r="G160" s="17">
+        <v>0.43445601851851851</v>
+      </c>
+      <c r="I160">
+        <v>4</v>
+      </c>
+      <c r="J160" s="29">
+        <f>21*60+36</f>
+        <v>1296</v>
+      </c>
+      <c r="K160" s="29">
+        <f>1*60*60+46*60+35</f>
+        <v>6395</v>
+      </c>
+    </row>
+    <row r="161" spans="1:11">
+      <c r="A161" s="26"/>
+      <c r="B161" s="27">
+        <f>AVERAGE(B158:B160)</f>
+        <v>1.500385802469136E-2</v>
+      </c>
+      <c r="C161" s="28">
+        <f>AVERAGE(C158:C160)</f>
+        <v>7.4020061728395023E-2</v>
+      </c>
+      <c r="I161">
+        <v>8</v>
+      </c>
+      <c r="J161" s="29">
+        <f>39*60+38</f>
+        <v>2378</v>
+      </c>
+      <c r="K161" s="29">
+        <f>1*60*60+58*60+57</f>
+        <v>7137</v>
+      </c>
+    </row>
+    <row r="162" spans="1:11">
+      <c r="A162" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="B162" s="19">
+        <v>2.6585648148148146E-2</v>
+      </c>
+      <c r="C162" s="20">
+        <v>8.2662037037037034E-2</v>
+      </c>
+      <c r="E162" s="16">
+        <v>0.60547453703703702</v>
+      </c>
+      <c r="F162" s="16">
+        <v>0.28195601851851854</v>
+      </c>
+      <c r="G162" s="17">
+        <v>0.39590277777777777</v>
+      </c>
+    </row>
+    <row r="163" spans="1:11">
+      <c r="A163" s="21"/>
+      <c r="B163" s="22">
+        <f>F163-F162</f>
+        <v>2.6932870370370343E-2</v>
+      </c>
+      <c r="C163" s="23">
+        <f>F164-F163</f>
+        <v>8.2835648148148144E-2</v>
+      </c>
+      <c r="E163" s="16">
+        <v>0.61988425925925927</v>
+      </c>
+      <c r="F163" s="16">
+        <v>0.30888888888888888</v>
+      </c>
+      <c r="G163" s="17">
+        <v>0.42494212962962963</v>
+      </c>
+    </row>
+    <row r="164" spans="1:11">
+      <c r="A164" s="21"/>
+      <c r="B164" s="24">
+        <f>G163-G162</f>
+        <v>2.9039351851851858E-2</v>
+      </c>
+      <c r="C164" s="25">
+        <f>G164-G163</f>
+        <v>8.2303240740740802E-2</v>
+      </c>
+      <c r="E164" s="16">
+        <v>0.69381944444444443</v>
+      </c>
+      <c r="F164" s="16">
+        <v>0.39172453703703702</v>
+      </c>
+      <c r="G164" s="17">
+        <v>0.50724537037037043</v>
+      </c>
+    </row>
+    <row r="165" spans="1:11">
+      <c r="A165" s="26"/>
+      <c r="B165" s="27">
+        <f>AVERAGE(B162:B164)</f>
+        <v>2.7519290123456785E-2</v>
+      </c>
+      <c r="C165" s="28">
+        <f>AVERAGE(C162:C164)</f>
+        <v>8.2600308641975331E-2</v>
       </c>
     </row>
   </sheetData>
   <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">

</xml_diff>

<commit_message>
new figure replacing the previous one for mapping step comaprison. I added crossbow data
git-svn-id: file://localhost/tmp/svn2git/svn@6680 defb5e50-622e-49ec-a68e-d72c7db87b45
</commit_message>
<xml_diff>
--- a/papers/saga-mr-ngs/data/GS_data.xlsx
+++ b/papers/saga-mr-ngs/data/GS_data.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="21405"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="6100" yWindow="1960" windowWidth="34180" windowHeight="25320" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="GS data" sheetId="1" r:id="rId1"/>
@@ -14,9 +14,9 @@
   <externalReferences>
     <externalReference r:id="rId4"/>
   </externalReferences>
-  <calcPr calcId="130000" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
@@ -938,15 +938,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="5">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="168" formatCode="h:mm:ss"/>
-  </numFmts>
-  <fonts count="9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -1041,7 +1034,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -1068,21 +1061,10 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -1090,27 +1072,62 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom/>
@@ -1118,84 +1135,29 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1203,23 +1165,23 @@
       <left/>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1263,60 +1225,60 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="21" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="21" fontId="0" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="21" fontId="0" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="21" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="21" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1324,7 +1286,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
 </file>
 
@@ -1332,7 +1294,15 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="1"/>
   <c:lang val="en-US"/>
-  <c:style val="18"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -1350,21 +1320,26 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:v>Map Phase time</c:v>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:errBars>
             <c:errBarType val="both"/>
             <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
                 <c:f>'[1]GS Data Analaysis'!$F$5:$F$8</c:f>
@@ -1457,9 +1432,11 @@
           <c:tx>
             <c:v>Reduce phase time</c:v>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:errBars>
             <c:errBarType val="both"/>
             <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
                 <c:f>'[1]GS Data Analaysis'!$H$5:$H$8</c:f>
@@ -1546,15 +1523,25 @@
             </c:numRef>
           </c:val>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="494438328"/>
-        <c:axId val="520478648"/>
+        <c:axId val="467605432"/>
+        <c:axId val="467141832"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="494438328"/>
+        <c:axId val="467605432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -1572,20 +1559,25 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="520478648"/>
+        <c:crossAx val="467141832"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="520478648"/>
+        <c:axId val="467141832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:title>
@@ -1604,19 +1596,24 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="494438328"/>
+        <c:crossAx val="467605432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -1630,12 +1627,22 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="1"/>
   <c:lang val="en-US"/>
-  <c:style val="2"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -1694,41 +1701,58 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
+          <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="494263112"/>
-        <c:axId val="494266152"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="424809208"/>
+        <c:axId val="424812168"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="494263112"/>
+        <c:axId val="424809208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="494266152"/>
+        <c:crossAx val="424812168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="494266152"/>
+        <c:axId val="424812168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="494263112"/>
+        <c:crossAx val="424809208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -1742,7 +1766,15 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="1"/>
   <c:lang val="en-US"/>
-  <c:style val="2"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:autoTitleDeleted val="1"/>
     <c:plotArea>
@@ -1760,15 +1792,18 @@
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:v>SEQAL</c:v>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:errBars>
             <c:errBarType val="both"/>
             <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
                 <c:f>Sheet1!$N$5:$N$7</c:f>
@@ -1776,13 +1811,13 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
                   <c:pt idx="0">
-                    <c:v>18.29333333335506</c:v>
+                    <c:v>18.29333333333334</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>114.0978909143999</c:v>
+                    <c:v>114.0978909143859</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>118.9120511601106</c:v>
+                    <c:v>118.9120511601373</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1794,13 +1829,13 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
                   <c:pt idx="0">
-                    <c:v>18.29333333335506</c:v>
+                    <c:v>18.29333333333334</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>114.0978909143999</c:v>
+                    <c:v>114.0978909143859</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>118.9120511601106</c:v>
+                    <c:v>118.9120511601373</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1849,9 +1884,11 @@
           <c:tx>
             <c:v>Local-PMR</c:v>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:errBars>
             <c:errBarType val="both"/>
             <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
                 <c:f>Sheet1!$Q$27:$Q$29</c:f>
@@ -1859,13 +1896,13 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
                   <c:pt idx="0">
-                    <c:v>4.097169079209209</c:v>
+                    <c:v>4.09716907931949</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>30.10003705732057</c:v>
+                    <c:v>30.10003705736206</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>10.54038909809311</c:v>
+                    <c:v>10.54038909769669</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1877,13 +1914,13 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
                   <c:pt idx="0">
-                    <c:v>4.097169079209209</c:v>
+                    <c:v>4.09716907931949</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>30.10003705732057</c:v>
+                    <c:v>30.10003705736206</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>10.54038909809311</c:v>
+                    <c:v>10.54038909769669</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1932,9 +1969,11 @@
           <c:tx>
             <c:v>distributed-PMR</c:v>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:errBars>
             <c:errBarType val="both"/>
             <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
                 <c:f>Sheet1!$I$57:$I$59</c:f>
@@ -1942,7 +1981,7 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
                   <c:pt idx="0">
-                    <c:v>12.10328698706824</c:v>
+                    <c:v>12.10328698715066</c:v>
                   </c:pt>
                   <c:pt idx="1">
                     <c:v>19.03239361660941</c:v>
@@ -1960,7 +1999,7 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
                   <c:pt idx="0">
-                    <c:v>12.10328698706824</c:v>
+                    <c:v>12.10328698715066</c:v>
                   </c:pt>
                   <c:pt idx="1">
                     <c:v>19.03239361660941</c:v>
@@ -2009,14 +2048,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="471996664"/>
-        <c:axId val="497280488"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="429777064"/>
+        <c:axId val="429782632"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="471996664"/>
+        <c:axId val="429777064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -2042,8 +2091,11 @@
               <c:y val="0.900806562677764"/>
             </c:manualLayout>
           </c:layout>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:txPr>
           <a:bodyPr/>
@@ -2055,17 +2107,19 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="497280488"/>
+        <c:crossAx val="429782632"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="497280488"/>
+        <c:axId val="429782632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:title>
           <c:tx>
@@ -2083,8 +2137,11 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:txPr>
           <a:bodyPr/>
@@ -2096,7 +2153,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="471996664"/>
+        <c:crossAx val="429777064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2120,6 +2177,7 @@
           <c:h val="0.256183669976036"/>
         </c:manualLayout>
       </c:layout>
+      <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
         <a:lstStyle/>
@@ -2133,6 +2191,7 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:ln>
@@ -2151,8 +2210,17 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="1"/>
   <c:lang val="en-US"/>
-  <c:style val="18"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout>
         <c:manualLayout>
@@ -2168,6 +2236,7 @@
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -2182,9 +2251,11 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:errBars>
             <c:errBarType val="both"/>
             <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
                 <c:f>Sheet1!$P$79:$W$79</c:f>
@@ -2314,9 +2385,11 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:errBars>
             <c:errBarType val="both"/>
             <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
                 <c:f>Sheet1!$P$80:$W$80</c:f>
@@ -2452,9 +2525,11 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:errBars>
             <c:errBarType val="both"/>
             <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
                 <c:f>Sheet1!$P$81:$W$81</c:f>
@@ -2564,15 +2639,27 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="497323128"/>
-        <c:axId val="497326392"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="429825656"/>
+        <c:axId val="429828744"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="497323128"/>
+        <c:axId val="429825656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:txPr>
           <a:bodyPr rot="0" vert="horz" anchor="ctr" anchorCtr="1"/>
@@ -2584,17 +2671,19 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="497326392"/>
+        <c:crossAx val="429828744"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="497326392"/>
+        <c:axId val="429828744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:title>
           <c:tx>
@@ -2612,8 +2701,11 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:txPr>
           <a:bodyPr/>
@@ -2625,7 +2717,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="497323128"/>
+        <c:crossAx val="429825656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2651,6 +2743,7 @@
           <c:h val="0.0937441673957422"/>
         </c:manualLayout>
       </c:layout>
+      <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
         <a:lstStyle/>
@@ -2664,6 +2757,7 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -2677,8 +2771,17 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="1"/>
   <c:lang val="en-US"/>
-  <c:style val="18"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout>
         <c:manualLayout>
@@ -2694,6 +2797,7 @@
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -2708,9 +2812,11 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:errBars>
             <c:errBarType val="both"/>
             <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
                 <c:f>Sheet1!$U$110:$Y$110</c:f>
@@ -2822,9 +2928,11 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:errBars>
             <c:errBarType val="both"/>
             <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
                 <c:f>Sheet1!$U$111:$Y$111</c:f>
@@ -2936,9 +3044,11 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:errBars>
             <c:errBarType val="both"/>
             <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
                 <c:f>Sheet1!$U$112:$Y$112</c:f>
@@ -3036,15 +3146,27 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="472110536"/>
-        <c:axId val="505333640"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="429872392"/>
+        <c:axId val="429875480"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="472110536"/>
+        <c:axId val="429872392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:txPr>
           <a:bodyPr/>
@@ -3056,17 +3178,19 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="505333640"/>
+        <c:crossAx val="429875480"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="505333640"/>
+        <c:axId val="429875480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:title>
           <c:tx>
@@ -3084,8 +3208,11 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:txPr>
           <a:bodyPr/>
@@ -3097,7 +3224,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="472110536"/>
+        <c:crossAx val="429872392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3121,6 +3248,7 @@
           <c:h val="0.241094286291137"/>
         </c:manualLayout>
       </c:layout>
+      <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
         <a:lstStyle/>
@@ -3134,6 +3262,7 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:ln>
@@ -3152,8 +3281,17 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="1"/>
   <c:lang val="en-US"/>
-  <c:style val="2"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout>
         <c:manualLayout>
@@ -3169,6 +3307,7 @@
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -3183,6 +3322,7 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
               <c:f>Sheet1!$E$142:$E$144</c:f>
@@ -3234,6 +3374,7 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
               <c:f>Sheet1!$E$142:$E$144</c:f>
@@ -3285,6 +3426,7 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
               <c:f>Sheet1!$E$142:$E$144</c:f>
@@ -3336,6 +3478,7 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
               <c:f>Sheet1!$E$142:$E$144</c:f>
@@ -3387,6 +3530,7 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
               <c:f>Sheet1!$E$142:$E$144</c:f>
@@ -3438,6 +3582,7 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
               <c:f>Sheet1!$E$142:$E$144</c:f>
@@ -3458,22 +3603,41 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$K$142:$K$144</c:f>
+              <c:f>Sheet1!$J$159:$J$161</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>692.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1296.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2378.0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="494041704"/>
-        <c:axId val="494692424"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="467059544"/>
+        <c:axId val="467065224"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="494041704"/>
+        <c:axId val="467059544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -3492,8 +3656,11 @@
             </c:rich>
           </c:tx>
           <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:txPr>
           <a:bodyPr/>
@@ -3505,17 +3672,19 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="494692424"/>
+        <c:crossAx val="467065224"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="494692424"/>
+        <c:axId val="467065224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:title>
           <c:tx>
@@ -3534,8 +3703,11 @@
             </c:rich>
           </c:tx>
           <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:txPr>
           <a:bodyPr/>
@@ -3547,11 +3719,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="494041704"/>
+        <c:crossAx val="467059544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:spPr>
+        <a:noFill/>
         <a:ln>
           <a:solidFill>
             <a:schemeClr val="bg1">
@@ -3569,10 +3742,11 @@
           <c:yMode val="edge"/>
           <c:x val="0.157538676943551"/>
           <c:y val="0.0536952733849445"/>
-          <c:w val="0.286364090052124"/>
-          <c:h val="0.38511215509826"/>
+          <c:w val="0.290523178440723"/>
+          <c:h val="0.418725600476411"/>
         </c:manualLayout>
       </c:layout>
+      <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
         <a:lstStyle/>
@@ -3585,6 +3759,8 @@
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -3598,7 +3774,15 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="1"/>
   <c:lang val="en-US"/>
-  <c:style val="18"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -3617,12 +3801,15 @@
         </c:rich>
       </c:tx>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -3637,6 +3824,7 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
               <c:f>Sheet1!$I$159:$I$161</c:f>
@@ -3688,6 +3876,7 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
               <c:f>Sheet1!$I$159:$I$161</c:f>
@@ -3725,14 +3914,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="497292232"/>
-        <c:axId val="508893288"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="428877688"/>
+        <c:axId val="467183480"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="497292232"/>
+        <c:axId val="428877688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -3751,20 +3950,25 @@
             </c:rich>
           </c:tx>
           <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="508893288"/>
+        <c:crossAx val="467183480"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="508893288"/>
+        <c:axId val="467183480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:title>
           <c:tx>
@@ -3783,10 +3987,13 @@
             </c:rich>
           </c:tx>
           <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="497292232"/>
+        <c:crossAx val="428877688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3794,8 +4001,11 @@
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -3809,7 +4019,15 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="1"/>
   <c:lang val="en-US"/>
-  <c:style val="18"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -3828,12 +4046,15 @@
         </c:rich>
       </c:tx>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -3848,6 +4069,7 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
               <c:f>Sheet1!$I$169:$I$171</c:f>
@@ -3899,6 +4121,7 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
               <c:f>Sheet1!$I$169:$I$171</c:f>
@@ -3950,6 +4173,7 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
               <c:f>Sheet1!$I$169:$I$171</c:f>
@@ -3987,14 +4211,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="505079752"/>
-        <c:axId val="520517064"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="429152936"/>
+        <c:axId val="429138792"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="505079752"/>
+        <c:axId val="429152936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -4013,20 +4247,25 @@
             </c:rich>
           </c:tx>
           <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="520517064"/>
+        <c:crossAx val="429138792"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="520517064"/>
+        <c:axId val="429138792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:title>
           <c:tx>
@@ -4045,10 +4284,13 @@
             </c:rich>
           </c:tx>
           <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="505079752"/>
+        <c:crossAx val="429152936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4056,8 +4298,11 @@
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -4071,7 +4316,15 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="1"/>
   <c:lang val="en-US"/>
-  <c:style val="2"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -4089,21 +4342,26 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:v>Map Phase time</c:v>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:errBars>
             <c:errBarType val="both"/>
             <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
                 <c:f>'[1]GS Data Analaysis'!$D$51:$D$53</c:f>
@@ -4184,9 +4442,11 @@
           <c:tx>
             <c:v>Reduce phase time</c:v>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:errBars>
             <c:errBarType val="both"/>
             <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
                 <c:f>'[1]GS Data Analaysis'!$F$51:$F$53</c:f>
@@ -4261,15 +4521,25 @@
             </c:numRef>
           </c:val>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="515563960"/>
-        <c:axId val="498741224"/>
+        <c:axId val="399992744"/>
+        <c:axId val="399973624"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="515563960"/>
+        <c:axId val="399992744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -4287,20 +4557,25 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="498741224"/>
+        <c:crossAx val="399973624"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="498741224"/>
+        <c:axId val="399973624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:title>
@@ -4319,19 +4594,24 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="515563960"/>
+        <c:crossAx val="399992744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -4345,7 +4625,15 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="1"/>
   <c:lang val="en-US"/>
-  <c:style val="18"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -4363,21 +4651,26 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:v>chunk time</c:v>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:errBars>
             <c:errBarType val="both"/>
             <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
                 <c:f>'[1]GS Data Analaysis'!$E$81:$E$83</c:f>
@@ -4458,9 +4751,11 @@
           <c:tx>
             <c:v>Map phase time</c:v>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:errBars>
             <c:errBarType val="both"/>
             <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
                 <c:f>'[1]GS Data Analaysis'!$G$81:$G$83</c:f>
@@ -4541,9 +4836,11 @@
           <c:tx>
             <c:v>Reduce phase time</c:v>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:errBars>
             <c:errBarType val="both"/>
             <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
                 <c:f>'[1]GS Data Analaysis'!$I$81:$I$83</c:f>
@@ -4618,15 +4915,25 @@
             </c:numRef>
           </c:val>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="500538136"/>
-        <c:axId val="472670648"/>
+        <c:axId val="467477240"/>
+        <c:axId val="428998488"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="500538136"/>
+        <c:axId val="467477240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -4644,20 +4951,25 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="472670648"/>
+        <c:crossAx val="428998488"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="472670648"/>
+        <c:axId val="428998488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:title>
@@ -4676,19 +4988,24 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="500538136"/>
+        <c:crossAx val="467477240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -4702,7 +5019,15 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="1"/>
   <c:lang val="en-US"/>
-  <c:style val="18"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -4720,21 +5045,26 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:v>Map Phase time</c:v>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:errBars>
             <c:errBarType val="both"/>
             <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
                 <c:f>'[1]GS Data Analaysis'!$F$5:$F$8</c:f>
@@ -4827,9 +5157,11 @@
           <c:tx>
             <c:v>Reduce phase time</c:v>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:errBars>
             <c:errBarType val="both"/>
             <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
                 <c:f>'[1]GS Data Analaysis'!$H$5:$H$8</c:f>
@@ -4916,15 +5248,25 @@
             </c:numRef>
           </c:val>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="501154392"/>
-        <c:axId val="483345176"/>
+        <c:axId val="467394152"/>
+        <c:axId val="467399624"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="501154392"/>
+        <c:axId val="467394152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -4942,20 +5284,25 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="483345176"/>
+        <c:crossAx val="467399624"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="483345176"/>
+        <c:axId val="467399624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:title>
@@ -4974,19 +5321,24 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="501154392"/>
+        <c:crossAx val="467394152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -5000,7 +5352,15 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="1"/>
   <c:lang val="en-US"/>
-  <c:style val="2"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:autoTitleDeleted val="1"/>
     <c:plotArea>
@@ -5018,15 +5378,18 @@
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:v>Map</c:v>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:errBars>
             <c:errBarType val="both"/>
             <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
                 <c:f>'[1]GS Data Analaysis'!$D$51:$D$53</c:f>
@@ -5107,9 +5470,11 @@
           <c:tx>
             <c:v>Reduce</c:v>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:errBars>
             <c:errBarType val="both"/>
             <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
                 <c:f>'[1]GS Data Analaysis'!$F$51:$F$53</c:f>
@@ -5184,15 +5549,25 @@
             </c:numRef>
           </c:val>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="494730680"/>
-        <c:axId val="515036056"/>
+        <c:axId val="467438680"/>
+        <c:axId val="467444184"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="494730680"/>
+        <c:axId val="467438680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -5210,8 +5585,11 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:txPr>
           <a:bodyPr/>
@@ -5223,17 +5601,19 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="515036056"/>
+        <c:crossAx val="467444184"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="515036056"/>
+        <c:axId val="467444184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:title>
           <c:tx>
@@ -5251,8 +5631,11 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:txPr>
           <a:bodyPr/>
@@ -5264,7 +5647,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="494730680"/>
+        <c:crossAx val="467438680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5288,6 +5671,7 @@
           <c:h val="0.157242725094146"/>
         </c:manualLayout>
       </c:layout>
+      <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
         <a:lstStyle/>
@@ -5301,6 +5685,7 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:ln>
@@ -5319,7 +5704,15 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="1"/>
   <c:lang val="en-US"/>
-  <c:style val="18"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:autoTitleDeleted val="1"/>
     <c:plotArea>
@@ -5337,15 +5730,18 @@
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:v>Chunk</c:v>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:errBars>
             <c:errBarType val="both"/>
             <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
                 <c:f>'[1]GS Data Analaysis'!$E$81:$E$83</c:f>
@@ -5426,9 +5822,11 @@
           <c:tx>
             <c:v>Map</c:v>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:errBars>
             <c:errBarType val="both"/>
             <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
                 <c:f>'[1]GS Data Analaysis'!$G$81:$G$83</c:f>
@@ -5509,9 +5907,11 @@
           <c:tx>
             <c:v>Reduce</c:v>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:errBars>
             <c:errBarType val="both"/>
             <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
                 <c:f>'[1]GS Data Analaysis'!$I$81:$I$83</c:f>
@@ -5586,15 +5986,25 @@
             </c:numRef>
           </c:val>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="494156504"/>
-        <c:axId val="494162616"/>
+        <c:axId val="400281528"/>
+        <c:axId val="400429848"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="494156504"/>
+        <c:axId val="400281528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -5620,8 +6030,11 @@
               <c:y val="0.869026548672566"/>
             </c:manualLayout>
           </c:layout>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:ln w="19050"/>
@@ -5636,17 +6049,19 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="494162616"/>
+        <c:crossAx val="400429848"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="494162616"/>
+        <c:axId val="400429848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:title>
           <c:tx>
@@ -5664,8 +6079,11 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:txPr>
           <a:bodyPr/>
@@ -5677,7 +6095,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="494156504"/>
+        <c:crossAx val="400281528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5701,6 +6119,7 @@
           <c:h val="0.142693540519824"/>
         </c:manualLayout>
       </c:layout>
+      <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
         <a:lstStyle/>
@@ -5714,6 +6133,7 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:ln>
@@ -5732,7 +6152,15 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="1"/>
   <c:lang val="en-US"/>
-  <c:style val="2"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -5750,7 +6178,9 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout>
         <c:manualLayout>
@@ -5765,6 +6195,7 @@
       </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -5829,14 +6260,23 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="497511832"/>
-        <c:axId val="494520888"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="400108024"/>
+        <c:axId val="400349720"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="497511832"/>
+        <c:axId val="400108024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -5854,18 +6294,22 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="494520888"/>
+        <c:crossAx val="400349720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="494520888"/>
+        <c:axId val="400349720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:title>
@@ -5884,19 +6328,24 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="497511832"/>
+        <c:crossAx val="400108024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -5910,12 +6359,22 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="1"/>
   <c:lang val="en-US"/>
-  <c:style val="2"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -5968,41 +6427,58 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
+          <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="494203880"/>
-        <c:axId val="494206920"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="424847000"/>
+        <c:axId val="424849960"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="494203880"/>
+        <c:axId val="424847000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="494206920"/>
+        <c:crossAx val="424849960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="494206920"/>
+        <c:axId val="424849960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="494203880"/>
+        <c:crossAx val="424847000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -6016,12 +6492,22 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="1"/>
   <c:lang val="en-US"/>
-  <c:style val="2"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -6074,41 +6560,58 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
+          <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="494233544"/>
-        <c:axId val="494236584"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="424876440"/>
+        <c:axId val="424879400"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="494233544"/>
+        <c:axId val="424876440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="494236584"/>
+        <c:crossAx val="424879400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="494236584"/>
+        <c:axId val="424879400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="494233544"/>
+        <c:crossAx val="424876440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -6553,15 +7056,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>469900</xdr:colOff>
-      <xdr:row>142</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
+      <xdr:colOff>393700</xdr:colOff>
+      <xdr:row>144</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>393700</xdr:colOff>
-      <xdr:row>164</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:colOff>317500</xdr:colOff>
+      <xdr:row>166</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -7196,15 +7699,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <sheetPr published="0" enableFormatConditionsCalculation="0"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y158"/>
   <sheetViews>
     <sheetView topLeftCell="A190" workbookViewId="0">
       <selection activeCell="H6" sqref="H6:J6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:14" ht="15">
       <c r="A1" s="1"/>
@@ -7977,7 +8479,7 @@
       </c>
       <c r="L25">
         <f>STDEV(E25,G25,I25)/SQRT(3)</f>
-        <v>0.95113318365910415</v>
+        <v>0.95113318380418077</v>
       </c>
       <c r="M25">
         <f>AVERAGE(F25,H25,J25)</f>
@@ -7985,7 +8487,7 @@
       </c>
       <c r="N25">
         <f>STDEV(F25,H25,J25)/SQRT(3)</f>
-        <v>3.8921515186908215</v>
+        <v>3.8921515186904561</v>
       </c>
     </row>
     <row r="26" spans="1:19">
@@ -8025,7 +8527,7 @@
       </c>
       <c r="L26">
         <f>STDEV(E26,G26,I26)/SQRT(3)</f>
-        <v>25.902892328855973</v>
+        <v>25.902892328850076</v>
       </c>
       <c r="M26">
         <f>AVERAGE(F26,H26,J26)</f>
@@ -8033,7 +8535,7 @@
       </c>
       <c r="N26">
         <f>STDEV(F26,H26,J26)/SQRT(3)</f>
-        <v>1.2000589337377248</v>
+        <v>1.2000589337380267</v>
       </c>
     </row>
     <row r="27" spans="1:19">
@@ -8073,7 +8575,7 @@
       </c>
       <c r="L27">
         <f>STDEV(E27,G27,I27)/SQRT(3)</f>
-        <v>15.299896648162512</v>
+        <v>15.299896648162221</v>
       </c>
       <c r="M27">
         <f>AVERAGE(F27,H27,J27)</f>
@@ -8081,7 +8583,7 @@
       </c>
       <c r="N27">
         <f>STDEV(F27,H27,J27)/SQRT(3)</f>
-        <v>2.2325377438638392</v>
+        <v>2.2325377438640941</v>
       </c>
     </row>
     <row r="28" spans="1:19">
@@ -8121,7 +8623,7 @@
       </c>
       <c r="L28">
         <f>STDEV(E28,G28,I28)/SQRT(3)</f>
-        <v>19.678437700520611</v>
+        <v>19.678437700522181</v>
       </c>
       <c r="M28">
         <f>AVERAGE(F28,H28,J28)</f>
@@ -8129,7 +8631,7 @@
       </c>
       <c r="N28">
         <f>STDEV(F28,H28,J28)/SQRT(3)</f>
-        <v>2.6636263501721773</v>
+        <v>2.6636263501725166</v>
       </c>
     </row>
     <row r="31" spans="1:19">
@@ -8927,7 +9429,7 @@
       </c>
       <c r="G88">
         <f>STDEV(C88,D88,E88)/SQRT(3)</f>
-        <v>44.339394594427489</v>
+        <v>44.33939459442368</v>
       </c>
       <c r="H88">
         <v>128.80500000000001</v>
@@ -8944,7 +9446,7 @@
       </c>
       <c r="L88">
         <f>STDEV(H88,I88,J88)/SQRT(3)</f>
-        <v>7.5428862071049236</v>
+        <v>7.5428862071048961</v>
       </c>
     </row>
     <row r="89" spans="1:12">
@@ -8970,7 +9472,7 @@
       </c>
       <c r="G89">
         <f>STDEV(C89,D89,E89)/SQRT(3)</f>
-        <v>58.385792408006402</v>
+        <v>58.385792408008861</v>
       </c>
       <c r="H89">
         <v>140.238</v>
@@ -8987,7 +9489,7 @@
       </c>
       <c r="L89">
         <f>STDEV(H89,I89,J89)/SQRT(3)</f>
-        <v>4.1344438965032166</v>
+        <v>4.1344438965032886</v>
       </c>
     </row>
     <row r="90" spans="1:12">
@@ -9013,7 +9515,7 @@
       </c>
       <c r="G90">
         <f>STDEV(C90,D90,E90)/SQRT(3)</f>
-        <v>19.678437700520611</v>
+        <v>19.678437700522181</v>
       </c>
       <c r="H90">
         <v>136.01</v>
@@ -9030,7 +9532,7 @@
       </c>
       <c r="L90">
         <f>STDEV(H90,I90,J90)/SQRT(3)</f>
-        <v>2.6636263501721773</v>
+        <v>2.6636263501725166</v>
       </c>
     </row>
     <row r="94" spans="1:12">
@@ -9270,7 +9772,7 @@
       </c>
       <c r="Q122">
         <f>STDEV(O122:O123)</f>
-        <v>1.0748023074035887E-2</v>
+        <v>1.0748023074035516E-2</v>
       </c>
     </row>
     <row r="123" spans="1:17">
@@ -9822,7 +10324,7 @@
       </c>
       <c r="G148">
         <f>STDEV(C148,D148,E148)/SQRT(3)</f>
-        <v>1.7540000000002831</v>
+        <v>1.7540000000000004</v>
       </c>
       <c r="H148">
         <v>1209.1849999999999</v>
@@ -9839,7 +10341,7 @@
       </c>
       <c r="L148">
         <f>STDEV(H148,I148,J148)/SQRT(3)</f>
-        <v>19.678437700520611</v>
+        <v>19.678437700522181</v>
       </c>
       <c r="M148">
         <v>136.01</v>
@@ -9856,7 +10358,7 @@
       </c>
       <c r="Q148">
         <f>STDEV(M148,N148,O148)/SQRT(3)</f>
-        <v>2.6636263501721773</v>
+        <v>2.6636263501725166</v>
       </c>
     </row>
     <row r="149" spans="1:17">
@@ -9875,7 +10377,7 @@
       </c>
       <c r="G149">
         <f>STDEV(C149,D149,E149)/SQRT(3)</f>
-        <v>3.5763333333362866</v>
+        <v>3.5763333333333285</v>
       </c>
       <c r="H149">
         <v>2187.7220000000002</v>
@@ -9892,7 +10394,7 @@
       </c>
       <c r="L149">
         <f>STDEV(H149,I149,J149)/SQRT(3)</f>
-        <v>13.902016196695632</v>
+        <v>13.902016196700965</v>
       </c>
       <c r="M149">
         <v>323.47300000000001</v>
@@ -9909,7 +10411,7 @@
       </c>
       <c r="Q149">
         <f>STDEV(M149,N149,O149)/SQRT(3)</f>
-        <v>10.873797593807824</v>
+        <v>10.8737975938083</v>
       </c>
     </row>
     <row r="150" spans="1:17">
@@ -9928,7 +10430,7 @@
       </c>
       <c r="G150">
         <f>STDEV(C150,D150,E150)/SQRT(3)</f>
-        <v>24.97066666666846</v>
+        <v>24.970666666666681</v>
       </c>
       <c r="H150">
         <v>4227.183</v>
@@ -9945,7 +10447,7 @@
       </c>
       <c r="L150">
         <f>STDEV(H150,I150,J150)/SQRT(3)</f>
-        <v>67.344362268343815</v>
+        <v>67.344362268369153</v>
       </c>
       <c r="M150">
         <v>673.399</v>
@@ -9962,7 +10464,7 @@
       </c>
       <c r="Q150">
         <f>STDEV(M150,N150,O150)/SQRT(3)</f>
-        <v>5.7530535177223436</v>
+        <v>5.7530535177223614</v>
       </c>
     </row>
     <row r="153" spans="1:17">
@@ -10094,7 +10596,7 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
@@ -10102,15 +10604,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <sheetPr published="0" enableFormatConditionsCalculation="0"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:I85"/>
   <sheetViews>
     <sheetView topLeftCell="A85" workbookViewId="0">
       <selection activeCell="F78" sqref="F78"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
@@ -10562,12 +11063,11 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
@@ -10575,15 +11075,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <sheetPr published="0" enableFormatConditionsCalculation="0"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:Z178"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A111" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E122" workbookViewId="0">
       <selection activeCell="E184" sqref="E184"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="2" spans="1:24">
       <c r="A2" s="15" t="s">
@@ -10691,7 +11190,7 @@
       </c>
       <c r="N5">
         <f>1.96 * STDEV(E5,H5,K5)/SQRT(3)</f>
-        <v>18.293333333355065</v>
+        <v>18.293333333333337</v>
       </c>
       <c r="O5">
         <f>L5/13</f>
@@ -10744,7 +11243,7 @@
       </c>
       <c r="N6">
         <f t="shared" ref="N6:N7" si="1">1.96 * STDEV(E6,H6,K6)/SQRT(3)</f>
-        <v>114.09789091439987</v>
+        <v>114.09789091438593</v>
       </c>
     </row>
     <row r="7" spans="1:24">
@@ -10793,7 +11292,7 @@
       </c>
       <c r="N7">
         <f t="shared" si="1"/>
-        <v>118.91205116011055</v>
+        <v>118.91205116013731</v>
       </c>
     </row>
     <row r="9" spans="1:24">
@@ -10987,7 +11486,7 @@
       </c>
       <c r="X13">
         <f>1.96*STDEV(V13:V15)/SQRT(3)</f>
-        <v>90.643966766199668</v>
+        <v>90.643966766195263</v>
       </c>
     </row>
     <row r="14" spans="1:24">
@@ -11107,7 +11606,7 @@
       </c>
       <c r="X17">
         <f>1.96*STDEV(V17:V19)/SQRT(3)</f>
-        <v>99.177635471794702</v>
+        <v>99.177635471802702</v>
       </c>
     </row>
     <row r="18" spans="1:24">
@@ -11207,7 +11706,7 @@
       </c>
       <c r="X21">
         <f>1.96*STDEV(V21:V23)/SQRT(3)</f>
-        <v>48.174196873825352</v>
+        <v>48.174196873891361</v>
       </c>
     </row>
     <row r="22" spans="1:24">
@@ -11363,7 +11862,7 @@
       </c>
       <c r="Q27">
         <f>1.96 * STDEV(E27,I27,M27)/SQRT(3)</f>
-        <v>4.097169079209209</v>
+        <v>4.0971690793194897</v>
       </c>
       <c r="R27">
         <f>P27+I34</f>
@@ -11419,7 +11918,7 @@
       </c>
       <c r="Q28">
         <f t="shared" ref="Q28:Q29" si="7">1.96 * STDEV(E28,I28,M28)/SQRT(3)</f>
-        <v>30.100037057320566</v>
+        <v>30.100037057362055</v>
       </c>
       <c r="R28">
         <f>P28+J34</f>
@@ -11475,7 +11974,7 @@
       </c>
       <c r="Q29">
         <f t="shared" si="7"/>
-        <v>10.540389098093113</v>
+        <v>10.540389097696695</v>
       </c>
       <c r="R29">
         <f>P29+K34</f>
@@ -11525,7 +12024,7 @@
       </c>
       <c r="E35">
         <f>1.96*(STDEV(C27,G27,K27)/SQRT(3))</f>
-        <v>4.2397511311659413</v>
+        <v>4.2397511312076928</v>
       </c>
       <c r="K35">
         <f>4096/11.2</f>
@@ -11542,7 +12041,7 @@
       </c>
       <c r="E36">
         <f t="shared" ref="E36:E37" si="9">1.96*(STDEV(C28,G28,K28)/SQRT(3))</f>
-        <v>27.301347690011074</v>
+        <v>27.301347690016893</v>
       </c>
       <c r="K36">
         <f>4096/11.6</f>
@@ -11559,7 +12058,7 @@
       </c>
       <c r="E37">
         <f t="shared" si="9"/>
-        <v>11.312186388587316</v>
+        <v>11.312186388288527</v>
       </c>
     </row>
     <row r="41" spans="3:17">
@@ -11663,7 +12162,7 @@
       </c>
       <c r="I57">
         <f>1.96*(STDEV(G57:G59)/SQRT(3))</f>
-        <v>12.103286987068245</v>
+        <v>12.103286987150657</v>
       </c>
       <c r="K57" t="s">
         <v>93</v>
@@ -11755,7 +12254,7 @@
       </c>
       <c r="I61">
         <f>1.96*(STDEV(G61:G63)/SQRT(3))</f>
-        <v>19.032393616609415</v>
+        <v>19.032393616362871</v>
       </c>
       <c r="K61" t="s">
         <v>95</v>
@@ -11836,7 +12335,7 @@
       </c>
       <c r="I66">
         <f>1.96*(STDEV(G66:G68)/SQRT(3))</f>
-        <v>24.167021097560671</v>
+        <v>24.16702109730387</v>
       </c>
       <c r="K66" t="s">
         <v>94</v>
@@ -11903,7 +12402,7 @@
       </c>
       <c r="F71">
         <f>1.96*(STDEV(D57:D59)/SQRT(3))</f>
-        <v>13.340925888849769</v>
+        <v>13.340925888907885</v>
       </c>
       <c r="K71" t="s">
         <v>210</v>
@@ -11958,7 +12457,7 @@
       </c>
       <c r="F72">
         <f t="shared" ref="F72:F73" si="12">1.96*(STDEV(D58:D60)/SQRT(3))</f>
-        <v>8.4817664826547219</v>
+        <v>8.4817664826773278</v>
       </c>
       <c r="J72" t="s">
         <v>209</v>
@@ -12498,7 +12997,7 @@
       </c>
       <c r="G116">
         <f>1.96*STDEV(E116:E118)/SQRT(3)</f>
-        <v>13.935673511291871</v>
+        <v>13.935673511292233</v>
       </c>
       <c r="K116" t="s">
         <v>183</v>
@@ -12523,7 +13022,7 @@
       </c>
       <c r="Q116">
         <f>1.96*STDEV(O116:O118)/SQRT(3)</f>
-        <v>1.6668740844330987</v>
+        <v>1.6668740844267127</v>
       </c>
     </row>
     <row r="117" spans="1:17">
@@ -12604,7 +13103,7 @@
       </c>
       <c r="G121">
         <f>1.96*STDEV(E121:E123)/SQRT(3)</f>
-        <v>7.8781625077026014</v>
+        <v>7.8781625077030064</v>
       </c>
       <c r="K121" t="s">
         <v>184</v>
@@ -12629,7 +13128,7 @@
       </c>
       <c r="Q121">
         <f>1.96*STDEV(O121:O123)/SQRT(3)</f>
-        <v>7.3775567566892803</v>
+        <v>7.3775567566626359</v>
       </c>
     </row>
     <row r="122" spans="1:17">
@@ -12710,7 +13209,7 @@
       </c>
       <c r="G126">
         <f>1.96*STDEV(E126:E128)/SQRT(3)</f>
-        <v>4.6431871871022583</v>
+        <v>4.6431871869798229</v>
       </c>
       <c r="K126" t="s">
         <v>185</v>
@@ -12735,7 +13234,7 @@
       </c>
       <c r="Q126">
         <f>1.96*STDEV(O126:O128)/SQRT(3)</f>
-        <v>5.9110665054272307</v>
+        <v>5.911066505387117</v>
       </c>
     </row>
     <row r="127" spans="1:17">
@@ -13303,7 +13802,7 @@
     <row r="168" spans="1:14" ht="26">
       <c r="A168" s="35"/>
       <c r="B168" s="29">
-        <f t="shared" ref="B168:C169" si="19">HOUR(B155)*3600+MINUTE(B155)*60+SECOND(B155)</f>
+        <f t="shared" ref="B168:C168" si="19">HOUR(B155)*3600+MINUTE(B155)*60+SECOND(B155)</f>
         <v>678</v>
       </c>
       <c r="C168" s="30">
@@ -13352,7 +13851,7 @@
     <row r="170" spans="1:14">
       <c r="A170" s="36"/>
       <c r="B170" s="31">
-        <f t="shared" ref="B170:C178" si="21">HOUR(B157)*3600+MINUTE(B157)*60+SECOND(B157)</f>
+        <f t="shared" ref="B170:C170" si="21">HOUR(B157)*3600+MINUTE(B157)*60+SECOND(B157)</f>
         <v>692</v>
       </c>
       <c r="C170" s="32">
@@ -13365,7 +13864,7 @@
       </c>
       <c r="E170" s="26">
         <f>1.96*STDEV(C167:C169)/SQRT(3)</f>
-        <v>50.306666666698277</v>
+        <v>50.306666666666665</v>
       </c>
       <c r="I170" s="44">
         <v>4</v>
@@ -13426,7 +13925,7 @@
     <row r="173" spans="1:14">
       <c r="A173" s="35"/>
       <c r="B173" s="29">
-        <f t="shared" ref="B173:C178" si="26">HOUR(B160)*3600+MINUTE(B160)*60+SECOND(B160)</f>
+        <f t="shared" ref="B173:C173" si="26">HOUR(B160)*3600+MINUTE(B160)*60+SECOND(B160)</f>
         <v>1490</v>
       </c>
       <c r="C173" s="30">
@@ -13446,12 +13945,12 @@
         <v>6395</v>
       </c>
       <c r="D174" s="26">
-        <f t="shared" ref="D174:D178" si="28">1.96*STDEV(B171:B173)/SQRT(3)</f>
+        <f t="shared" ref="D174" si="28">1.96*STDEV(B171:B173)/SQRT(3)</f>
         <v>196.65333333333385</v>
       </c>
       <c r="E174" s="26">
-        <f t="shared" ref="E174:E178" si="29">1.96*STDEV(C171:C173)/SQRT(3)</f>
-        <v>57.0349148427022</v>
+        <f t="shared" ref="E174" si="29">1.96*STDEV(C171:C173)/SQRT(3)</f>
+        <v>57.034914842674318</v>
       </c>
     </row>
     <row r="175" spans="1:14">
@@ -13470,7 +13969,7 @@
     <row r="176" spans="1:14">
       <c r="A176" s="35"/>
       <c r="B176" s="29">
-        <f t="shared" ref="B176:C178" si="31">HOUR(B163)*3600+MINUTE(B163)*60+SECOND(B163)</f>
+        <f t="shared" ref="B176:C176" si="31">HOUR(B163)*3600+MINUTE(B163)*60+SECOND(B163)</f>
         <v>2327</v>
       </c>
       <c r="C176" s="30">
@@ -13502,21 +14001,20 @@
       </c>
       <c r="D178" s="26">
         <f t="shared" ref="D178:E178" si="34">1.96*STDEV(B175:B177)/SQRT(3)</f>
-        <v>129.82113096274134</v>
+        <v>129.82113096273829</v>
       </c>
       <c r="E178" s="26">
         <f t="shared" si="34"/>
-        <v>26.54656621432266</v>
+        <v>26.546566214442457</v>
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>

</xml_diff>

<commit_message>
rumtime comparison w/ changing total number of workers
git-svn-id: file://localhost/tmp/svn2git/svn@6785 defb5e50-622e-49ec-a68e-d72c7db87b45
</commit_message>
<xml_diff>
--- a/papers/saga-mr-ngs/data/GS_data.xlsx
+++ b/papers/saga-mr-ngs/data/GS_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3880" yWindow="3960" windowWidth="31800" windowHeight="18600" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="1160" yWindow="1760" windowWidth="31800" windowHeight="18600" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="GS data" sheetId="1" r:id="rId1"/>
@@ -4252,10 +4252,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
+                  <c:v>4622.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>2327.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4622.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -10867,6 +10867,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>
@@ -10884,7 +10885,7 @@
   <dimension ref="A2:Z204"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A159" workbookViewId="0">
-      <selection activeCell="L202" sqref="L202"/>
+      <selection activeCell="K201" sqref="K201"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -13980,14 +13981,14 @@
         <v>4</v>
       </c>
       <c r="L190" s="49">
-        <f>G191</f>
-        <v>2327</v>
+        <f>G192</f>
+        <v>4622</v>
       </c>
       <c r="M190" s="49"/>
     </row>
     <row r="191" spans="1:15">
       <c r="A191">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B191" s="17">
         <v>0.28195601851851854</v>
@@ -14019,14 +14020,14 @@
         <v>8</v>
       </c>
       <c r="L191" s="49">
-        <f>G192</f>
-        <v>4622</v>
+        <f>G191</f>
+        <v>2327</v>
       </c>
       <c r="M191" s="49"/>
     </row>
     <row r="192" spans="1:15">
       <c r="A192">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B192" s="17">
         <v>0.9258912037037037</v>

</xml_diff>

<commit_message>
updates done mostly with section-3
git-svn-id: file://localhost/tmp/svn2git/svn@6865 defb5e50-622e-49ec-a68e-d72c7db87b45
</commit_message>
<xml_diff>
--- a/papers/saga-mr-ngs/data/GS_data.xlsx
+++ b/papers/saga-mr-ngs/data/GS_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="-20" windowWidth="21600" windowHeight="14120" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="36920" yWindow="-8220" windowWidth="21600" windowHeight="14120" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="GS data" sheetId="1" r:id="rId1"/>
@@ -10844,7 +10844,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>
@@ -10860,7 +10859,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A3:K85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A90" workbookViewId="0">
+    <sheetView topLeftCell="D52" workbookViewId="0">
       <selection activeCell="G71" sqref="G71"/>
     </sheetView>
   </sheetViews>
@@ -11340,6 +11339,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -11356,8 +11356,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A2:Z238"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="P235" sqref="P235"/>
+    <sheetView tabSelected="1" topLeftCell="F203" workbookViewId="0">
+      <selection activeCell="O241" sqref="O241"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>

</xml_diff>